<commit_message>
ready for rewriting the main paper
</commit_message>
<xml_diff>
--- a/CML_prob.xlsx
+++ b/CML_prob.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,44 +543,44 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>logistic_regression</t>
+          <t>logistic regression</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7433198380566801</v>
+        <v>0.7417004048582996</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7425343018563357</v>
+        <v>0.7386091127098321</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7449392712550608</v>
+        <v>0.7481781376518218</v>
       </c>
       <c r="F2" t="n">
+        <v>0.7352226720647773</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.743362831858407</v>
+      </c>
+      <c r="H2" t="n">
         <v>0.7417004048582996</v>
       </c>
-      <c r="G2" t="n">
-        <v>0.7437348423605497</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.7433198380566801</v>
-      </c>
       <c r="I2" t="n">
-        <v>0.7322064056939501</v>
+        <v>0.7313167259786477</v>
       </c>
       <c r="J2" t="n">
-        <v>0.7261698440207972</v>
+        <v>0.7256944444444444</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7455516014234875</v>
+        <v>0.7437722419928826</v>
       </c>
       <c r="L2" t="n">
         <v>0.7188612099644128</v>
       </c>
       <c r="M2" t="n">
-        <v>0.7357330992098332</v>
+        <v>0.7346221441124779</v>
       </c>
       <c r="N2" t="n">
-        <v>0.7433198380566801</v>
+        <v>0.7313167259786477</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -589,7 +589,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>[1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+          <t>[1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -599,17 +599,17 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>[1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0]</t>
+          <t>[1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>[0.877546304764949, 0.05851705021219207, 0.3446443491478341, 0.45863521142754216, 0.4549470092861245, 0.9730971615918019, 0.7089465684222105, 0.36353652675625314, 0.2997495972247737, 0.87283286753496, 0.8040881491835951, 0.6923889040859931, 0.6371418372366413, 0.6072009677378271, 0.9536914082574661, 0.3016892542701188, 0.7490560003537088, 0.7971905129252401, 0.7471037684246807, 0.30717262415268526, 0.9045101529287418, 0.7990717101336955, 0.7549739076623734, 0.12053765216899259, 0.40490801541707017, 0.016689808831731674, 0.9529300085602261, 0.6287260697910386, 0.7279800616709476, 0.2710806128491044, 0.7111148784768294, 0.09265590017820659, 0.5053417456174573, 0.8510201616667413, 0.8150516029778497, 0.8546961282707163, 0.4671552773984634, 0.4299353428021231, 0.6556116786247076, 0.6548563517167182, 0.579026677716633, 0.6924712252030546, 0.03624026565389024, 0.4136000799962244, 0.8386742316810593, 0.015252186157927974, 0.9190199543174228, 0.8866387122862669, 0.02330913285655244, 0.7961894129436756, 0.8644724780769878, 0.9485529436217203, 0.4888031402867006, 0.9603209628667506, 0.6294466630151654, 0.5896138497824848, 0.3250401682567881, 0.9756853671780789, 0.8663836506107796, 0.6935534015893164, 0.48505887242261353, 0.6295904633993292, 0.2004367759412461, 0.5130930729624232, 0.8787744280932103, 0.0656019381782799, 0.5136730382542308, 0.7828164372228797, 0.4705444420065616, 0.7294240677505424, 0.5897116328266027, 0.7159081180255588, 0.8728754146455627, 0.9882590573406385, 0.8904542470917668, 0.7157074768398125, 0.9535178241938859, 0.9047592113382414, 0.9242371639978934, 0.2719242655768378, 0.7194810684200585, 0.5056773941420211, 0.9789128168911687, 0.7217973314453051, 0.8383529619461364, 0.6159409471964632, 0.7193572994078823, 0.8240210747293368, 0.5057650252607974, 0.5281539775592644, 0.9866133224360812, 0.015730990364494678, 0.4575450940810278, 0.5175696676050772, 0.44667132599821147, 0.6420633643483515, 0.5019135697914335, 0.24168582976834532, 0.9393250639770254, 0.7818221126808792, 0.6305756030332769, 0.6531358029791767, 0.6004058505239072, 0.5773032476123572, 0.47317857375216343, 0.9129256838392142, 0.21778070687795828, 0.5343977184414171, 0.7278269907165004, 0.670470463480782, 0.06675233876615908, 0.01178572438268505, 0.5491764344023178, 0.9716351824755427, 0.4802845990861253, 0.3161160023746913, 0.8774608823085206, 0.4266624647940935, 0.747892192063044, 0.5656879957250023, 0.4405473014766765, 0.5621195213906228, 0.7383108714544754, 0.59950068173449, 0.4296637077844851, 0.6447703775666767, 0.6017621015735529, 0.45550719787596666, 0.9212636453277864, 0.34631465046894044, 0.5078441265730906, 0.8892578596024684, 0.5499952608199763, 0.43215897177992124, 0.7415202484891945, 0.8148441307237265, 0.3907843613176202, 0.9000149772775315, 0.9810093526309775, 0.4774327498962904, 0.9624661341832955, 0.9169786154330951, 0.8349076305498551, 0.4885830406836242, 0.5491673469410595, 0.7456271817924358, 0.919355874248191, 0.6865266425362155, 0.9030100558557579, 0.12134203271514084, 0.08366438645478223, 0.9882360501777679, 0.06212934294154111, 0.7659091508030262, 0.06993930397310967, 0.9667498842179766, 0.5735413727441022, 0.07570203324774284, 0.43243790682252414, 0.48328848284987064, 0.8470178416764789, 0.43132411572479545, 0.8121484640833948, 0.8911292967481144, 0.24400191022115636, 0.513841462419622, 0.7138931895191998, 0.9962489006731579, 0.6292606487053509, 0.595353912520805, 0.9792565527365084, 0.6224747520511459, 0.5186109095836988, 0.7068377496645959, 0.9193113133232809, 0.5343806237327418, 0.3292452669343151, 0.7294580584976799, 0.7093020374202308, 0.9832745711591587, 0.8220603890224094, 0.39502113631962893, 0.9222756631609003, 0.9172672046385433, 0.11193336350340109, 0.3768771778394016, 0.8720906020670092, 0.6093609640701203, 0.7700395438778728, 0.8487117983594986, 0.8819260876479967, 0.765316859680217, 0.39306064412401726, 0.9654985299024623, 0.27371311288957945, 0.46064410560789587, 0.9303679200630549, 0.5918681531823772, 0.9360977587622357, 0.1245345348238142, 0.9277074706405425, 0.4828878498026712, 0.8923319444470064, 0.7992062713852971, 0.7667609094673573, 0.731923259732805, 0.6139302866101934, 0.763288509879286, 0.15792485281691823, 0.8107802990598036, 0.9112504032691282, 0.23708432967516418, 0.8397793768502861, 0.599122889085892, 0.7353994562193645, 0.9503374985983312, 0.6347871251233556, 0.8015992599483951, 0.9325162045744415, 0.9983446869823812, 0.8478503847219512, 0.2498425188541626, 0.7109756901366632, 0.8920624683806098, 0.3602787063991872, 0.7610525907864937, 0.3947876404068894, 0.6731457585918482, 0.5370664169960558, 0.9357183731862092, 0.6062762604846648, 0.38706222932125217, 0.7545508075649812, 0.9629343944769603, 0.18445162681178973, 0.8797504024353233, 0.2663606440322694, 0.4758430112916275, 0.7977593536811423, 0.6100694883565532, 0.5092577241866287, 0.1276772116134062, 0.36056431963934016, 0.834061129260184, 0.7021747452892677, 0.8674974066451262, 0.18069858272141234, 0.9047592113382414, 0.04723091327006877, 0.11978382585570638, 0.9328641642361046, 0.8625964929050286, 0.8808965760443255, 0.6920489922546874, 0.8858372994163887, 0.22752240766583928, 0.8170029626486638, 0.6960586051870695, 0.5037952885814316, 0.4486209979269096, 0.43292465373657407, 0.09783992557996568, 0.8301100080601506, 0.8130919406228113, 0.5994137331209355, 0.2814448772872763, 0.9164509751532942, 0.25070383790387235, 0.4139833210074489, 0.8097709166867596, 0.6885595850498444, 0.07663978149398673, 0.5190642526590318, 0.05618266658087177, 0.4076421284503023, 0.8020167442707198, 0.9980256785638467, 0.8804171035647435, 0.9886565308964802, 0.5790940402910789, 0.28069985203595826, 0.7523256995606471, 0.933758492443763, 0.8720533392495451, 0.8091802548766008, 0.09262813279278277, 0.8234654741389283, 0.8649626824029559, 0.13239657583835843, 0.05081614991462957, 0.6775810559724206, 0.14779199991792863, 0.8910319709520116, 0.8774511943511646, 0.8706824116106756, 0.8273817337959689, 0.9477197191577028, 0.7342930870841352, 0.4730358562466996, 0.22346753749001355, 0.14194368457720904, 0.8256201260771368, 0.2717234498756487, 0.25233908109735737, 0.6101008763327024, 0.9132762968954462, 0.7192330664412302, 0.7394362417383565, 0.342283173462447, 0.33254745056150325, 0.4998331598057203, 0.04187591263134332, 0.2176146964661014, 0.9636870279512324, 0.9518424485179532, 0.02637120447290766, 0.016430880770641212, 0.6797223104847132, 0.7537955050356497, 0.5225759186370587, 0.7740267386124533, 0.6644065583039478, 0.9637848070096251, 0.8593089616356044, 0.6671466811500375, 0.8389733438901948, 0.9131666604835251, 0.1703990083605776, 0.3362362500934706, 0.8800654388851922, 0.43714840664452814, 0.5865867302847906, 0.567107814977619, 0.8428301349853538, 0.38588117054187965, 0.5075924739364844, 0.9748278924295362, 0.7997549994583345, 0.5929571622964138, 0.3656309711856504, 0.10702807544150517, 0.29890159916948406, 0.6621657373139607, 0.8515747025799878, 0.869498168828245, 0.7967952298395342, 0.8260708166974974, 0.29568355549560943, 0.7053756289537151, 0.9495278284762234, 0.15571930771496872, 0.9828321120657921, 0.7128505686197842, 0.8030993763998268, 0.8499669013582651, 0.940151490091712, 0.8221114367639455, 0.16647535902077154, 0.5988258258488738, 0.8502105739824293, 0.4785318304486327, 0.4159025307734114, 0.6909629234320294, 0.8487679044385713, 0.9332702995176372, 0.31149306505782426, 0.6952818643339626, 0.6488338080030234, 0.28804985079791257, 0.6398188321263696, 0.8744912266255265, 0.9683852138227148, 0.027812172786638622, 0.7482188090689061, 0.9649047945297551, 0.7490040227419646, 0.5899299005638793, 0.5497830742018395, 0.8451347810184571, 0.49533449556848863, 0.6627986332835479, 0.8278115713473844, 0.8111553349945271, 0.06463115611998799, 0.4843338671309439, 0.817911995382224, 0.5080589720911111, 0.3900002462957396, 0.8365638182991412, 0.9052238684919608, 0.928749891831226, 0.19771255851740893, 0.638791934196862, 0.6494797598512198, 0.46214726053139715, 0.9495092035646936, 0.5768269828512966, 0.9484656277699799, 0.1240877913228814, 0.3301920871202918, 0.1382976727494802, 0.5344136924660767, 0.4931627294871943, 0.8752808924791752, 0.4708131334113489, 0.3271202857765858, 0.7011927255863702, 0.3342973159092425, 0.8225171689089481, 0.48152209454483874, 0.5594762306681772, 0.14882685404863455, 0.5059340032181725, 0.7153558403620689, 0.8725040697021055, 0.6348539592211363, 0.5428778794409025, 0.725220287521496, 0.7119265997481442, 0.24084822363312205, 0.2409145254809293, 0.9857996853462978, 0.8021346663115388, 0.7123072753216082, 0.4942237957027726, 0.982462708679555, 0.6486579528054931, 0.5510966204170072, 0.12024358472194996, 0.6424215145582637, 0.669975455334768, 0.8980220815098929, 0.8613846402413706, 0.8075457007459288, 0.6097033974751827, 0.9650961704302191, 0.9161148379559864, 0.920976586420663, 0.6589582004513869, 0.5270006681662556, 0.8458613950530462, 0.8523008485092414, 0.19807175093184656, 0.8550892556463398, 0.8305855967571644, 0.7369272450556581, 0.7743961085587989, 0.8730478324875268, 0.8889218195659954, 0.8042470198186338, 0.9002525014120673, 0.748514831714709, 0.4145007461642177, 0.8233594839969887, 0.98138736330967, 0.22175121343960638, 0.9090338725045869, 0.3613034642152364, 0.839010192062657, 0.40769979232812825, 0.7710409074867548, 0.9787022644425868, 0.8419085852906543, 0.22457510324119798, 0.8292180567043813, 0.8386125889112371, 0.012843866093566879, 0.6245712208610517, 0.6559069952457429, 0.9733314342429661, 0.9198104523819917, 0.9473977438358909, 0.662352335082189, 0.14709845205493058, 0.1403103809453235, 0.17661191384708091, 0.3456331857266407, 0.6940568463671777, 0.9442767282883552, 0.10760409702243458, 0.8889699752562306, 0.1484435319220388, 0.888302075335397, 0.43868941504961523, 0.03707036070440541, 0.6203417341728032, 0.6549325436463683, 0.018359719334589207, 0.9363923986121593, 0.20427800401664134, 0.5974739836206915, 0.07181820801456545, 0.2595924436990716, 0.5311476745184098, 0.6747001559421681, 0.8271485502552527, 0.8874862826389865, 0.8374004831775189, 0.9039228117767963, 0.8578571803010572, 0.4386127180131861, 0.3701779771146128, 0.30494330245256623, 0.3668314036878573, 0.02662721060437607, 0.2881737775275016, 0.9594485401080294, 0.7503467299810634, 0.6917379683998102, 0.9935229683488045, 0.9360707527281177, 0.9222702383781356, 0.4329225917354415, 0.8955997131041825, 0.7236136564603299, 0.19454650464451734, 0.9821086053821722, 0.30554101963872554, 0.4743319393523288, 0.7866447315026006, 0.13191706521289598, 0.9102144271226953, 0.5779690169784397, 0.6912728433702136, 0.8696817008675014, 0.3312089643927946, 0.4347280349653062, 0.5680527919221845, 0.5904158628533368, 0.6061369512359376, 0.9711479254107642, 0.6416157339504932, 0.9226235258189813, 0.1314233748777054, 0.9259342473229615, 0.8923319444470064, 0.5828464920051859, 0.8326342775236878, 0.4504078631806394, 0.7086611899557143, 0.15360196284201735, 0.03518503486274292, 0.5332522486823474, 0.7209088330043546, 0.12610745471437723, 0.869808590436586, 0.1698887820456143, 0.6729224208999119, 0.7114055602376937, 0.1738677095862815, 0.6891770254687041, 0.9679024645714805, 0.3432958269257134, 0.8914366903125202, 0.36414702666862986, 0.9465524459865515, 0.07000014212063116, 0.9567470515834899, 0.9578486759344351, 0.7629231398942958, 0.885425372741941, 0.6571541007461685, 0.44054974592154206, 0.5057614756590553, 0.42596005761507033, 0.9425797384248519, 0.9428507056177392, 0.6208894117718448, 0.9291105308172714, 0.39902896489023437, 0.10097403838360798, 0.9045758354334228, 0.7341245049486482, 0.13745118657670521, 0.7604681143868709, 0.5936894021932836, 0.9469209666115754, 0.9587403322858266, 0.7053145826318769, 0.8882915629999064, 0.9274705279178699, 0.8850032548867053, 0.9439592284850938, 0.897858302761838, 0.57790946301815, 0.48825584864578736, 0.5721344955741898, 0.8950043251184098, 0.15667066667216664, 0.7668063398188418, 0.8330021999962609, 0.41681988998434716, 0.672408211324824, 0.32302428997724014, 0.9861574023853182, 0.13158503799804244, 0.9860714832897887, 0.8917150738820631, 0.5968463900620403, 0.7298052477225652, 0.7206313215040074, 0.8717361330941699, 0.5313641878318446, 0.037562062651783225, 0.4404341192519513, 0.653873262926775, 0.08436983623116272, 0.6552463072098236, 0.0742744799905559, 0.029011804786057603, 0.09882424065463692, 0.7100691090635287, 0.12690701522899342, 0.9808727986700188, 0.16800525705080271, 0.19090097723456714, 0.9863101196611727, 0.8032340157098633, 0.00901149911985877, 0.6324562465592569, 0.8571195821567577, 0.03552681527229692, 0.20617523887937445, 0.9009005956245487, 0.6917144856129054, 0.4991289937445146, 0.19790413864927825, 0.38944508712013143, 0.6622672624655797, 0.7128223678565023, 0.9634545993134803, 0.7472400841285021, 0.6867176534113706, 0.9590955072851405, 0.9356817128911539, 0.9504871376834878, 0.1712797330031344, 0.7132946415256947, 0.40274191730006464, 0.9623628053816684, 0.7716375640505573, 0.8016166497577607, 0.6083762329830056, 0.09999586448294447, 0.9471561449627912, 0.9365673634015151, 0.6419689189443837, 0.038232377393681245, 0.9304354519417503, 0.017595658083944962, 0.7141664952421997, 0.4164443544035568, 0.9828029056105925, 0.578496424511513, 0.9313635592426106, 0.3835931812356902, 0.22249747617139956, 0.5786663809112108, 0.8620236066148008, 0.3689569744621481, 0.6102524259146243, 0.9242275148400564, 0.4764193927902527, 0.44368473266828684, 0.5823897062081674, 0.13720234696105907, 0.9437964316265942, 0.3479676718585079, 0.8210827281212874, 0.5751965198755294, 0.7805179510610271, 0.41564219311650935, 0.9427610478290995, 0.6542651049138984, 0.8936446348184862, 0.5235108369947408, 0.8981652121427343, 0.8535164479712368, 0.8394484899156092, 0.02391689002649527, 0.7625376547742202, 0.11261593732443721, 0.2929820973616, 0.6379100054979933, 0.4467547607971714, 0.9460706735869313, 0.7854198383960177, 0.08275163595793801, 0.21204198221541212, 0.5841382598625008, 0.9878764178692229, 0.9089554303968133, 0.7328250221501406, 0.17310086816455672, 0.15993613732907885, 0.8226455427887193, 0.11368091379131134, 0.8073635759789928, 0.49441835784892185, 0.8958163406352176, 0.8159982594950197, 0.8317969529058848, 0.8080643237346878, 0.2408703215130914, 0.4848830967794734, 0.3261846283438132, 0.8472052554387263, 0.0437648102111827, 0.775188059029517, 0.4597701965887338, 0.4245286560905208, 0.8177449635358611, 0.31397207478289796, 0.8698680716878977, 0.8419699320058694, 0.10099041837281307, 0.9508426335508694, 0.5297245271120439, 0.1519270230020755, 0.15067425229075238, 0.5287743421978737, 0.7926684518571585, 0.5376818227918148, 0.14240953364575948, 0.8624119146620435, 0.8468175812059229, 0.9026894334575594, 0.3801184145670528, 0.7195777687924616, 0.8466793150068441, 0.31793843259430216, 0.5636495742674792, 0.7974611332902707, 0.7245264851358143, 0.7586831944831656, 0.8861051537579253, 0.04681960839217044, 0.6724967720138889, 0.9931017538231667, 0.9060297048580674, 0.7145135201155077, 0.3373349834878057, 0.7216941482996986, 0.5289548992802622, 0.5762168529919995, 0.828441530312563, 0.8747334153261164, 0.7686713799996477, 0.15021531554988385, 0.7887974437474798, 0.875351777625858, 0.14088321144087115, 0.9488129985639756, 0.9340866135694843, 0.6916709872037639, 0.8280042734312848, 0.7062575642377777, 0.47022907267402836, 0.8737648871523721, 0.3337013769889109, 0.7533976849100801, 0.3680005024325995, 0.9483580740746956, 0.2556471178725003, 0.4238552936894582, 0.9076331252837772, 0.1212392028941755, 0.5099558636055989, 0.6016775371675087, 0.9418876213613349, 0.794721534518028, 0.13846229051364453, 0.38879151472674084, 0.925867320873485, 0.826060269776037, 0.8976065842705854, 0.4597701965887338, 0.02241533622058593, 0.7274099047052891, 0.6326044410522961, 0.8727651698439274, 0.9599167174076516, 0.6620327135129551, 0.8782522474830818, 0.839219033119521, 0.05474644309069787, 0.05253536965889152, 0.6963038464731095, 0.6647337751581894, 0.41707292889677705, 0.6298276918983242, 0.5018671125231405, 0.3087933251245964, 0.04499126030368072, 0.7103156467849472, 0.22279113380377288, 0.969356377421119, 0.8789265755141964, 0.49161759297027097, 0.05427570649608922, 0.6132684675326769, 0.230858887030258, 0.9558673693517727, 0.911375128932354, 0.2251227656359767, 0.7696437609832415, 0.6018486663337779, 0.733022007645436, 0.12934341491623214, 0.9108340840186663, 0.7137798534720217, 0.19869123996387994, 0.5036951346737477, 0.8824741091470931, 0.8281733835347078, 0.3433539411949943, 0.828381343501289, 0.3432020587213231, 0.09627215906739656, 0.5411650578032041, 0.7462591846606078, 0.8994603836538724, 0.5571053912567757, 0.03160436321215191, 0.8391039802668869, 0.472811347828998, 0.9282777549163329, 0.02216835219724185, 0.9635371681084131, 0.9291527730396477, 0.38923261440655654, 0.7461858660261153, 0.7961945154570531, 0.09791036942450575, 0.11007067208382001, 0.2475771057701104, 0.3070986857360549, 0.8969716659798301, 0.2946896636166547, 0.8173015337523655, 0.30249247005900093, 0.39655878794340543, 0.7322819277614868, 0.02152322667788998, 0.3962024185745842, 0.19054222962026043, 0.4185483302785237, 0.38014650254414445, 0.10025002438161827, 0.10195455222561871, 0.3949273302954, 0.09395387469179817, 0.05138706865060097, 0.6311175377433232, 0.5973832124786485, 0.8093047574813051, 0.3537322779066222, 0.08449567437330725, 0.5161508605665212, 0.9141025754511577, 0.8432453093708911, 0.2305319475093085, 0.4279272577883564, 0.6443550640450117, 0.7719783743358288, 0.21597200484528467, 0.7573028646189766, 0.6018614517684843, 0.8841960818410627, 0.13183378746572383, 0.9168330308600094, 0.6185565800194431, 0.8796688815882586, 0.05434339266806493, 0.7791376639108661, 0.8749713272048448, 0.4608791137440662, 0.6128664740353728, 0.4740323035861646, 0.6841898495808397, 0.9206932129153617, 0.5290811221118987, 0.11327289964372439, 0.11213768431961521, 0.42519392613819823, 0.20736892139489807, 0.39914877553272404, 0.16716618960587065, 0.7110009876971946, 0.09692768393174934, 0.7268219148222451, 0.5000433542810423, 0.24125801915586897, 0.43419567636676487, 0.9193113133232809, 0.46872829367779845, 0.6986921483060387, 0.8230282187666493, 0.407402120363402, 0.7977250485442556, 0.16720521889453885, 0.8761110003432624, 0.6298857423953919, 0.6933699401264845, 0.4375547053275526, 0.9614257179381817, 0.35786668438465574, 0.8526731706439017, 0.595364709754864, 0.8345568336963031, 0.8673113382743624, 0.49499272799738897, 0.7683367152017345, 0.480605425279481, 0.5025396536673223, 0.4088834339288662, 0.37758761653499173, 0.8895726559101577, 0.24988595534027655, 0.7486444661897352, 0.6269232538069774, 0.009066300323645742, 0.5731346088097535, 0.8994901296386785, 0.710072918174986, 0.21569097290322237, 0.5152031029920713, 0.9555940648760425, 0.8494288286430297, 0.4144554113427599, 0.738589783594311, 0.9549313873103844, 0.7291749315311818, 0.961881111658699, 0.6847158702719703, 0.7707761552968921, 0.7337145065601661, 0.89560633327391, 0.5826043289039663, 0.9711240173061219, 0.6347871251233556, 0.5926708561030976, 0.7808835981144857, 0.48743108481447184, 0.7540662126800268, 0.29016202008418, 0.015260050439380054, 0.12879085797883538, 0.7764890261611086, 0.6441491468286221, 0.8912783761323879, 0.23687750524644502, 0.8278115713473844, 0.027567031580574722, 0.6065630125107007, 0.4326047437884065, 0.2922798701450856, 0.8982045041721148, 0.7822080736545947, 0.8038182409621377, 0.9711593278310964, 0.4070795998267889, 0.020670372690563314, 0.9826758122351089, 0.9144590255067481, 0.8299599140178635, 0.35744293624484463, 0.05930974125544584, 0.6063921654167219, 0.6982413452050501, 0.16828402339195228, 0.9895278210926923, 0.551471198096423, 0.7993474309210237, 0.6607607849258476, 0.8719962488022143, 0.7285983647542217, 0.8364040771846277, 0.8633045009258296, 0.7421510852498183, 0.9231183216685089, 0.5365443486979968, 0.7687812541054363, 0.5618368895996122, 0.9192410708841338, 0.8126531587983938, 0.925713701243188, 0.7890929189129133, 0.0541773045282515, 0.7634561060492052, 0.7958650121600273, 0.8011947693519267, 0.7169971365980704, 0.9510839701844522, 0.7458299002886722, 0.9014007904323559, 0.7122322035554196, 0.7124766555186148, 0.47513211612495476, 0.8148743467335562, 0.5628148387794861, 0.5970440253643312, 0.7653518481457381, 0.04018277912106944, 0.016386049479488504, 0.8723793437044269, 0.8319292724649199, 0.9635546187409434, 0.8745019699769125, 0.28776932116364695, 0.7770326030824815, 0.405828423010163, 0.25249770395550103, 0.05779252770005503, 0.9458881857129127, 0.1957848400154579, 0.6530105103904584, 0.8349398269641581, 0.3817679474887198, 0.6784070813830209, 0.8975224933534425, 0.6230895038253611, 0.44666411203262885, 0.8194499484882612, 0.33181366237739074, 0.03318912035013781, 0.2710464445099198, 0.8875396804840645, 0.7918722872602473, 0.10357507905187181, 0.5199761252710153, 0.7497565431547522, 0.625123600600461, 0.9036205225208905, 0.43019423352719954, 0.8088638085979131, 0.04047242446663475, 0.9107994941796619, 0.5053986789005097, 0.7737099060218295, 0.3520466441649709, 0.20450968842027187, 0.5123873603137249, 0.7308011323297021, 0.16425591826514305, 0.8975142636402003, 0.34399272578244483, 0.7668160293093056, 0.7791826519595023, 0.5307882638821572, 0.7349817633222843, 0.14026857786490585, 0.8906114762917805, 0.9639671174027182, 0.8795071931932397, 0.33787870966010863, 0.6373565677164232, 0.422585274016933, 0.5311674005573345, 0.08040682933346907, 0.684199904556233, 0.7401426065056138, 0.9393235648376767, 0.7731063146808621, 0.3095284170938172, 0.827304385255511, 0.051433735072575607, 0.7695040804195594, 0.3296286083196602, 0.8022943615881577, 0.17488742732320828, 0.4601892161611704, 0.23654436971188533, 0.9613859569326861, 0.7228092229689522, 0.80346533284821, 0.9470023771032519, 0.5343193773612953, 0.3882429945553379, 0.5621528240889923, 0.6220473897112038, 0.9408739024681629, 0.1372968660217683, 0.9254513502564727, 0.6512729901914517, 0.7811754267173289, 0.593242832115843, 0.9646987413721118, 0.028687808750451037, 0.9089259711864182, 0.881480792048983, 0.8399733037904566, 0.2458113952899276, 0.8219181935616934, 0.8051132385819544, 0.9278079600919572, 0.8431139334514995, 0.24875008674428878, 0.6722870196275661, 0.6292186401965367, 0.7965401823899311, 0.5464985857752124, 0.841326601972558, 0.9370731173721768, 0.40478203063145796, 0.21348713176035744, 0.21665220526881282, 0.19395116881675098, 0.06947157623168236, 0.571820647830205, 0.8451512563711719, 0.8684853760639903, 0.9736187845779588, 0.6016784484349995, 0.7450065138416416, 0.7633050426513588, 0.5114791579750346, 0.15506437936071993, 0.693561498722337, 0.5825909562731512, 0.8629113039761308, 0.726936577094558, 0.9169066614263979, 0.8968736949470233, 0.13260931335135695, 0.9264842194564605, 0.7679130199593492, 0.677036526632798, 0.8797934353663688, 0.6181658657476125, 0.5461901368201262, 0.9392361231978265, 0.311418979593029, 0.1175208788897126, 0.8923319444470064, 0.9014030692466378, 0.8068730321800566, 0.8535343705488595, 0.5048653190105235, 0.7327716909225027, 0.7177572035941386, 0.42589058250592576, 0.8651560487177201, 0.9093530242265697, 0.8574491859531008, 0.8617816276818011, 0.7146728201925953, 0.5010273103209172, 0.1797751367223389, 0.8607140456010565, 0.9131635980669339, 0.8955922847680303, 0.6140568783967023, 0.4605040857777309, 0.07013655288689824, 0.61469738892879, 0.2521838352636976, 0.3075450619299786, 0.7037415361727953, 0.7865908555112348, 0.5923530989060686, 0.7708513539222399, 0.8248951543806028, 0.8586900448496028, 0.32236023857121526, 0.9321068421850117, 0.6741627422425814, 0.6610276986078492, 0.38755034873482425, 0.7980930088827494, 0.7457651800257575, 0.32902411579720586, 0.5013261273538542, 0.4660392708748032, 0.1930464845926113, 0.9648690403476499, 0.5197283583751193, 0.9137773883261887, 0.8243375470585936, 0.36247954319143744, 0.4218531823601084, 0.6638265564741754, 0.9384357619010668, 0.07327608357791646, 0.9331478053435475, 0.3535816531122428, 0.892110534627039, 0.6254768900862654, 0.8526808467269749, 0.6297842652767269, 0.8391563071658579, 0.774717780972308, 0.9061009916939068, 0.7541476963470832, 0.8273316911832305, 0.8178934468513586, 0.9609668373043566, 0.4040750219123903, 0.37543185074957586, 0.9410702242851661, 0.10861934984528722, 0.35639690440360905, 0.9084301851787429, 0.9654985299024623, 0.7799427242042202, 0.45639779054050506, 0.5996117783771873, 0.5931225549540361, 0.7459091708480283, 0.5893155286475442, 0.35500494065207444, 0.04111196730358092, 0.343991637494702, 0.9214880579738685, 0.9213503194965342, 0.32589703335612596, 0.007713772447836578, 0.08051520150261317, 0.9954314851704061, 0.6870411218419967, 0.032718104013320815, 0.8552550871162682, 0.8349666022130078, 0.8649696963622656, 0.3712916234349487, 0.7528836973573231, 0.8173955216631343, 0.1897619556320649, 0.563481108418667, 0.7750117030298791, 0.941871896587179, 0.09663476341505652, 0.44427083844957793, 0.8839624486946714, 0.40359592437333763, 0.7198533654971526, 0.25481176526143906, 0.9518704702434763, 0.5782409347033014, 0.2534651637209439, 0.4884019225214971, 0.4916078799505112, 0.8063457746661461, 0.7021747452892683, 0.8928655452186333, 0.26857346793778714, 0.7255768921669095, 0.9672734647101024, 0.7449761231310025, 0.21443847872899677, 0.7316503900947233, 0.4259810797711782, 0.12644327039742842, 0.7355340814286208, 0.885461729951144, 0.913673274774688, 0.9654985299024623, 0.893970777196389, 0.2097229809259881, 0.4934426595165187, 0.9623937596434571, 0.011652038004593758, 0.8929150241340315, 0.9548667469689261, 0.7376210065367871, 0.8765739952635268, 0.9032274892447757, 0.6252712043838574, 0.3647433658318032, 0.9917862334144834, 0.4527251241008775, 0.2042156579646508, 0.640277712307071, 0.625434515144233, 0.6045142109520368, 0.5955018664512846, 0.3364443349885367, 0.671047407421786, 0.30682402229433503, 0.8564893749270748, 0.7906474074471277, 0.4167684428182529, 0.011076820674891354, 0.07243180390734666, 0.8732815928723939, 0.6601034414535062, 0.8850032548867051, 0.760312969804649, 0.9792631724471278, 0.18652045736629885, 0.8628386320234255, 0.7603826437722088, 0.46037146441628685, 0.5541069594352124, 0.7091126687217741, 0.7601991976953151, 0.45510847748676503, 0.6001769332263883, 0.18597579908112746, 0.47061679555966307, 0.841754034932539, 0.8863142314586911, 0.33329055430584015, 0.35120340670856154, 0.10088623159460562, 0.1354461605269888, 0.5851596830248433, 0.9198525389931961, 0.6166922602762008, 0.42565398507632773, 0.6840678007745358, 0.7021747452892683, 0.8619367939630947, 0.5672260269062324, 0.9303667192575046, 0.35400765967354914, 0.7691228136162818, 0.8077857553071929, 0.5224138459541277, 0.3949002106833696, 0.9087085728858622, 0.4571287399655389, 0.5318895534940681, 0.6246978637021349, 0.6047434564223912, 0.6509344691415999, 0.023313029080238426, 0.9609376572564429, 0.3862351529569527, 0.580803149770764, 0.95880941881513, 0.018504450320260078, 0.4240728686330368, 0.7418413456687533, 0.10389002918219357, 0.6836723254899374, 0.19731667410484377, 0.5433231798347807, 0.3994335357391629, 0.8489881455963268, 0.925981314651065, 0.8502236948071202, 0.18669339843941263, 0.7175087959040356, 0.40409385656418206, 0.7994548705305182, 0.7840564052830984, 0.6142465955220353, 0.8713085079318066, 0.20888153844869553, 0.6285270364939166, 0.9238582272002287, 0.7377445500244261, 0.26010346712471316, 0.8689253645039197, 0.788220931678358, 0.24317384341510523, 0.9917905576345374, 0.4011509239761857, 0.9422750044457707, 0.14555917210914135, 0.7466930835517394, 0.8487796994475866, 0.31771805805233744, 0.3444389202723949, 0.9414158324542727, 0.4031068480122612, 0.4228654253661134, 0.44349400062940225, 0.4083148501459777, 0.40547347790868776, 0.9122920387798577, 0.08390839564019863, 0.7915044230880093, 0.4424566134721975, 0.8071035227757689, 0.6886729427098304, 0.7799910498934332, 0.9706712609271065, 0.4664198338170833, 0.5731359528420676, 0.5171486501638496, 0.9372158701105177, 0.8923319444470064, 0.48613421374317833, 0.7337347101163959, 0.38059377837583386, 0.703795488680456, 0.7359668340455822, 0.4549741455811564, 0.8428882535352177, 0.622498551021576, 0.09625050906102148, 0.7754128294134183, 0.4873639667504588, 0.61308797156122, 0.6440869816144597, 0.1424980959926775, 0.62817783952058, 0.9572291068086829, 0.6124357258864769, 0.7455092902602046, 0.9641317463883211, 0.7545230483738273, 0.2605235374797005, 0.46857664138280847, 0.9348548150745992, 0.8774511943511646, 0.8573054312382031, 0.9195820259077696, 0.4578198288529614, 0.5779235262178114, 0.7199874330097601, 0.5372026922985045, 0.6527298395905498, 0.14050452579570552, 0.3627917357058301, 0.3276065444867839, 0.5102772621953423, 0.9250809785026823, 0.1330783598488746, 0.7931823502064024, 0.9925959930279529, 0.8366562317887812, 0.6987730239766852, 0.8073546076951942, 0.9635697657353283, 0.6779322920384577, 0.5463134809794503, 0.27393145890256293, 0.6060023641188121, 0.8379575447887397, 0.9772334871394426, 0.1591175002843462, 0.2785568712097873, 0.08261991433007743, 0.3753319541139463, 0.5472693361686793, 0.9308356402578383, 0.8442872377718589, 0.8006345042871206, 0.17705788440547318, 0.8799056529646183, 0.7094993390311758, 0.16785454626116098, 0.6083208828332455, 0.2592732744373853, 0.14049258624825153, 0.6067438646060457, 0.7750053871101688, 0.21383986420794715, 0.6271011549065469, 0.48167766606880397, 0.47064075578936043, 0.6307001376786232, 0.3992165850633317, 0.9705268437950131, 0.6009282767358111, 0.6251198609543018, 0.5736054797544893, 0.9418214474383506, 0.2607173616044941, 0.8041926068315775, 0.6877454000965931, 0.5756180046781366, 0.5833229453666036, 0.356591670397996, 0.6780335975479617, 0.9557759298817013, 0.12371163748765823, 0.6784961002604635, 0.35320813110158755, 0.9334222447461135, 0.1908813466426898, 0.07172394808608372, 0.3168857499823764, 0.45708882257466876, 0.7432849523374101, 0.17605999982229212, 0.11769439863192392, 0.4683697565688271, 0.41703318671571504, 0.9141978527993345, 0.38706818517546165, 0.5106263668367312, 0.9453474936695815, 0.5949673995241306, 0.21514007406988683, 0.2430599614270794, 0.24065317790234467, 0.6939807331582103, 0.2263074583017149, 0.27561005974468555, 0.7577529663016015, 0.9367013619814165, 0.8498919585280807, 0.9296520593009389, 0.885461729951144, 0.40667713559115204, 0.9672691242137835, 0.22458160078630143, 0.9718446624547573, 0.39371870807680487, 0.7505884828932131, 0.3867348862433569, 0.5128765929460786, 0.9330412177464644, 0.3179900413826183, 0.9188388701235065, 0.4193150946529644, 0.6011955453014526, 0.5783226884758238, 0.5682416820566776, 0.6795209913546923, 0.4673821584683952, 0.9717993539636453, 0.8383488127420743, 0.593342384783459, 0.9925618536586507, 0.3997291986462006, 0.09764393428267511, 0.5929210498516011, 0.9653697127544765, 0.6311212307793787, 0.5338917468779764, 0.4841851925019006, 0.15849125148407442, 0.4603909647920365, 0.7521159082227333, 0.9797170132807045, 0.017688935886902034, 0.16052058788631257, 0.8062909986543665, 0.4596112245310487, 0.7375787517169967, 0.31080910320458704, 0.5827406552304795, 0.3809444167438303, 0.6290698644498122, 0.2116662309659339, 0.5976394025938696, 0.07411088990594956, 0.7728721472357726, 0.3473550279642954, 0.11974939825219795, 0.3368694654252327, 0.7592793674867822, 0.049417889363309195, 0.36103130200051975, 0.28750594557447545, 0.25012632182765937, 0.30444365980555466, 0.38221643660288496, 0.36997974213804785, 0.7148502183276907, 0.3867192323492328, 0.3368442529483241, 0.19575834715001508, 0.2546533040358724, 0.44930767418992185, 0.3527348510974505, 0.7592973659280893, 0.40691687867627097, 0.11730455036993309, 0.7732165421509211, 0.39674542011627734, 0.10441387511534542, 0.1614946689273983, 0.23686425130710678, 0.015559924828516418, 0.4474504380732523, 0.27333159676307067, 0.0845778792856072, 0.1773944907900621, 0.04274068857649272, 0.12051229683655719, 0.12075844199544451, 0.27563313320143323, 0.13160093817704083, 0.36039193716577306, 0.05632165461850138, 0.41761728257608605, 0.04042375350906321, 0.4728753859145881, 0.016864450078196022, 0.24228315435443545, 0.06397764320430858, 0.5800238410235748, 0.30462242162530273, 0.23174156403854593, 0.4210560074607004, 0.48863573090374396, 0.4519040869041778, 0.4922948485796133, 0.6309893964566861, 0.1647679498768174, 0.8001216299436968, 0.3927150435467111, 0.23155482664389776, 0.23744550286888688, 0.7313379964181916, 0.5406589194714616, 0.6003790626269048, 0.5821892987852052, 0.040251170799183826, 0.1837353792272091, 0.248915907622607, 0.19663221975294248, 0.2592469321194181, 0.165490752284916, 0.3938704561845213, 0.36401713861643414, 0.6606314030833881, 0.25701891762447143, 0.024712829530885414, 0.27236960785226666, 0.23382187804559876, 0.37663407002820604, 0.3791466978060857, 0.1476096102967597, 0.6096537746581792, 0.41869466025490887, 0.5968804910279482, 0.021786103129098004, 0.197503</t>
+          <t>[0.8828513463881672, 0.06183629229345817, 0.38001546300011874, 0.45693007141502023, 0.4492150145566317, 0.9758347305173654, 0.7112709716715935, 0.36860740883102766, 0.3766913505539761, 0.8955878822317486, 0.7685874323352752, 0.6901383194857781, 0.6144288784290767, 0.595204750599652, 0.9486287293787395, 0.3148745948053469, 0.717899211312997, 0.8239145807964056, 0.7932384305693906, 0.3020294262669245, 0.8851452583468138, 0.8072655593134022, 0.7530478310656621, 0.12394167506521866, 0.38974085200316183, 0.014695228020637887, 0.935505788524809, 0.6407027580076389, 0.7317131606083591, 0.2836461715747051, 0.7356988747323022, 0.1136597746280907, 0.5760457612219048, 0.8601719881432334, 0.8313181423543364, 0.856486471628815, 0.4873695025766852, 0.35678540228096706, 0.6879752358088034, 0.668009629273842, 0.5949674264189859, 0.6871015912985003, 0.030736279170219042, 0.42006531967378075, 0.8558302393271704, 0.012796749950993603, 0.9215935254871498, 0.8939191341343261, 0.021789655121082635, 0.8008810860008636, 0.8723438187699807, 0.9593939554223743, 0.5084051534537675, 0.957010437814279, 0.6154632255840794, 0.5908814862173565, 0.33434677345226377, 0.9751217474070004, 0.8612501347969911, 0.6974298586176854, 0.4937727699805813, 0.6712548274455041, 0.19626128251469183, 0.4991296047902517, 0.8878436374913766, 0.06551394329303009, 0.5149982606838315, 0.8064328315098961, 0.47908021697302927, 0.7220610130319121, 0.535740026320413, 0.7161873145304756, 0.8471266826076671, 0.9899380119423974, 0.8825956185033562, 0.7281637714529992, 0.9540736919975807, 0.9084566087370192, 0.9181544282819245, 0.23920423935603732, 0.7209350332776516, 0.5418351455940562, 0.9805013979979109, 0.7199500393158315, 0.7991440563482501, 0.6292796073146251, 0.733667760409697, 0.812160666831968, 0.5141116445041639, 0.5947153080342878, 0.9875540362929476, 0.013067032435103187, 0.5304102371396439, 0.5002974555771568, 0.4556532918104444, 0.6439623861652786, 0.4816549039624786, 0.2347041019503143, 0.9420730913549403, 0.7500227418421516, 0.5965986418027902, 0.670411011637496, 0.6442107133455793, 0.5917462916640612, 0.47775514270265707, 0.9079902329100683, 0.2261674779589266, 0.5099884891839291, 0.6992252587857525, 0.702784612565761, 0.07526304958305563, 0.010433484512832004, 0.548988317550295, 0.9638353547467671, 0.512805576145837, 0.33038330297490137, 0.8520431481261805, 0.43267794034929097, 0.7058934375620725, 0.5975794297912987, 0.435510145005617, 0.5558796129099093, 0.6635527559879076, 0.5749527969120151, 0.42735922591326414, 0.5427633430456577, 0.6039421564477397, 0.4112179823771682, 0.9091975695769835, 0.35485475731715416, 0.4956817189238541, 0.8812154348244174, 0.5323485448994754, 0.41270159868103073, 0.7573458479925785, 0.8170255765253839, 0.41306889451722323, 0.8881912592501567, 0.9754133216161285, 0.5954541529740155, 0.9687708675781739, 0.921671568612817, 0.8428663057001008, 0.5225605059067524, 0.5259188909531162, 0.7473185317740427, 0.926653454490203, 0.6866564318697136, 0.9143335059698271, 0.11502687370473366, 0.0954607269651739, 0.9922715095325264, 0.049443738606380634, 0.7831979330448111, 0.056782629022276924, 0.9668175797994008, 0.6593957372430158, 0.0699088800992483, 0.4408345359279171, 0.5414165671171592, 0.8400459199078215, 0.45311743222700224, 0.8269399090529618, 0.8731380592295186, 0.3878363191293344, 0.590343851887012, 0.7064693186616258, 0.9962898957680603, 0.671634057395429, 0.6149946305169941, 0.9804951049821791, 0.7073688019884353, 0.5735294044032506, 0.7098351641233268, 0.9142579937363475, 0.5390724295032291, 0.33218605315469835, 0.7530327203266551, 0.7220430332769144, 0.980970292231087, 0.8129317191804207, 0.40784380051101726, 0.9243278971560648, 0.9059959073114807, 0.11589672627415183, 0.39075508591026337, 0.873803205245828, 0.5897194811727526, 0.7177396114492671, 0.859318765928572, 0.8723247099796463, 0.6853163826239164, 0.4440991819755288, 0.9608555728087206, 0.293412985034666, 0.5049018842273915, 0.9342980707387928, 0.6242577086373569, 0.9197819394591874, 0.15670365561830468, 0.9292815727395966, 0.49137426891998987, 0.887958908859688, 0.7584834031149735, 0.7291814631359445, 0.6936207668969812, 0.6390787013968324, 0.7400412803314785, 0.12787467382683232, 0.8295325557566754, 0.9317003257316693, 0.27597190750888173, 0.8644014289836027, 0.5876757119650217, 0.7575814225403003, 0.9535214961568896, 0.6666501937367502, 0.8188950711043864, 0.9363438443945511, 0.997933448913558, 0.8677595548612707, 0.26291752015464365, 0.6818217835710894, 0.8812617956748793, 0.36710858457100043, 0.733572883683903, 0.4044490326517519, 0.7014953758869038, 0.3961926388533474, 0.9498813906550152, 0.6294924610064261, 0.41347774828879164, 0.7568515519191681, 0.9606238519816597, 0.18021199715655375, 0.8602091489473647, 0.26826950016689854, 0.3969599614210435, 0.7656398373457628, 0.6454925421839359, 0.5371112978710818, 0.14922555071255963, 0.3878097301609109, 0.8452689191405619, 0.7276679888388623, 0.8748241311117096, 0.19157920017228788, 0.9084566087370192, 0.03242698597803539, 0.10131396674798833, 0.9110733064937653, 0.8624943572044305, 0.8828441909380241, 0.7042494418571752, 0.8790335015398643, 0.24025652952486465, 0.820978274815857, 0.7135823089188236, 0.5190778418922568, 0.4460544108419821, 0.4731103290067387, 0.10149356388765397, 0.7642439820674463, 0.7975910459851389, 0.6063112017534565, 0.2661580255947553, 0.906319067055898, 0.23982386929439642, 0.42097836851175513, 0.827044221168667, 0.6822300469108061, 0.055937544566567916, 0.453932839430659, 0.07641533007680953, 0.43031645068196506, 0.7781930584715263, 0.9974003706353165, 0.8900084809255139, 0.9909656671412685, 0.6158342001089144, 0.31204077042492995, 0.7555402565372525, 0.932718125320903, 0.8545877471476939, 0.8041236697528495, 0.07060583730619281, 0.8106331880565998, 0.8503105846276054, 0.06620731170754998, 0.04992660833731514, 0.7262789373918574, 0.15414317153941584, 0.8947842909216709, 0.8736254707587376, 0.8536760003733546, 0.82648412369615, 0.9475945103555591, 0.7405163581359884, 0.4975612935667302, 0.2248652671844684, 0.13740164247315545, 0.816309050185299, 0.24871956222184438, 0.285056354978716, 0.6407753076934078, 0.9078798950523871, 0.7626682449142292, 0.7715889437882818, 0.3840317049089722, 0.4309924803643574, 0.4988215884180778, 0.028584714311436443, 0.19782199073330425, 0.9627147994722315, 0.9459040618525744, 0.026863549369162614, 0.018414884175934284, 0.7554493533725068, 0.7653663132905502, 0.5090879915673214, 0.7748564708614886, 0.6766101411291979, 0.9647834672003005, 0.8782883419491232, 0.6749707307273751, 0.8291801355802031, 0.9169519576729995, 0.22013495321443596, 0.32574932475647533, 0.8801292487960674, 0.4863162038747877, 0.5863426890001059, 0.582134234243461, 0.7898978764812291, 0.40782293138609416, 0.4918010392632464, 0.9638280095407162, 0.7891915538829918, 0.6111078140631822, 0.38381447596545903, 0.11251040115601023, 0.2170150718043584, 0.602171629187746, 0.8444814297422759, 0.8546543430418375, 0.8040326456196832, 0.8192973680084882, 0.29823180450145326, 0.7727352367149725, 0.9388647613377847, 0.1436803544848365, 0.9782704050061017, 0.7026246486107575, 0.8014056639672364, 0.8542284689585601, 0.9375396972075212, 0.8178210594742871, 0.16515646408136517, 0.5965214544321429, 0.8699924241891144, 0.5190220261887063, 0.43755503465562423, 0.7087650081847504, 0.8309684943518482, 0.9284611546527675, 0.28464632127747497, 0.7217144731564026, 0.6099845826458067, 0.4106891263111157, 0.6551909077331128, 0.8608465436614664, 0.963050705325774, 0.02844730230830005, 0.7689023091806702, 0.9668122908091555, 0.7417250904314294, 0.575749543588746, 0.5438209993697001, 0.8427966821312991, 0.4528438570807203, 0.6332111555926652, 0.8263979508930915, 0.8219171437055558, 0.0589430525196657, 0.5372805268599715, 0.8309164304043734, 0.5424692469471606, 0.3905587853882237, 0.8346739271571374, 0.8958879892896562, 0.9339933464377703, 0.2095421104491771, 0.6198361523153202, 0.6310346499250417, 0.4949855101329962, 0.9442133778652625, 0.5862908263613493, 0.945788479610153, 0.14527299551991038, 0.30111826307994116, 0.1410584347814474, 0.5345446272744433, 0.5095848981975896, 0.8705289215298936, 0.46591564708568545, 0.3199021305440401, 0.7078050194650125, 0.34087274888434804, 0.8461721447292502, 0.42022996901084586, 0.5379545700011444, 0.1508810515290486, 0.4941847161486722, 0.7234857470254918, 0.8733662564699828, 0.6427581893734293, 0.5906499170157049, 0.6331517030353394, 0.717809411630336, 0.19238438717932058, 0.230021960207079, 0.9903296439263519, 0.8110287064930443, 0.7070956142796442, 0.5874807713580106, 0.9885509429920657, 0.6595716520487629, 0.580719527965884, 0.1297277096015534, 0.6451733101885474, 0.7312626189180413, 0.926943989960598, 0.8569221450466163, 0.8206590730232018, 0.6346688146639927, 0.9555452075415024, 0.9216661650474254, 0.9395709630979723, 0.6605523980275921, 0.5441821623100433, 0.8558766901553303, 0.8109955150050969, 0.15018923701608042, 0.8651080514452815, 0.831562460573868, 0.7225111610058587, 0.7686859985528901, 0.8797909859629255, 0.8953020440991782, 0.8059785391087924, 0.9000119444084557, 0.7386352662615585, 0.39958518242862956, 0.8222613701047033, 0.9776885841697845, 0.2868071933191821, 0.9135863759344803, 0.3644115822606335, 0.851947985328749, 0.46407220226134327, 0.7595179047993628, 0.9761499263590633, 0.8256704495051272, 0.2265199686633486, 0.7280502667384674, 0.8170942726485144, 0.012461876910858033, 0.5990718056140161, 0.6960411636966974, 0.9701044938304377, 0.9363568159070261, 0.9439642497567388, 0.6664495336878649, 0.15771581075566524, 0.15708978063023676, 0.17884196937377136, 0.34855218022548107, 0.7035080162996203, 0.9430829714429948, 0.09377166509295184, 0.8791538798026366, 0.16014959759476066, 0.8819065384560084, 0.4302993026897752, 0.040321355395701176, 0.6314462507253, 0.6395174640975265, 0.017363950147433506, 0.9430059836834661, 0.2090818860755099, 0.6053501165622656, 0.059727834035796686, 0.249238729836089, 0.5398420590079755, 0.7064099134603865, 0.7717672958241737, 0.892568413941392, 0.8415732066129746, 0.9028038331051768, 0.8568627442573947, 0.4719374788270051, 0.32829367737646015, 0.3257907987616955, 0.38956502680556737, 0.020179685327840747, 0.256009389689137, 0.9603565995489811, 0.714564706453464, 0.7980336786344908, 0.9933374600172276, 0.9369893219621223, 0.9147264659019343, 0.46798147672941914, 0.8982405745918565, 0.6931978098865482, 0.19728431942818764, 0.9790056817054041, 0.2785415289776229, 0.4026105136055468, 0.7932562007275963, 0.12473010389114149, 0.9114385894386139, 0.6092988193642981, 0.7063573176428088, 0.8661799745983775, 0.36769590514528877, 0.38774273570300694, 0.6051763306872611, 0.584519615280946, 0.6346940820121446, 0.9728987456383672, 0.6146631401400905, 0.9260629728383333, 0.1702724719574105, 0.9255417150332572, 0.887958908859688, 0.5680864916306184, 0.8344329528404577, 0.4528384884760597, 0.7183277234469044, 0.15636586883879475, 0.032419810075781, 0.45472992251365213, 0.6373765208308019, 0.10480691955024121, 0.8515644433574497, 0.1785772576331377, 0.7190126913080439, 0.7289311559604584, 0.09341263299131751, 0.7894173290736829, 0.9704917843930562, 0.35656627614181285, 0.890354622467268, 0.32818140769451537, 0.9435268247221099, 0.05384131525476995, 0.9480354504852438, 0.9511298384630882, 0.7569656527387874, 0.8766298567493226, 0.7285350206203884, 0.4268205806593383, 0.49643299205668323, 0.41410847922078725, 0.9455981527237839, 0.9424288721960272, 0.6141906194981153, 0.9258250482873788, 0.4211236512176746, 0.11149259884080595, 0.9123825073829731, 0.730719566616803, 0.11301494269713877, 0.7580979961843977, 0.6640646736069802, 0.9472530098640299, 0.9641377511411106, 0.7123916224488809, 0.8917334616631605, 0.9326383378651799, 0.8808868883599277, 0.9256379915201594, 0.9282048574798526, 0.5324236296002808, 0.5294286528060537, 0.6153593246613709, 0.902610895742818, 0.18035429956907312, 0.7833390474365246, 0.8029477635273503, 0.4400987685428257, 0.6719288317472143, 0.3350871850093402, 0.9838000408545724, 0.11560222835100872, 0.9886646488399872, 0.8569009342538385, 0.6102715307363, 0.7524479237218552, 0.701344315058279, 0.8552609319056425, 0.6298179419799281, 0.032533498563400126, 0.47257221761099916, 0.582086261810428, 0.09276192871100834, 0.6772393550161191, 0.07162530170836134, 0.02636626035754259, 0.10250587518736519, 0.6996022875623208, 0.10760558089748702, 0.9793077103895964, 0.15738025584193094, 0.203047737173223, 0.9856940251640516, 0.8218498788787341, 0.00733221628421701, 0.6667061446506429, 0.8657885779189936, 0.03820708582077759, 0.21958539296953838, 0.9170622289671301, 0.6723899031559615, 0.5819931345878315, 0.19109815921163167, 0.39486495871230853, 0.6489387251543864, 0.7091577474569634, 0.9671390671608582, 0.7518851542130414, 0.6983438018186614, 0.9586537136158385, 0.9371647094239325, 0.9457501302092755, 0.16944802043674514, 0.6844114216539872, 0.40522069486234114, 0.9616916234834804, 0.7918309632484931, 0.746308018123594, 0.6039560757508404, 0.13462659449788975, 0.9444873963314061, 0.9156035959872232, 0.6639242705157359, 0.03743173748833925, 0.9150897302866705, 0.014868860520272385, 0.7325112297560903, 0.4106746119394648, 0.9843223925347737, 0.577552340218851, 0.9261720153835907, 0.3789068021306266, 0.20940696405240264, 0.604427182554581, 0.87978529558343, 0.3922416991960443, 0.6451481808726334, 0.9245835321936232, 0.46965717090617976, 0.3308359539496518, 0.6038902201671364, 0.12671807395388696, 0.9268644427489926, 0.34256334814459555, 0.7942739584247308, 0.4882913868508808, 0.7812443655867224, 0.41723383005237086, 0.9431153604836193, 0.6899686749792427, 0.8467539085603322, 0.4921502975841351, 0.89530175316044, 0.8507595294742861, 0.8568241831328977, 0.033535176774465845, 0.7694033766464359, 0.17264021584208816, 0.3031705951098112, 0.6550176254809673, 0.4466767618917722, 0.948425627549064, 0.7858436122508713, 0.08864144182814443, 0.2348368746782931, 0.5608273875065506, 0.985374753354733, 0.9110472018366254, 0.6872445983623706, 0.19939292506198417, 0.17822971121014797, 0.7935151083168053, 0.11741328147807983, 0.8001930719365135, 0.544939125440844, 0.8533074375828381, 0.7951263432299157, 0.8176642543421673, 0.7842251152298589, 0.22708867285032924, 0.5361032108810206, 0.3358879360787508, 0.8662481465806371, 0.04730849782188834, 0.7929358548125138, 0.5025597735336857, 0.44592820668720207, 0.7578769991578336, 0.3295817857655108, 0.9144851558057902, 0.8466920009281214, 0.10213313991281066, 0.940494681352023, 0.5477345133297081, 0.1307759408051056, 0.10779122975008593, 0.5515604503101716, 0.8176350332118447, 0.5430546773410068, 0.14757914645501266, 0.8363590309412243, 0.8571714087500869, 0.9148191739650599, 0.3468333793061339, 0.7235136512335922, 0.8728382698507511, 0.33287127740795713, 0.5541421690818786, 0.7924839046664742, 0.7478744855044791, 0.6947129641407321, 0.858425141272048, 0.03094472497269449, 0.6791720825838573, 0.9926362066394964, 0.9005123079985075, 0.70429728779604, 0.2889826242914412, 0.6849834419323827, 0.5189475209538776, 0.4822508316766796, 0.8102398580677725, 0.8742642303862069, 0.7190461477854341, 0.1825662527617982, 0.7775757703936926, 0.8673735848301076, 0.12407918471889723, 0.9495618125776264, 0.9189775026926745, 0.6858759984216544, 0.860476835625626, 0.6889464250999661, 0.4984442455728084, 0.8663792712571907, 0.3152280173281389, 0.7534715748937606, 0.34663129994906516, 0.9515885908203591, 0.2288950083829992, 0.36486140696927233, 0.8918006235396104, 0.16361045934422266, 0.5458764101823853, 0.5766226240589176, 0.9397274059873607, 0.7800405696975414, 0.13839710318876886, 0.3356923557660397, 0.9306113113472106, 0.8381571976766875, 0.890883549246461, 0.5025597735336857, 0.020834760690966975, 0.7304792456420729, 0.7206188103637622, 0.8587253747194968, 0.9591411507424958, 0.6735830257032114, 0.8660683993925855, 0.8681651228926831, 0.05756449237213202, 0.050526887839304736, 0.7440513015953719, 0.6796782679236253, 0.3608554003911614, 0.7210111009234227, 0.5439269627648782, 0.3242715583099854, 0.05186161870000858, 0.7264735714722124, 0.22231046796076914, 0.9593176642313621, 0.9145932063977583, 0.501036700990144, 0.048207347238038344, 0.6266541004617456, 0.23482015526760613, 0.9445090337750278, 0.9078267682657356, 0.25203119678694585, 0.7787910042776603, 0.6114066018581122, 0.724387312152029, 0.12717770676139808, 0.9259785673682854, 0.7070054359384177, 0.15833001816216674, 0.4943739284534388, 0.8765554750606105, 0.8437232352395998, 0.4687586520809164, 0.798340677501218, 0.3695853973003753, 0.11290014333051321, 0.5399444323487994, 0.6829755442597754, 0.8948647112400064, 0.5872081143851169, 0.029205352589698436, 0.8411480524220026, 0.46798933964539263, 0.9285036659213881, 0.02443779409057072, 0.9577113311623758, 0.9316549361380354, 0.32762309138420526, 0.7055652502420824, 0.8363238977170411, 0.12765539911678717, 0.11647112563911666, 0.20870213633323417, 0.3230625774614003, 0.8711176512680762, 0.28923147491748524, 0.8044881733329791, 0.3164556145412522, 0.43319921898490643, 0.7368140862825495, 0.01861748607117415, 0.3562433763764787, 0.20725926511453266, 0.353705373731779, 0.3787788297474769, 0.10526780773396456, 0.08504067277641565, 0.37636488528535317, 0.0931575010962778, 0.04010885928053499, 0.635237850743531, 0.6146895808834429, 0.8257720833881644, 0.3725459602823775, 0.0866702059677342, 0.5246666996423756, 0.892913990234158, 0.8133685545687341, 0.2472174135817707, 0.4277848674820358, 0.6974717980040971, 0.7739242537360037, 0.18925170232265678, 0.7770052715847948, 0.6916309854432678, 0.8810026108660642, 0.10081855244321129, 0.9183947678792294, 0.6305172768363156, 0.8848088732828785, 0.05055646047989413, 0.8340132683666213, 0.8862828106457944, 0.4590390932198788, 0.6105050027478081, 0.47691506696908714, 0.6731605693265357, 0.9235270380467743, 0.5703871152262326, 0.08910727887264262, 0.11648978367669337, 0.4895264290084873, 0.20612586988857817, 0.41789183419513176, 0.1332524284347226, 0.6970030967201275, 0.11032123203732308, 0.7388749527213258, 0.5401052712172563, 0.2116286053538779, 0.45747750654533476, 0.9142579937363475, 0.47436750327883537, 0.6962707047374073, 0.8514087905587809, 0.4292862403572964, 0.7144007106637669, 0.14596163330003287, 0.8759604517377692, 0.6629629967076586, 0.6938923002048987, 0.5344548531227505, 0.9475778557733384, 0.36649018043348247, 0.8129578639649984, 0.5337880217281407, 0.8355517787195126, 0.8743950700323831, 0.4608906062310444, 0.8083673984984379, 0.49310088647810646, 0.46964223319773635, 0.37181145405444677, 0.5203420419680685, 0.8814609840356711, 0.26502925577937686, 0.7448300044173013, 0.6354726304608053, 0.009546872405784375, 0.5818481296950273, 0.9062234348262971, 0.7084761484835678, 0.2055884295911057, 0.511343975025798, 0.9497635548425779, 0.8440446382115996, 0.4049921413988754, 0.7636487133030208, 0.9506153047455593, 0.7352891765702413, 0.9624347190447239, 0.6911667870288675, 0.7526197852022619, 0.7282122044925631, 0.8952236875630817, 0.6007097764674995, 0.9718279235916382, 0.6666501937367502, 0.5686963592620464, 0.7462547669095064, 0.5014357153612293, 0.7586927974267429, 0.2467370542215808, 0.010968794331425318, 0.12929555078041113, 0.771489583723797, 0.5878744286733966, 0.873584404304773, 0.21047854325018536, 0.8263979508930915, 0.020253752042231614, 0.6003620962963824, 0.39814457863493635, 0.294095601584008, 0.8994586202038647, 0.7754288204532722, 0.8138269761432698, 0.977117618269748, 0.44300031318775196, 0.017804753295220074, 0.9816650436058969, 0.8889521948566431, 0.8964380045230043, 0.4248498547226422, 0.053421442914387496, 0.5511465058672594, 0.702073316743887, 0.22131528482179802, 0.9894990049153449, 0.5989077076113919, 0.7876748644442042, 0.6448057105823881, 0.8811730687200844, 0.7348555642138952, 0.7927204789288408, 0.8617907986151945, 0.7237599580295582, 0.9117973616466803, 0.525624053481644, 0.7595786348273119, 0.5817552625770628, 0.9125632197070578, 0.821005691623077, 0.9252935244798884, 0.8116410299716806, 0.052293131200151, 0.7464655843574263, 0.7899022577965237, 0.7848416734373227, 0.711868291911801, 0.9401364675129994, 0.7595740225938532, 0.905352716857997, 0.7100794864617586, 0.6731664443588202, 0.4098635604839478, 0.8081853763927264, 0.5601715133990811, 0.5968577766088462, 0.8002276912928818, 0.05408925905542006, 0.015953299213182448, 0.8720012144239943, 0.8111128815684606, 0.9632238573955293, 0.8675710176020015, 0.2982613619878595, 0.7883571839731925, 0.4519966972563884, 0.2537412367741822, 0.03398990828439213, 0.9366987772331221, 0.1963206254881612, 0.6711763595390491, 0.8528106080593892, 0.37252558187803353, 0.6651025454633858, 0.9013449373013716, 0.6285819936071687, 0.41515934238721947, 0.8344669949527868, 0.3060385117788596, 0.02441426548469089, 0.25027959160331936, 0.8777913350348073, 0.769412897752243, 0.15375892922413895, 0.5395592619980305, 0.7544704190567475, 0.6527190474269119, 0.9006776185463318, 0.4010869094254136, 0.7629806163872719, 0.03582272309525263, 0.9139138603498831, 0.4493504792040717, 0.7599934573382935, 0.3333845614089927, 0.20016036210546984, 0.5969470574390275, 0.7400797603454922, 0.19786845018488164, 0.8841030648157014, 0.35406365436279097, 0.8198799596914883, 0.7783853160802251, 0.5219540472329548, 0.72757232114698, 0.1637533411047227, 0.9021371032895114, 0.9572348236523244, 0.8799132160469543, 0.3379937174582007, 0.6511163938859241, 0.4235006958855193, 0.5305809654780619, 0.1222072710326179, 0.672916640353016, 0.7362580570829299, 0.9280070486675724, 0.778537566998724, 0.3802176894112184, 0.8193095713621994, 0.05166251974982172, 0.7207122131832409, 0.3047766707803071, 0.8127908736025725, 0.18677869220108534, 0.44065922913327493, 0.2289924270289172, 0.9472329055993233, 0.732572968353033, 0.7818796906471368, 0.9500128426163876, 0.5827881706290917, 0.35980241598529145, 0.5992390509296394, 0.6556198869011663, 0.9413946320262507, 0.13534131211290662, 0.9203147348029037, 0.6458935996278388, 0.7832377489038007, 0.6222450301812954, 0.9642342325158745, 0.025832122917402955, 0.9217431402150918, 0.880656822629161, 0.840686222693206, 0.20795020363068875, 0.8293141318193902, 0.7795042367493832, 0.9311625326957637, 0.8306523613460269, 0.24797894783864186, 0.6209429031948499, 0.613426598787528, 0.7976396588459586, 0.5383568531777657, 0.8370142236160462, 0.9452299555408546, 0.3966816743984021, 0.21195548459121064, 0.23749991973946627, 0.21693679439046207, 0.08230932504290625, 0.5884771225695241, 0.8727565991334977, 0.858747075785419, 0.9675897054317996, 0.6042571154308486, 0.7849860398015146, 0.7795680507772789, 0.5333968589038636, 0.14967024128582332, 0.7093817897541603, 0.5401614878780107, 0.8376586176593698, 0.753012411005184, 0.931827139948436, 0.8960044963753642, 0.12106095731364926, 0.928698120390974, 0.7705763087861811, 0.6247466429856864, 0.8689023658819782, 0.6209453470517577, 0.597814522422026, 0.9515483044178935, 0.332467708668732, 0.11065440497827077, 0.8879589088596882, 0.9074103489219287, 0.8051214573768798, 0.8817076912072674, 0.5298633350579537, 0.7339693368435334, 0.7482651991962695, 0.4396722796703375, 0.8594254112011752, 0.903422229594927, 0.8630747290460451, 0.8332039359399565, 0.7096058194223568, 0.5507399172988027, 0.20226625821736746, 0.8567440432239055, 0.9045203527538035, 0.9096282722202815, 0.637827019816856, 0.4406097275674847, 0.06791990103353857, 0.5890280279047272, 0.2606220869562848, 0.24816144027917414, 0.6755615308537717, 0.7832311478064983, 0.5908618926476227, 0.7732349742421524, 0.8500839437742096, 0.8369866956523158, 0.34332462725797513, 0.9391853466068497, 0.6596997488321843, 0.6290260267843577, 0.41637672697115086, 0.848348260833856, 0.7541643987821657, 0.35652197390554763, 0.5326081986363851, 0.45439874429109817, 0.1932693415824839, 0.9618817105512109, 0.4701160369487616, 0.9259200991816859, 0.8529912420476964, 0.39910436930229565, 0.4616728365183412, 0.689177115667523, 0.9539316720879507, 0.0707449132790412, 0.9176340080083434, 0.4188160049946503, 0.9012641026095007, 0.6098390891059243, 0.8100538157163275, 0.6341064294668709, 0.8343407510939247, 0.787306469563548, 0.9122830712906858, 0.7484311501812155, 0.8286892990151152, 0.8354047878939924, 0.9617964157145173, 0.41453505485109504, 0.38615355059391643, 0.9353241947180793, 0.09210551001132836, 0.3753970803392133, 0.9207291705307943, 0.9608555728087206, 0.7798900400011273, 0.42551864170929316, 0.613886496614762, 0.5715195909168245, 0.7487913051819355, 0.5609757268070266, 0.3291245495217413, 0.033774640431698234, 0.3568765284984731, 0.9195924740573156, 0.9007932130675377, 0.3571688516599409, 0.006229644581926962, 0.10259310874726207, 0.9956011344814424, 0.6805236028293834, 0.01660682885892861, 0.8777429930722832, 0.821814665130588, 0.8612539620400201, 0.36612163341534565, 0.7843077109204145, 0.8159184234038622, 0.1931201265679241, 0.5642280464127278, 0.8027663140176077, 0.9401238852896958, 0.09341866097638239, 0.40079358687155375, 0.8778473826088822, 0.30350025397672653, 0.6775272198764786, 0.22353752186534798, 0.9397451730446738, 0.5121190507854213, 0.2745225952658942, 0.4029057203657495, 0.5571109907714829, 0.7995438217225889, 0.7276679888388627, 0.8606279734708084, 0.2976378626240128, 0.7451393741266901, 0.9632621894071415, 0.7701996469660395, 0.2233256002658006, 0.7567779356376193, 0.45652242501713247, 0.0968863465879995, 0.7023261639332414, 0.8911073966419883, 0.9179756125933187, 0.9608555728087206, 0.9199150283175369, 0.21648150866999316, 0.5079713812526663, 0.9641074394521925, 0.009854184553946644, 0.9096330192536853, 0.9713023989826828, 0.7675722139617347, 0.8717247162872377, 0.8990206124922471, 0.46385139782699086, 0.3694669349400599, 0.9917101967703454, 0.46377679965055113, 0.2012637337235797, 0.6094150821929887, 0.6149750618087753, 0.6444554061357654, 0.4519105983451752, 0.39054211812624084, 0.6515079173696862, 0.3048543875803874, 0.8718295573724227, 0.7669345142341395, 0.36911038947976993, 0.012592511993022245, 0.06628354178805622, 0.8969585893504908, 0.6863571598765912, 0.8808868883599276, 0.7623609416208081, 0.9824652051365473, 0.10772825460702315, 0.876283087512439, 0.7445822484455861, 0.5085646123678578, 0.6008683128825515, 0.7160880060756326, 0.7823443257780106, 0.39353292636419807, 0.6256154155212788, 0.1981449847872944, 0.4674383047499123, 0.8478893790957162, 0.8829301836214611, 0.35462632297273, 0.35875832360720844, 0.11492447587909801, 0.11470439298226917, 0.617634596078319, 0.8964641241103062, 0.616375010169679, 0.4845613329483055, 0.6901853598538538, 0.7276679888388627, 0.8493075588431787, 0.5735786537531732, 0.9110878934158209, 0.3701088443260404, 0.6990106319710079, 0.8099123137447668, 0.5128878893751389, 0.47072056764437975, 0.8949983515860889, 0.42434068812938625, 0.5527992611213777, 0.6411033524751768, 0.6806914562026446, 0.6318555520858103, 0.02182603344287828, 0.966446180592212, 0.3372667637550863, 0.5408706552274175, 0.9468308705879351, 0.01580475250397158, 0.47404572191940675, 0.7509101771334656, 0.12644831527792608, 0.6788784038706196, 0.24920395496626413, 0.5025919145861072, 0.4843187448206965, 0.8585587633315703, 0.9468999329847533, 0.8622301286862475, 0.1671481075480581, 0.6978372407618675, 0.39440315901902123, 0.7871595007379504, 0.8100366817742053, 0.5700601216455635, 0.8859239459553165, 0.1920366471777148, 0.6254786336299172, 0.9293160623237018, 0.7273327497835973, 0.2771586901224791, 0.8744882429240017, 0.7800474476616822, 0.24856124102439545, 0.9900826863346581, 0.4077790754597071, 0.9467009825426853, 0.1340005914530943, 0.7706848236319318, 0.8474258109545628, 0.41438369485775617, 0.37719777626526874, 0.9385994109817329, 0.39488135092702953, 0.48044637180496624, 0.4317056428982617, 0.415395321835219, 0.3719041188224918, 0.915592751760729, 0.12464278076363433, 0.8121713220505491, 0.4237011243110747, 0.8273820833014021, 0.6801493299000784, 0.8126615634433954, 0.9671429804884755, 0.4700063198324922, 0.5992003193510335, 0.5324835961446134, 0.943080768642271, 0.887958908859688, 0.48124146561180176, 0.7564821892766846, 0.34154256990214044, 0.6805410442126882, 0.7048865622343122, 0.5950932297207416, 0.840431737931265, 0.6452773282808317, 0.09800739940840338, 0.8055141081874393, 0.47843293004163795, 0.6923603034409106, 0.6158496748640075, 0.12715872953535615, 0.6459552747572294, 0.9566229372841576, 0.6134896409929695, 0.6566676615852343, 0.9679593886088338, 0.7630983794657412, 0.25189698071619676, 0.3787796365902094, 0.9394721194462238, 0.8736254707587375, 0.8609572964748169, 0.9203320819607741, 0.44953486449269464, 0.5636162060687022, 0.7441004967438746, 0.4585101862819958, 0.6287698204546216, 0.15153022690098306, 0.3115926561499572, 0.28542813965406416, 0.4936967342953964, 0.929822844224065, 0.12801293916852038, 0.7705655864943822, 0.9925795566839783, 0.5818116459460831, 0.6368347699947319, 0.7971773476576239, 0.9446935496359133, 0.6574304630602367, 0.5750092860392798, 0.2899489975673339, 0.5885248578497217, 0.8435227652839676, 0.97789651130315, 0.1627562304647675, 0.28971189521232854, 0.045847112859911485, 0.39895735287473827, 0.5836824835127796, 0.9320563867145215, 0.8350380122230006, 0.7753202716047142, 0.17971353382583458, 0.8672562143860264, 0.6819877919891443, 0.16595604898895663, 0.6544352629195669, 0.3932245916181636, 0.1268894155394329, 0.6147617968942489, 0.8168412731380448, 0.2197356626037324, 0.642974523382992, 0.5224692347531947, 0.5070278442457353, 0.5740265737624133, 0.4080282808616592, 0.9677286079301548, 0.6223920862038395, 0.6462750308571044, 0.5744114630652996, 0.9430607903903757, 0.24605291971896243, 0.8435214303628678, 0.7219871631089274, 0.5564300033188272, 0.5212787176909656, 0.39768066259056273, 0.6691738721674204, 0.9581175289756148, 0.12386298052910533, 0.7630189811963914, 0.37014530155048975, 0.9089441088666302, 0.19221458525581403, 0.05382057303801117, 0.31714372531049584, 0.47755844754467625, 0.7284612001696777, 0.1703253275271455, 0.08793549884767972, 0.4220352584989261, 0.4508687903350388, 0.8774793623921341, 0.3593830857124181, 0.4765506130291584, 0.934266738047365, 0.6426326973693076, 0.186217645304922, 0.24315291431006683, 0.24833966901970225, 0.7024781858336093, 0.2742863414440476, 0.2763112940033612, 0.7660115902413376, 0.9286202084905623, 0.8379944934248553, 0.9269336758264125, 0.8911073966419883, 0.27777552377932074, 0.9636808344102444, 0.3273162042375195, 0.9698096833409903, 0.4192855784958721, 0.7972525810300144, 0.38869106728940617, 0.5108070574459055, 0.9249683354805556, 0.32532513267267915, 0.9220795442623136, 0.3319403919647482, 0.6086209584823885, 0.5787440492217076, 0.6167566618290943, 0.6666273010151136, 0.4583281468140404, 0.9689733596804362, 0.8545938690542787, 0.6051957162442942, 0.992041297522711, 0.38623477431920306, 0.09808719768392692, 0.584833487119901, 0.96069430821548, 0.5927791560379332, 0.55856870589357, 0.49337457944522295, 0.15315188204538513, 0.5122587167350299, 0.7397721331257877, 0.9772914427081718, 0.07362088141913446, 0.12173551571742398, 0.348555518438886, 0.13038904455636743, 0.31715624452539465, 0.2549055572901537, 0.7405131369418068, 0.1677340206646449, 0.06382760422324783, 0.31572181801894345, 0.3711890299296813, 0.06029758671134427, 0.49350679649612056, 0.04018391249485956, 0.6799842312848585, 0.03256604213827274, 0.5275155089167315, 0.30423663962417147, 0.09036679421774789, 0.2127266112578104, 0.2255208855130746, 0.35394943908433707, 0.43703561115261735, 0.11555324004257297, 0.016206957544140088, 0.04654684022711511, 0.22024176162909959, 0.25059151490816967, 0.7654191292154946, 0.6449681592103108, 0.030791298228197147, 0.16599462098198703, 0.05620738029604905, 0.38935192251181766, 0.03552258295825463, 0.11454137116921882, 0.21770659916155535, 0.08230540170361339, 0.1524359652211414, 0.6192436429566149, 0.2126316511599213, 0.42649889819808307, 0.5281158345302464, 0.643704731847632, 0.5708904481326963, 0.3953539814516225, 0.4387330519393016, 0.2748071912477927, 0.16318721301635009, 0.3064848087514917, 0.5154926633385309, 0.07623574828274034, 0.029333691617926847, 0.22257547902249858, 0.06861281920911295, 0.2568576042320215, 0.6324843378110153, 0.9345134027051194, 0.6670168335455534, 0.735571977195928, 0.02579961895968415, 0.5209575784687839, 0.46318086868416125, 0.5661968300749355, 0.2063318612098657, 0.09871370390252178, 0.5950249785186751, 0.47030688556660105, 0.8801332965134316, 0.04488251434170479, 0.29474280017119336, 0.3026069523115878, 0.721888313920486, 0.11112080102186361, 0.08457269428583933, 0.45852102796287525, 0.6662382658625106, 0.23018939103112862, 0.434431659503762, 0.448298350081767, 0.32494806897194245, 0.2768114037183133, 0.6220124709208618, 0.5362849851326872, 0.14492033300377885, 0.03483300315879387, 0.25199532050122525, 0.31209145879619044, 0.3985768362276341, 0.1456005273570103, 0.5547273036645095, 0.7263727527989269, 0.38759965203063995, 0.5768942471046636, 0.6202716948972231, 0.5359</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>[0.5248347633510431, 0.6356110478360651, 0.10092603779330166, 0.991145761215201, 0.6404137424446494, 0.8378183346343703, 0.7535400535090132, 0.31970666343015497, 0.7766942104931794, 0.06383774063457151, 0.8847794671279396, 0.6483196430168312, 0.801406008523635, 0.9628681557260758, 0.9481832327213549, 0.18163501900508502, 0.5573698865073546, 0.32567634246191346, 0.13095284871173132, 0.6790685803466355, 0.8190040413534818, 0.44340126028313287, 0.9562368119644067, 0.32720104466430233, 0.06530176731276006, 0.3520125990938107, 0.6490331894255433, 0.30640866722289156, 0.5072455549246805, 0.45166850361101013, 0.2718517076178263, 0.5622447703880936, 0.7927925797468658, 0.8267327614818627, 0.7269494290188099, 0.8489155201559733, 0.9011720402032231, 0.6489594242949721, 0.8240162366937004, 0.8512734985166737, 0.8706211110596188, 0.8636121326549753, 0.958931232953173, 0.11345761718684752, 0.6695364301145715, 0.5443439091660951, 0.9687985773775337, 0.9101723213435132, 0.9001207580907185, 0.7374915844926626, 0.8391887670497286, 0.7578149159545436, 0.8279757127364946, 0.5171018381830644, 0.9681683012727501, 0.8944135343452975, 0.8602935334988732, 0.7727611263594162, 0.950761369082067, 0.5259065260010032, 0.6234804029377748, 0.9491865289804001, 0.6524494460022872, 0.6535188133425294, 0.9391628039876773, 0.9676244273703104, 0.9149682093472089, 0.2577075363755299, 0.957068913041924, 0.519038302837049, 0.5286919467438792, 0.6511965666099697, 0.7734772126287393, 0.8765575798975124, 0.9607865032210534, 0.948537300957522, 0.9407951929794226, 0.9883904828685695, 0.8807094301207766, 0.611268457139356, 0.31648315435079305, 0.8822041950742295, 0.2738717641157794, 0.8234080233786382, 0.8333006362098926, 0.7827479736713648, 0.4188980624732988, 0.28830680128526287, 0.9853856043713177, 0.9306001771929525, 0.714830063505455, 0.8610845036596255, 0.5515093472032688, 0.9723567102576632, 0.7593501734054734, 0.4539998535304236, 0.1854292144172285, 0.5811414139001821, 0.8299142261547806, 0.937936075003819, 0.6247354998390009, 0.5129339876922729, 0.6362669533198851, 0.5121727643675675, 0.826370979175463, 0.6958713535353652, 0.9762644107795243, 0.7823735440690734, 0.041560889446859865, 0.8172483488262953, 0.15677534516801533, 0.9562910222497789, 0.7126461150927991, 0.844023742761289, 0.9247222832458787, 0.8665761312862351, 0.30836306017391746, 0.7379389652705158, 0.462500470056207, 0.28579681286259007, 0.8453685005184542, 0.6912823055393944, 0.8531680534816842, 0.9942927762577216, 0.9168550780667967, 0.9698433489403211, 0.5330320984434179, 0.930078898442763, 0.7178922891147932, 0.9860224393620343, 0.3032526124343806, 0.26513265678578674, 0.04152506399621376, 0.5407442572915824, 0.6094138491893648, 0.8266084398015535, 0.8766010845963061, 0.43039130810581766, 0.5246402990413974, 0.8134818822402939, 0.9750137255442651, 0.9517995403663883, 0.9001467589759106, 0.6251154051112005, 0.6750561872932018, 0.7554539090737958, 0.4664600411094339, 0.5204616333630387, 0.9788876663032717, 0.8651346782029542, 0.9406585045466499, 0.10046893654116582, 0.6290420414769318, 0.387244927188142, 0.8881888123565544, 0.7759061827105476, 0.02010637053820013, 0.9196575015352811, 0.9138626530756339, 0.6841203797532237, 0.18224981777585422, 0.11070984052347252, 0.05600307519222104, 0.7809398439876799, 0.4010864701735219, 0.6836761750586196, 0.3556127431025147, 0.7826184386795227, 0.6916383682007357, 0.9128275937234978, 0.08982119905018042, 0.9283036649334241, 0.6558887299976486, 0.38875268905295246, 0.4303226766083269, 0.5119181097012099, 0.11919533816528537, 0.44980296461948593, 0.832271321058815, 0.8592516431192971, 0.7226640788379526, 0.7852829878868516, 0.2818671319253725, 0.9287457956098952, 0.7713039957081819, 0.5598711798909253, 0.9445378636135908, 0.8668186946844261, 0.08663355105388396, 0.8629863128651126, 0.935262986244856, 0.9200304964239236, 0.7911646514548168, 0.050237002846096626, 0.7928859011374807, 0.6728104145163378, 0.8269641411186662, 0.6660219682397422, 0.726423395564406, 0.8781792064139472, 0.25756804698407604, 0.8104479941086231, 0.6004102069294555, 0.6121848813484375, 0.4891456339318494, 0.5865530181138534, 0.8946136292095614, 0.1319272255439225, 0.6377109069241675, 0.9865300688284827, 0.47213603499106777, 0.9459297717647831, 0.966680256415216, 0.17497901851740508, 0.9541585473031124, 0.9547837794794607, 0.8488853408417665, 0.8057772573420928, 0.6361313168577059, 0.5929620185509875, 0.5711831989013189, 0.4025153571794018, 0.6768708606238145, 0.65389400221104, 0.004425864028093308, 0.6684322566327809, 0.5734046092227136, 0.23132124371008317, 0.5162433415967868, 0.1270018649606143, 0.9201056897185083, 0.5544224848962884, 0.9577332744266496, 0.6938755334526328, 0.12005106607734684, 0.031456884075638694, 0.10694307518241776, 0.1196940687049158, 0.029960182408981663, 0.12429484575464295, 0.6121482700234643, 0.06297020069352273, 0.08575638721902618, 0.14979288988818887, 0.775682815671292, 0.8806621043938312, 0.8572280710340718, 0.5616081505958862, 0.6924717093208858, 0.9222383305115068, 0.11977787281574451, 0.9131096549530852, 0.881809729941589, 0.4267242950053971, 0.7202026509169529, 0.7582148816168682, 0.037744796856135424, 0.7992244852733309, 0.9921070842222182, 0.9252699622674426, 0.2153179705909353, 0.05726399664053743, 0.9282073373402916, 0.41874808784009376, 0.006262585025754759, 0.06677540871591167, 0.6101896802149266, 0.11720175939383946, 0.4065350409849919, 0.1108077260399233, 0.22991884750241928, 0.691960494746297, 0.6254376697653498, 0.9350023377704704, 0.9088851584818401, 0.09110717212704861, 0.21159365442437844, 0.9788646758668437, 0.7264906209978903, 0.892888866907768, 0.022492415220493243, 0.12943634533428405, 0.958465471626458, 0.7861869516818986, 0.06396137926389316, 0.6775146100375987, 0.40221660503221773, 0.9836632764238115, 0.15407335750877707, 0.6090893853780703, 0.9261876916484417, 0.6776524166392658, 0.19437167234130154, 0.8703966531202398, 0.7353580765688429, 0.698683056580949, 0.4785318802396779, 0.41444838825596186, 0.25471359523239523, 0.05196304808627879, 0.04564608438777111, 0.19270762687559523, 0.8807060669169748, 0.4088715452987179, 0.20059369049733414, 0.8749141988093753, 0.833158130901206, 0.4753052179701201, 0.8703194224344992, 0.9747080227316145, 0.13043931789274588, 0.7430890289517227, 0.25830384596111816, 0.9418583018721945, 0.7886559685598094, 0.9395354808360581, 0.5492507482080208, 0.9448651431242203, 0.36125677192794986, 0.9774481632952051, 0.6536180800942802, 0.390573827801502, 0.9795787238948993, 0.9853470726248887, 0.47992223144554463, 0.7943923098901672, 0.34891415734041936, 0.6332611851236548, 0.7989682769960617, 0.4622012644603757, 0.47726130582901877, 0.898887921721679, 0.9862054838856515, 0.43966188987259675, 0.5932194830342336, 0.07484300636852308, 0.6145111305037291, 0.6737816449689679, 0.5633266691005372, 0.02366890716457297, 0.1618792775302293, 0.5485162635711204, 0.6456783569377433, 0.12707836807488407, 0.092398431352957, 0.4740730670009878, 0.3858023543077351, 0.9732653335831946, 0.9810909490720413, 0.9620494347430293, 0.9364442006515783, 0.9685216458125601, 0.3221170881031022, 0.9834737056215975, 0.7491379571471474, 0.40510188753198395, 0.870262726507593, 0.06398197560732957, 0.28868421594826676, 0.9252255835034835, 0.8218600982546752, 0.25886198714935404, 0.24698487524666998, 0.5615990986812959, 0.809044452529311, 0.9157835029638287, 0.47069619440538973, 0.39024246441411653, 0.5966627874537267, 0.6075316073619283, 0.5637225608402809, 0.7227291975000548, 0.7951311502253593, 0.3187863052955516, 0.8373959673877391, 0.701162687984737, 0.12567397574464786, 0.9586978586662205, 0.8066550802852852, 0.4122828387638471, 0.7509309529836067, 0.9002192525774207, 0.9857790744903424, 0.6903179369119236, 0.7542506266908628, 0.9481576735195106, 0.29407442523877114, 0.8050062221729704, 0.4097718491491959, 0.5746304975358928, 0.024767089450561285, 0.8739839046295238, 0.3615857657738849, 0.9336557248632946, 0.611262442890268, 0.9189449100435002, 0.9068188904485642, 0.4102070133429001, 0.9662743859988239, 0.868835831533879, 0.0575270672875587, 0.9418110482562185, 0.7735241601902703, 0.8337098875264991, 0.7491018095877477, 0.04343807879581667, 0.2488594802983674, 0.46500326939002135, 0.4298506233010541, 0.20337361670607568, 0.9842118633647866, 0.8465787125869354, 0.8793780107815578, 0.9368069893627113, 0.4809649190955851, 0.9564683039535944, 0.2339744175054286, 0.6126018325214135, 0.06485964549656371, 0.8155842052258298, 0.8360940804090004, 0.36466327264861825, 0.9070183276239497, 0.21471999876011896, 0.3565282877872413, 0.32553311063939744, 0.31556036608034904, 0.04633935026530777, 0.00781632086341576, 0.04392463756513557, 0.48544223287534943, 0.011622188650514795, 0.9027522134461782, 0.149688099215992, 0.6357625831548168, 0.8594692292181959, 0.005709605859394068, 0.3387196487526656, 0.35348936501322303, 0.7332107625941267, 0.7607196646137684, 0.1912983389658097, 0.9659294021748855, 0.7993911827541599, 0.8061873014588895, 0.7752413029260078, 0.8614070730838586, 0.9777219898973126, 0.4349288239435242, 0.9674198070498492, 0.4084070862487995, 0.32079894430071143, 0.05292006651621021, 0.9631964559631658, 0.4484548620060233, 0.1804876859020067, 0.7080002335153226, 0.49137753594521166, 0.5932140526219187, 0.9021183552751478, 0.7910493897948377, 0.09005052398401117, 0.5371165248758875, 0.5569061480837942, 0.09287619067289675, 0.19897486632552083, 0.40091302473582324, 0.2734655274018805, 0.6235126772785323, 0.4907288402322086, 0.8407445429353927, 0.8711104884039393, 0.5728437494088059, 0.9223706872144763, 0.5224717934285992, 0.2715417766665816, 0.7856072859468534, 0.2716672420926313, 0.2401838788601317, 0.23983934550896377, 0.1700554257547603, 0.9431056869103404, 0.04141281481519977, 0.3919262061080191, 0.8397669739785585, 0.1194045569440843, 0.5192030333223623, 0.7880895408260713, 0.8348748141898416, 0.11667371791495085, 0.9395708721916112, 0.5044876551416483, 0.5823704504196487, 0.6141957786711606, 0.9171889704039586, 0.6710366344741358, 0.601543144975622, 0.8930165596104253, 0.26382090413861664, 0.8947876179902361, 0.22413767009220661, 0.8273194986183389, 0.15994837310761192, 0.8683664233220647, 0.62071915590681, 0.3416011339885461, 0.4833206101792296, 0.7306591410690846, 0.06756452935652149, 0.873457381462022, 0.3427210543239378, 0.5509403235276285, 0.8145868599869792, 0.07792771857467039, 0.4757616340972621, 0.6893104934614532, 0.24911868268870208, 0.6093817310688546, 0.6846608052181555, 0.30528580403630823, 0.49747132179584375, 0.9752739702716723, 0.6808259392649936, 0.019152026526523095, 0.554578115228625, 0.46080826694702504, 0.5398956999998262, 0.7049297705699191, 0.2898182642871855, 0.5550851866271407, 0.0559464312415938, 0.514933469277788, 0.8088464975540586, 0.8788732914166333, 0.5552267840891016, 0.35987191843740446, 0.7549617003989564, 0.8720338833067189, 0.9480991394256116, 0.10445173810567705, 0.1376402471375076, 0.3034448755147035, 0.5893890976487975, 0.1119345325234556, 0.08292331117935332, 0.16459124380661963, 0.8071663050939963, 0.32563714737886884, 0.3939463519201699, 0.918195628120692, 0.7505334438601554, 0.32773163416074785, 0.8596817303652983, 0.18066212392427505, 0.7434726675280334, 0.7531714995220978, 0.35832681754870366, 0.3972238030627993, 0.1391274686395656, 0.2049281771632519, 0.761344288385066, 0.48872666937572357, 0.9867833076170527, 0.9388450383921535, 0.9498964453410425, 0.3734981895198182, 0.7555816564032931, 0.9710746084560249, 0.32160581640796293, 0.6077163126283118, 0.5956677433337282, 0.5908144494631958, 0.674920506670117, 0.24585143804461715, 0.8271802350892801, 0.8893295260267764, 0.9776407602020968, 0.9688939545368097, 0.9844100635756045, 0.7260387739235379, 0.7840460587768737, 0.4565415408036285, 0.937313685483305, 0.7406449514275495, 0.8602443619951051, 0.9519886517840628, 0.722770541017733, 0.9163859616867219, 0.06147380494609046, 0.7268477952402642, 0.7932485081160762, 0.41317498097395344, 0.5663561729759088, 0.441937999111502, 0.7999692916080298, 0.7303843701585434, 0.9925174002324301, 0.22766088653375943, 0.09781231530020393, 0.8190413463727658, 0.7788641463453186, 0.24716134612091178, 0.34352902918791733, 0.7859583066637914, 0.5004093573319163, 0.7704987601414076, 0.9345298947173426, 0.9827940402912869, 0.4398852340199819, 0.7779764468730771, 0.9818182594591119, 0.9303097336300732, 0.7198057135557814, 0.043327491836830205, 0.05886519596638329, 0.205980365195056, 0.6120175666853093, 0.9443159965903717, 0.1262677420366684, 0.4023865385607786, 0.8070326815374185, 0.8272279294364328, 0.7253457031254181, 0.22784817060361032, 0.9841577547554611, 0.6666421382828523, 0.5932839932568034, 0.6445786197788873, 0.9894537627992059, 0.581590686844259, 0.8566692291873406, 0.7085763610514245, 0.8163509318815043, 0.04511493130242221, 0.8905387798129589, 0.9872403886848423, 0.9310446765658612, 0.9849637501863792, 0.7628128136642537, 0.9676769511173882, 0.20369358357776207, 0.6366551016328039, 0.8148976751867468, 0.23101656499125764, 0.8262549544313325, 0.8009842706997743, 0.6796479298655891, 0.7865086882667556, 0.8359512990446081, 0.05508679154603352, 0.4266087771876618, 0.9885879773415945, 0.04923371771511628, 0.8543497539568685, 0.9441079860751547, 0.5557683397452493, 0.325285488630086, 0.43414822891722493, 0.2290721080077652, 0.8595864536738679, 0.543232482673848, 0.6121450520183876, 0.8959743250766838, 0.1206651744312929, 0.8429041084369343, 0.9621629450134245, 0.9798159207393462, 0.374004094984096, 0.9731089583322385, 0.3034579288220405, 0.8482453182345178, 0.43103025816944135, 0.8078425491641639, 0.6520915429780639, 0.870681120535812, 0.986163175700503, 0.8220374489509751, 0.2111253627516565, 0.9535341331942258, 0.8385145673204616, 0.9910213800047115, 0.03927219858529336, 0.7050871847999816, 0.9545084777080356, 0.9955375478511472, 0.9867300816338122, 0.4390344409292153, 0.7164313257697614, 0.5227350093982519, 0.8443251676572687, 0.9117583384403792, 0.5410533576277289, 0.9804653976590919, 0.9810879579824472, 0.43084510266515774, 0.748555533235115, 0.22774205205665202, 0.39157502326894233, 0.9191574024374785, 0.9719680694540583, 0.14979393511459788, 0.45968017255155535, 0.7320783224237339, 0.7124707481800404, 0.8373286973810684, 0.691017001710207, 0.03262793432931417, 0.9638290698325006, 0.38780272115569325, 0.48328905676006906, 0.9541952872192778, 0.853947340553696, 0.46756584406556706, 0.3903339104141124, 0.8734838558782249, 0.9686033026278613, 0.5513055008920554, 0.7263506905917964, 0.9381817769727194, 0.34892141698953205, 0.8710889680027794, 0.627683271159904, 0.745209926748173, 0.6864456675820159, 0.6754043722428452, 0.8091557522774433, 0.9777589998178041, 0.8705662647700727, 0.6228667387236339, 0.8246788718752369, 0.8272649868160168, 0.5709853814405417, 0.6008727834044432, 0.06365271402141717, 0.8085734527278732, 0.47598261950620996, 0.8344908359571794, 0.3339853107086929, 0.1976099800563482, 0.14499186673684805, 0.7234805377414874, 0.9622223058798536, 0.6131173513359975, 0.13050922788029792, 0.45006991110491545, 0.26297821983039843, 0.9318613222813219, 0.19455462020197817, 0.9843435652112729, 0.43739850714860273, 0.768008993674148, 0.9853106248188361, 0.22917089153732953, 0.41787261484343063, 0.8711659103095525, 0.9507829078432937, 0.600272966000673, 0.7588036867466731, 0.44952440721561093, 0.919953000137248, 0.9000960725295017, 0.5981944267890847, 0.7697044588706585, 0.43409785981033555, 0.44253609146778256, 0.9713358549698403, 0.596862297199299, 0.591175524420882, 0.559856026869088, 0.8386701542653642, 0.19423481808075643, 0.594272088732564, 0.9823001170087672, 0.7157893521871589, 0.8827852878824342, 0.5724534173128173, 0.9654815859653232, 0.3985938361301162, 0.2436774952339583, 0.3802685415634568, 0.43849963979061135, 0.5030098460531778, 0.31944201707873277, 0.8948710474828631, 0.7628714976747448, 0.868119905674962, 0.8662679638659971, 0.7193635029307318, 0.9847215495434501, 0.7931302923081854, 0.9067660517965415, 0.903401483068001, 0.7024775802032903, 0.4921922640523477, 0.3778105696053367, 0.5447378258571584, 0.9548504209492337, 0.7924287661695533, 0.9666655422467971, 0.5958235777990452, 0.902677424271782, 0.534363564707601, 0.39853098028674555, 0.872295122335913, 0.3804290137216658, 0.4105182638643926, 0.8979657780903411, 0.2013412125610074, 0.7269549428484022, 0.7448500822100693, 0.7468280004681601, 0.5892463117368708, 0.7535816179785173, 0.5277201345870783, 0.9625497750046379, 0.9428549249588288, 0.2014103512587555, 0.9842974338535841, 0.825552143147593, 0.9027574124427084, 0.5657739769148903, 0.3406965695737281, 0.7522671116048822, 0.4925236081644022, 0.8990250957533555, 0.5915803872226907, 0.9654499988133651, 0.5394483306947532, 0.4262930061221845, 0.40971852399086894, 0.960229381649431, 0.5620137355057364, 0.7715241575845713, 0.46356346615257765, 0.6392085400695978, 0.4648329551761937, 0.848054889191994, 0.9339625119940385, 0.9139018053360148, 0.1372942052640442, 0.021856791848707285, 0.9706436175709824, 0.6460426890925942, 0.6962619062580848, 0.985154133192133, 0.9211591456985504, 0.8030326194365274, 0.9694276009734872, 0.9751964589012174, 0.5443847114032045, 0.7747184633288188, 0.802832495852755, 0.5344852371935377, 0.35361215260201007, 0.708891643837649, 0.9870662936081318, 0.9886096684963875, 0.4405979295648049, 0.5436230203411696, 0.9525650612426826, 0.6108306566750794, 0.2852629103731753, 0.9621103133415813, 0.45586225640664374, 0.8854761418441123, 0.3054872633418877, 0.8185688951738027, 0.7777136324213093, 0.7699287703585435, 0.23489227050184655, 0.7485371117889933, 0.8092485466123099, 0.9136241879758893, 0.9289836771001613, 0.4177723938121609, 0.9081121205967846, 0.9576536845631027, 0.9260639286727244, 0.6597564227372296, 0.25877310826551914, 0.17904184076462912, 0.4113434466598989, 0.631212410753468, 0.5470934729159204, 0.4640640080722058, 0.8327988032589767, 0.2367525671365077, 0.1348732333084759, 0.5661470408777272, 0.5000921103348243, 0.4712421499162289, 0.9802302451703306, 0.9269706783115309, 0.8088072282959821, 0.8224404878151601, 0.5288230901021601, 0.7000785549517187, 0.5441951818049126, 0.8222590627894323, 0.23315921238165993, 0.16904667597126025, 0.9438679144546013, 0.8355718603505822, 0.9294992400145101, 0.8353144734214465, 0.9590204559018065, 0.8909051836006304, 0.0883293242331428, 0.9635835050451615, 0.23467883440666432, 0.9212475587539916, 0.9214958802274908, 0.5575499454643227, 0.7263825296827041, 0.9475533439915192, 0.7792273952331878, 0.6243374119867331, 0.8351118682562643, 0.9031701575344051, 0.49857609592425467, 0.7191327747983087, 0.788037363690153, 0.05484991902660831, 0.20908388192088742, 0.7980931470398257, 0.17375042215140274, 0.9560767585896615, 0.9414193062028208, 0.15275875823817506, 0.5997230640502635, 0.8356185734330837, 0.8505937454299896, 0.9554344276708413, 0.9430224260587997, 0.43587177605028266, 0.40111947892892014, 0.6862635286136197, 0.6299242810338265, 0.11501061728096977, 0.9867288722512831, 0.30752817897320406, 0.906046728597399, 0.2745021670683906, 0.514851343417491, 0.720755963873047, 0.31203081798171844, 0.926459771948186, 0.9588404477778175, 0.7114198682058054, 0.45285392003123937, 0.22219313385648692, 0.5619451590430586, 0.7514777344671222, 0.6497582812400436, 0.8633198035131351, 0.8478780680113852, 0.2018420243548737, 0.6830134827447399, 0.18551900309232588, 0.2692311997188636, 0.6834698503636057, 0.47892366863935004, 0.1467847749175432, 0.877439447760118, 0.3551115801175475, 0.7389274386745369, 0.3610707914723244, 0.9638336344002204, 0.4142978031219304, 0.7382823531744158, 0.8533292122554987, 0.8661230066705231, 0.8419878939251498, 0.2049743892192254, 0.15705711711055592, 0.3903485505030245, 0.8678308658338847, 0.9044540866641266, 0.8713729593931206, 0.01444300026598962, 0.808967732287225, 0.15922478187657926, 0.8867675458831805, 0.6675183497869306, 0.32320990144865314, 0.8394457543974256, 0.644091069420722, 0.4078585125717723, 0.7480479068579996, 0.9550737314633239, 0.528329245463507, 0.7486363618074517, 0.8120663908549568, 0.22854497496629259, 0.2019323070587914, 0.07478590550724948, 0.7895869250953589, 0.36357912318763635, 0.22610681614440314, 0.5366432990511644, 0.8561155989403658, 0.4899894132760497, 0.3183481606126503, 0.6974768522971008, 0.8450412151714941, 0.803849002255275, 0.35035012793387565, 0.33094938028537557, 0.58713504654045, 0.46603698412391914, 0.2532988937972076, 0.6432368307812446, 0.9115945920020542, 0.5547682239767001, 0.914433980461877, 0.5771758360145457, 0.379785945034663, 0.2807079410629272, 0.6301865085995906, 0.5667730120913788, 0.786389696368155, 0.8370611658090186, 0.7823579839012814, 0.9583032650575881, 0.5261781526890525, 0.7386385988183595, 0.8283432207900654, 0.6777864896691078, 0.9575816534145446, 0.553168830384011, 0.8105515174024314, 0.8929928703214162, 0.8848235284264679, 0.6847361298823351, 0.838081165445737, 0.44460674004447953, 0.6943194127639492, 0.8857479551921881, 0.5019071191497748, 0.716631060251531, 0.3238333170729525, 0.501590688453044, 0.8688733399415534, 0.7808230965842653, 0.24950873125374926, 0.4851371886333508, 0.6191562167372956, 0.9127512982322374, 0.611537176534941, 0.9383384015422842, 0.7460226790552472, 0.9778036456535216, 0.5064499468810957, 0.48321921878063806, 0.9270845698998543, 0.7138112996518586, 0.92693711873106, 0.6672253318548242, 0.8744446530221089, 0.7912148641318145, 0.27306290412904693, 0.7004413999209945, 0.8029792932228489, 0.2682383797608175, 0.6427437440380179, 0.9428408945838259, 0.42590736503852417, 0.6252027903987872, 0.2793128212046009, 0.7051420630798528, 0.728008202888463, 0.698954905542286, 0.7115339739878871, 0.8827499828404024, 0.3466805143043107, 0.38270273404070754, 0.4986441103151791, 0.9195178697557332, 0.8230060283027881, 0.5585810838160716, 0.7736632106281123, 0.45791640957934043, 0.8100905431993817, 0.9056700038979325, 0.7002688097415739, 0.9633252568223827, 0.2588054504961393, 0.9401853528342657, 0.3716090668713618, 0.8577369637266306, 0.7775004901671612, 0.5627498777067856, 0.8442007954749251, 0.8076632536627206, 0.6466855975839357, 0.5485021372645417, 0.9252733142137489, 0.6058277151166621, 0.04203492403839814, 0.6947153898362274, 0.6463663158986881, 0.5554678742283, 0.7989935661499885, 0.10787212351740677, 0.5409439881697744, 0.28640389154323564, 0.5838994673181855, 0.863739019088763, 0.3317327439122225, 0.4144434587098896, 0.46808645105121754, 0.42234075329131476, 0.7257613912203567, 0.4971809543090053, 0.6758078180062338, 0.7378859133315703, 0.753671202727884, 0.5798851161783455, 0.33332172968142604, 0.2686314038901909, 0.8434530187608598, 0.6879454870069599, 0.379973056100794, 0.8144852104879968, 0.4707469945794664, 0.5423455982001557, 0.8001393600688703, 0.29138015618247043, 0.8987262864584118, 0.561590125988598, 0.4682858800570236, 0.8261167556477625, 0.8637739038857268, 0.6018471864519536, 0.6783727248796719, 0.7264495340268801, 0.05953883969221017, 0.4590083452570568, 0.5311706715876311, 0.9163219594208567, 0.4505053049073027, 0.39548304439519166, 0.7512001111682223, 0.48417712476946323, 0.49907083861533813, 0.8897702524125461, 0.31163097733413386, 0.7287675599623135, 0.9374676676512479, 0.8005762315470032, 0.8480596668314642, 0.7316243828632057, 0.25019190305927075, 0.7301592559863239, 0.13357464491893922, 0.4185352773258327, 0.6798005674487472, 0.7930796432965638, 0.8392066617639267, 0.4249979608430918, 0.6630300128192773, 0.6420916929463644, 0.24223155278615696, 0.9170330185877674, 0.22664327737919585, 0.6115927443027767, 0.3635428758673965, 0.12030756825143923, 0.7922979110749954, 0.8165048343835771, 0.3655840337486277, 0.7791394991822794, 0.03375457090124942, 0.8316096476486137, 0.686444673487521, 0.6343571181729362, 0.7851906195957489, 0.2131296220196578, 0.39324183212270936, 0.024416372335831417, 0.5965941864080047, 0.27539685643669415, 0.7148000595926062, 0.3339853107086929, 0.12855252389812588, 0.059645053636358254, 0.7331513362738741, 0.9372074830626178, 0.5630623846180748, 0.7975390154175769, 0.4680198184951762, 0.8029683465746954, 0.5920770349124816, 0.9661596439541819, 0.4796551940144375, 0.6756134062286656, 0.24529012090435884, 0.2743853720942695, 0.43990332353030054, 0.4357900839811348, 0.8057543911040695, 0.7760852699662713, 0.2454095061632777, 0.6814875383767008, 0.2427390660818652, 0.3069508582505901, 0.429962650068998, 0.6007673748586436, 0.9089187790049787, 0.2985615209008822, 0.11905981461817593, 0.7479890001335595, 0.7277176474891693, 0.5705168216680483, 0.9744792385776394, 0.2882732079118999, 0.5714395295624144, 0.8946575334258281, 0.0742079698666063, 0.6779733176290325, 0.4769463256054319, 0.2877796089666747, 0.3237399217270849, 0.1674227983537129, 0.6344361367834406, 0.19804064612558217, 0.49695890062945164, 0.5661638891274684, 0.8890298706960349, 0.7941090052071866, 0.8262964838269218, 0.5328201625073042, 0.7733123154742373, 0.4501384197461176, 0.337336926033961, 0.19317432352896502, 0.3152105656071218, 0.4898392881490591, 0.24358324250784602, 0.1651740422922886, 0.4616334501978091, 0.6260887119291849, 0.8448045877796646, 0.8875086937214526, 0.9569204265255813, 0.8583614584663615, 0.7454214625504887, 0.44847700414885794, 0.736465318300746, 0.298996383797972, 0.5829462195927423, 0.6319086778565632, 0.42840612706845654, 0.4798941881532769, 0.6115143475319381, 0.194842574349035, 0.78748916738129, 0.9337432341525704, 0.12462224010244669, 0.08865480062505408, 0.8506079104840115, 0.10833999271847607, 0.5827104672931156, 0.8076176848147082, 0.8758731273266455, 0.06249392546345528, 0.9376864684138569, 0.5126473749592868, 0.7533868964323371, 0.8564017310351467, 0.9668327534499386, 0.4598539915382624, 0.9289362233036723, 0.22841621092888623, 0.5100667009327895, 0.5703110702542661, 0.1281392352773042, 0.5353525110500984, 0.03178088952656153, 0.5925859580067542, 0.5398966404253286, 0.4702651079358588, 0.7478545619134783, 0.37893099430582244, 0.7320189633325638, 0.9751869582744495, 0.7817715464528946, 0.7735571260013164, 0.9607880490665768, 0.9394917137812057, 0.5488958452564265, 0.4417420495779112, 0.33016051951146264, 0.46454089751956146, 0.6415320570808709, 0.11970220957311047, 0.6092402507619357, 0.6033085188935152, 0.282030987320365, 0.5460941400652941, 0.5328455008291471, 0.16548664233739557, 0.35541008089960113, 0.2543429319214324, 0.8118371802129276, 0.3016220128232416, 0.6823465739170657, 0.4842749571118772, 0.9388687321433997, 0.7422833592478096, 0.47730457887612515, 0.565904790039254, 0.8678717732103194, 0.9059237934631864, 0.7591499249546559, 0.6235462754249615, 0.902833013153899, 0.4052950648400916, 0.7239782387565041, 0.37378454389346555, 0.6144489933397779, 0.7905915975697372, 0.713530595418023, 0.9509756055873841, 0.2605294353889972, 0.4992564372754758, 0.8175358735077926, 0.8858177068125441, 0.44006437934329573, 0.6669615473723743, 0.5725199852843543, 0.1287624311259, 0.8043460828946329, 0.6806957100377596, 0.591034055652471, 0.24452687341699914, 0.5494948464099858, 0.3359131915042288, 0.8119000295370797, 0.7553680137578407, 0.04651072340470949, 0.6840892563688249, 0.6051143940331879, 0.19766132963360766, 0.21584633422619218, 0.9436078842211498, 0.46144174316358494, 0.654303243783584, 0.4066064644380243, 0.7300226573354549, 0.5657611803221022, 0.517319943676148, 0.07229332445901801, 0.3467912427679765, 0.5456343858965179, 0.21576363623627892, 0.8880473707557166, 0.8011737249971406, 0.8996584707516603, 0.9763691514592256, 0.8485301285480044, 0.9224104089835437, 0.24276151562454534, 0.7614152321776811, 0.32634172188348487, 0.6782377916375154, 0.33806547249720387, 0.5564654545246481, 0.8244942479020365, 0.8054237026025775, 0.9040170760453716, 0.9329730316244826, 0.4526591487583528, 0.5047039763821337, 0.35596895334949974, 0.5750291780770277, 0.4884089733748289, 0.894321809025103, 0.2596275723053589, 0.41016055784387223, 0.08241836672354516, 0.6673157195904279, 0.4162510596369788, 0.6434076505619961, 0.9450501438844507, 0.4818422698929155, 0.7520026997550064, 0.42826635223929804, 0.6393313469869188, 0.7547230220451036, 0.1856837183176025, 0.0032021684534628975, 0.5539409395381298, 0.06717533133098894, 0.9467745469420854, 0.5070348354256019, 0.9284183357867076, 0.6080051392848859, 0.5804688749244391, 0.271466991459375, 0.038471669030322495, 0.7850903637157398, 0.6920331636963356, 0.5810324228611465, 0.9299698084063382, 0.9375258477311266, 0.5171595120405628, 0.19462488632052333, 0.6464733210603558, 0.18017046557548594, 0.01048688716533385, 0.23303210402666324, 0.4138009500288487, 0.05060143284060895, 0.2879349518248186, 0.04320048428879737, 0.12250792060494733, 0.5648050613968041, 0.41274447945584414, 0.6506943204108897, 0.17626208623478987, 0.2722823168439713, 0.2798233553752671, 0.8487510100520308, 0.2228610739885683, 0.5659679441512675, 0.455193382469363, 0.3851741066402977, 0.9827764429279281, 0.23735673779103122, 0.29795533326619794, 0.6256048695264618, 0.26751651839414053, 0.11598178745069791, 0.37172303890996733, 0.490200272431638, 0.25537892563773285, 0.12933471527168097, 0.7061315980934053, 0.5510380170513474, 0.5952257985256588, 0.40442525947040137, 0.4034582415552023, 0.16396581433230137, 0.0696033612056323, 0.37634313101317124, 0.6305300590459321, 0.2935695725886229, 0.4431024548313214, 0.5501839515225913, 0.08138327620249837, 0.08478175993570336, 0.28239072020238437, 0.2383184781572384, 0.751828759933559, 0.8168324305722042, 0.11138999461447388, 0.33681525754337105, 0.09480701199382485, 0.21688394328616972, 0.27654745800826447, 0.32746905362919254, 0.4203224590556732, 0.36658898655096706, 0.04519026898082502, 0.3745237806869271, 0.09501042227497628, 0.023338651909088678, 0.9723509218190695, 0.09401551705210953, 0.49714179719765417, 0.07989600909561846, 0.2180418642802576, 0.24051971093915225, 0.6572667998752273, 0.6089120623206872, 0.5385042561954457, 0.6299654197194743, 0.5559674948375231, 0.10360676912955677, 0.8863731836625508, 0.46623808860742116, 0.28269681892059273, 0.2323973401827282, 0.22397671878584718, 0.14699871184130295, 0.11264831116963035, 0.15222578463070283, 0.4900524762025242, 0.3467250764253939, 0.3716741006291789, 0.8760514282145069, 0.7322960020582586, 0.29700581343433535, 0.26234013699876735, 0.3609382094672238, 0.28882123154457134, 0.24715116618740043, 0.074150691596693, 0.1877364591460827, 0.5975062837719228, 0.17831602479866515, 0.6652230441456962, 0.1657826052525834, 0.6149119497250476, 0.3427006423949688, 0.13602586106080333, 0.46100807621280704, 0.44546070817643685, 0.14234690762987748, 0.5183360267380727, 0.6580607221819245, 0.7537746825308342, 0.1695771644022048, 0.22754140494699243, 0.5642405802838937, 0.2916179779421427, 0.24561860912667483, 0.32651176126446696, 0.5079014441823055, 0.3400280228297853, 0.11207851832819041, 0.653532424406224, 0.04426811910008972, 0.6505999826892177, 0.03978985133627003, 0.6325822505832972, 0.35635258750469, 0.9551242890415118, 0.16467659128533943, 0.28467143221948177, 0.18496422835086676, 0.3437751248991377, 0.1489967761119895, 0.07591847876721403, 0.6107979817617271, 0.5154022668508889, 0.3744046008441108, 0.904945441643859, 0.6576792755301105, 0.7107737789179046, 0.3965105857976064, 0.2364839298223994, 0.34632367719988455, 0.02942226104599106, 0.2242460609478228, 0.07676677184731003, 0.4545140289643748, 0.6819534155260006, 0.0621970733355503, 0.39453000955420836, 0.3014418772736327, 0.6393716913715913, 0.9053209204431757, 0.7816507882643264, 0.694023092541776, 0.27182749549435226, 0.05202909107072356, 0.40506976187353627, 0.8908106087917109, 0.12052441804377126, 0.03672912059293631, 0.4347818155197854, 0.5235743472851302, 0.5591898766443947, 0.2751778392753225, 0.4586072262119472, 0.5666830192588578, 0.2558948962531558, 0.4390212786460714, 0.05562359593891943, 0.33463373106115774, 0.5393800596519595, 0.4592781888318605, 0.4896490981641464, 0.03787229729195549, 0.44067697250836246, 0.0420084720999284, 0.5879976245353381, 0.7080844311268623, 0.32554399263539663, 0.02391443393517213, 0.3564038388941197, 0.05234857127558486, 0.29524383526133335, 0.53923953167942, 0.832548663998778, 0.025184255359066585, 0.2675609583683608, 0.5605113386301857, 0.5489213043300105, 0.7017796837428363, 0.48916106453353336, 0.2824529629919752, 0.367024360463113, 0.14734066222414516, 0.5232679937014778, 0.5963186728081795, 0.2447295510396471, 0.5530466395060961, 0.18673296662742755, 0.3953924928011752, 0.7064692960302841, 0.10938871929447587, 0.27639676705754646, 0.3101941788287516, 0.24715712598676076, 0.878457791144506, 0.6737120614584453, 0.3373011909707462, 0.547263843207008, 0.188190184328505, 0.5254804657938296, 0.6950931372146364, 0.45251976899213087, 0.32627854777753235, 0.028532346942236983, 0.8255780844453109, 0.16219018059349166, 0.26130214855488393, 0.04477828220185625, 0.2008106340775549, 0.06540325661161059, 0.282525163075737, 0.07787294886079531, 0.593535382536</t>
+          <t>[0.5222559148666296, 0.6881888303306357, 0.08619003684737968, 0.9907612455696236, 0.6285012200404044, 0.8366293342983186, 0.7883225050277324, 0.3004624531601982, 0.7719113360845763, 0.08517211103266799, 0.8689567852448683, 0.6992715946371852, 0.8077864772798771, 0.9631032900540073, 0.9426994977151234, 0.20930632775828456, 0.3938263667851605, 0.32887564843067596, 0.14071670910285952, 0.6753866698168709, 0.8023716121570698, 0.35778512744600555, 0.9487505307537597, 0.3002754914135645, 0.059758566411667866, 0.35525819290820526, 0.7011967971176895, 0.32732098599970194, 0.6168704809890986, 0.4985205118285779, 0.2690952813943193, 0.5822788496460776, 0.8012447527066927, 0.8033934909232121, 0.7907695839196125, 0.8769212544372537, 0.8994769919636483, 0.6815054779959637, 0.8061754516496126, 0.8258890207397237, 0.8354660792824875, 0.8461739924975623, 0.9563698837232887, 0.12008367460945452, 0.6634815055140973, 0.5549641061186622, 0.9668073896827267, 0.8962893159875595, 0.8618432159061155, 0.7350164043496824, 0.8483483916533685, 0.7553926770248396, 0.8014709986375503, 0.48933576769815135, 0.9709158450613109, 0.9203436416027355, 0.8953295937889781, 0.7567529930272111, 0.9550233040817517, 0.4638562215414024, 0.7425960963958803, 0.953778092937943, 0.6786245669097577, 0.7500239753019311, 0.940814020741551, 0.9577271547736202, 0.9241512244231864, 0.3247253729402209, 0.9395018993813882, 0.5443684560405789, 0.5397834347886633, 0.6329484869849636, 0.7648354014262805, 0.8406490926468722, 0.9560710510163978, 0.9531714901721022, 0.9278151698997126, 0.9890147644138316, 0.8876114136942329, 0.7403288774977947, 0.3513575925444804, 0.8902000107483401, 0.269649988489729, 0.8155006176426433, 0.8331804219624102, 0.7249599938872361, 0.47044389667437353, 0.27997593732540327, 0.9856635371407637, 0.9249268696157024, 0.7260077470605294, 0.8489968287341555, 0.44383970947623586, 0.9718940714072641, 0.7716868696611678, 0.5152599630002305, 0.2713985657943165, 0.6949398999532183, 0.8738246654231767, 0.942066844841723, 0.6769823814424185, 0.4587117642438351, 0.643421138735452, 0.5705894549330399, 0.8503228749859587, 0.7031809869169643, 0.9763595252028149, 0.8652729435576524, 0.044408289694877694, 0.8285265874588055, 0.20480789365178773, 0.9572418984327118, 0.724433255974329, 0.8426328700663185, 0.9279242701888321, 0.847099103085505, 0.23310456724642742, 0.7470699342477343, 0.4903925576998933, 0.23782176974387498, 0.8605322240935603, 0.7444695059621368, 0.846858362074887, 0.9945269443458168, 0.9312771478701789, 0.9582872322108162, 0.5645389246528646, 0.9138953641738327, 0.7077705757197176, 0.9879062209806767, 0.3844229912091994, 0.24717736921491854, 0.03368834464085001, 0.5424583078598689, 0.5935923842572051, 0.8551588345796034, 0.8760059960558688, 0.4052684702403691, 0.539819768206388, 0.8126855300698878, 0.9771538241921846, 0.9545385834657603, 0.914566774754986, 0.630314066357475, 0.677353863188806, 0.7655963440964075, 0.4972969959253654, 0.5651171588832389, 0.9693865661111519, 0.8670946095454164, 0.9674651441418688, 0.08176603334265269, 0.6474291031902523, 0.4074694597289005, 0.889870215955426, 0.8104032850615133, 0.026007990074367476, 0.9435795324854287, 0.9150285403900806, 0.6717350493385874, 0.14738603738173542, 0.12978339293611701, 0.05544565257035077, 0.7759685643516077, 0.3795275385254955, 0.7011940404119775, 0.4236450672001863, 0.7044469285173637, 0.6629056582184735, 0.9028212946550727, 0.09400147029111626, 0.9209891432812217, 0.6294929137147911, 0.39895984634504644, 0.374411413908452, 0.5853083730110271, 0.11516755257486821, 0.5595199321377164, 0.8443336224816427, 0.8277243705637565, 0.7256968685654669, 0.7836658940031637, 0.29493142158850716, 0.9236776399873247, 0.8018046675329096, 0.5768238315826059, 0.9516951222427485, 0.8447206382601525, 0.08103778351823489, 0.8741924084654639, 0.9363707289529472, 0.9319275236044842, 0.7703759569943751, 0.07539587145186681, 0.6310915360411532, 0.6380739236887848, 0.8241051295924778, 0.6996860388599652, 0.6881911768913208, 0.8851890902672689, 0.24360471795863076, 0.8193747183789755, 0.634907673580121, 0.5889006805911937, 0.5402947347028398, 0.6085643703757755, 0.8810176465768992, 0.12970628560624242, 0.6906448459403036, 0.9855133879118323, 0.4393664731902737, 0.9373538727375943, 0.9715221452545775, 0.17533881884630687, 0.956865759754995, 0.9499931511579284, 0.8726185015404544, 0.772344596324687, 0.5552520697259854, 0.6302373382717054, 0.6071311481394467, 0.2437231130778051, 0.612629277515103, 0.6750108475033942, 0.0030414071887191955, 0.5641704713526913, 0.5299880308182151, 0.2676416245265211, 0.5104314701233287, 0.13265248665346843, 0.8940048737698295, 0.5434341868410355, 0.9511406764378018, 0.6763827267301031, 0.11145505021755177, 0.03325646644423224, 0.09784671060772684, 0.09068599712484797, 0.018569119621637188, 0.1283184982124193, 0.6217953699571813, 0.06250572777803393, 0.08708030274434604, 0.12971678089284616, 0.7572693630939394, 0.8891099936314381, 0.8891822834366071, 0.5724085682738519, 0.6787289423367685, 0.9153327250250061, 0.10121541759024845, 0.8937285302886717, 0.8875005399520555, 0.4218484047178935, 0.6991299505694829, 0.7353768028532016, 0.043858862155253364, 0.8171372184326569, 0.9947220671375057, 0.9350548594697141, 0.2640480809326021, 0.06340675627945085, 0.9186312692517002, 0.47785796715821344, 0.006280552099495135, 0.0656945829176645, 0.6073820092606149, 0.148423596767467, 0.38262293668302727, 0.12895139139794184, 0.25707486589573286, 0.7114011231174527, 0.6737807756660433, 0.9509775404920563, 0.8959504627677801, 0.09049978350756623, 0.20605056240383032, 0.9762605751963552, 0.7182007441361001, 0.853194122222274, 0.026516460410403613, 0.09860208254721184, 0.9539867911174733, 0.7826265633038674, 0.11139420956983724, 0.684450045988784, 0.40999788213097194, 0.9855300615865504, 0.15089931436055112, 0.608581047292871, 0.9347069559474078, 0.7315438847798071, 0.25262552425438317, 0.8685271853794945, 0.736070387570856, 0.7030918249547982, 0.4976258667677201, 0.4382719578827652, 0.20029554768296773, 0.04999681617803239, 0.04477616911360058, 0.195683268125496, 0.8937502437575505, 0.44868538240055283, 0.24172886310392844, 0.8885048492568743, 0.8404849040658029, 0.49072393375335527, 0.862386282983713, 0.9760885751719879, 0.11960563483039256, 0.6662439797603599, 0.2824609036601953, 0.9508941643982538, 0.7475889682758329, 0.9410451362030922, 0.4848902598457274, 0.9414443475939948, 0.26844817865160125, 0.9750755615490468, 0.7412213883229496, 0.4194069289926434, 0.9789942911403935, 0.9822063519698901, 0.49043254713729156, 0.802267392322149, 0.40918566819705965, 0.7605476136180832, 0.7819915458605022, 0.453649422102472, 0.5152174312405774, 0.9222280662078522, 0.986725026339961, 0.4215677854074135, 0.6124128544856908, 0.07582774644883904, 0.6226102852786302, 0.6607528537682194, 0.5647096471105193, 0.020905828312931397, 0.22367903821843643, 0.5091070127003073, 0.668303999148497, 0.11589921375679442, 0.10154238960788559, 0.4118595630373926, 0.3233606359505509, 0.9729864281462385, 0.9784564105281519, 0.9466702585417994, 0.9160598614156948, 0.9604647326970348, 0.27057611099561624, 0.9744257273687388, 0.7834264406049483, 0.43479673048984124, 0.8658090878275312, 0.08223045887590312, 0.275064885280565, 0.9199485010719769, 0.797881955191999, 0.28726296345837565, 0.2419776548723126, 0.5676879516288365, 0.7848005454941369, 0.8990951487443416, 0.4827387224141541, 0.39544614572238546, 0.608441285149847, 0.6464976704146909, 0.5889634036285142, 0.7055547504803844, 0.8053186311312984, 0.29597389024097115, 0.8782844645720771, 0.7224569063071478, 0.14018562145109784, 0.9633742810151473, 0.7522905756183845, 0.4111190473728782, 0.723855153261405, 0.908465127249623, 0.9855968737353, 0.7589530554046621, 0.7307129439745454, 0.9550697487504481, 0.3111814531784073, 0.8319514240450596, 0.4593227859740595, 0.6054343572617568, 0.02602307362416298, 0.8604132508582683, 0.43626392665705055, 0.9341619773073044, 0.5874116980666156, 0.9278157485417434, 0.9156156110241171, 0.46075975078481735, 0.9621154306127712, 0.8940156946164254, 0.06233623102757897, 0.9296905096607507, 0.812570336622375, 0.8567661952351117, 0.7716552477977928, 0.03594856708089934, 0.25318839734778614, 0.4646220937935422, 0.45050186249735363, 0.1657371056801563, 0.9858384898559827, 0.8450996954012878, 0.840257115367256, 0.9477340354968464, 0.53813895718333, 0.9460073227426008, 0.20402855887460397, 0.5854702706101569, 0.06789370638930965, 0.70609532797403, 0.808311373615574, 0.3688593714392218, 0.8901324774358288, 0.21406522801266975, 0.3827626032862136, 0.30887637967085246, 0.2799412960528026, 0.05924337735371716, 0.008337909476762042, 0.045802488026445584, 0.4892371800010675, 0.011333727624695696, 0.9262139925033235, 0.2022806274025099, 0.6157448148572299, 0.8721558476729453, 0.006230602411398131, 0.495972461302935, 0.3345470774242774, 0.7471821540684885, 0.7564783307200791, 0.195083568924436, 0.967503390172017, 0.8296641422442659, 0.8522715577993363, 0.7951738679718614, 0.8630555878399143, 0.9763152587118951, 0.42845873387277944, 0.976721033804008, 0.4307575504240516, 0.3235222681770004, 0.05251235498309744, 0.9594998964734156, 0.37685767427562905, 0.20252963870992288, 0.7253249068321415, 0.5179951540712374, 0.6393576763690919, 0.893619550057172, 0.8117611703345777, 0.08993053451080567, 0.5441375283628306, 0.5240379164832343, 0.11515960071947759, 0.1917739120117615, 0.39648809885620334, 0.32411933351667177, 0.6677384859732843, 0.4461618568209198, 0.8610164395393712, 0.8793725931435554, 0.558934448077533, 0.8981724591511817, 0.523116707376604, 0.2667218505618064, 0.7833589294232723, 0.31867158305576276, 0.06895749280178633, 0.23291007114405643, 0.1738820060554177, 0.9379649647427855, 0.041139687558089624, 0.39463396585929583, 0.8511149535077724, 0.1238864053960408, 0.4616506754316289, 0.7803910561733233, 0.8155109972018019, 0.11798173860063262, 0.9390545722152808, 0.590185111461269, 0.5595210124615586, 0.6771157180271666, 0.9099066250488073, 0.6671179983908441, 0.6163458129727698, 0.9213162153220169, 0.22411544969910024, 0.9004781705169955, 0.2502545214509191, 0.7875949804583289, 0.2577541880114281, 0.8671555371154259, 0.6198145487609292, 0.3735530241768628, 0.5184560270931432, 0.7291911480501811, 0.06079746608886574, 0.8209011687595364, 0.35072419547824724, 0.5743720546350223, 0.8447034236791504, 0.10201430028971921, 0.5341023426782596, 0.6603374416112986, 0.26019307018435195, 0.6611272524158178, 0.6217620235399826, 0.32442613114587643, 0.48386406323163994, 0.9730280244751546, 0.705891283031606, 0.01631364141369546, 0.5629578018792405, 0.4606169429735701, 0.5677521787949091, 0.7184793618306031, 0.2789227101719856, 0.574813604550208, 0.058966848158170576, 0.49206335982915794, 0.8212812739327426, 0.8873897676278776, 0.5865168202889477, 0.4120349536839423, 0.7474825382484304, 0.8514452062840664, 0.9334671223431267, 0.12603012887008155, 0.14399488164929272, 0.35017648552535835, 0.5903994460567467, 0.11683984070081495, 0.07648739047198536, 0.11374031516331785, 0.8132675536582088, 0.4052809186407532, 0.2881593722211369, 0.8956753796215973, 0.6614582738899675, 0.2511052583006493, 0.8482759461069203, 0.16691431166018827, 0.7461286723244861, 0.7424336284929309, 0.40164215013053794, 0.2704394416650606, 0.13110154431430368, 0.253270404648338, 0.7218378750402271, 0.4251116253098255, 0.9824532162410685, 0.9312868796143504, 0.9468248083449473, 0.3239227542506685, 0.7841805382465353, 0.9689396410680916, 0.2165868631413703, 0.611723615752986, 0.5519864476671903, 0.5749522118862819, 0.7387029237221265, 0.16559555341564536, 0.8088710791951282, 0.9129424458435154, 0.980229739870284, 0.9761921025382903, 0.9786171987110083, 0.7129838954959441, 0.8055794975770345, 0.5124138128925503, 0.9368233342692945, 0.7199352519127256, 0.846642772265491, 0.9478266125508401, 0.731406824729748, 0.9221708460232577, 0.0644319241770957, 0.4739972368833307, 0.7850611459418537, 0.38995384283472684, 0.5299461565539859, 0.4731350138030495, 0.6508097625130292, 0.6527058853423406, 0.9927197322688287, 0.22548264812250604, 0.10122105955894459, 0.7915398169212574, 0.7605950597499079, 0.24516532418932915, 0.2814312287934776, 0.8446876607618875, 0.4365450048269571, 0.8126660096105983, 0.9333111172647283, 0.9823796974692384, 0.4616148878362177, 0.7994948190291636, 0.9792823353704079, 0.9372033179154721, 0.7264554112780429, 0.04908022391374409, 0.0532694614610018, 0.20282962867713952, 0.5897653087242353, 0.9566933786528795, 0.13002090080226725, 0.36388986271498985, 0.7965484395442515, 0.8277970818578453, 0.7486401178720254, 0.2201896424402976, 0.9845873066731173, 0.618010331943053, 0.6364187263882536, 0.6406762587950007, 0.9879297390727095, 0.546119874958919, 0.8857895419128525, 0.5946967849567362, 0.8504810826771808, 0.04030346811943554, 0.9086849445919916, 0.9815177247387052, 0.9328372166408174, 0.9852473303127537, 0.720937184182207, 0.969504659437664, 0.2449473039509442, 0.6804703176931842, 0.7962089836866769, 0.21951058662148906, 0.8485086880801339, 0.7568580688356874, 0.6713122742767217, 0.7784976566403271, 0.8404513106495551, 0.053161416990606926, 0.40710666878908214, 0.9861492161649111, 0.04828393954757527, 0.8731612580883614, 0.9457234234243866, 0.5625682631130553, 0.204653553099178, 0.49254273123993625, 0.2241666616638066, 0.86959850506855, 0.6755241427576487, 0.6376129790980665, 0.8986540654549879, 0.10671661701896856, 0.8455324803711964, 0.973073517651439, 0.9759520818429068, 0.41826665272985086, 0.9696916912880339, 0.26788760739368384, 0.8037852033529933, 0.5502735784669084, 0.7970257880541968, 0.7028932080964628, 0.8440279342332987, 0.9871224233957459, 0.7771636675419553, 0.15460268094624874, 0.9530820160579435, 0.8285149104711077, 0.9893965612207278, 0.04148679396048745, 0.6881202223690396, 0.9471335249473328, 0.9965816601847689, 0.9828393623742343, 0.40653277626169326, 0.6475928980241783, 0.5338473693235644, 0.8226106805203746, 0.9180514977348291, 0.5395789139390832, 0.9754538233544363, 0.9785760691527549, 0.4847765082384238, 0.7629122963136623, 0.2948899200025969, 0.3922872862598755, 0.929974389272699, 0.9719566714986806, 0.19879180082907696, 0.3353303547936236, 0.7558432804550345, 0.7410213620848504, 0.8197193714401928, 0.6047834356610597, 0.037602728148319935, 0.9569297248437867, 0.39375706211732403, 0.5184573750009451, 0.940787025760847, 0.8204610859835187, 0.49100935815689856, 0.45309009641603326, 0.8337332828686497, 0.9659503297196885, 0.546812126183172, 0.7498969203859609, 0.9409968682348128, 0.42081252427164373, 0.8498000805400567, 0.6821874922584166, 0.6957996672955526, 0.6576178103116969, 0.639775327701615, 0.8325001837377685, 0.9822277866323292, 0.8448384127718458, 0.592136865528627, 0.8451267058481183, 0.8099253855524601, 0.6028237201808355, 0.6826016495044824, 0.05941884725979708, 0.8440795279856145, 0.48179971930878873, 0.7899269868026477, 0.3544556614731711, 0.19465610992277718, 0.16204449462571777, 0.6605795051091845, 0.9622668589283071, 0.6049773628317894, 0.12887267848212708, 0.49475010600346225, 0.26983621913136957, 0.9073961010838814, 0.1902666354168397, 0.9846051556802561, 0.4451308525474345, 0.7282000599467854, 0.9856694907634053, 0.23622585288248246, 0.4277693230990873, 0.8741337412552909, 0.9482781423451508, 0.5321786950669559, 0.7696407516413142, 0.45374941235615407, 0.9227865720177161, 0.8989108257036779, 0.5577229038847552, 0.7866661855331937, 0.4446679848490898, 0.44218178092502236, 0.9690288031134826, 0.5776733764297526, 0.586024630446389, 0.4919829034847323, 0.8384614157688014, 0.20170671731847203, 0.5508980957182452, 0.9819458865898453, 0.7128170027175363, 0.8773573529060574, 0.5910554068193735, 0.9658793433721458, 0.4259311306926934, 0.26140594257307004, 0.36384149760866297, 0.46667789428905043, 0.5484811391819362, 0.30978355483641395, 0.8994962128406188, 0.7423921469825683, 0.8512941188639034, 0.8688366292594913, 0.7331938933403293, 0.980781549972055, 0.7996871629367723, 0.9213543258226121, 0.9082496804603879, 0.7055582161643837, 0.4929057930287804, 0.3576822472929641, 0.5601154680109931, 0.956505756785581, 0.8075272875318698, 0.9591329337558088, 0.6064765360041682, 0.893570057632708, 0.5428651576592106, 0.3617297643739007, 0.8804529225679648, 0.40884246707198973, 0.44625109843487887, 0.9146557856686512, 0.19399850466523458, 0.7216885814405659, 0.7317206301418336, 0.7624400487098446, 0.603670815780089, 0.752201216630103, 0.529180793069277, 0.9621319558255237, 0.9430934213735622, 0.21728604643168573, 0.9830003737037619, 0.8355550454749848, 0.8952481156581288, 0.5864607183479374, 0.38857078627440433, 0.7347444689625003, 0.4998394593093752, 0.9089087922790371, 0.645660744540383, 0.9616715081662109, 0.5512118001017096, 0.45618072661808934, 0.4525068339466281, 0.9713153669319253, 0.6019426555453288, 0.7647222520660254, 0.49201727500745507, 0.6422254766802519, 0.46897247302996253, 0.8517834092275532, 0.9309231218956574, 0.9114503622764372, 0.13448696808925042, 0.028202019098269214, 0.9759253251484191, 0.672985741541884, 0.7108883519372058, 0.9870881100323939, 0.9333098503473919, 0.7724861524841846, 0.9622448843803458, 0.978294056839238, 0.5388161083719267, 0.7525237718401745, 0.7943697366861424, 0.5134458005264022, 0.34236102237615523, 0.7420430551304436, 0.9854085170577868, 0.9857222347943554, 0.46289302334682586, 0.5754327233235073, 0.946818950423356, 0.544418487663996, 0.3237355999244597, 0.9545694378077643, 0.4559404288357898, 0.8780809740392947, 0.37639008546452873, 0.8237878498594099, 0.7887611339458084, 0.7347417960830501, 0.23906320408553294, 0.7903277260382681, 0.8063674100021209, 0.90216938640809, 0.9360324598665176, 0.44917648583200054, 0.9167531607370316, 0.9505324632414861, 0.8956314893387424, 0.6894826892806253, 0.28145146655257974, 0.18388934984674155, 0.43774258814822564, 0.6092326727857268, 0.584473606062962, 0.46577385027622303, 0.8933001998904865, 0.26701642984717827, 0.14918395241988958, 0.6031070091638627, 0.5236252776008563, 0.49297919725125056, 0.9841704252403326, 0.9335372901915762, 0.8005050387256234, 0.8259387396289298, 0.5373506811855239, 0.6902990493434041, 0.5562715403176322, 0.8119260410298139, 0.23513766778526451, 0.17601721327779932, 0.940192434321937, 0.8317053801069347, 0.9224034853068406, 0.8268578086895213, 0.954575754636986, 0.8935423017159811, 0.09043657414917645, 0.957009980131217, 0.2502884462703165, 0.9265438675149525, 0.9112086071623237, 0.5504651448315724, 0.7385563283511337, 0.9477766228372381, 0.7663769628421383, 0.6427531673725305, 0.8273895112398251, 0.8963103778002888, 0.5183230261716076, 0.70544174601189, 0.7734664663127557, 0.0639477082518681, 0.22046713368198279, 0.7679293814751247, 0.21025049760472334, 0.9524151886927846, 0.9484435194120516, 0.23115092546322485, 0.6193707073519628, 0.8122157386373157, 0.8513715130544092, 0.9500856310623487, 0.9438354370091981, 0.5158550648912561, 0.41480512886231097, 0.6979954518827777, 0.656636500584487, 0.17499518841031372, 0.9891724261935164, 0.3963866584272157, 0.8899341535426534, 0.3263239401566317, 0.5420923657018973, 0.6868352370259002, 0.28918850561474224, 0.9320504904993793, 0.953193972362393, 0.7273993736028593, 0.4614794667546601, 0.20613168751673977, 0.5403361465294898, 0.7256752695025316, 0.6549341524062089, 0.8536991306145402, 0.8433698502576438, 0.18135798102693843, 0.6636166610760335, 0.19136114437556592, 0.27832869052611525, 0.6931837216179555, 0.5236348351594227, 0.1638272578261897, 0.8691927564391984, 0.3812781959650864, 0.7360688860153916, 0.37403028877060385, 0.9621508636787214, 0.46421501473384985, 0.7350875682676947, 0.8483351028559398, 0.8226260692812479, 0.8636702481582675, 0.1988214435162283, 0.1688158907882244, 0.32483457863760035, 0.8668326409967494, 0.8938473903000949, 0.8450668813800779, 0.01578848392081493, 0.7962086682022755, 0.158057891291653, 0.8972674219265119, 0.6594315791093148, 0.3872765694392812, 0.8274101029064391, 0.6600107339704351, 0.40616144322951353, 0.7220455848991026, 0.9465853101904697, 0.5653927885381039, 0.6954012866966267, 0.7873831915204478, 0.24929637494146104, 0.21700138428439109, 0.08906700415658095, 0.795416529586218, 0.38078913687151444, 0.14193891761334754, 0.6187315581759965, 0.8605664917161244, 0.4999676947910985, 0.32665958917751, 0.692970637489907, 0.8298797682078026, 0.813304265776872, 0.3560495145697516, 0.32138684927627864, 0.5913192573846034, 0.466395080713275, 0.27545080399874083, 0.5907026077624303, 0.9053471591378341, 0.6198130807729069, 0.9148097030177491, 0.622233561728012, 0.37295759287069785, 0.2858999841609487, 0.5747862765649435, 0.6054506792679263, 0.7646016956602419, 0.8310698811098619, 0.77941435582539, 0.9630108710037897, 0.4836657623217477, 0.7694674771491241, 0.8235853242507921, 0.7251729346536204, 0.95351138579618, 0.5017875145521604, 0.8068218086357373, 0.8928023420823021, 0.8514844081496857, 0.793248459586959, 0.8402693733065904, 0.4463900859758284, 0.6867101961347494, 0.8961551140163421, 0.5096022502207103, 0.7229482267631421, 0.30198072072682497, 0.5401379480758892, 0.8744269277016073, 0.7905243336226673, 0.24821589631145144, 0.48637568927968167, 0.5802147652939296, 0.9126547651649782, 0.5318004630194831, 0.9320958867596147, 0.7657130230443534, 0.9711460270022982, 0.4013292275637882, 0.477703767929641, 0.9252888858432738, 0.7431309561462929, 0.9070763956935314, 0.6321949417123202, 0.8635132962168417, 0.7893833888084791, 0.2798012096014836, 0.6662582261551705, 0.7942738267772841, 0.23468658618495283, 0.667267570205867, 0.9389456468195959, 0.4662148734940208, 0.6141336096957568, 0.2948699349440681, 0.7079248682823213, 0.6995807002635007, 0.6801554130880041, 0.6535805527366912, 0.8814231449492574, 0.35051911338590286, 0.39349959064356277, 0.43359984889217384, 0.9251728998124205, 0.803178296287693, 0.575797970426874, 0.7847605224171095, 0.46448110604591064, 0.7653805358834271, 0.9037205813422541, 0.6277899874316617, 0.9560951602740679, 0.2581128333277595, 0.9400568816313039, 0.3489093640067406, 0.8467346912421077, 0.7747226628176419, 0.579657170750095, 0.8182967623880943, 0.7565488694723255, 0.6132792866517913, 0.5011740613132185, 0.9092437490284085, 0.5744917691382754, 0.047965923714405195, 0.6906610544164433, 0.6418800412985649, 0.49358751898547293, 0.792247954711174, 0.11625813407242805, 0.541569641610427, 0.3481892925104904, 0.6453779815452798, 0.8422549908641459, 0.34379236494750687, 0.4095521393857954, 0.49454184771538057, 0.4128245454782881, 0.7300241873635266, 0.5202834648910583, 0.6659552143613215, 0.7371754544798375, 0.7951723980056346, 0.5754845083815953, 0.34389907973608486, 0.28876537021314763, 0.8651319910552988, 0.709420710677396, 0.37099994954019927, 0.8498293418220482, 0.48732006958009194, 0.557273484154091, 0.7547966196761738, 0.34499953684657125, 0.8917082399276349, 0.5544791901659443, 0.4574406628385566, 0.8226584545903388, 0.8409266017472852, 0.6030633132667328, 0.6842103968211429, 0.7269522915453985, 0.06022609822702683, 0.4446595369172561, 0.5314987030442868, 0.9270414663275063, 0.46189434940104007, 0.40088515670510166, 0.755894999306437, 0.5038999200903818, 0.49511402535649246, 0.8885064500397581, 0.32842397173105153, 0.6624233294761129, 0.9267590170878364, 0.8058898793702776, 0.8258960331233068, 0.7038009895885989, 0.222123307982002, 0.7394982111873533, 0.12908320677908525, 0.4835932589574323, 0.6768307126743549, 0.7633247847486216, 0.8395711776216866, 0.4771598269668634, 0.6689018086768694, 0.6260075753452745, 0.26580155170337233, 0.9067401578681417, 0.23542522948929617, 0.6407004263330768, 0.3834236702540002, 0.1249572350305128, 0.7694802270960901, 0.7895334555284721, 0.3776370025772536, 0.7926518700901793, 0.02899737770156266, 0.791018501728652, 0.6839414225010922, 0.623797016673997, 0.7531646495666177, 0.23596856080497386, 0.4320464877097913, 0.024877380443200453, 0.6023258445151143, 0.28827284831654837, 0.6905753424599509, 0.3544556614731711, 0.12214115432410541, 0.06412936947039878, 0.7146587141660868, 0.9377498533142263, 0.5442416221025016, 0.7526728894866269, 0.4698272414859367, 0.7937043907006994, 0.5605307276727813, 0.9621512226825689, 0.49179091878255665, 0.7151894591550131, 0.25478728630464875, 0.2820178083111431, 0.3818951187354882, 0.3821418935498773, 0.7992453061197174, 0.7821093461628834, 0.2561582981924215, 0.6595660466857698, 0.2521452474397218, 0.32111464047740007, 0.4156323244097353, 0.635942821078552, 0.9168301767659367, 0.35273501049902095, 0.12914948375987945, 0.7345389938226191, 0.7312613459457228, 0.6393092543933261, 0.9698773785993892, 0.3175225742236497, 0.5569167432260699, 0.8794731317414621, 0.07591385140745759, 0.6800888726043882, 0.5212845887578913, 0.297621918690672, 0.3519411382684339, 0.20224767406720412, 0.6767614351666768, 0.2004927921685233, 0.5343446394785558, 0.6416380873033077, 0.8980812324188112, 0.7820326115055669, 0.8059598217011915, 0.5396229058479591, 0.7457916518698477, 0.4997101409527351, 0.35129864100478814, 0.22640982828026487, 0.375193158697639, 0.44376421520822795, 0.24245278357109598, 0.19576073381085876, 0.47333847520330247, 0.6090520314964971, 0.8220348095415264, 0.8793701477404412, 0.9539411778301778, 0.8609661194918335, 0.7046696772957222, 0.4559886718115199, 0.7345472387490417, 0.3259069341806095, 0.5323967083099718, 0.618817878296661, 0.4476174853305728, 0.5128918699404439, 0.5860834831814273, 0.26844029738322817, 0.7861918829649672, 0.9367051773390213, 0.12041706989491814, 0.05764075386522621, 0.8317674834505404, 0.1324108518770282, 0.6309039198438482, 0.7676354123997551, 0.8773541921893185, 0.0623522110066202, 0.9348229843882299, 0.6072586890996181, 0.7674245193632626, 0.8376192223875857, 0.9627361452323675, 0.4419459236887462, 0.9200570066700471, 0.23766666122150132, 0.5795652871862579, 0.6018252014071472, 0.1412563316980416, 0.5441301465545725, 0.03977926750689134, 0.6318135830436601, 0.589198831600827, 0.4657663389618918, 0.7435660490529747, 0.3837261651418459, 0.7401440533339234, 0.9731798364566533, 0.7862513326189552, 0.7955563842197574, 0.9544789078973398, 0.937024282582344, 0.5118259706665579, 0.455746215501251, 0.35248352326173726, 0.5073725939905216, 0.6553661559010919, 0.11790051465472837, 0.6317003387580239, 0.6160868903079492, 0.3165992643278972, 0.580693891468578, 0.5843540129085034, 0.15353626143382657, 0.43606709530037646, 0.3014929111655163, 0.8349524445161329, 0.2844494657439396, 0.673483192127729, 0.5107930464851451, 0.9338172867016842, 0.7608113147503377, 0.3846472613350784, 0.5632639393582224, 0.8583957837832352, 0.8879454840230572, 0.7569182891270747, 0.5601530582244096, 0.9172532138683529, 0.4197307130732088, 0.7137979735297039, 0.378114508577424, 0.5978344542725613, 0.7833262583069984, 0.6703240878919935, 0.9444687269047197, 0.27413516486786427, 0.5394116966467614, 0.8183498216685209, 0.8287236948396357, 0.4554919452756739, 0.6142988653574175, 0.6011758522025268, 0.15636927769354295, 0.8054563585263302, 0.6895310695988256, 0.6120425201350266, 0.23265406133564218, 0.5367041013802345, 0.389560522694046, 0.8071375809290571, 0.6830933379598423, 0.03972737554876427, 0.6040709532138658, 0.6246256872148603, 0.2061584450073018, 0.2662823685776749, 0.9346821720863385, 0.41049221445647555, 0.35956230109567955, 0.41167531314476835, 0.7099952321363695, 0.5960286319755861, 0.5070782232633911, 0.09518634887578574, 0.3443449305442898, 0.5840499990861563, 0.20613518962076993, 0.8905611706789105, 0.8409604699083911, 0.894249327979678, 0.9757855249306807, 0.867781895536914, 0.9090625839469973, 0.1818819345035311, 0.785731503372176, 0.3341739846419868, 0.6946377835597984, 0.3309832448258242, 0.5520600020069834, 0.8201278559885192, 0.7867376456241156, 0.8746835047601618, 0.9137973375900443, 0.4675572606684581, 0.5123787128985791, 0.40157614195292723, 0.6231671615962701, 0.5918724468653458, 0.8703791555876346, 0.355641292226443, 0.4294828392866448, 0.08602051573687493, 0.6763472389471914, 0.47370856378611276, 0.5957523372450935, 0.9425983140392123, 0.45974111775046833, 0.7680947337680546, 0.4328857529149277, 0.6562697161316773, 0.8102661656516806, 0.2052359702158717, 0.0014188160520548557, 0.5618623263833441, 0.07151120028039185, 0.947788539379902, 0.4436200217909075, 0.9270350311541703, 0.6095181597180842, 0.5868533614432048, 0.2581150062151854, 0.04266487617865883, 0.7981956432914564, 0.7045659343813584, 0.5678692989137945, 0.9237884532993116, 0.9270648448403039, 0.5005612511029621, 0.19009303513738504, 0.6012901691374818, 0.02595589411782358, 0.9386208696002404, 0.5133882224285292, 0.40976582250508176, 0.09245940204138965, 0.12312266211161785, 0.26544716185435113, 0.21405504918316323, 0.7453092216599447, 0.3678280725646996, 0.36883282324416045, 0.7682149793221135, 0.2605707391482312, 0.13527803226955895, 0.11067672397332792, 0.2607265976598444, 0.1936078254643784, 0.8260981555557126, 0.035309895198002136, 0.34929057177092626, 0.5118546350446229, 0.13428413563562297, 0.16345213281648624, 0.5217284978914289, 0.49896323302931267, 0.17181050341296872, 0.11987023033544673, 0.14736850097110787, 0.6660302544522275, 0.35048975324213405, 0.332493136795436, 0.23952002968626085, 0.041857759601781674, 0.49953180391794155, 0.6844596409109426, 0.502970390718219, 0.3539925696500554, 0.4993593720697925, 0.24360443212962155, 0.654531066901554, 0.6368252230399394, 0.11137092402243437, 0.45082717651168164, 0.5549476832885135, 0.401691813911908, 0.04939012257182876, 0.3475363605584505, 0.29149481473655287, 0.4488979819768508, 0.26031129598878483, 0.30514441149109145, 0.13693045523860134, 0.18793435949101633, 0.8086528244683568, 0.0865504379874036, 0.2731210138794278, 0.48703090666066, 0.15394319120231761, 0.28027255502654036, 0.3026771822963598, 0.30628120362537803, 0.14697110043632264, 0.5716667747942599, 0.4020884884955254, 0.21342108786418815, 0.6410702503765916, 0.800954132754481, 0.08619285784267976, 0.7499248139438622, 0.4865250828170044, 0.30448052966811806, 0.5741675383161748, 0.22722434939928118, 0.4277636443932723, 0.16237446844733508, 0.17436984788222887, 0.4788198251771096, 0.0681431800775362, 0.33031958093717423, 0.1449352136594336, 0.4576663833207147, 0.6583695119999704, 0.5032108479171911, 0.40086704217607744, 0.5029267591045752, 0.405862838962784, 0.4750186361793595, 0.2778428784718422, 0.41777901129493605, 0.39277526501259896, 0.7096625006963923, 0.40099598746027226, 0.11462850560667062, 0.2825328395557569, 0.583196511698778, 0.4439649554507215, 0.3627082702121073, 0.6142682916684387, 0.05865480993297513, 0.1429086701031607, 0.3311300667292493, 0.23805796187616005, 0.49938599434602154, 0.17919314656714763, 0.6604936738094648, 0.14203163499854543, 0.5021074922059103, 0.06201726054967138, 0.5705744125933752, 0.32658234973562433, 0.12502375609921074, 0.0998263856145567, 0.056668913664483164, 0.07224754296819136, 0.3255674188612855, 0.033919572709698094, 0.2958155414323879, 0.7761624698535315, 0.5269287988514617, 0.0731537625322381, 0.577585602636258, 0.5487214392604051, 0.5391991521082129, 0.07549993072162167, 0.15227637476714126, 0.2015806142467344, 0.08890449249432791, 0.3107921519861983, 0.2243019906227395, 0.008409226622259293, 0.06514122292162926, 0.575038051591366, 0.46969070479721997, 0.6802905283432757, 0.8653971500372535, 0.10618475646548108, 0.5216614961511061, 0.026661397001076243, 0.2220133700066379, 0.33787340910872066, 0.04911264541311718, 0.6128789022090281, 0.3042690992126972, 0.5073405921393357, 0.413793798188538, 0.7436000693364825, 0.5669912853160168, 0.6527894675849079, 0.6711721471364201, 0.4026504719686943, 0.4254853221947078, 0.06682300609686338, 0.5320368789419009, 0.7617377164565236, 0.34261432937686354, 0.3717133722603875, 0.3562109716535475, 0.39819246466144836, 0.10009370530447173, 0.26397990093875895, 0.6502964500083042, 0.024347605372324995, 0.5409432488348008, 0.27170935747085767, 0.19563895200422782, 0.037007693263610426, 0.9582487723699291, 0.3868228026318793, 0.3445706467901605, 0.8459155610172393, 0.26575453238476543, 0.3738746909248912, 0.22981518967652878, 0.3604384860477572, 0.08559751665481725, 0.13379453954633372, 0.19260000966004906, 0.1575023844501758, 0.11643604259161378, 0.05150803391013262, 0.5623529169664236, 0.4612146654343318, 0.1492685225029524, 0.34740632291803786, 0.4090976671776237, 0.3904839101729193, 0.17178988165416564, 0.32559429660916434, 0.4537720925670491, 0.2189853584318692, 0.18498283903655247, 0.30353848467132954, 0.9245344210629588, 0.1606137884956872, 0.07158288527161231, 0.4848643619596667, 0.2790221509896458, 0.062122009278880896, 0.4516719714112971, 0.4230237324633874, 0.14646532867160605, 0.5771771894255263, 0.03196582817757092, 0.10352012867333416, 0.7013597987338398, 0.6833272043597507, 0.11195444847411677, 0.3241450358436107, 0.6535640031602961, 0.44056982850502424, 0.16191916755184033, 0.4727154899537409, 0.450371591051897, 0.33141330331839414, 0.13186930073815029, 0.05901443644</t>
         </is>
       </c>
     </row>
@@ -621,44 +621,44 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>svm</t>
+          <t>SVM</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.751417004048583</v>
+        <v>0.7595141700404858</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7278063096111519</v>
+        <v>0.7344550109729334</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8032388663967611</v>
+        <v>0.8129554655870446</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6995951417004048</v>
+        <v>0.7060728744939271</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7636643571978446</v>
+        <v>0.7717140661029978</v>
       </c>
       <c r="H3" t="n">
-        <v>0.751417004048583</v>
+        <v>0.7595141700404858</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7326512455516014</v>
+        <v>0.7362099644128114</v>
       </c>
       <c r="J3" t="n">
-        <v>0.719195305951383</v>
+        <v>0.7306689834926151</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7633451957295374</v>
+        <v>0.748220640569395</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7019572953736655</v>
+        <v>0.7241992882562278</v>
       </c>
       <c r="M3" t="n">
-        <v>0.7406128614587829</v>
+        <v>0.7393406593406593</v>
       </c>
       <c r="N3" t="n">
-        <v>0.751417004048583</v>
+        <v>0.7362099644128115</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -667,7 +667,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>[1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+          <t>[1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -677,17 +677,17 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>[1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0]</t>
+          <t>[1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>[0.9939700039884991, 0.007040215014294723, 0.21818980971448151, 0.6677697616274344, 0.6532673747841214, 0.9945739939198248, 0.9656655773794033, 0.12837401945334978, 0.5, 0.9596697080868682, 0.8592828502995099, 0.6551346458896868, 0.9502642243603241, 0.8453568178927254, 0.9337635980177915, 0.0597749799805915, 0.9661382927951323, 0.9518507844648437, 0.8903791437028343, 0.18274526671561886, 0.9829369467331133, 0.8984722610493485, 0.9545331062604977, 0.532696081225553, 0.6785310943807218, 0.09588975735964035, 0.993141835025617, 0.9631386915898171, 0.9724424534738866, 0.46010934957069594, 0.9112464398934342, 0.17787803685088174, 0.6678444514297461, 0.8817954686558133, 0.7673875248050787, 0.9613649990001358, 0.6905854599801718, 0.6652028531313777, 0.7821657761380805, 0.9535252685745069, 0.8283777418640089, 0.5287956812868708, 0.1644530415889885, 0.41216500554865615, 0.9604732290094403, 0.32021062257832034, 0.9847862684387111, 0.8476373293808144, 0.0018897472157972774, 0.9675471931619367, 0.9682433393283777, 0.9954840744184524, 0.39796457398809126, 0.9042589361455999, 0.8266402261711474, 0.4830475413132054, 0.24697566343343197, 0.9255194529420074, 0.9734500313383435, 0.9253319155892812, 0.7042816046447702, 0.8817454034502942, 0.7108027101973711, 0.3719989466684966, 0.9626664491307434, 0.46898317994970395, 0.7938814044285359, 0.9856203945748064, 0.7909759979911083, 0.8685191841409609, 0.7237895422374557, 0.8578450996966023, 0.9038728651152287, 0.9801661206415915, 0.854742484697973, 0.9466307259369171, 0.9858413739433737, 0.9692459472047366, 0.9915982448764381, 0.019767809176028172, 0.928484076576622, 0.7403229834552384, 0.8478094964709764, 0.9318502697117466, 0.8013762117123088, 0.879280208713989, 0.8109311362601415, 0.9884552293424046, 0.31356593530029425, 0.7235954254463817, 0.9698058837895767, 0.4096099775329562, 0.8018123767912958, 0.8096797397146123, 0.2125957984544897, 0.6783742633408302, 0.5810814226174473, 0.47662364349907554, 0.95994887529424, 0.8697796503886921, 0.5710714025734769, 0.5390730936860071, 0.6402653910438373, 0.7314212733420469, 0.22203642548753996, 0.96677724144593, 0.03192727028874992, 0.8551225917219929, 0.7449669245854298, 0.8659441997078898, 0.5553452432080366, 0.0006059408295522378, 0.8648969739587445, 0.9803804259634614, 0.8552814652804877, 0.8399649001732488, 0.9535367807393927, 0.9284903345342569, 0.8699269421370439, 0.6706158178987041, 0.5385404139218227, 0.7038674352891426, 0.8517810005308859, 0.7927907872242178, 0.3837115414646036, 0.615358872923436, 0.791372619429463, 0.8867545759131099, 0.6994055230722394, 0.17632126901241718, 0.6362609720096969, 0.9636467412719215, 0.8028349653001469, 0.7423853080184232, 0.9544206197822528, 0.9772848596580465, 0.22021984835268782, 0.99055015405313, 0.9833874321896336, 0.575459946333637, 0.9896743487406412, 0.9945797201537012, 0.9343702700603534, 0.1591567363040032, 0.7949129008125245, 0.7698712922026805, 0.9962451772720997, 0.45018509831166864, 0.9757339789839228, 0.29328886426617495, 0.05161947555593942, 0.9666186440360554, 0.031143970727222064, 0.9243903801413462, 0.010642247551256456, 0.9944169013357007, 0.6341259910174106, 0.258903775338716, 0.6907373065902203, 0.5148433781241467, 0.8833468246252492, 0.5742129725574667, 0.947349330517481, 0.9908643170770125, 0.19828292508177972, 0.8189282398797518, 0.9177471818762897, 0.9343810606559643, 0.8981434469964389, 0.6347435543304657, 0.9925529721079822, 0.8053255087330697, 0.24638514377759874, 0.9505103859506346, 0.965717342504876, 0.7001643590199126, 0.8653479445793522, 0.8681344029609314, 0.9179341163316784, 0.9402232661858356, 0.8772187435534679, 0.6968587104225498, 0.966950172433708, 0.9930971668150533, 0.016273776129881137, 0.5934300711634085, 0.9587257936458988, 0.9789978247217326, 0.9125508059280198, 0.9511789073348557, 0.9897598202228768, 0.5890125614981122, 0.4292351391861632, 0.935405766589857, 0.2797712607889015, 0.5903834246939971, 0.9778828489570431, 0.8234203611258095, 0.9022055982361067, 0.1385305120937664, 0.9656555694728202, 0.7828703357792691, 0.9683173626142305, 0.9267358312330616, 0.7964533793551045, 0.9649373374955493, 0.8249705642639219, 0.9960323147053032, 0.20630340570839556, 0.8389243235286699, 0.9407443904973736, 0.2773755931260577, 0.7399631636974054, 0.9347036556233239, 0.8921237341392709, 0.9915676769865696, 0.830170950747839, 0.9837973267628805, 0.9618278941376249, 0.7843824213436529, 0.8801072924889584, 0.15374756800920752, 0.8096407248416001, 0.8071690384104127, 0.4918790827869045, 0.9403787872731139, 0.09275720831675448, 0.8774781729286529, 0.6160900484448454, 0.9814116302530724, 0.9059261058680136, 0.19142686669054307, 0.9404409914482053, 0.9933627238673428, 0.622348816289001, 0.9819800746852292, 0.5531791656815546, 0.9528979843805527, 0.8199091278038528, 0.5993396700847083, 0.6305898208560778, 0.8360978280450578, 0.3184470958582644, 0.9638119974215255, 0.9043047375487432, 0.8542830349540468, 0.9399745933116891, 0.9692459472047366, 0.7592728048359845, 0.014223788175868928, 0.966896741898561, 0.9885764362841489, 0.9897556481357894, 0.9583098794150313, 0.9875835754620164, 0.4626059105694757, 0.8940645010930626, 0.916901713729224, 0.714159979467136, 0.6082448745003297, 0.5, 0.36577625662466656, 0.9584341538038672, 0.9680701746036121, 0.8195543793475917, 0.23109258075549244, 0.897081438311815, 0.027226571850866976, 0.7534445960392449, 0.9931944383387297, 0.5912888789490569, 0.5289572469244008, 0.538625333706829, 0.07502307388793268, 0.6691365853846465, 0.7714444016280276, 0.7815523734877254, 0.9599282419114248, 0.9810706130989407, 0.8671943372939085, 0.13695094997872156, 0.937987856507791, 0.9629703857594772, 0.9868579617411071, 0.9726593338235568, 0.5173113006193443, 0.9912125165146067, 0.9679314029632774, 0.34908020838693915, 0.516051827827224, 0.8682299285036557, 0.45504061118524963, 0.9288441744570846, 0.9681516844396554, 0.9853440104292459, 0.860961047471842, 0.9605385040282098, 0.9639990148938224, 0.4793469868272322, 0.4437810825930173, 0.03081566130747394, 0.8287602461050125, 0.02656250528080084, 0.04905071132450791, 0.6467873103681732, 0.669658120023652, 0.9440603625394358, 0.903652817363948, 0.3813472747526008, 0.5520099621666548, 0.4016340065246028, 0.18013000629050552, 0.6705604327347372, 0.9390419468791068, 0.9794038330881942, 0.16113002170811444, 0.6111239620623088, 0.6366284243742122, 0.8060470246250837, 0.5529355709652448, 0.8834703141796519, 0.8493831576711013, 0.9820381197198709, 0.9610971904427483, 0.9139564129205203, 0.6864187671870878, 0.9882057858065983, 0.25893365978615046, 0.23752479867072657, 0.9814724360227255, 0.44546211271665237, 0.8437299543225074, 0.7086591286461615, 0.9172421098593453, 0.17603735722269775, 0.4645436990653916, 0.9904770862296504, 0.9798310102746994, 0.9772273183481517, 0.24502791125482096, 0.6517052109382266, 0.8133702025517362, 0.7674522891785182, 0.945034342438183, 0.9492887660812905, 0.7013702046927934, 0.8933066715745361, 0.5825981606759177, 0.9169524016168119, 0.8808262471302828, 0.19105692301848423, 0.9618273539680571, 0.9326731308552745, 0.9325512723412765, 0.9289765607657159, 0.9873988009295, 0.9808233144299264, 0.051153425968210174, 0.7341559555810844, 0.984028450369758, 0.5502680455644403, 0.28226399980618694, 0.8792533285572184, 0.5075322285017454, 0.9858297220414921, 0.8237075124646631, 0.8206869860432996, 0.812993405196322, 0.6476494994672406, 0.9666039749971427, 0.9709756930348966, 0.9933475274899385, 0.11717659210589997, 0.934547735449174, 0.9635610002634921, 0.8408308762476084, 0.8177337281016087, 0.894076633777024, 0.9651694017038055, 0.47085657294027466, 0.7845421158549939, 0.9622798861833811, 0.8600720457005933, 0.20659600752930324, 0.5252435522200819, 0.9603251330621031, 0.384959487122825, 0.5776947925527367, 0.9638499563517711, 0.9839837786599599, 0.975274151864776, 0.16573420647884562, 0.9156146604296266, 0.9279862243920965, 0.22066612408798217, 0.9523596834665691, 0.7658547465596501, 0.9425540675852543, 0.47909559905370125, 0.1799383729560695, 0.8876168834962405, 0.21366427708923594, 0.8488207598102269, 0.8112794449894244, 0.648165064558034, 0.7477505481108576, 0.8419186914185487, 0.15316971363939028, 0.9575477407288007, 0.33247765662269846, 0.8815354462235584, 0.058058243920126845, 0.6926408670391206, 0.8935781847557485, 0.9502572479641898, 0.7841732905619602, 0.3354025428165637, 0.8585009073505203, 0.9142726028951688, 0.3581122378026038, 0.4744171921729853, 0.9683376668708885, 0.944772818315531, 0.8547803641248831, 0.7412431424230153, 0.5128466835146003, 0.7439539668088583, 0.6711464165876877, 0.1386009298822547, 0.8863002553230502, 0.8302625752271119, 0.9851595746828173, 0.8771878144914268, 0.9588732710546204, 0.936581813676816, 0.9412389488317486, 0.894000770572676, 0.988018737255845, 0.8306184358727283, 0.6076354175084425, 0.9696096795246543, 0.8753154291842694, 0.8727156383099687, 0.8391665213213849, 0.7413291418372224, 0.9503589872241212, 0.9837287238824114, 0.9302611952465243, 0.95843881278829, 0.7786311793039916, 0.9836512740919269, 0.9214759639446007, 0.3215638530721482, 0.6765316873573811, 0.9804424760429544, 0.7700003826597865, 0.9969855225924331, 0.18956907112217083, 0.9053295624587769, 0.7305033916223889, 0.9687888441931302, 0.9753192600500199, 0.9318020508053424, 0.053983284583490276, 0.9682838074111026, 0.9189820952388758, 0.07890668486246462, 0.6040460404118165, 0.6138567455546459, 0.9768154303338067, 0.9933674389571776, 0.9843753268128848, 0.9848918327612041, 0.2718272452342596, 0.48906857967400424, 0.012731619788336604, 0.24267425338533458, 0.6263553943244949, 0.9234976651442655, 0.1649930244025246, 0.9838474140330526, 0.4103441415654676, 0.9808682498285332, 0.22537980672903113, 0.6617361886830622, 0.9896342732022426, 0.9322277348291325, 0.009943051369034894, 0.9908079068034751, 0.08995494936713411, 0.558256551040855, 0.08333590821344493, 0.13362076028703063, 0.5221542801032859, 0.6086010044915303, 0.9223258746007282, 0.9821205951086885, 0.6750377668857358, 0.9808308891542089, 0.8692877902398268, 0.40311208381889774, 0.3327514943232077, 0.05138813281932916, 0.16958322014502436, 0.5, 0.5330883730112371, 0.962445045850846, 0.9280317171500748, 0.8263298189841313, 0.9794024634653138, 0.9807077991218653, 0.9952174388092809, 0.3191892749507167, 0.8956051477294656, 0.9061822288246083, 0.3347863645520829, 0.985177792875905, 0.7159894577036472, 0.645372348590199, 0.9512395785157659, 0.160393747994085, 0.9853563235455155, 0.5763947209742841, 0.6717463979804836, 0.967737745639756, 0.4670719825050563, 0.7596089073264474, 0.7088417476377407, 0.4542788414277254, 0.7628245752134584, 0.9557159644568476, 0.8087902678678633, 0.7139112230004273, 0.4609559003809899, 0.9669884497943272, 0.9683173626142305, 0.5848795586278462, 0.9661063837947376, 0.7815847625773613, 0.8313820059139347, 0.007830968937585912, 0.008119387677302236, 0.6425179465225999, 0.7271125015798034, 0.6233209659742759, 0.9863136686608246, 0.19511332755998217, 0.7261391756030589, 0.991057039971179, 0.09116179370903266, 0.5490728581597896, 0.9885679447976549, 0.4247339053217269, 0.9268434158396119, 0.270422891860164, 0.9774372043680081, 0.2294612420144062, 0.9865304542577921, 0.9814405743587998, 0.9548979275113586, 0.9518616961672873, 0.9264256583334722, 0.6492417187832499, 0.5681541690387184, 0.6192085752989913, 0.9891534231343517, 0.9814082678062818, 0.6868788597420513, 0.9772708925567377, 0.23962757158122291, 0.26903646256809854, 0.8884217842700177, 0.8556315513631803, 0.013114295689770721, 0.906164939027516, 0.7777135879680293, 0.992123983373205, 0.9927554141741639, 0.9741629728402064, 0.9647623474483868, 0.9828120476445358, 0.9683463954379397, 0.9744895611752128, 0.9321991842481712, 0.9553284897920038, 0.20726686122623814, 0.7859420142538873, 0.8898799881568547, 0.09887849761259679, 0.9434697122398076, 0.9494585933872869, 0.7920784530223867, 0.954882146979969, 0.6658028443122547, 0.9965473473092636, 0.09053389388550884, 0.5135403773110909, 0.8351708020092345, 0.4549148830394246, 0.9240165016351909, 0.9191565535451777, 0.9671960657534928, 0.6559873965547659, 0.011034453303403004, 0.7198425007019595, 0.7874801224644207, 0.2648191708059934, 0.8915879670773496, 0.46156795167979847, 0.0006786513039658656, 0.42027424028047483, 0.8230975678154858, 0.3355827797459459, 0.9877223471044871, 0.3594047167454368, 0.9138244328547424, 0.9927930434838402, 0.9488944308565121, 0.2425448827768392, 0.9702272004640109, 0.9674278435009677, 0.7266860920634873, 0.0810395878625873, 0.953857145833808, 0.5711412588905921, 0.7884031986139837, 0.47897962401970745, 0.33158556898797714, 0.38821155625607173, 0.8740373100433192, 0.9920374676268999, 0.9090787745079808, 0.8847165425831678, 0.9642279049056081, 0.9950932356681526, 0.9916450807167304, 0.10200356095399075, 0.9125951429726173, 0.7197831493825168, 0.9632177796763205, 0.9001316250517606, 0.936419668889893, 0.6285766289681678, 0.07158507558446878, 0.9786300168508094, 0.9877379822801775, 0.5273918939521979, 0.017298334496901126, 0.9877483304166367, 0.5578165036484691, 0.9878111517423678, 0.40496410142040845, 0.9822464838460742, 0.5150467479397848, 0.9536261752508068, 0.8114674178460424, 0.08434618276447274, 0.28723602190842185, 0.9686349739245425, 0.681566893981792, 0.9209769871631063, 0.8486223548890225, 0.5297869163842339, 0.38744269618470684, 0.8928799862286418, 0.15872339538278532, 0.9934570011850791, 0.1892574534693046, 0.8800415559846295, 0.881807881420739, 0.9286387494083451, 0.3887426283509424, 0.9596866679619053, 0.6323742077146015, 0.8098656972346419, 0.9192791427096483, 0.9727856854409787, 0.9662512585584512, 0.9176818284398538, 0.12395377839090567, 0.8823713537328867, 0.10085657791307163, 0.04249376739525866, 0.21199899112232007, 0.679721200245439, 0.9866799725894556, 0.9871255516094337, 0.048132241332777694, 0.054580642748635444, 0.02073373997786678, 0.9947111651924929, 0.9717735765597343, 0.702299986624916, 0.30597754060767485, 0.0252790537207643, 0.7752979717238406, 0.22521019363583944, 0.953881150414702, 0.7943806357126793, 0.9609235745300387, 0.5843098091064479, 0.9661097248646745, 0.8620770650044641, 0.30977681310728233, 0.5, 0.23468223766216847, 0.9386787085889517, 0.21522224439346732, 0.9468674158860209, 0.4212841836645902, 0.30543408420496954, 0.9651136566530841, 0.05497790652479786, 0.9257704422180545, 0.935858824542919, 0.07808901054562155, 0.9697691485428402, 0.8002096083602726, 0.48856110040657663, 0.26498399781809256, 0.7357232313550854, 0.9686113143866064, 0.8041499236307127, 0.16579719242426127, 0.9389771875665935, 0.9833863045733016, 0.992792624045233, 0.8225764200686949, 0.8796102722901565, 0.9361992294370197, 0.18777479382244341, 0.8320835822334933, 0.9044122515155066, 0.9804228065551707, 0.9082986043982065, 0.9753346631687755, 0.6929092482370788, 0.7202139843239784, 0.9928877364892461, 0.9763343259897208, 0.7319329796016842, 0.8063197162480519, 0.9493083100737305, 0.48380992695797814, 0.3382907691201283, 0.9700624725687897, 0.953121285757595, 0.7559589596591583, 0.06823859459832501, 0.9640579192927259, 0.9732120598782642, 0.0810515884272748, 0.9475077204563693, 0.9745251161468461, 0.7394100821771452, 0.9869710363776127, 0.9266048200274077, 0.33854258309325314, 0.9851793321011755, 0.28187645776856846, 0.9341172695345085, 0.6498068472442883, 0.9578849083413294, 0.2026076331862267, 0.758552760544293, 0.9877521123739138, 0.0346918900179752, 0.41009954569853796, 0.19592785487677833, 0.9919310365519416, 0.886860413205702, 0.061548537299313116, 0.32971401424709645, 0.9842724815235597, 0.9621849218561007, 0.8585291681499156, 0.4212841836645902, 0.11201887963169153, 0.9029329056868577, 0.8553664369890391, 0.772123199565135, 0.9446339904260947, 0.8377044184669735, 0.8523052073733934, 0.9850858317521913, 0.6854292498070365, 0.06839364772262695, 0.8957211798997425, 0.8508318561982139, 0.8369490620533627, 0.933687261731219, 0.23473808425138618, 0.2807565285437627, 0.1372781127393954, 0.85515227686777, 0.07114020359380505, 0.8719174772641365, 0.8716286215523072, 0.7754979049903272, 0.6841502815361697, 0.6631999260237479, 0.3570911556072076, 0.9905942706759472, 0.9919746917740925, 0.3561859047257792, 0.9308823407119571, 0.6978016992040678, 0.9080153290459815, 0.026509865105717907, 0.9518327208283628, 0.7600311257096058, 0.12376140545878062, 0.42987717238332396, 0.9923515936228792, 0.9734240350299778, 0.15880519370956941, 0.9893995070716626, 0.8462351081145545, 0.6555700736277535, 0.48248453796143154, 0.8408263448685573, 0.9680652645053527, 0.6745200822910337, 0.47429517728959425, 0.9816230248182115, 0.5678514917474256, 0.9609597828569177, 0.10340927263513836, 0.974158679114361, 0.9911011157604039, 0.7981498719816748, 0.9339329685268144, 0.8037616225914287, 0.40513599257531424, 0.19817713267388037, 0.2854798447766856, 0.35825082487487625, 0.9385879144413855, 0.24602565952037117, 0.8270795688340722, 0.09533927332522632, 0.16373003175332568, 0.9274108837145532, 0.041868122992243226, 0.2765137990715215, 0.1404725017723768, 0.6533963786159604, 0.4798681816525491, 0.5212236483781371, 0.05338439843664028, 0.728249449925087, 0.010572595235008727, 0.13419557817358782, 0.12313296799466025, 0.7374527182058287, 0.9112998301158791, 0.5715341350680233, 0.0010510641163393153, 0.2936063434276513, 0.965019524065094, 0.9746970603115427, 0.45048122098037474, 0.7586219006319594, 0.9130401513803149, 0.946435166274178, 0.7179540764423966, 0.9390800962532176, 0.8912778733367425, 0.8332778722145401, 0.22513042049455226, 0.9871612967052666, 0.8094304751945277, 0.8751438696496536, 0.026200619780992727, 0.8399843890093807, 0.9947790611075296, 0.6657312872103406, 0.6562604298329939, 0.6879037102452635, 0.8405632780765296, 0.9643123607747817, 0.7435943424390863, 0.8474191228463315, 0.36129542664664915, 0.6678473935471456, 0.7775972550797636, 0.11491454266699508, 0.2405757046645044, 0.8440674238972424, 0.8032360988950756, 0.9855342971064075, 0.23287320531429562, 0.6039980278273231, 0.40666414959404973, 0.965717342504876, 0.4358057247835761, 0.5714891997506913, 0.9830382173520128, 0.2603150821055892, 0.8410010070342835, 0.26338637540538945, 0.9786521065247206, 0.8136989901433889, 0.7142788489544184, 0.3431205398374364, 0.9175545816432491, 0.34890409670760325, 0.9610681066667938, 0.8404501126793671, 0.8535225436608234, 0.9292246188284101, 0.888862936293348, 0.8800679838674894, 0.952200306906764, 0.7266526152560373, 0.5705603693457824, 0.8910865990567789, 0.9205382764987217, 0.18764273135500187, 0.9478593391206984, 0.5367599783059038, 0.0045436446707037585, 0.9363688553071549, 0.9488260018221444, 0.8753578876726725, 0.37183702999646284, 0.4353291541516788, 0.966465876686662, 0.9845108353178095, 0.3936447490784512, 0.8888252532744295, 0.9726550949187437, 0.9555255911729771, 0.9646896147175289, 0.8276624269146213, 0.7902416085738083, 0.9607133183371458, 0.9799192382496953, 0.6092142764641606, 0.9886464039689347, 0.830170950747839, 0.3497308986101271, 0.8454502554021183, 0.40654306792611183, 0.9035555883061646, 0.4518848600790036, 0.005382599591733259, 0.2599323687276034, 0.8727139579025126, 0.7786728024552566, 0.9961244631619944, 0.06708961019203315, 0.9622798861833811, 0.05147818533340302, 0.6248670020004957, 0.767717705134797, 0.738025638211017, 0.9548750159434299, 0.5404753064443064, 0.9185929380546549, 0.976141984949125, 0.3562184291387655, 0.06008895704924261, 0.9454786147912925, 0.9674831096656977, 0.873223296108149, 0.3173671008550834, 0.07572291168321878, 0.7985948526445794, 0.8655042115121072, 0.36690347065649503, 0.9721919639041422, 0.7451218649811145, 0.9318777164300412, 0.9313451056308112, 0.9701166088565251, 0.935133650937135, 0.7674941226692302, 0.9587527353636459, 0.8789509716924687, 0.9521943296900393, 0.1730537450773256, 0.9614007664270198, 0.707356796601087, 0.979487559423896, 0.9476930232288545, 0.9326516982798562, 0.8095961454056549, 0.7802017541159896, 0.47957962926504855, 0.975683564185117, 0.8775008803828371, 0.9187505848359608, 0.9828128928648324, 0.9175073533803333, 0.9753601263690127, 0.9612128628672789, 0.2828844578329054, 0.5449637986959214, 0.9878639077618194, 0.7895651372236161, 0.9223663880150944, 0.9158260705232977, 0.240929216726186, 0.2838579974811082, 0.9793431305177883, 0.9597904330745354, 0.9759907028692262, 0.9554823000142104, 0.5452657493844214, 0.9904076286869041, 0.43355889971378025, 0.7611002956576052, 0.5131680787684759, 0.8887017783835179, 0.10874807507683983, 0.37773130422422246, 0.9914844509027833, 0.6364728433669979, 0.8114378959833556, 0.9756287304324759, 0.9055305599881419, 0.8044957957003379, 0.9652150592389264, 0.07570630800410974, 0.137967246650615, 0.37070158927361946, 0.9773018044526167, 0.9501257420717759, 0.3493069206554257, 0.5710678235085284, 0.8606685095316373, 0.7204960769359671, 0.980949568120919, 0.9072118396664172, 0.9507795852595949, 0.07235108686513654, 0.9687199116600855, 0.39821538779406057, 0.9555635810131096, 0.5487664297544206, 0.7713116859151199, 0.6097834690284564, 0.9130183803937767, 0.11421930020264676, 0.9349028753270425, 0.5101426927822619, 0.8350997929759769, 0.9674048149259926, 0.509171124774369, 0.7204613281335062, 0.804990157083295, 0.8803032900557184, 0.9009986338092414, 0.985229347245814, 0.9658216679121477, 0.6963456518901822, 0.3302503943082442, 0.6974134863029414, 0.04543812279919366, 0.8534053816948448, 0.8834744073827042, 0.9964923305100117, 0.7025158597780777, 0.5, 0.9676160375913604, 0.2656013656451591, 0.37168019484529546, 0.06096458756847016, 0.9410716015392477, 0.8715124751769509, 0.7489320041946982, 0.6191177016698447, 0.9891018179991911, 0.9522889658942308, 0.9914990693931154, 0.9912034238408652, 0.33961648420153184, 0.5, 0.9710265642372966, 0.9556001423135547, 0.9888940378207806, 0.0408151592415646, 0.9643381574779042, 0.9363104709680297, 0.962675243720443, 0.6505024874907938, 0.992229921686264, 0.007210572749005128, 0.9254145185757461, 0.9717858558271606, 0.8443756467061417, 0.3695136502433837, 0.9906167435614718, 0.9829734558618216, 0.9773428708956977, 0.9883397312728002, 0.11159739064325541, 0.9229764331348793, 0.5972284651440133, 0.956334213238089, 0.7232513794714988, 0.9481681650353132, 0.9924317633831865, 0.7057350255267593, 0.08016248924150232, 0.427735605571638, 0.29551060494875453, 0.05861111219709692, 0.7773543771209969, 0.8427845575988153, 0.8873291101800768, 0.9880893398884049, 0.8299836394073653, 0.66602478049705, 0.8674210749200325, 0.7341431335721338, 0.7592285114251925, 0.6369650425031792, 0.6806995883936978, 0.9828679674388682, 0.8925971008022454, 0.9867839122157529, 0.5244680179226627, 0.17616359788840882, 0.9909034991656579, 0.9076035416864099, 0.7430998031222569, 0.8557016166601501, 0.6838441979268401, 0.6906645055075563, 0.9999894695989162, 0.8697221609740653, 0.04518322360272123, 0.9683173626142232, 0.8088595837811808, 0.970329560741316, 0.9799639765398425, 0.8479525442925543, 0.7650697791000346, 0.8904550327797907, 0.6939132406455196, 0.8642428745488909, 0.9368223977210196, 0.9519719634608251, 0.9580067883585752, 0.9259920527770983, 0.13795087949288426, 0.47202515846482795, 0.9655075873748096, 0.8215555124727301, 0.9651449463175853, 0.8340889154244505, 0.6414882023429577, 0.13393120340683012, 0.8266593578021284, 0.0563080615774097, 0.655384500005263, 0.16585998716212427, 0.9840342111903815, 0.8396152066581355, 0.9229119806139032, 0.9226822415291173, 0.991597919502799, 0.17054463439557097, 0.978423116160554, 0.8440811712095584, 0.9537347259161492, 0.31462884561638865, 0.7852867045675326, 0.6433654403958524, 0.13689171989524404, 0.36243202725528756, 0.579060727980308, 0.2730646283357022, 0.976758808091472, 0.817317045473594, 0.9797564119452973, 0.9556838858523526, 0.48899779724692083, 0.08854303675504266, 0.7875052143934773, 0.9598892969566568, 0.5310002671614488, 0.9957076876630444, 0.5607606527456231, 0.9939071722832592, 0.8945133366361723, 0.8237171310638697, 0.5761534416073416, 0.9438846742701591, 0.9140608250628928, 0.9417083956209553, 0.8686757816395942, 0.9863386178118002, 0.9867299456982127, 0.9708875409473244, 0.4581212605324756, 0.5572381240311018, 0.9776170370203937, 0.07146843794269425, 0.17059471183937078, 0.9616568230551071, 0.935405766589857, 0.9803124245998134, 0.4862084659606625, 0.35218800788057564, 0.8932760519681903, 0.927622288663814, 0.6314525631640822, 0.21025466215659883, 0.01992499002166339, 0.1678798410718379, 0.7762064102476552, 0.55312921409593, 0.38888751178425923, 0.18070743503239614, 0.7636599886744166, 0.9893489185796819, 0.6014189015576985, 0.22594449121455792, 0.9971654695170948, 0.9549930266839787, 0.9775092350514045, 0.450587434817112, 0.8341135136334777, 0.9212934655874817, 0.2595156819386914, 0.1681321461877764, 0.9083423502114559, 0.9934318177208089, 0.23080700041822516, 0.17300221070140823, 0.8140176077568346, 0.5947494093346827, 0.8560288101070472, 0.7645279241104178, 0.9959427301621171, 0.8925804250760854, 0.892658144963987, 0.5, 0.808064803409763, 0.9645537815633047, 0.9043047375486697, 0.9812042016337235, 0.25931656748298554, 0.7041851011226928, 0.981618990754407, 0.9441429995901433, 0.005154013222362999, 0.9151083062927632, 0.4237124673974289, 0.15369130494585176, 0.8986127292416939, 0.9695884175792352, 0.9831025081311943, 0.935405766589857, 0.9267021937197154, 0.8655338310220148, 0.7846947581306604, 0.984760283590356, 0.1362165803738829, 0.9723930340249491, 0.9296371356943371, 0.9399074986481807, 0.8493575264841751, 0.9827941860241317, 0.838257862216439, 0.8028453946182562, 0.9266847163050906, 0.34971223414859365, 0.2697802687877593, 0.9354129397136193, 0.48471759296419353, 0.7995889930492549, 0.8322488690878376, 0.37314816784356497, 0.9045094249319451, 0.3736355463284892, 0.9629871670978796, 0.9687635820643301, 0.6819716711664279, 0.38419062096722195, 0.26967486228263643, 0.7135390760081789, 0.5281136540610287, 0.9683463954379576, 0.8705726466034794, 0.9884401282634869, 0.05856125906976884, 0.9627000459595892, 0.9696010459564637, 0.6882788369196997, 0.779122256608167, 0.7519759277646034, 0.833962894511512, 0.6691040385708728, 0.5742414649399775, 0.19658718816789786, 0.9791760432159483, 0.9091441135232878, 0.9873067773072861, 0.2564990154346835, 0.37918562996353056, 0.017193179133337972, 0.16951330050227884, 0.9554053594103915, 0.8863636292626235, 0.6877653213008582, 0.3942451881481574, 0.9514501505230573, 0.9043047375486697, 0.972687669776602, 0.7464714747416591, 0.9660336621376243, 0.6390139707107796, 0.9237760379910014, 0.864755225584049, 0.5244483279267884, 0.45635728143905135, 0.9911903346299117, 0.5595430936247942, 0.3145096210067668, 0.757683923850064, 0.8957129300395706, 0.9596133928018463, 0.14903951528727707, 0.9665034696393321, 0.1092646558491317, 0.8363980195502092, 0.9001017759517462, 0.0021003438053303815, 0.6103710961026496, 0.9330681204706134, 0.12197868837556225, 0.8494528484007493, 0.5583400606488853, 0.8702947517608448, 0.2957481004477054, 0.9824554336050918, 0.9770376907969298, 0.9304398108928355, 0.09927111895269772, 0.9726100572520802, 0.6959120144360048, 0.9316836359148046, 0.9699033507974564, 0.512157302889149, 0.9657754664112056, 0.7954407925779852, 0.835822108279117, 0.9546683433470842, 0.9229445403568681, 0.8121863711789475, 0.9921467944220935, 0.9720542528824627, 0.053966001046089694, 0.9925051605843479, 0.5689460815820104, 0.9634073257423059, 0.024152912449988666, 0.9347478149184786, 0.9688341444972748, 0.4764544382244541, 0.6394430743600186, 0.9896735911731904, 0.2251088469916353, 0.2820308940136136, 0.4618496258116548, 0.46413095125483467, 0.2437741468600175, 0.9574279278713475, 0.7220299311346483, 0.9710902005452585, 0.7153037800298132, 0.8702963633076054, 0.8269733447908753, 0.8326786440722841, 0.9892686439934467, 0.4056442961981892, 0.5387688005380699, 0.8841145775189575, 0.994810740403122, 0.968317362614223, 0.37319288398365824, 0.8349874281315957, 0.8055399044696094, 0.9842481422330811, 0.9840244009665189, 0.5183142494514733, 0.6382420086420634, 0.8167085617842174, 0.12994794292463202, 0.8113667323572893, 0.8101293595439225, 0.7260284695432093, 0.9204267303931909, 0.02260801943431621, 0.668478420939794, 0.990165297809639, 0.9371421257146361, 0.8469377830880283, 0.9754467426426487, 0.9351629982900503, 0.6007394691689665, 0.22218821838388325, 0.9691199914771663, 0.9681516844396554, 0.981162371444655, 0.9818353403658863, 0.7142920351993961, 0.7950547035551963, 0.8531231312829847, 0.8051653589846918, 0.5499779178913542, 0.03420147407903498, 0.12799174783253645, 0.1753718732175904, 0.8006670776702104, 0.9514952450629307, 0.05495359863679538, 0.9628765247502584, 0.9840887394162323, 0.8658144271134024, 0.44729855738830443, 0.9536788787824383, 0.9794901375642174, 0.32968142857149724, 0.7165099994857254, 0.050654571474409285, 0.8405495421772519, 0.9431662074075648, 0.9748247614030296, 0.09754734972538642, 0.18557008780347917, 0.012429504894371614, 0.15932871951924044, 0.8279761192191906, 0.9914087527279178, 0.9618031798503879, 0.7608602872962174, 0.09731929492363153, 0.995806338086363, 0.9913409000457748, 0.5497480311300802, 0.9626519527985338, 0.5207441948750245, 0.03442071124691784, 0.9220500066520246, 0.899294733941265, 0.11653988207111234, 0.4897814514067016, 0.5401854407543462, 0.27853405138028375, 0.6361635233207656, 0.5301450198778751, 0.9043411624553769, 0.5214436073776779, 0.1784207169726985, 0.21449776102029852, 0.9896126427994396, 0.6392940943675962, 0.8398468564815346, 0.8659376234902295, 0.16606284392039583, 0.7381307135770664, 0.942631138885247, 0.7753455214285889, 0.9261160800493528, 0.012414607751091142, 0.6997051533900421, 0.10220815170369113, 0.9715186328596855, 0.026226363747055056, 0.20223743044872808, 0.38138286911529706, 0.6919702577598145, 0.9051455701775276, 0.32326503208672003, 0.030232142768507053, 0.47503892144788346, 0.7559137217863998, 0.9757011290006016, 0.8664651426053906, 0.9072006999275796, 0.926305688186832, 0.8212917836629778, 0.8972222930469228, 0.7051280606380754, 0.3542057076320183, 0.9176196188106049, 0.4914877869256747, 0.15343918796800876, 0.8665204015385922, 0.9934625509947932, 0.8702555726446732, 0.9864585622526337, 0.9695884175792213, 0.1436604538733995, 0.9932066963400951, 0.07073570906657606, 0.9999840173415036, 0.2706252023502751, 0.8738877402853997, 0.7334473468457247, 0.27739237898514946, 0.9653981702813077, 0.3643765588034646, 0.9883583771217958, 0.8365418447159465, 0.8086464449415485, 0.69721300011791, 0.8041771186866951, 0.9394253164411086, 0.2223922784740407, 0.9927516556080487, 0.9347349335976074, 0.9499944474855063, 0.9492427722040642, 0.13056935163201097, 0.06668755312834167, 0.9238899552414067, 0.9931309812005785, 0.574851487650293, 0.6616646593075198, 0.43659414674795355, 0.08767259413869083, 0.7196687373495865, 0.739941103358039, 0.9939839188041071, 0.09081205150916634, 0.005201681902894329, 0.8029002631874568, 0.5848779803129165, 0.9022394429763183, 0.013832207839827445, 0.7192070242782133, 0.470011047119812, 0.75353764609245, 0.27559426566454687, 0.7818191208015335, 0.08616582962385355, 0.7809580716297295, 0.09649773008004142, 0.09017003271004746, 0.1476223022592255, 0.9006682971836827, 0.42299486262200164, 0.3404111709463234, 0.328705409331714, 0.4620041437661404, 0.027591635866031285, 0.637661900596052, 0.2927258163025557, 0.9249201619469032, 0.23066900661125586, 0.20346299681797325, 0.004426084632791338, 0.05296031128492924, 0.2507746202706609, 0.30203449564281964, 0.8789834395426519, 0.05299113667746082, 0.04433630739261258, 0.9320698262197932, 0.6103572006583917, 0.25361161086379985, 0.4502667505936749, 0.06135327965073744, 0.5339071088050356, 0.5559461263579103, 0.02423629460878744, 0.003921700231199374, 0.021178989264982656, 0.006045989795785208, 0.11115072116113399, 0.019851193980435455, 0.3502715855661125, 0.13417686911709398, 0.06130763198808499, 0.03960264017587402, 0.24467644705801117, 0.011900851294145849, 0.837574361786304, 0.5465785449695666, 0.5480417942935071, 0.36300672554093144, 0.735235780714244, 0.3065524289142347, 0.09607399609073049, 0.4935882493494249, 0.48655488710393757, 0.2716289243685595, 0.6567656821325264, 0.7378188178145445, 0.15161243408755148, 0.9356867051657475, 0.37468366835422284, 0.07812067419188706, 0.03518475189602243, 0.8513974555981908, 0.11488039773992394, 0.45062504404528186, 0.7390331290306366, 0.08089254701024808, 0.009590863085467239, 0.08659547284896112, 0.030804673101457052, 0.3151190443068023, 0.08321493524342205, 0.1513650853015306, 0.06223950748580752, 0.579306643009164, 0.018747931752745698, 0.4117212337322475, 0.6464842393824716, 0.041606719138370225, 0.537715649461015, 0.7900108142259106, 0.09508696631934613, 0.20748884012309798, 0.5131177560400343, 0.48982350965060917, 0.13738068988590502, 0.3066964380647352, 0.20011606005068577, 0.5574208759943556, 0.4368966624646397, 0.24138719887200447, 0.8142778547036936, 0.6250334415882413, 0.7711070243185012, 0.</t>
+          <t>[0.9966840138408032, 0.005229344788635329, 0.33458883528652267, 0.7078892266049546, 0.706177903242992, 0.9956343787809875, 0.9214822205945364, 0.15442585749396048, 0.6433318488607205, 0.9660718004739057, 0.8178793599893805, 0.625233778788459, 0.9730995168739112, 0.8594078537359293, 0.9750746092182161, 0.07749272998616162, 0.9445577586665633, 0.963999922282188, 0.9554062293760124, 0.09598532491773272, 0.9474219285405932, 0.9187082179300308, 0.9666243724150476, 0.5168526922830228, 0.6830812524055648, 0.0711497511423278, 0.9961986958447314, 0.9713887455928789, 0.9783489768288408, 0.4786224844499359, 0.9187717666942979, 0.10391155038619501, 0.7850353497885665, 0.7836160469557224, 0.7906352345659003, 0.9646032817659508, 0.6753641915276849, 0.7188864610494183, 0.8729073636233939, 0.9541207315053966, 0.85396921863461, 0.4145741239965991, 0.11171957250135718, 0.4634941529372916, 0.968229714191186, 0.3129679575001952, 0.9852982865654181, 0.8554942652747151, 0.0016965737256956538, 0.9677113504408856, 0.9651720018823362, 0.997028041443528, 0.28286205188404134, 0.9333212473827341, 0.9600167977551769, 0.369284852428912, 0.17758076532616807, 0.9254356755758668, 0.9876395963657156, 0.9582730936648078, 0.6461518326219615, 0.9037624857864355, 0.4157266056046201, 0.9423626610722468, 0.9801894669069326, 0.17901541505228527, 0.8199689036778987, 0.9856853134979475, 0.7867517202541848, 0.8422648304569351, 0.787384084537048, 0.8692545557738268, 0.895096565797284, 0.9886183603721345, 0.9344187331836731, 0.9275430394347254, 0.981519329177711, 0.9623993753986165, 0.9959729214278407, 0.028207802713241116, 0.9246480015072844, 0.8121307829673554, 0.8701128060943841, 0.9482077985108981, 0.8432296191857058, 0.9340930068453404, 0.9107875621500541, 0.9957087921903826, 0.5383124744304577, 0.5121652385172436, 0.9624077825226828, 0.44968448368615954, 0.8283736871391011, 0.8224872239596245, 0.19475363864091225, 0.743076164411123, 0.5, 0.36218077774205204, 0.9606075658689794, 0.8657294196218253, 0.38718595428320174, 0.6911107218017232, 0.6987052519042648, 0.7214947135906645, 0.27379446700190174, 0.9485898533682657, 0.030252920187047696, 0.81815137315199, 0.7009997643090481, 0.860015079518614, 0.2787449811344654, 0.00082691670339661, 0.88183568191068, 0.9740460497942619, 0.7441559864905801, 0.8394374259562366, 0.949748047105682, 0.8838176332101674, 0.8606436219615586, 0.7057589736394793, 0.5740092480294345, 0.6932333644267268, 0.8212556275434737, 0.8051099366823405, 0.3717730490686301, 0.5575659217661587, 0.7587000794987004, 0.866579814784379, 0.8920393947139494, 0.28262639235794645, 0.6803450881148413, 0.9656003335873882, 0.5954136090856523, 0.7270479350872954, 0.9639681508660921, 0.9667543124566764, 0.21360787759871938, 0.9915782263324795, 0.9841160461103616, 0.8358579229440594, 0.9873475843999491, 0.9951440117795872, 0.9561593025637495, 0.2140994825245686, 0.8743785650353177, 0.8456172882324287, 0.9946032269582379, 0.5787177693149818, 0.9859927324978854, 0.22369237193495103, 0.041211845067516524, 0.9456174957535198, 0.0336133818476459, 0.9416316841563528, 0.00756318727021983, 0.9958479438023152, 0.8138789227570188, 0.20753479570772246, 0.8540621286706245, 0.5670439263329625, 0.8861025779629836, 0.4522747996539616, 0.9665837949071628, 0.9813245143923743, 0.5866895171535421, 0.8859097287351108, 0.9551292623757874, 0.9293502575776245, 0.9522999248683461, 0.846670435499682, 0.9947031020907056, 0.8859864578996421, 0.23482776722182, 0.9650882948924918, 0.9458604089796692, 0.8088276331578019, 0.8855946609688289, 0.8935547689291234, 0.8970774967953778, 0.9525935009230325, 0.777296827089582, 0.5695226207472824, 0.956908378262095, 0.9786515244264712, 0.020081105528796404, 0.5926840399606956, 0.9667922047144429, 0.9805883430375668, 0.846332028782178, 0.9591894670420015, 0.9908433157237, 0.8734677525071587, 0.40079217143021345, 0.877533499823363, 0.18020966983918113, 0.6788998627746815, 0.9848493553049514, 0.861017434120669, 0.9362447389370122, 0.19651149865986844, 0.954186123604418, 0.8365018553770791, 0.9537531648443908, 0.8889338301260915, 0.6927250491673694, 0.8772251057291943, 0.7868235409710012, 0.99572123175909, 0.1062997847098519, 0.8200769710603386, 0.9227931369606989, 0.35797595773412144, 0.7526658681765491, 0.9211366143788445, 0.9261667559320855, 0.9928498319417646, 0.8478283314312642, 0.9814237168485701, 0.9687016248174936, 0.7758601689535217, 0.7664483766697572, 0.06677183359758274, 0.8060296234605684, 0.8309526761789188, 0.47554164758287076, 0.9400093472294629, 0.08300325676508104, 0.8895178548565793, 0.4660288660993604, 0.9924941557420895, 0.9172688790994971, 0.212611033136338, 0.9754683189366963, 0.9927324391853903, 0.800859603633665, 0.9869076146654097, 0.5708780692548476, 0.8966531630537892, 0.849850105977704, 0.8717965873953576, 0.7870827318357979, 0.91283148133958, 0.3486409012251989, 0.9625479179426546, 0.9127927154813232, 0.8737347613173916, 0.9649575298343024, 0.9623993753986165, 0.8333900373929164, 0.021376553466423042, 0.9371818747239489, 0.9856078500219402, 0.9827564767121068, 0.9493900887762418, 0.9845971889086996, 0.43713861184758623, 0.9078233968936131, 0.9258048139905916, 0.7337367840339388, 0.6887454140107988, 0.6904404811268875, 0.373533744841383, 0.610556516737953, 0.9620767254761082, 0.8748284280483454, 0.13881712521453493, 0.7879886635749795, 0.03416307673129104, 0.8745402271788552, 0.993720523971977, 0.7250470246884205, 0.418473906630068, 0.5497043657496755, 0.1758728505206005, 0.7029475866999145, 0.7687587257574552, 0.8053771256297935, 0.9508487303453188, 0.9921187242754571, 0.7143193567533382, 0.14185316327538294, 0.9280602448602812, 0.9972222857043771, 0.9881344379539063, 0.9765458721214993, 0.3804892622853406, 0.9867225525025513, 0.9650743792303869, 0.3171861370435188, 0.6118504601775064, 0.8922895474633655, 0.6064500412033408, 0.9824805143591309, 0.9551727298985959, 0.9785621117746817, 0.8499099287290022, 0.9827168865423257, 0.978679201382943, 0.5058582603302817, 0.49288720113033896, 0.04097587232196394, 0.8921969096672335, 0.014277210548530822, 0.05965235717554316, 0.7615381304377631, 0.759632072515637, 0.9761763777469095, 0.9359191335724479, 0.8151080925192502, 0.6460306133129953, 0.17893315273314522, 0.26327874534158197, 0.643219753929629, 0.9008828855785587, 0.9815038350600976, 0.09684007932702662, 0.4580330971929258, 0.4785984610420445, 0.8208584068375018, 0.5495359325386152, 0.9223456924226089, 0.8466698389629176, 0.9809184873582075, 0.9391974444303288, 0.9543940037254145, 0.7327877555766641, 0.9888300763718113, 0.2405825937269811, 0.24809753293956047, 0.9865676298351435, 0.5180295035293935, 0.8215402843731653, 0.6988904310212962, 0.9098043041032604, 0.4564069579243114, 0.6618878362701119, 0.9824246770408414, 0.9789310075844126, 0.9863402524253551, 0.409644113932929, 0.6092546530108389, 0.7822290994139419, 0.7648071133677316, 0.8599939688282575, 0.9448569136382444, 0.7837786303196711, 0.9640265004887921, 0.7859482333856299, 0.9440097563233991, 0.8874374208871446, 0.22075979082873629, 0.9822940394357217, 0.8712163036652686, 0.9740943045761941, 0.9361437734844966, 0.9936750173060955, 0.9869061480958015, 0.04522928084734595, 0.7828944548757575, 0.9959063601231649, 0.4524361338755098, 0.2752896295506928, 0.847310382004999, 0.7860269899113569, 0.9835796341295572, 0.8472143569690905, 0.7415822159873954, 0.7336672783311347, 0.6212299359672799, 0.966760812484197, 0.955572009151518, 0.9947389443862446, 0.19422846279656006, 0.9386770102323125, 0.951478409355235, 0.8654254188574259, 0.8508993801042934, 0.8450940490409646, 0.9541131201430646, 0.47724731991489117, 0.770477260894843, 0.9517612068930108, 0.8837884258696821, 0.16927080964233293, 0.5066165309438581, 0.9599492935239896, 0.3780785234816886, 0.7300142029523086, 0.9530902028730669, 0.988415862705222, 0.9775433131201761, 0.1329303639526245, 0.8462870821729723, 0.9114133990214576, 0.3088491923061178, 0.9679362989351903, 0.8239794971819772, 0.9559378924723176, 0.5874318840329371, 0.17576974675954835, 0.9024323350278975, 0.2615648052026995, 0.6934729172957816, 0.7571829214341512, 0.6587103643213861, 0.7400129896788598, 0.8498669157069748, 0.21686238635972985, 0.9780203302806031, 0.48568646414312033, 0.8348021463535548, 0.06285358859873964, 0.6375717608937361, 0.9068186257969889, 0.9473334478784903, 0.8648235295625437, 0.39801957260917176, 0.8705638094603434, 0.9041524028726422, 0.3729218742955738, 0.30617665086949464, 0.9520864419721377, 0.9679579202894942, 0.9201654410069917, 0.7764230679140625, 0.5930250769172717, 0.777146065445012, 0.8032201903207065, 0.29970481842543695, 0.9012025225417164, 0.8765369376556347, 0.9890972211308616, 0.8897101390381487, 0.9586673410147277, 0.9400295620012316, 0.9596064282431938, 0.8432100647974677, 0.9942165710135802, 0.6416854112991588, 0.5983019457149275, 0.9724702942860164, 0.89467341273243, 0.8799849969235584, 0.7178989432360007, 0.8873211304482632, 0.9575398710222304, 0.9819731396144687, 0.9190918989508934, 0.9617016201668751, 0.7027257658327429, 0.9860883395267775, 0.9352978530910766, 0.2809212240108029, 0.6061530033678332, 0.9753772413088971, 0.8230220276498209, 0.9999823727267746, 0.23527155326027663, 0.953278333178085, 0.8030245654790066, 0.9582400568717312, 0.9826846418200701, 0.9397969930265697, 0.044777924583647565, 0.9533463872402421, 0.9540010653680008, 0.061895659570542265, 0.5566002867701313, 0.8566747930291746, 0.9664535100127112, 0.9737763369954197, 0.9845569969110245, 0.9713549531718503, 0.33063631422703205, 0.20626998588727197, 0.010728494565958846, 0.45333766435129613, 0.6045719563232715, 0.9672934810019843, 0.1668179762829327, 0.9859511397910904, 0.27189849880269523, 0.9849960944944454, 0.12731620498372587, 0.6585780243679202, 0.9928734818551906, 0.8984323253041601, 0.010804366365865752, 0.9999839573713053, 0.20872396634447515, 0.6144347577678515, 0.06372470718024253, 0.26405263640103466, 0.37465670865106737, 0.6969774941024102, 0.6850306953353323, 0.9870875404970735, 0.6369512854052327, 0.9787299619087445, 0.9306597418437336, 0.3482944373887017, 0.33158085361023876, 0.08742432672660042, 0.16336373895106515, 0.4077122603840944, 0.5595750893390237, 0.9591483356202309, 0.9291732562611656, 0.945244999542452, 0.9856681243799557, 0.9827009391733719, 0.9937401836875738, 0.1641055600392444, 0.9005897734224437, 0.8805542288199926, 0.5150078413181597, 0.9859729517692756, 0.6392111350897979, 0.6565293560566534, 0.9614052914584209, 0.2141750742777388, 0.9832254814254082, 0.5347702027385296, 0.7559116654406512, 0.9553723931687669, 0.4841027759750837, 0.7406570020725901, 0.7370918250482628, 0.575720201001169, 0.8284970392751344, 0.9624442320700061, 0.8968638772043112, 0.6974504241427569, 0.4679396759822203, 0.9597003738946345, 0.9537531648443908, 0.6154426344412407, 0.9767471186739572, 0.808531438248906, 0.8581180713859148, 0.005413163298447084, 0.0054711951112222145, 0.7824643974891763, 0.6674563424297301, 0.8435009889459258, 0.9866938925935168, 0.31482645074805377, 0.7869565676280474, 0.9904323823492672, 0.07229231227652823, 0.6186777046756509, 0.9906019157247079, 0.44161638210542375, 0.9341735350215169, 0.2953853204464444, 0.9838276158648355, 0.1695732267673319, 0.9895749638900275, 0.9941142334367427, 0.9623144559398839, 0.9400104900386809, 0.9576657281427562, 0.48841497289102737, 0.5900838113336616, 0.43725272137539695, 0.9869381451205381, 0.9873286690046281, 0.748577224871461, 0.9819652969046178, 0.2328932590938331, 0.2551977405968692, 0.927206736467428, 0.76100096916889, 0.01727835164621062, 0.9229477825726781, 0.8670978630542477, 0.9880503077171404, 0.9969528279441511, 0.9733574593828661, 0.9550081517294832, 0.9916603362207645, 0.954640856754157, 0.9637845917773508, 0.9304273892628291, 0.9773032965852708, 0.30362391857840393, 0.8127356223685959, 0.9201227571100202, 0.07385142098071934, 0.9708834448380216, 0.9413540318434539, 0.6719295728905329, 0.9485003100181176, 0.7561958480177551, 0.9954748062682027, 0.10076314626401632, 0.5, 0.7913564913208972, 0.45360942460037795, 0.9297165353095639, 0.8961344887899256, 0.9717095394701305, 0.7873459308946136, 0.00852667469309278, 0.7680424823801129, 0.7607663332622941, 0.1779033416297289, 0.8325556436429027, 0.2982105619166818, 0.0004165448871668969, 0.32789160446913135, 0.8603192959142193, 0.3667921501825223, 0.9804161593175919, 0.1970581887220285, 0.8941632095436306, 0.9956792728889851, 0.9708176368768413, 0.23363263297001588, 0.966749032790492, 0.9648287434364219, 0.6825549069520275, 0.06738471826789373, 0.9803361380399027, 0.5306612061823839, 0.8079894534677156, 0.2051969494945372, 0.2542931953789865, 0.27554306736952777, 0.8411402900989341, 0.9903798435968414, 0.9113046390810144, 0.897534422729902, 0.9664624904798876, 0.9999871291672875, 0.9894092240346679, 0.1620341904396337, 0.8925402558530982, 0.7300274354419927, 0.9745699637153721, 0.9318157888292453, 0.9581834256815256, 0.6329858922436793, 0.053706876632683614, 0.9859262767240362, 0.9860921939711186, 0.9282052587610999, 0.02334298095011562, 0.9884395122959219, 0.6134878547477912, 0.9929084758191604, 0.34519406974372635, 0.9818232914294879, 0.6700253941805426, 0.9325474475307973, 0.6738790679870584, 0.34372421398263214, 0.4389584617124704, 0.9528328257832692, 0.6531192615865972, 0.9328068428377113, 0.9018336925675339, 0.4894384484721305, 0.2504551016594465, 0.9232176930283401, 0.09053192591351406, 0.9874629760399591, 0.13307034840933496, 0.9055319423687592, 0.8145976917519253, 0.8628600135810939, 0.4125832485348574, 0.9422040148727522, 0.6298551418136683, 0.6990918022308235, 0.8283600216053265, 0.9584140138759984, 0.9548350630812581, 0.9524197088795135, 0.0929587050000745, 0.8695103561867369, 0.1578992222942506, 0.04168308731307351, 0.19426139564650893, 0.7676199355205043, 0.9899757009830497, 0.9888014943140637, 0.05223710931593358, 0.02139020810296113, 0.03515469086884608, 0.9954029244128488, 0.9856532530172979, 0.5, 0.3811978076663641, 0.04788861955361141, 0.7915187999081648, 0.16079714631363948, 0.9669072942307549, 0.7645050440759479, 0.9619707199308702, 0.567022085751167, 0.9670087417047228, 0.8655791988396272, 0.30763491309450647, 0.6194080888821165, 0.4430877015762604, 0.9668092251062544, 0.22836602222951258, 0.9490371014315786, 0.4524834499807976, 0.2983380725493001, 0.9529750957931354, 0.07557977085622287, 0.980743370436409, 0.9032257818206771, 0.09527587876472383, 0.9777869896299038, 0.867650092443676, 0.546581887209222, 0.2026229012180483, 0.5895739089548254, 0.9695247028926725, 0.8451510263915093, 0.14213995042114133, 0.9373909558709745, 0.9914986204006322, 0.9966861527797707, 0.6979011237594667, 0.9158422792810107, 0.9677997473900961, 0.21876124372428676, 0.8469744866598783, 0.9511411648952857, 0.9862801185737587, 0.7212076023302347, 0.9541241151360423, 0.6061139390029434, 0.7607758995716154, 0.9808894293604506, 0.9798249512342151, 0.8149171667503201, 0.49147640471503967, 0.871313733937986, 0.46502190071643557, 0.2464793652661342, 0.9605418336280048, 0.9858905844155246, 0.7995633253533875, 0.0841154722406492, 0.9773002833864098, 0.967946078527523, 0.09894024047952125, 0.953768326722516, 0.989060857200384, 0.8605712052901386, 0.9915865109767679, 0.9578387056395427, 0.41545802248408276, 0.988707815397895, 0.40046325593869103, 0.9760502524575795, 0.6621560340789991, 0.9773196622165703, 0.15257180365496234, 0.6930449817829667, 0.9640740630090391, 0.08241159285070505, 0.42065933681874507, 0.1484594082528384, 0.9934351791126914, 0.8703966008567348, 0.04149028649140419, 0.3136807418885563, 0.984152462289884, 0.9613611153123708, 0.8472403219602517, 0.4524834499807976, 0.09388137536121625, 0.8920385227851733, 0.763340071953688, 0.9163918379959987, 0.9121965864731966, 0.7223712312179444, 0.9195743688549984, 0.9917268271534598, 0.7650204134624179, 0.0685561726414804, 0.8992485609341023, 0.8793336686402056, 0.8253731255645718, 0.9450282025463912, 0.30825507200316055, 0.6946747071222815, 0.4535669438897029, 0.8925547319019455, 0.1012407135918101, 0.863289203555238, 0.899173170932212, 0.7840720894343491, 0.696803620581048, 0.7662597474985307, 0.4724218764060928, 0.9828372285548477, 0.9888348049704253, 0.8185988929695802, 0.96143314082416, 0.8173917199685587, 0.9119901009332444, 0.175897500961445, 0.953869544008973, 0.849898502289866, 0.07702901889441337, 0.4640789505519888, 0.993889242581671, 0.9801105361275224, 0.3788920372571777, 0.9838730597004058, 0.9300552153986452, 0.7432463025184853, 0.5065772485184697, 0.7225335122565809, 0.9525005667688862, 0.652664639562518, 0.5174674169536065, 0.9693305807058207, 0.49468382544774053, 0.9477635461046304, 0.0942011351602075, 0.9855603183458616, 0.9937380140110066, 0.7627948563965322, 0.8777691923344838, 0.9188523937900359, 0.44270581358093547, 0.1671202058422012, 0.2742546882087678, 0.3545984510203019, 0.9650114802118529, 0.4258540349190463, 0.8959173302982617, 0.09000237961273083, 0.1558830464937443, 0.9174057922737775, 0.014920310461265449, 0.1497299038979215, 0.16506640522045798, 0.8424866544668205, 0.5970025917249114, 0.2728112278688751, 0.02252165106108269, 0.6362895411003842, 0.006837857680826397, 0.11544667689804664, 0.28582786937109894, 0.6249235819807634, 0.9443620051957031, 0.48155269747744256, 0.001151211786108812, 0.34119241257141536, 0.9748145040577136, 0.9739044924130595, 0.6613044339674798, 0.7145082505077617, 0.96468376155398, 0.9365224100888075, 0.8326631083090632, 0.9425082132195579, 0.9342517276908879, 0.8751040292204451, 0.1572517360235748, 0.9925699963263329, 0.7990872458519258, 0.9186356525077948, 0.03556419802235055, 0.8182411038242271, 0.9958318121664904, 0.5947580324306433, 0.8691354307329606, 0.4061337194629126, 0.8575541248052797, 0.9758623007503466, 0.7847710332524079, 0.7773158458169951, 0.2691295099421365, 0.6520503812115013, 0.7960321983895956, 0.10853851827821527, 0.1649611347903278, 0.9369367589074811, 0.8402037134881626, 0.9858168300780863, 0.2490114454447967, 0.46038136956316045, 0.5356101416904561, 0.9458604089796692, 0.28982017634816315, 0.7317576289637122, 0.9857526040499343, 0.2534605757489281, 0.8652325994097517, 0.22883110120717035, 0.9933158292734569, 0.8864532850257442, 0.7552136770173391, 0.5336187984803532, 0.911767565964372, 0.4155930646405362, 0.9568579635588662, 0.625412745783228, 0.8999239457480981, 0.9523645315628309, 0.8752008254431048, 0.9435830209985954, 0.9018837898420005, 0.9566228465815911, 0.5192974565149495, 0.9250819177775208, 0.9222583769372582, 0.4823746364347363, 0.9520359882662371, 0.5446809749650922, 0.008335799100919295, 0.9521041559265737, 0.9561980940587618, 0.9239322423638218, 0.2154514593299089, 0.35122893565569807, 0.989491299579931, 0.9790562762264178, 0.24299586552881094, 0.8887535064782409, 0.9619977120860268, 0.900678416335098, 0.9772141876560695, 0.8405325819648819, 0.8672532895504385, 0.9756597656230832, 0.9758737060762144, 0.5886723096801055, 0.9808994273100736, 0.8478283314312642, 0.3814841132010811, 0.636126421660371, 0.3767288601221677, 0.9620201318134833, 0.5933219099765643, 0.00237342672065168, 0.27686418618058956, 0.851453567900738, 0.48687661789370046, 0.9963359498414105, 0.027697668953419255, 0.9517612068930108, 0.041832178443146316, 0.5916403782656553, 0.8014143667473879, 0.7881977652249219, 0.9746216547110137, 0.69148335606061, 0.9460999094887116, 0.9802239789303843, 0.4451443608835241, 0.03540057855704171, 0.9285400460766257, 0.946147094613511, 0.9686098291623834, 0.27668920153002047, 0.09195868616049362, 0.9427369614829264, 0.892083767360447, 0.40023924691674234, 0.961036602562987, 0.7672765683180881, 0.8058953158358272, 0.9374606208384119, 0.9529774001706042, 0.940542966612602, 0.7778665460572286, 0.9652492663211277, 0.9023804834269356, 0.9442422940633225, 0.120086457022848, 0.954073243849963, 0.4888501101446397, 0.9868715343924181, 0.9551236368211261, 0.9806072856159359, 0.8632195626064115, 0.78964559832499, 0.5682327050580491, 0.9640474667898188, 0.8551153908769131, 0.8978012327139704, 0.9797168110053786, 0.9078733568502807, 0.9734340482162068, 0.8546924122061432, 0.3038092088281488, 0.6244048858775828, 0.9857207911045212, 0.794585388807271, 0.9205541773771154, 0.9527998456532576, 0.21926439960943833, 0.21558728243290898, 0.9781969296390668, 0.975694424696, 0.9775539199908534, 0.9612732957603093, 0.6678764084272059, 0.9718507936685993, 0.4898911983585633, 0.7950991693674403, 0.8035772142378675, 0.9134744987953278, 0.08302415589118334, 0.45840493322505604, 0.993584994032968, 0.5509353826411185, 0.864672050553172, 0.9859060974413428, 0.9165590434053695, 0.7950562511825978, 0.9778784078271038, 0.06894996946059916, 0.17018262011505678, 0.3534298118802743, 0.9748168092302687, 0.9109884347862611, 0.4166379749233121, 0.5456210463822246, 0.9305731478785473, 0.8023409140294119, 0.9830249010977701, 0.7811718834657658, 0.922831666080241, 0.11879202295672553, 0.9609557624553436, 0.4256637225291153, 0.985808573158621, 0.7122167575303423, 0.7543411321882896, 0.6126068913677294, 0.8882832692083199, 0.20231163974927754, 0.9569696999826307, 0.5494198914465781, 0.9463028491091324, 0.9693758286813231, 0.3576542445644808, 0.7483311018839355, 0.7600975516791812, 0.9049224113114595, 0.8215238722872427, 0.989826437735466, 0.9774765166112811, 0.6880626018978885, 0.19754280507978644, 0.75303016187049, 0.08578828875171753, 0.863592373432294, 0.8941261877915774, 0.999985312039747, 0.8380825187422118, 0.6611225930411466, 0.9609470681318311, 0.583461293962483, 0.4251377359240563, 0.06802181441914695, 0.9561465178253308, 0.7741781791030772, 0.6820250003808417, 0.6024780220945686, 0.9916563760282381, 0.9493330047133506, 0.9888697402832687, 0.9957843727176848, 0.5, 0.6073018053750088, 0.9850895692359539, 0.9771278598568612, 0.994461940283873, 0.041994831286545464, 0.9425065307933269, 0.9251673947106032, 0.9502191511325582, 0.7034486078883198, 0.996599701188606, 0.008522446660180373, 0.9508057045229539, 0.978493454756276, 0.9062187024777069, 0.19834283928972923, 0.9892093044017581, 0.9727157172507485, 0.9786638821249906, 0.9795196020166922, 0.12222610414129144, 0.9289444813773101, 0.6080618703769047, 0.9746635325961298, 0.9028421765456952, 0.9596387998455256, 0.9964739480011986, 0.7132280847141012, 0.06767133701444537, 0.34081841412792807, 0.3332847226307377, 0.28506765630089886, 0.76262534683719, 0.9182304402723886, 0.9497559106918729, 0.9825318185137217, 0.7000798823901362, 0.5819604736186581, 0.9279829130846878, 0.723924424702484, 0.7542873132821689, 0.6880361053994271, 0.7624283156733749, 0.983127335446901, 0.9252385814557291, 0.9924069825210446, 0.6597172420700843, 0.24163853102885702, 0.9905227733711611, 0.9472099753968438, 0.7624627760505188, 0.8983597623461687, 0.5957233422326457, 0.8387949836784068, 0.9999963256643699, 0.9004202209592601, 0.02923232007354116, 0.953753164844391, 0.896526727646186, 0.9784977796732, 0.9915410428720419, 0.8775460422607109, 0.8483642985429884, 0.8979042772455808, 0.7659651978844783, 0.9063043284750516, 0.9724556021489996, 0.9511908244220901, 0.9777674308029876, 0.9469263110335778, 0.16034063395208237, 0.4474265887479675, 0.9737582400959298, 0.8878949726846938, 0.9647316393928422, 0.8375799949344122, 0.6186653935205938, 0.12859484120510203, 0.9342724850478964, 0.059818338141133805, 0.7132340352299155, 0.23893463833897433, 0.9888343363787432, 0.881874000212225, 0.9486004946608161, 0.927199359967064, 0.9803623206492728, 0.2780971481224581, 0.9912096665491831, 0.786586889612415, 0.9092436872676344, 0.31134448667740705, 0.8713944272480506, 0.6818712378754263, 0.18445887270505437, 0.47466333476295525, 0.5918790019390038, 0.6000485940545726, 0.968635811445636, 0.8530590452072183, 0.9919499165131679, 0.9268590809655471, 0.6156738148610345, 0.16542950386256727, 0.8973941208247069, 0.9752981831856254, 0.5826136187501608, 0.994359485479015, 0.7603177836633171, 0.9935551800204735, 0.8697670146160497, 0.7919688417280609, 0.4900464158491052, 0.9474673917394201, 0.864510018460939, 0.8833725937206416, 0.9407818564230576, 0.9858179356980922, 0.9886755299319017, 0.9582160853930165, 0.4920943192424595, 0.5575100928920296, 0.9817071731844292, 0.051058803650318486, 0.168379058250014, 0.9712363628885577, 0.877533499823363, 0.9774078694906122, 0.41030112739195035, 0.22668499392942842, 0.8821790093163973, 0.9294525870563102, 0.5390382276985022, 0.1831151426844845, 0.02563329023104158, 0.15349760303071894, 0.8696910953444429, 0.35664806211609534, 0.5466147983149097, 0.1467538860583731, 0.7432714879804215, 0.9846923912530282, 0.713557369449623, 0.23824439332775268, 0.9964466515121319, 0.960764438994381, 0.9603277619333898, 0.34346848573839045, 0.905313482230427, 0.9756030672821482, 0.2792905861601585, 0.16145037556483535, 0.9611947060391328, 0.9972995331882434, 0.24099871941194317, 0.3875140523822345, 0.9120385677494287, 0.3341990225249468, 0.6858266720328355, 0.6862110412790071, 0.9953016738694722, 0.8803595562263409, 0.9204993777085044, 0.4184345215094513, 0.814043035466093, 0.9763969996818992, 0.9127927154813763, 0.9868725673643094, 0.27816437578966363, 0.6623901715206613, 0.9808153560726712, 0.9585118599846807, 0.0038712126341416656, 0.9122979052194137, 0.4841820306832771, 0.13249414640212862, 0.8462212054589541, 0.9649020404005525, 0.9828547210319523, 0.877533499823363, 0.9441092021416787, 0.8941746970216221, 0.7967156970186031, 0.9880419099699108, 0.12954002013454477, 0.9903316236951867, 0.8921537429735493, 0.9402553418504805, 0.8846918042263977, 0.9906222951921266, 0.7064621692612383, 0.8395537355744596, 0.8896523152846912, 0.41447496785301385, 0.24613005236301497, 0.9579658520506975, 0.6481390582443532, 0.8011356520416293, 0.4519590139912806, 0.5086446127616235, 0.8949019370434991, 0.2774407397750149, 0.9833541585053005, 0.9335107740564251, 0.7356522848913066, 0.41818555580767736, 0.32297779233502566, 0.696715038432223, 0.6788178969400899, 0.9546408567541342, 0.926984900568075, 0.9895521470844887, 0.02812919958766077, 0.9667617167046428, 0.9816949644153128, 0.7475346791114046, 0.8277802016964618, 0.7887965670660486, 0.8775851027071228, 0.44627212431059426, 0.6161143183761529, 0.17097629100602338, 0.9743407095765649, 0.9534680526792038, 0.992565069353025, 0.20000247003479896, 0.37673731262175963, 0.016128070804388286, 0.09790583210223373, 0.9393570987780446, 0.8378159069451312, 0.5800470761840141, 0.5528984357902269, 0.9440580457164106, 0.9127927154813763, 0.9682851981790257, 0.7558431609845512, 0.977545359755801, 0.7745478744819437, 0.8797898663100986, 0.9255257699596097, 0.5605528150294504, 0.63850501486085, 0.9963601531793955, 0.38545792786967586, 0.3611284407971735, 0.7726522819543054, 0.9529341863667227, 0.9862434545710282, 0.10598243011412387, 0.7343708416069693, 0.1312686303972336, 0.7424929633413009, 0.9083712134439131, 0.0015529617458510982, 0.7520190741837932, 0.9420274504132689, 0.08948819265140368, 0.7998921860207221, 0.6226256961951618, 0.8650269533748033, 0.2998901220796753, 0.9839036531592442, 0.9818713982379144, 0.9487167534681361, 0.25196765272351224, 0.9720779428643902, 0.7383381055254563, 0.9452758829224591, 0.9839635042600304, 0.5146925605964339, 0.977521188499767, 0.8393857802697197, 0.8572691157019664, 0.955764436048342, 0.9205047197191817, 0.8740725053486168, 0.9932877345123664, 0.9595017637270936, 0.041994622133412714, 0.9952657493119863, 0.7815603479740999, 0.9752998265754661, 0.031096995964217108, 0.945083788795248, 0.9703601534001327, 0.7327124560435678, 0.6293993101560406, 0.993783421774301, 0.2570735242095753, 0.33028472189494756, 0.4460294690087832, 0.48767337480029527, 0.304417114032626, 0.9431323066273481, 0.7348825648755547, 0.9798952469269131, 0.7755990916537403, 0.9318824951552653, 0.8406998453970324, 0.8549585695418689, 0.9875875065915329, 0.3937852317116619, 0.598531337116557, 0.8456321406664898, 0.9967243614612513, 0.953753164844391, 0.4526185990751324, 0.796690800067566, 0.6544639047293409, 0.9883393995248516, 0.9764468282638881, 0.7461791881731836, 0.6874818519647817, 0.8336082587120773, 0.12311845888496832, 0.9239467626049057, 0.8125253167994485, 0.9043361273352137, 0.9219558373147108, 0.01626313361183084, 0.7467304096963827, 0.9792935094598841, 0.8939621571360897, 0.7186762067117356, 0.9830335545088503, 0.9016450825109915, 0.5830590599044441, 0.10262254426271866, 0.9704546355483403, 0.9551727298985967, 0.977769920921095, 0.9747961248778151, 0.7642291804917403, 0.6752686655363777, 0.8969781799879366, 0.6746741194132891, 0.3714918683477587, 0.05466538244508464, 0.07730638890190318, 0.144252382349496, 0.8419869887576352, 0.9495099965955113, 0.04582834811856508, 0.9626555373719515, 0.9778442757828729, 0.8801438785740943, 0.5654169695618958, 0.9381436978399239, 0.9477065319547294, 0.39994290936736004, 0.7830408489209848, 0.0584685628777598, 0.712510178991754, 0.958328448856297, 0.9863406641478666, 0.10093639718507602, 0.3000655060536386, 0.008377902857824585, 0.1710395444138286, 0.7968909849440456, 0.9908233734724019, 0.9482890003468785, 0.7312828161769942, 0.08342352676364628, 0.9946365645588336, 0.9882853029350152, 0.40596950160790923, 0.9746952444326415, 0.6904324041496488, 0.04052912122496602, 0.8038263749035994, 0.8989110240281863, 0.12331695908674183, 0.44564414064738334, 0.5840043192481774, 0.362075736318177, 0.782699907062587, 0.6152907588745665, 0.9616629404684527, 0.6264187213929908, 0.21733327255874987, 0.3415260481648696, 0.9902137962677175, 0.8310548684398492, 0.8646275892915458, 0.869488302006668, 0.1221921286625228, 0.5601384651296331, 0.9851634601694464, 0.808864559266783, 0.9329024132817196, 0.009829873536667292, 0.8345979009113621, 0.19868044569254104, 0.9865522292246528, 0.024732459273447357, 0.24157335274004652, 0.3227977227617153, 0.8622557443848704, 0.8619816881715362, 0.3606035926326183, 0.05354039485923774, 0.4512311111427822, 0.7611833605127395, 0.9657037556492462, 0.8125843080910542, 0.8635000487507161, 0.9417625854046552, 0.9015978238206197, 0.785190409610882, 0.7345390207911078, 0.3053928641184306, 0.9287304942561918, 0.5226604363423953, 0.2194548766815444, 0.7982457647408283, 0.993798366715157, 0.9221844986005695, 0.9885171328964548, 0.964902040400552, 0.08583468663082128, 0.9932917953153285, 0.09416747059114791, 0.9972699050957385, 0.2518384913361151, 0.8643671263871545, 0.5861726999804644, 0.27100080825279393, 0.9664082372089178, 0.4192477642355343, 0.9885152598894005, 0.8332459511655712, 0.8751190638680109, 0.6938297126532951, 0.9029065316860511, 0.9697646342722699, 0.179790563314671, 0.98392804756172, 0.9570186338405083, 0.9561605902092541, 0.9089590215114397, 0.4297522264712767, 0.06095516238213982, 0.9272928874623672, 0.9763216335563767, 0.3961247597727388, 0.7839494856656912, 0.40434828686083046, 0.08376904063133679, 0.6952575442917466, 0.697306292605696, 0.9909595430156406, 0.12603478500236692, 0.1275783401510722, 0.13244274485777607, 0.09709708320735551, 0.06557303733701272, 0.1955745920101217, 0.7406910899812547, 0.7899984085673373, 0.0037525126660617066, 0.10740986586068464, 0.07048492313816665, 0.6217122032067074, 0.4016442368498943, 0.022075475415354866, 0.843704751042054, 0.10709829737522844, 0.735359293916331, 0.05034546107209769, 0.26343163744046805, 0.3197077723026889, 0.2912715026724884, 0.19577621939916684, 0.128546824625944, 0.028060029915681, 0.33623458095871056, 0.0020882237705241516, 0.36625835141791857, 0.24177995795944202, 0.9213488341112147, 0.7664093181067498, 0.00904651921679811, 0.31629225730928784, 0.06813075259016836, 0.5898406183955517, 0.0052402004888586935, 0.02581144080332403, 0.17764291827996162, 0.16475727944954008, 0.18446065017771318, 0.8477202191838058, 0.020873507001824856, 0.2344439858770095, 0.8200753367961177, 0.6449192475518746, 0.4297554720478005, 0.09256529716581052, 0.42456073353410395, 0.09196541573283223, 0.068990008408817, 0.18500929486248469, 0.3603904845715474, 0.1384338848785122, 0.007273375229140113, 0.026857381318350682, 0.1464078762823441, 0.404462342071306, 0.7966899878616229, 0.9867634927361267, 0.440813679667033, 0.698055580878743, 0.0633600179463362, 0.3961354524522722, 0.6859032751354698, 0.6292919386430226, 0.010316151136714715, 0.025554438519915124, 0.5530597120168792, 0.8765667673047947, 0.8723316178431151, 0.5898050886362891, 0.40272820389672453, 0.08465901775662511, 0.741585740968056, 0.02615480995603816, 0.02171466575525662, 0.21055565280485292, 0.8121016015937991, 0.31569665294002874, 0.3938802862641569, 0.7093019231681456, 0.2528156715017729, 0.27130680335453866, 0.48754367862562764, 0.6179285390468646, 0.024426136549175158, 0.005548398700092798, 0.6568679215716879, 0.1480472369876471, 0.39009898242323837, 0.0057396434444144375, 0.6092763672225203, 0.8919132984901182, 0.6253092247745086, 0.7883702124157534, 0.8016967746380491, 0.842007173077333, 0.11466847948931767, 0.3006837519856008, 0.5383625575440787, 0.16071712858011752, 0.13088307141993594, 0.0014879761279041645, 0.27873247547484115, 0.</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>[0.6579772347289935, 0.48114264395586587, 0.02543772216127315, 0.9192765664494514, 0.7699080276188961, 0.8762040910998263, 0.8564791066996827, 0.930027924186432, 0.8106194310386252, 0.016065180718173297, 0.9426079539059897, 0.8966926787100138, 0.8357199850388684, 0.926430872696366, 0.9877833433154123, 0.36843137740627685, 0.7541425266543056, 0.6739957599509406, 0.5559201797089462, 0.8743639201527933, 0.9059467649417015, 0.7540550182769213, 0.9857428812802643, 0.4407450511513664, 0.5397218296390848, 0.28538979546412835, 0.8371314461975409, 0.8898165416366676, 0.522634435995873, 0.694084617708979, 0.311693197578041, 0.8351145671552731, 0.9736055818154993, 0.9755913606607433, 0.846600847230253, 0.9678810092619728, 0.9810339370177953, 0.3298422077397186, 0.9911305124328033, 0.934361989692899, 0.9575615048834487, 0.9893935008250817, 0.9545650949381572, 0.09830248348789378, 0.9174972535907704, 0.794025324545912, 0.9918022716264684, 0.9910718803038139, 0.8967737523884943, 0.9058520110398941, 0.9584872405044963, 0.6154825281382659, 0.9815145499845915, 0.8509783211151334, 0.9717892763225865, 0.725175636692712, 0.9228598083225802, 0.5187581944396611, 0.9754026147347635, 0.9515560073163181, 0.9304813012062239, 0.9363522946161488, 0.6012259961532948, 0.882987658108431, 0.9885714592203546, 0.9999841868702952, 0.986556520193386, 0.2759836931419265, 0.9807074359455332, 0.7753745314536659, 0.7960837835412857, 0.8903274776572639, 0.8264861422532652, 0.9470292746487697, 0.9921931840119186, 0.9952749389116221, 0.9808975161758355, 0.9743797010342322, 0.9254793009653609, 0.7890542199443714, 0.13241277982800673, 0.9858116344291377, 0.663825854534055, 0.9010242209682503, 0.9609566651393031, 0.5, 0.7976785804293554, 0.6855408471882284, 0.9761340579318183, 0.9734811676730888, 0.9163726123088107, 0.9085840462960885, 0.9771415361056414, 0.9949920632587027, 0.9361638501668981, 0.7083085837413137, 0.8283263334794649, 0.6703956054573469, 0.8661719055835596, 0.9304373768822428, 0.3191394472020225, 0.2327909002493385, 0.9156570906876896, 0.7317030109529307, 0.8965387364241592, 0.6630021346728607, 0.9882877366711224, 0.4182179540284743, 0.8146357626679872, 0.9811731623907155, 0.3546744560534673, 0.9918207766042617, 0.3637402630071615, 0.9717910174683683, 0.7540453884199549, 0.9962389395856669, 0.8288300645765204, 0.8009831206183448, 0.8294387383363596, 0.3037849767473747, 0.9478846753052275, 0.6071243673302266, 0.6820057757756259, 0.9435352076671778, 0.9481496773040953, 0.9461833008178262, 0.21351040695153428, 0.9365167967353545, 0.9445103195954159, 0.9829009304707709, 0.27586825477086335, 0.5844474531851628, 0.22352726060702544, 0.9243636418284514, 0.7226998848979063, 0.9391722314897298, 0.9793607535158252, 0.832220824268988, 0.9028528945928029, 0.7189438170739152, 0.9899592162511918, 0.9378524360690359, 0.9635227721078726, 0.7096888211585843, 0.8296485768365645, 0.6925499465926583, 0.7320897509634874, 0.6251947912939733, 0.9250848149061793, 0.934849066397746, 0.8249238031929245, 0.780617468626822, 0.7064938129272638, 0.6140241089458705, 0.842424922930321, 0.8933526783754318, 0.6899257918516005, 0.8932539996543968, 0.9093280071298223, 0.2871198707285353, 0.04336151477338093, 0.05215387881962094, 0.06079821421998276, 0.8631775901749029, 0.5431908877305952, 0.7350576062139369, 0.24068888432881405, 0.8522605874092999, 0.37236453800882036, 0.9906622002623272, 0.10501190805705828, 0.8315540282753644, 0.8334521139697557, 0.4949606808149152, 0.8797952628930845, 0.8633926341716405, 0.12937462860692908, 0.8386491840924492, 0.9375511009614953, 0.9780842706108409, 0.9350763954345402, 0.7878784148315477, 0.254793779942668, 0.9905137877964885, 0.8968364568259805, 0.3853159638911171, 0.9004548119865775, 0.9391874883334597, 0.05938216359471348, 0.8800257642940076, 0.9864619435851107, 0.9294574147061625, 0.5833294772572098, 0.6245936044523146, 0.5761372427015646, 0.8921195257358523, 0.9894548527955463, 0.8316471892328281, 0.6757870671898161, 0.9934940019323927, 0.4183348891916422, 0.9191756507615035, 0.8864284711863974, 0.7876355191185874, 0.16998144109237423, 0.366305469799229, 0.8136235266899168, 0.05391316914224661, 0.770760890915357, 0.9942744136212641, 0.5, 0.9601087920572002, 0.9854133859794376, 0.30399031968110796, 0.9655527369574928, 0.964265001290019, 0.8188483316308326, 0.9697587290580323, 0.14535556870202007, 0.7346214857909549, 0.619680538329318, 0.08081622915378213, 0.2618318658201175, 0.8968803497989054, 0.044715161423943335, 0.787681930046121, 0.852490750093727, 0.17340868183091715, 0.3733787550891862, 0.03674846666959894, 0.9380592293667056, 0.3155538626540462, 0.9768710356593264, 0.9911966538442974, 0.5741842759042796, 0.4323236022990606, 0.6332248879585912, 0.7647838202545166, 0.025895844982122336, 0.7888928637180742, 0.954236895597531, 0.09189415147574698, 0.13936999394734165, 0.07802589964571796, 0.7156350784794663, 0.8528688779913521, 0.6752057673046493, 0.4265109668172001, 0.8554977501697152, 0.894381588671264, 0.31632871528611617, 0.9957577631081391, 0.9642429130845506, 0.6955757422050892, 0.8939724315500728, 0.7783133499637145, 0.6767584872203609, 0.8081003089585616, 0.9877086134334596, 0.926085895498517, 0.727508475267638, 0.0491358003028682, 0.9668680819955885, 0.6025670765494975, 0.5276549373185576, 0.4089155721623454, 0.31061211645065884, 0.16881074704748167, 0.19708940603489866, 0.31790820240555345, 0.16299453475766087, 0.36613129174276654, 0.9493304028271529, 0.7170955503098768, 0.6816945265436499, 0.16454343077749534, 0.05958190851643675, 0.9429709866518535, 0.8568629283229799, 0.9635769451593554, 0.6729486314660797, 0.45504540663561993, 0.9575041867214938, 0.7957864787371061, 0.33268870044948357, 0.44839527235934773, 0.4290474838152151, 0.9861484561586263, 0.02704917882420155, 0.9270695629738577, 0.9999947826772189, 0.1377277201473648, 0.1219866417796459, 0.9950908426188413, 0.9146611271016307, 0.6922841234557661, 0.9683375606408692, 0.23257180845515688, 0.19892729261321257, 0.6150298815264068, 0.09872308666802025, 0.258511897731826, 0.953832114247785, 0.3168516275035404, 0.03849378474621119, 0.9653826793524143, 0.8792486947904841, 0.3817562185275494, 0.9570608228612283, 0.9862249073039208, 0.12863445915158303, 0.3988980553077669, 0.034527948985602956, 0.948635552122945, 0.6242693812260272, 0.9760755606638357, 0.85880300461796, 0.9032819216793815, 0.8588135306708001, 0.9901931013747202, 0.7336481157142939, 0.2821962620166092, 0.9999830360979557, 0.9873438178233327, 0.18844546020930972, 0.9930853769952099, 0.1678383595587859, 0.8127771273065095, 0.9080254073521258, 0.6119743244421455, 0.5854469192311658, 0.8474970173573052, 0.9818649085571841, 0.7330305449398768, 0.7900096929618339, 0.4900271581122435, 0.5939510349001822, 0.8683785782769906, 0.8612514301906949, 0.7114822826971883, 0.054293542584566194, 0.7792865206563278, 0.8277927825662016, 0.4635313031487055, 0.2158539172857097, 0.7251447980511724, 0.9297742149976151, 0.9884451655850155, 0.9409881367130368, 0.9487028033000635, 0.9828430699500826, 0.9912779978267303, 0.44162542002546407, 0.8367977805867401, 0.9416899904152938, 0.3228349264285437, 0.9834322298610748, 0.5505500175872446, 0.7716421093303487, 0.9569070029190231, 0.3869192207916157, 0.4325157981082257, 0.12330486766595415, 0.4575021294924773, 0.9118391694571918, 0.9887030177241317, 0.8106330216161162, 0.5575178674425236, 0.6479823085619507, 0.7403689780353376, 0.7742437970760497, 0.43550405175800844, 0.7792083663216886, 0.6131829499947131, 0.9446511969353303, 0.916505503368245, 0.41093282826774047, 0.9837670090944737, 0.9803542308644855, 0.2424034831176183, 0.964832511735413, 0.9339215795112912, 0.9908122763056664, 0.7816285841340085, 0.9436659069987477, 0.95750999031032, 0.7316701572777394, 0.6080101704146101, 0.9811032982775757, 0.5836690116873618, 0.37735787658976955, 0.9914140813121858, 0.3695430400990789, 0.9918264028325874, 0.7980010059161508, 0.9808675479989856, 0.809571514949846, 0.43642100800734435, 0.964843499599926, 0.8514207919372646, 0.4253639045228773, 0.9665237067306877, 0.8136078825280386, 0.8276306303604515, 0.8983808220868493, 0.5499502522950388, 0.10544579494204905, 0.46186373298066374, 0.19059910005664246, 0.3008370787323987, 0.9966200726779292, 0.8314107146081738, 0.9918005866896028, 0.9151008920885272, 0.7816031429531957, 0.9787452035274484, 0.7969471312846493, 0.7889622766029415, 0.24990253608206778, 0.9780729250140014, 0.8386115460474025, 0.5, 0.9734966420030198, 0.2008176448933076, 0.16185974410076495, 0.29308239241542766, 0.771928695544341, 0.6676185128786488, 0.533312252378426, 0.16866121343416526, 0.7710574052797734, 0.21057748331071108, 0.8648571187792123, 0.023399265063890787, 0.6321018069615053, 0.9645734587363151, 0.25638853397669265, 0.8468155466270808, 0.5792354281125711, 0.7778377220038395, 0.9598661332159815, 0.02205297473296911, 0.9867191398155372, 0.5747966408566704, 0.8816908910204401, 0.9680146718246915, 0.9742383580227497, 0.9883049112995426, 0.744047730612235, 0.9516050384830745, 0.30218145729716694, 0.15626505461977877, 0.04235360283504757, 0.9232068171943586, 0.16206129687086027, 0.07846676947715713, 0.8485097692323647, 0.36458286984348864, 0.44631554204485724, 0.9066452508640095, 0.9374659466018747, 0.02895610030170319, 0.8060635880451327, 0.7767909833596938, 0.2841399226976253, 0.5496499098162378, 0.33206194413074613, 0.658825035296657, 0.5335358603028441, 0.9305554348268156, 0.9797705661597964, 0.9915370232666763, 0.3945563629879823, 0.9779463318890653, 0.4565325426199538, 0.29219666471493244, 0.7513269546892146, 0.017594236906435815, 0.847177638294861, 0.8271716831423218, 0.05210833346936846, 0.9772243310592024, 0.0069318284012700165, 0.037966433992899194, 0.6895446001105745, 0.7728330394879113, 0.669163905513706, 0.7152087293094169, 0.8605993284040828, 0.005005024473291276, 0.9508559850804588, 0.7585997596509119, 0.8339202059566004, 0.8296897608356374, 0.9753697244536158, 0.4775919925799932, 0.39274934985171595, 0.7207964645688305, 0.2668224706698352, 0.922166957968445, 0.032752884053949695, 0.7683172313546461, 0.07974756942035503, 0.9857743368867782, 0.5251237449586121, 0.5884852701975962, 0.41900593588720186, 0.89239538442867, 0.05072477851964912, 0.8789149652311533, 0.8347265860199249, 0.7289720217143543, 0.9857184617312738, 0.30332577726016174, 0.9293187634521465, 0.4551421339951575, 0.03616724802717052, 0.2944077958607463, 0.8836450284840306, 0.7412749781276748, 0.8558301785356783, 0.9588953877547673, 0.8699775375012668, 0.10363136534383628, 0.9675347117128501, 0.7280131466848294, 0.919911641037262, 0.7539203441045433, 0.4177160941124562, 0.8664499557982445, 0.859050902807614, 0.8355474766998932, 0.7670480346813359, 0.9357944481369749, 0.41743741633778175, 0.5984482572736588, 0.37975414320372386, 0.9672051702270406, 0.988401313956915, 0.5202138470961041, 0.1587232673527053, 0.05153067338551794, 0.9179593738689739, 0.17524040973718708, 0.4827960107415952, 0.809460677649837, 0.658985192651093, 0.5276763444146501, 0.648114112605422, 0.8597364623269739, 0.9245015790975374, 0.573236609032384, 0.6442535149714816, 0.1515618356000955, 0.15669725014207042, 0.9583356296587744, 0.8465660320769895, 0.5, 0.27692880460352537, 0.11940344613882509, 0.6324948110593654, 0.7313819647093295, 0.9502823864784328, 0.8795936938898362, 0.9913423753336702, 0.4860600655815191, 0.9426742799075961, 0.9999860025492731, 0.34446356001239387, 0.3818405228747769, 0.9472670881899674, 0.9006629861548892, 0.9740625824615802, 0.1129961678784296, 0.6091602695264133, 0.9191810154846567, 0.9386460029923793, 0.9158503712278366, 0.9641542286148279, 0.8402103061675115, 0.9720789962041961, 0.05060080047148257, 0.9784998003651212, 0.9585479048185699, 0.9738495312340525, 0.9939384448625412, 0.9652791512884809, 0.980076989227785, 0.004174303109554609, 0.8584892963910088, 0.6512017454970531, 0.507250189883069, 0.9639772161826999, 0.5643560108684972, 0.9316071973136182, 0.8044809865999651, 0.9858179505024992, 0.6941161304754172, 0.3607143625796979, 0.9483037499481722, 0.9757179696888896, 0.01813245769818397, 0.4801160049305215, 0.9481705042723382, 0.8499121654911228, 0.9327938835755164, 0.986167543438496, 0.9916712193104371, 0.7132267196574213, 0.3787161700544881, 0.9870908081753119, 0.9854770679164144, 0.8079366246278182, 0.014852661188562492, 0.21905200724714682, 0.08804045101578434, 0.7975024795294287, 0.7946292705518571, 0.12271792304442065, 0.2192018071830231, 0.8195832271346483, 0.2743701291170325, 0.5472037545803963, 0.5692176972437832, 0.9844727893571644, 0.9957054019677429, 0.8373864659147267, 0.9118646086960623, 0.9833267968722817, 0.8688912590922165, 0.9018100086955688, 0.9288076536160375, 0.3774850207465607, 0.04095894582022929, 0.9707169232241653, 0.9913234335601635, 0.979973764689061, 0.9812787276661256, 0.6681096222607795, 0.9805399584308226, 0.09235671196599347, 0.7459140098622483, 0.9568701555511225, 0.14719237651983139, 0.8872561559842056, 0.8225718560009373, 0.7649521727885161, 0.8987694390087287, 0.97822280990993, 0.6244723807692366, 0.48049002359666837, 0.9440769376370293, 0.0031617011348878308, 0.6452082794957101, 0.9822307475671737, 0.3496004244830788, 0.17811706488968754, 0.9043316047016123, 0.7476356273239464, 0.9757313035936086, 0.45135557523211917, 0.7900367828242073, 0.9861506906609151, 0.5920245935337513, 0.9801358604782975, 0.9489157147703982, 0.9932452439519877, 0.8808071572181689, 0.9947065761683849, 0.3155738049175033, 0.9228441829148734, 0.7317043569993275, 0.8935008017017341, 0.9274052277975584, 0.8684660338427963, 0.9786404376987765, 0.9229307900195771, 0.4828259400643173, 0.9852628289909247, 0.964912244909343, 0.8623554417625015, 0.7969737926205938, 0.9483992586416405, 0.9939477599848999, 0.9909296179539192, 0.970963746003884, 0.7083236516380544, 0.8291381462229261, 0.9141321020032259, 0.9568175349200313, 0.986115722845199, 0.828419825303015, 0.989333839730876, 0.9948811177577617, 0.8665123183001233, 0.9440504028931468, 0.9044689888342669, 0.5157442613194313, 0.9629743356906992, 0.9853823331082749, 0.2877620479251654, 0.8856473594006454, 0.9185353727735929, 0.7362631593941668, 0.8846765640109667, 0.848216418095921, 0.7407700603326224, 0.9776004789496443, 0.27634268019374064, 0.8768446336454297, 0.9872215018416014, 0.6101319582098693, 0.26554327042215686, 0.6600270885735443, 0.8639666411512162, 0.9973549836027821, 0.7820722152856052, 0.9424032545146542, 0.9383587558591183, 0.38564217682791463, 0.9774515692058169, 0.8153744817617578, 0.8877160954004502, 0.9806434660013994, 0.37868737411122905, 0.9606335973523279, 0.9629712502442372, 0.9803873358648014, 0.5971354131746152, 0.8305772561017127, 0.9388540958196827, 0.8250108630464006, 0.6158845001013785, 0.07694550517170098, 0.8835756043274353, 0.6074136688214988, 0.9200059309415174, 0.08545168891052031, 0.12409029802591182, 0.1016212415082675, 0.8370561262597735, 0.9525507881066427, 0.8559200239820759, 0.47448452632781096, 0.23310885033149967, 0.23360082244627722, 0.9260528393228746, 0.0612384368701199, 0.9928662946346181, 0.24504262896149126, 0.7782397725324028, 0.8552802308482186, 0.0736645244282844, 0.3044515739683381, 0.8465378485057657, 0.9962073101922139, 0.7508737657132897, 0.8185936537299162, 0.17241666015358434, 0.9938141593567477, 0.9532338648382046, 0.7843072265541629, 0.7734866402560108, 0.16050570071840176, 0.026030634354152954, 0.9780607647232143, 0.43752876489421516, 0.3898906690224406, 0.3302274192498786, 0.9201570398375002, 0.010492108009077017, 0.7552933465410281, 0.9866123310137427, 0.8336218840230584, 0.925880114819992, 0.7403089211039715, 0.9593524349024977, 0.7402458472541122, 0.0972933769917632, 0.07046383994666468, 0.38229194889961776, 0.6672802905235413, 0.06435733638239464, 0.9893708271303222, 0.8103217063556358, 0.8742947603251013, 0.9853191892352461, 0.9260012495707456, 0.9868633118918919, 0.8348026258684037, 0.9864348999516731, 0.9809301566800204, 0.711427497698679, 0.3581109103459012, 0.3996936393493575, 0.4272827343917318, 0.9142439947472585, 0.9517639950350988, 0.9627684262450729, 0.5465681026460556, 0.9625596866927424, 0.5, 0.111034100384178, 0.988743252715589, 0.1500070660392701, 0.2980319991038065, 0.9676103733387922, 0.16015127103240243, 0.7541194060204324, 0.9662598673691699, 0.9632785159101784, 0.5698799502642722, 0.7643619112756578, 0.28731744397285236, 0.9660125502054528, 0.9856959166513501, 0.040245436034503215, 0.9904729393174418, 0.9899268151144017, 0.9597327849569006, 0.6060331385329968, 0.12370532956399172, 0.975248054514517, 0.6841138237862047, 0.9864489090496028, 0.65511486717032, 0.9939615186032076, 0.7325687840111076, 0.27127300245753116, 0.376516800273019, 0.9855947128473749, 0.37423137302512927, 0.8605891218015854, 0.5298350883382538, 0.9040591659421259, 0.7240952450855511, 0.769805383458556, 0.9111307158606994, 0.9704431377894014, 0.9939770653447629, 0.06193542235215458, 0.9952172791418945, 0.7707249836742166, 0.8637790272950271, 0.9846103107835077, 0.988754628632847, 0.8921426680505216, 0.9772180646550084, 0.9718154855756661, 0.5877937640454746, 0.813982394903251, 0.6659598562029816, 0.31063504515122387, 0.07454838236293239, 0.937835485496985, 0.9597219682800087, 0.9909235469760213, 0.35513809896059534, 0.7939821928503158, 0.851692529943141, 0.6340423639298248, 0.2784077136506174, 0.9816467099974827, 0.4467714475931049, 0.9687067495388673, 0.1006757063701708, 0.8273053234944608, 0.8356634119748547, 0.9490100286797846, 0.0810996650802555, 0.7430766470671989, 0.6717010347922977, 0.9296392621656658, 0.9506143013922513, 0.27680987782122396, 0.8409044802958354, 0.9925769284525635, 0.920567419313237, 0.1267072301887896, 0.6242616498859235, 0.03810725053381626, 0.7483564607003401, 0.5744338106366952, 0.19796003065682644, 0.4405957499720207, 0.8882627549413386, 0.03685713588524965, 0.257174889810965, 0.39698348358638413, 0.127666874763787, 0.28122616692719454, 0.9933104662266548, 0.9387243799314064, 0.9629641465110701, 0.9146771011320846, 0.38319576017560025, 0.7958991791656594, 0.38414796726856715, 0.8717990236576483, 0.020065558151152876, 0.6814762459575857, 0.9575996727330924, 0.9160907453620919, 0.9299167731040843, 0.986528409031281, 0.9916099169745825, 0.987774565066026, 0.4413849053968897, 0.9922062299206428, 0.3101321535674482, 0.999981736182634, 0.9803091737819543, 0.6476564229788098, 0.5964095393433695, 0.970678216071576, 0.9590882284028642, 0.3612622676599284, 0.8126581282467219, 0.991623435243008, 0.06652766195597265, 0.9521932537097494, 0.7086861326139419, 0.36856524371158794, 0.009212569497336337, 0.8734325988613975, 0.023093662910594982, 0.9868586261031344, 0.7967409206849234, 0.11062570360318545, 0.46118183945467855, 0.932319654744064, 0.9708386353834058, 0.9901342207675707, 0.9807888521639381, 0.1593256934455507, 0.08807967821541601, 0.5653023057846488, 0.6143086696858966, 0.07174382666121476, 0.9999819169221016, 0.46409907548738955, 0.9478435458472801, 0.5448683474559733, 0.918197631136494, 0.9281841150242921, 0.5400816443830236, 0.9887118072479861, 0.9444374838515488, 0.7561278055220543, 0.11192556476727403, 0.061242834456233186, 0.46319454101041, 0.943845597389245, 0.6130892533512624, 0.9130790902683721, 0.7694546328056139, 0.1995693086596233, 0.890120461424073, 0.017476945317062346, 0.10411920085375709, 0.8182859561804708, 0.7129553894179216, 0.6300490074805558, 0.9741125913301864, 0.8356587719428709, 0.9207512301556504, 0.047151933882855275, 0.9827781052151011, 0.17372978672001493, 0.8560124797371635, 0.9128112804475941, 0.9752675750893111, 0.9497633650900558, 0.04972226114497762, 0.10934071181801545, 0.23448965846845016, 0.97040074655519, 0.9498943198963248, 0.8941309761410895, 0.9569983366485905, 0.9781671250516526, 0.13944208333385025, 0.9815721083232286, 0.9115297731336071, 0.294612669172932, 0.4750761377963313, 0.8913353290955224, 0.21828076579218172, 0.8283669144875053, 0.9909041937846642, 0.6227050647775965, 0.786876800312327, 0.9152496688799128, 0.0065838679209087635, 0.023012525673343946, 0.10883737496088601, 0.7683321102799663, 0.7087512023977147, 0.042652716944265937, 0.6854842339355449, 0.9716076014376407, 0.593083418340698, 0.0864264956857995, 0.1647742754997699, 0.9353796223381566, 0.9733389364109802, 0.16192033781302795, 0.5118718743749173, 0.2373236045268987, 0.2357465234793416, 0.07965692217913264, 0.27335952874153213, 0.8616087614055585, 0.7060836169602911, 0.9852697623233297, 0.6916269983724711, 0.43712302711378576, 0.03509768825322657, 0.795137941685327, 0.7605963547652782, 0.8547425278083218, 0.7709312865532816, 0.8752683120967389, 0.9812590036017826, 0.6537625315153638, 0.7955212567710097, 0.8455762702305316, 0.5408849637732166, 0.9931188084264889, 0.595741548945716, 0.9413187572961667, 0.9832556613666611, 0.8294358779918446, 0.8402905722115348, 0.8981091979684526, 0.20627594685024656, 0.8981377171456197, 0.8404497268927611, 0.5678886777661385, 0.8047607405280031, 0.038442491805890364, 0.752054391519249, 0.9880880473656709, 0.8280510492706836, 0.11970528515368854, 0.779707184036694, 0.8109983389298868, 0.9849849561388785, 0.597523485530367, 0.9928155326033579, 0.8323784324671691, 0.9837207489519769, 0.3193093281714593, 0.5477282232389898, 0.9464286931880763, 0.8727607820844376, 0.9597081540331277, 0.8841978747924493, 0.923017545547697, 0.9180426134184385, 0.044824602461457086, 0.9154756509271988, 0.7639764363360672, 0.028542847959355317, 0.8350014424617974, 0.9912888879949145, 0.4566591586733643, 0.6699526736680329, 0.09260846237499765, 0.9007416156861029, 0.8483522158650747, 0.6812055517265849, 0.7562910151909732, 0.9536889998033693, 0.02466891408271, 0.4200672807676282, 0.8385701612976405, 0.9869677487429658, 0.9569111946017468, 0.793332694727415, 0.9154212462949115, 0.726093466381721, 0.8738651399024109, 0.9911166941370061, 0.9246873794592388, 0.9718765811640563, 0.1805712516082058, 0.9461599774192081, 0.4590044160340908, 0.9180278870370667, 0.7837790363947663, 0.7424438973311092, 0.9508145843076158, 0.9705264636941247, 0.722040628997185, 0.5483305453258224, 0.9572931131801496, 0.7770732312734061, 0.7507853608137159, 0.488839626420964, 0.8175117515453701, 0.4025681581102188, 0.9461165568243591, 0.025888258623367324, 0.73762442430251, 0.7158034873380604, 0.9253657096144079, 0.864126047932374, 0.18231568328462408, 0.6367412743843399, 0.3312507360018429, 0.076061871068957, 0.9300932283162443, 0.6432383685083248, 0.7794595601692385, 0.8461286382065777, 0.9286590000057169, 0.7370135238538896, 0.09437242728126743, 0.7353121327156209, 0.9241436743041213, 0.87167679948978, 0.5924003561101805, 0.8057728931051954, 0.9171051219974186, 0.6323151381913769, 0.9448659848817593, 0.14266406097327408, 0.9706073786195113, 0.772531299275302, 0.8002103435864207, 0.586871908312844, 0.6009948524517044, 0.5685398505564452, 0.9328168880995695, 0.9037508047809016, 0.033004090547393145, 0.5191178267283167, 0.7868063543124234, 0.8028812383688327, 0.36582529016115406, 0.3323949950238411, 0.9318285072940872, 0.5625715824284934, 0.7892969631634706, 0.9887099403910129, 0.2930622798425056, 0.8460121896858515, 0.947766100069279, 0.8510777528418944, 0.9112021898961293, 0.8301964150653088, 0.008481437386979424, 0.6707909375299941, 0.04660155072884157, 0.4306899514075481, 0.645038058774859, 0.9067612403782725, 0.9301484563916381, 0.26834702097002966, 0.627394431939463, 0.9089497738411638, 0.031193859059014586, 0.9860343836748603, 0.058482498671078215, 0.7771915104519567, 0.30555700395513236, 0.022229717319599197, 0.7938973270855856, 0.7502873876007782, 0.10877349323365425, 0.3622030453861979, 0.01015608078558567, 0.9573771906649103, 0.4189846030271227, 0.8406048710275041, 0.8904312396559212, 0.13974397411045117, 0.07997815459873736, 0.0002464932427553153, 0.7724464117047352, 0.24550910680547844, 0.8670984126208835, 0.08545168891052031, 0.025131124232408906, 0.029777153713789927, 0.9362114531509784, 0.9754477697441527, 0.7018918733084829, 0.942096203056747, 0.42945537726918415, 0.8345571493849945, 0.6080856875619968, 0.983323689726059, 0.05948201185034754, 0.44613439745115613, 0.0430979424112299, 0.02838922505726533, 0.13310299687641955, 0.1239715542297718, 0.7812978339679884, 0.8618898785967307, 0.02586810892357079, 0.8166822271167129, 0.4514758190699567, 0.46458732308139894, 0.1449640669667942, 0.4263625109354563, 0.9902896113459949, 0.16527347600286046, 0.0034504289800669657, 0.6921742976850151, 0.8334438694862407, 0.9435702259541633, 0.9823804284027735, 0.19834170954021074, 0.0921381444902582, 0.9766249162473319, 0.017902374164971414, 0.766679630507367, 0.882319757352464, 0.02341642112910734, 0.07041205035321176, 0.15594911863770858, 0.3126575370589549, 0.35255035147646635, 0.8964266767736906, 0.3766369316478057, 0.9761881962875133, 0.9854564639628508, 0.9412425290179004, 0.8923544963235442, 0.9167838985967743, 0.06367888066893009, 0.05980403027640643, 0.5505184047565183, 0.06864053836373651, 0.056318711892078106, 0.12364124718481251, 0.08046389366419904, 0.2401933305629695, 0.815321777478455, 0.9464237918964914, 0.965941140528055, 0.9384306302476546, 0.943076923722727, 0.17373413312822356, 0.28993519081973995, 0.8719933056088752, 0.14327395001055673, 0.9244804520159428, 0.19813128910813294, 0.2800135816689681, 0.7331162302979546, 0.571772336016884, 0.07904599068538608, 0.9504041231862034, 0.9672291601352951, 0.027656435298013954, 0.010918982126287566, 0.907576565888423, 0.018349528438747067, 0.20538529720793805, 0.8108820025917265, 0.9519092477304864, 0.08911278019064339, 0.9715953325621219, 0.6718975446909045, 0.8346245120210245, 0.9406725645763273, 0.9676316862689043, 0.2719815826392526, 0.9762183611029738, 0.02133983811974891, 0.547032171137448, 0.8259168445326893, 0.008452803595214659, 0.1633585059017584, 0.13754718231451182, 0.8202259597449578, 0.29797247732074333, 0.6678785945950284, 0.7431632154830751, 0.6750474643210485, 0.9367729876128358, 0.9831769356625308, 0.9821983870929181, 0.868703409608067, 0.8932703675379028, 0.9864715156937491, 0.21976142559230993, 0.38655161903687046, 0.25015239740672074, 0.4017940806007928, 0.9010677204469402, 0.03571533577489129, 0.19169629108221967, 0.6047637019029721, 0.04740283581547606, 0.4074754613311964, 0.31589534852992185, 0.028970458493334763, 0.07586319274437181, 0.054520329904630134, 0.8511752494185153, 0.21993551990788654, 0.9339413896667079, 0.41038382977817617, 0.9869084082889392, 0.6324439445857742, 0.8766981428400823, 0.6508230053051488, 0.8633127919494832, 0.9328107463194458, 0.4381738365125939, 0.8835871630197664, 0.952788003576271, 0.11536355882492268, 0.8473498674922488, 0.21913223948025468, 0.825367460491279, 0.906890935309292, 0.8924298338232937, 0.965591247697942, 0.45877278745494726, 0.36634934234547334, 0.9737028414473128, 0.9629712189490224, 0.664628244249058, 0.5574816625541039, 0.9412087182345853, 0.038254003258232784, 0.7018128661677953, 0.8750779162170231, 0.6729434123550723, 0.0794290876920131, 0.18209156976704238, 0.36735343053997904, 0.9317616672685478, 0.950639218269488, 0.0004050241153816868, 0.954306037009032, 0.4949010143301583, 0.030849031494862924, 0.5163459655844258, 0.9529971364575077, 0.6779341438384262, 0.8561336016763614, 0.5395697765536571, 0.6973133624289786, 0.5804014822299547, 0.6354061706961996, 0.05563846780103065, 0.18697982187956033, 0.7458920519130788, 0.6136968369448882, 0.9876309220444363, 0.9301404246813362, 0.7711884571570342, 0.9048575094229484, 0.9357836701932726, 0.9856920752286488, 0.6319727438044174, 0.8761500364402403, 0.6228901563498044, 0.5837954014367286, 0.0899819567766713, 0.5429987175668662, 0.9740563263238844, 0.8768822197923888, 0.9453205817622812, 0.9655315465729353, 0.34657875998237647, 0.350136541382925, 0.5710091103307054, 0.22611991728395103, 0.562316115019302, 0.970411084810915, 0.19584607135452206, 0.2654331746229478, 0.00957990458028789, 0.7627473414212028, 0.42168476165636076, 0.8183755016029268, 0.995616666037774, 0.34188292743639864, 0.7683777726825941, 0.1592959921168926, 0.26012546318590424, 0.9455170938144335, 0.2645439309100312, 0.84720463620994, 0.352712893067771, 0.001810026751804259, 0.9494202888033938, 0.7182339277924567, 0.9834223902077848, 0.5609476903800193, 0.5737410808134129, 0.15843828520961944, 0.006184334812917753, 0.9653239885204419, 0.8986583770156207, 0.636527814013925, 0.9823681460579252, 0.9767671117373168, 0.2802406986912386, 0.07577564555477034, 0.5838314540385593, 0.017683444417917363, 0.014868281086170835, 0.34066728354478737, 0.5337555618512684, 0.00043718854482740203, 0.5693526484913987, 0.014375839992135393, 0.030901837281972336, 0.17499475570741263, 0.2853992991182829, 0.9125783113574711, 0.056700030687815144, 0.015976676449320864, 0.007215578021852352, 0.9050616719396806, 0.15288187765635555, 0.28767847924367973, 0.6161663403212319, 0.703897610454365, 0.8519123572865321, 0.08128844135301018, 0.11714375229077682, 0.5572762374274921, 0.10514660386001017, 0.013000841962512923, 0.17789262426603755, 0.7076204561330439, 0.24518615201364122, 0.5345650466512885, 0.7538361724193349, 0.47292187053606566, 0.4518885289757574, 0.972921239134833, 0.6605198695630663, 0.6558928614748235, 0.007159395317989835, 0.21109374314233284, 0.5699648120882145, 0.09702867337812923, 0.1374843426618587, 0.16245099288166415, 0.012975451707218812, 0.11079760520264664, 0.03081097542269354, 0.02153404857706842, 0.7887698387552384, 0.6866525251436438, 0.014715632543370404, 0.13346774598085687, 0.4024291659543112, 0.022820813963412543, 0.11441068325281115, 0.07142406811470542, 0.2986752415252825, 0.4395704944972381, 0.0007485904559475189, 0.08926701312770993, 0.015112045037735711, 0.11433033194751102, 0.9846391592014907, 0.010324572036095629, 0.2789316715203005, 0.008520598958333823, 0.44223432982195243, 0.08408031612040397, 0.7676730512251588, 0.8105831356514296, 0.29243220275638493, 0.527317035622272, 0.4326216461872414, 0.1744360986191274, 0.9040165875015723, 0.23401933215606757, 0.09588196223255055, 0.14847100591043755, 0.2451483218630653, 0.013713237326448554, 0.2889979041578061, 0.10963721285280374, 0.26653180617079875, 0.08414057622774489, 0.4484533942414451, 0.9257053629473821, 0.751696667759628, 0.1382539169525757, 0.07566320527942193, 0.56374997051303, 0.2819737215089028, 0.06202786290693147, 0.010430416592759286, 0.30929814736448974, 0.7833181240690092, 0.013841623123600589, 0.6460013498295974, 0.031894224529891387, 0.7158469467185918, 0.10266749180738774, 0.41635077320093156, 0.3410045334669637, 0.3057158567410302, 0.019748186629960682, 0.3072267519173362, 0.7175751329833396, 0.7967117065852596, 0.01266744402481088, 0.007283031931290942, 0.7970426428406748, 0.2797220243928408, 0.11627401163528477, 0.252642839275831, 0.40800318450190604, 0.12254854104371773, 0.4330661573508889, 0.9440479617040264, 0.15362317951792143, 0.8882513209363649, 0.0023077619756102364, 0.4077671186432899, 0.08591963598575401, 0.9617223686403384, 0.061691133611889624, 0.020399684505868855, 0.013035305591336845, 0.1654228888743843, 0.05967844756259126, 0.005956613432569102, 0.8432793075369744, 0.11539710980589095, 0.15302235615190168, 0.9875891316720462, 0.654768014794146, 0.5372019741444524, 0.29025365706611905, 0.0660825561476574, 0.4783596661430139, 0.04883270788080807, 0.09868217330390794, 0.20971666648132967, 0.23060018478388403, 0.6616863883266829, 0.02830651931420296, 0.5152094884270927, 0.06106342049128006, 0.5424565210817215, 0.8079801293094345, 0.7793426744760614, 0.4903803652436704, 0.03623455495701777, 0.043722588535791446, 0.8494943854470545, 0.9306434418872616, 0.04573633021941223, 0.004273246323419483, 0.352186535379709, 0.22437969271102307, 0.550756349456231, 0.6126185705438041, 0.10113393270928854, 0.5175506745548226, 0.05512078139209161, 0.29547081628940075, 0.008389519190140679, 0.08598607686384362, 0.9264011035746426, 0.6220746535806921, 0.8990440065728718, 0.7200961890442794, 0.2568006919930407, 0.00033020094776176637, 0.7263069246662175, 0.44118554982293373, 0.12092145475323868, 0.04313337581769782, 0.17856333126528318, 0.4699058469910749, 0.012500452160610914, 0.6834075805488837, 0.8879027915883266, 0.026493388943160848, 0.21605615159486652, 0.7601798084778113, 0.6404729779474141, 0.277209966904278, 0.5772336306767993, 0.0960242618700872, 0.5618047867738991, 0.08700516730660289, 0.24199969224836052, 0.7717449927508485, 0.46457124857296495, 0.13169983042211714, 0.00635552386368016, 0.8435610329647042, 0.5634652920338208, 0.012931308272969884, 0.11423709948027615, 0.5415723258842841, 0.017296329588128614, 0.8292488654575185, 0.2532368239860039, 0.09967247991681394, 0.2768856930476898, 0.017000055977339883, 0.18501210261339382, 0.8482104312156563, 0.048348905929616076, 0.08635415357670546, 0.0003317527470437516, 0.8543542970492304, 0.010943324973693156, 0.016620240102485532, 0.35609557338842046, 0.3279781030206108, 0.0015195920056553162, 0.26967207888989586, 0.0040882988854287</t>
+          <t>[0.6679286204917539, 0.6130637817454652, 0.021332861994310295, 0.9381956470795609, 0.8250068023627983, 0.929798549294047, 0.8067022417628178, 0.7384446083321692, 0.8204572008121618, 0.035163738045006235, 0.7903644549712319, 0.9425108419509846, 0.6838106507424278, 0.922540188580495, 0.9896390362516538, 0.7771192750944776, 0.7096290941215586, 0.6341202966304548, 0.51109649957174, 0.8173184027111826, 0.9017635137665507, 0.8368581552226567, 0.9867652637910622, 0.280273993412854, 0.5980714934534295, 0.43884667862598603, 0.943339395018948, 0.8628730700073929, 0.8483515264460804, 0.4192952774275773, 0.4483559971696189, 0.8762746235536534, 0.9633630069827748, 0.9831919984710952, 0.865698037463634, 0.9757082280317926, 0.9857838296738475, 0.5, 0.9876109823047732, 0.9614364718952713, 0.9472832176942716, 0.9867980838979916, 0.9576248252276146, 0.06851107897307561, 0.9519471863095545, 0.7719386692756511, 0.9842474100873269, 0.9917369902779106, 0.9242478361495032, 0.8802182721508621, 0.9794772465289472, 0.5360003591049816, 0.9695808761647954, 0.7706198527973878, 0.9782734950390046, 0.8217076403672373, 0.9010892000681912, 0.7867914718115869, 0.9808352098069628, 0.9584801251650741, 0.9591691858385885, 0.9449962306342561, 0.557141000927075, 0.9531975547138205, 0.9748434474766919, 0.9999866156078633, 0.9765822457269754, 0.19295636512824418, 0.9312892979183172, 0.6860226873452105, 0.7585201602021865, 0.9171757963248949, 0.7692471104523897, 0.9290297627730368, 0.984712117286139, 0.9933132922879152, 0.9749366862769357, 0.9747317788039249, 0.9216199591894139, 0.6465238255634873, 0.21855840527212744, 0.9878110407545736, 0.4210514258150559, 0.9054797022974829, 0.9600701996962516, 0.5302998900375984, 0.8313372783501838, 0.8271546387585801, 0.9586293543792397, 0.9710790190963752, 0.8984714551390963, 0.9390755228778611, 0.9354213259247978, 0.9910698590783521, 0.9808849228134974, 0.7099172195395945, 0.8361305882670105, 0.6544228219974649, 0.9465067385189402, 0.9393923168007653, 0.42230344030232925, 0.09651883066400828, 0.8311807228679083, 0.6152374854181679, 0.8528070753596599, 0.645260976816809, 0.9937422805366304, 0.39351966174425485, 0.8425452773502092, 0.9822941754599619, 0.33179767939959615, 0.9830354024403984, 0.155818006405037, 0.9832777994291045, 0.8321948351793232, 0.9956294383909235, 0.8567154842438736, 0.6670557898894209, 0.853011494672485, 0.5590069280683708, 0.9582451703060147, 0.7147250462147616, 0.81731795486012, 0.9657366060318334, 0.9624145647713989, 0.9283598825830035, 0.16813178837045312, 0.9168694695334914, 0.9427383381248979, 0.9828936823865813, 0.25169680051468807, 0.5361704293125203, 0.27289732347882345, 0.9566088755300842, 0.7554220810730049, 0.9307542001946175, 0.989159949700793, 0.8429762718842088, 0.8789912896294124, 0.7574567100251133, 0.9902711442612883, 0.9311903498826565, 0.9627953629156393, 0.7839375372041559, 0.8815364751868434, 0.7128297581619764, 0.5349164377334849, 0.6169353635775268, 0.9575239681960601, 0.9564189004630409, 0.8402280541637914, 0.6696711717204775, 0.7927838375168887, 0.6915684056450261, 0.860858397132776, 0.9641048062506304, 0.7074582989658529, 0.9207402105292983, 0.872532648806977, 0.2895751468800344, 0.027218438043620875, 0.33866769706322897, 0.3458871229377132, 0.840145746129065, 0.6007732508905589, 0.8573657023001999, 0.3697799847831923, 0.7252906003388734, 0.40603673187995715, 0.9932114361321323, 0.06261880966311528, 0.7857084264441719, 0.7631615667649927, 0.4165506707633816, 0.8456120277559226, 0.9258795116540004, 0.1486673112561573, 0.8608617383847325, 0.957982759011415, 0.9365814215243382, 0.9714393803569866, 0.9075884093260269, 0.6472554528666294, 0.9915145291099791, 0.7702323223038386, 0.492780896080988, 0.9543734742185532, 0.9319974680231775, 0.07620324082775061, 0.8703422686376854, 0.9882665662006306, 0.9081843098963361, 0.6653529268782273, 0.5329882638706296, 0.5, 0.7896988883253555, 0.9907830212957874, 0.7187487804687391, 0.6029982233842154, 0.995392136576008, 0.36408645369482456, 0.9019551137107295, 0.8580600978314157, 0.8340181985427281, 0.4496759562160888, 0.4484083026057191, 0.8394103480592565, 0.09779285797385262, 0.8620234546284087, 0.9954015116271151, 0.3791718347893305, 0.951420238579113, 0.9890661635235524, 0.29027848095821335, 0.9725591544121321, 0.9493263136013098, 0.9007136191983043, 0.9388587952896232, 0.13854092895494835, 0.8730586482126872, 0.931428007844353, 0.0596259494665689, 0.52618794669549, 0.782707386485467, 0.032777990082004264, 0.5736155405586816, 0.7557304177966426, 0.17829818188559313, 0.20563237302931836, 0.04214870732473512, 0.9306979292186568, 0.16685961755818143, 0.976861497472116, 0.9779019978741736, 0.3401221677674824, 0.4171757540705296, 0.626458154095364, 0.704907568154463, 0.029796322466555458, 0.5826240484827493, 0.9355564332967335, 0.18938942477545329, 0.18492594992398512, 0.04884602973679694, 0.6474897068308423, 0.8129613859097142, 0.8267014355474137, 0.4202284579278127, 0.9052997787681284, 0.7495998034678264, 0.1641730956153245, 0.9952478203142501, 0.96114342965195, 0.4032903206491821, 0.9537199367319931, 0.797664938757335, 0.7673365746747873, 0.9568513991320985, 0.9933106465608912, 0.969213658723956, 0.7592399020400779, 0.05558610921945499, 0.9545394195443218, 0.6994343578640362, 0.6676167822923258, 0.1638947061428318, 0.32299134733580775, 0.23255667891404283, 0.2244720898664778, 0.37238109746270975, 0.0923671785501054, 0.3834707011593513, 0.9873588727773814, 0.7790328016091763, 0.6032684441002377, 0.14576736489459136, 0.08528438526619234, 0.916267189486769, 0.7998720680435482, 0.9761382554541314, 0.7329713084881747, 0.5496470403193837, 0.8894475196782243, 0.8077586952479792, 0.36659333941180355, 0.6471027248209699, 0.39186207985144944, 0.9909462146176695, 0.07868883344218346, 0.9073727230090851, 0.9999990433470992, 0.13978266188075053, 0.0721548496235714, 0.9918861854271301, 0.9312662431667436, 0.8913860390185716, 0.9510255214735742, 0.3043301733318518, 0.17590537987653293, 0.6566024595841855, 0.3364792802714154, 0.3208258644579154, 0.9733646850942289, 0.3033056368047648, 0.25230027578778436, 0.9411530032795643, 0.8705241033925435, 0.23828809570611734, 0.9643625997679504, 0.991360158568862, 0.5612113813148646, 0.4746361685318668, 0.1227564216314968, 0.948234220374509, 0.5637090941209869, 0.9842473936649, 0.7668674253083144, 0.8186297781083276, 0.7579057888035989, 0.9951901402347055, 0.7061827232337815, 0.6177924125894246, 0.9999841522667919, 0.9806872031016243, 0.09599717747315681, 0.9891957233475017, 0.10499004818284575, 0.8669914891425718, 0.8451316813066643, 0.6040223011848552, 0.7738170569236791, 0.8746616909211713, 0.9864936014756954, 0.8570918659402311, 0.8888120312503602, 0.4050667712549857, 0.6515530217850731, 0.9315026811534665, 0.8901117162009554, 0.7005095954173208, 0.10560828753396748, 0.9076774975135491, 0.847342611222551, 0.3466210999041826, 0.30003354341992083, 0.7661359087517977, 0.8785024065126983, 0.9633120106248604, 0.9018636057387016, 0.9725476158423306, 0.9730737665113605, 0.9851356766606271, 0.4032265021259311, 0.842388973752976, 0.9662600232567128, 0.3756482144597089, 0.9755169499149282, 0.5394424752065464, 0.6781040969803906, 0.9360826503847733, 0.38502605921061517, 0.4677092430451712, 0.029224031270575983, 0.25583628913884165, 0.9060366024333011, 0.9847306880069182, 0.87925917565482, 0.7022130528690361, 0.7983631666428097, 0.43134781574586295, 0.7365289284550014, 0.41359435780391435, 0.8367708248309298, 0.555926750494494, 0.9570976646778365, 0.9427444138541483, 0.3405497375131249, 0.9722993004379509, 0.8948385625724498, 0.3593376292303843, 0.9615642592974928, 0.897365081777333, 0.9910470347930568, 0.8281419484610285, 0.9690819360577811, 0.9384736809729809, 0.7223159437886824, 0.6140512445492418, 0.9679785513863892, 0.8110030176211613, 0.2751092820906806, 0.9930739288945066, 0.7554613761275234, 0.9967297590590095, 0.8921644361006089, 0.9654381798498117, 0.8865221676214738, 0.45720152745256254, 0.976975227636651, 0.8713264854150767, 0.21413280776906196, 0.971666031073433, 0.8032528236847413, 0.8409014572558287, 0.8890906866789696, 0.5, 0.18502516057484916, 0.3509367294922568, 0.23445898967533824, 0.36825698109389515, 0.9918883920153296, 0.7544829908094053, 0.987876782495658, 0.8977157526498803, 0.6006371609511878, 0.9591263378249412, 0.763252104412662, 0.7416149074163275, 0.30211564889520504, 0.9826932280300354, 0.8385624578642183, 0.3811049892639442, 0.97490037615139, 0.31173185345448146, 0.2034524362874617, 0.6354979275283577, 0.7985658308284841, 0.6473118771895428, 0.48636469572004787, 0.5267784360765748, 0.883226451601723, 0.2756924074503195, 0.9420100735312464, 0.027093478568656924, 0.3947386042491491, 0.9825937984958242, 0.45822350943537526, 0.2452780552373445, 0.430714137729955, 0.8971127259538062, 0.9588044813527671, 0.011839998843444876, 0.9917396422318475, 0.6312463161925717, 0.9240073074162798, 0.9809234204154802, 0.9795635485120755, 0.9909632361187211, 0.7549138943455791, 0.9592840577706694, 0.29058282800934454, 0.08683360326799895, 0.11126688117413869, 0.9657709985894483, 0.23960352418480327, 0.050278493126838984, 0.7565246074325632, 0.3755625889420669, 0.4337445983159223, 0.8249235360518866, 0.920422560514888, 0.013082018949128301, 0.8829762729122386, 0.845940841224504, 0.2479833189387726, 0.290802848041387, 0.332609211331783, 0.5237397417216, 0.38032634594932696, 0.8664744390764644, 0.9833296398790132, 0.9902426246535964, 0.3849273857674271, 0.9766245800790366, 0.4722173833786909, 0.2273599998624146, 0.8348467259832207, 0.10182558357968391, 0.8665544191717104, 0.8725646843578162, 0.06410201062485268, 0.9609702313839973, 0.02062631678287952, 0.03775242501315454, 0.6122554134885327, 0.7657489875685821, 0.6733230157098007, 0.5952020408819333, 0.8445634054845175, 0.004610411801106383, 0.9752380796167521, 0.6890296726226255, 0.8691962019317276, 0.8191792875262591, 0.9723262617799457, 0.6529852396697398, 0.12018189464584528, 0.679632808084407, 0.21605225897116506, 0.8919425837545473, 0.046466123251811854, 0.7314501559937879, 0.09491862863814732, 0.9278178616512619, 0.4165616974125639, 0.5294681541465854, 0.310736173080592, 0.9627699992005867, 0.0635502010686641, 0.6218282160345829, 0.7971946297380728, 0.8480456670984959, 0.9902220210846961, 0.3734756165166193, 0.8935460720374031, 0.4921058631733444, 0.08327467010239384, 0.2793868581285128, 0.8694085523046292, 0.759328754524462, 0.8862123593663713, 0.9730257711011185, 0.8873726392674024, 0.14373602790883677, 0.9481175293164956, 0.8102601373388667, 0.8827454149862394, 0.8171944122648173, 0.7897957465726712, 0.8055234112238515, 0.8994391214988111, 0.8817683527534685, 0.9463101328541125, 0.9604017896649116, 0.3971415007014945, 0.5997533012525856, 0.3536581102622961, 0.9515071543392851, 0.9876636297306847, 0.2288037815330131, 0.29470623729506906, 0.05846546906133806, 0.9042229883119818, 0.195509156416891, 0.4286620031579153, 0.7996608778981006, 0.6306180110891251, 0.5394643643695157, 0.6019405413285343, 0.8472415634431943, 0.9516404254932312, 0.7652885929841682, 0.6460756721773399, 0.20975450826693465, 0.31016703225515746, 0.9448346462435965, 0.8172139790665441, 0.6979755585951241, 0.5665919899393368, 0.5933157325470234, 0.6660251680396176, 0.8157069133545736, 0.8795735601204083, 0.9565389113595758, 0.9927959391266382, 0.6178939388047036, 0.9440617755414543, 0.9961329135688041, 0.4241605739963245, 0.36218252682328866, 0.9470513545328404, 0.9077428886502719, 0.9613307554542693, 0.12098957402985998, 0.6697940883315581, 0.9353212575460506, 0.9577587888884979, 0.9374120521222463, 0.9763093255135482, 0.9258455533092169, 0.9872464734171637, 0.11360987430575564, 0.979343044416413, 0.94531116240537, 0.9717824816489921, 0.9890155267464429, 0.9530702041786887, 0.9812803104788727, 0.002879208420620465, 0.8762195917059531, 0.7331759589076161, 0.5186189476503736, 0.9551459874387475, 0.46360023340090994, 0.7820530565032836, 0.7534776848718079, 0.988716019022113, 0.46650822827399746, 0.6669259239129002, 0.8687929430045687, 0.9787944925653587, 0.017651643839002636, 0.5193496351653727, 0.9761087465970834, 0.8615987469161603, 0.933814924340174, 0.9925384928751841, 0.9922555454529757, 0.7686795601007842, 0.2938319608390502, 0.9858783852432612, 0.9869604399106062, 0.6289879615026176, 0.026472906027948096, 0.22040582489607363, 0.07252661954240225, 0.8328895360187073, 0.7800865081066016, 0.36706430208001317, 0.2718578981625349, 0.8350280226289117, 0.6782396309843862, 0.5338501578596266, 0.7411642021922527, 0.9865791566188252, 0.9900693100096203, 0.8710157278672382, 0.933826189951142, 0.9847671873352619, 0.8991474191067154, 0.9815259463187472, 0.9070200997916824, 0.7779589432927312, 0.02155555772048378, 0.9671496134939532, 0.9913290582442328, 0.94544786026816, 0.9521189752481746, 0.6618260241264563, 0.9844078066344745, 0.13303629776956877, 0.7961896395824021, 0.9252945651705221, 0.13613365181545894, 0.9028124001248043, 0.7256926688815288, 0.7316181044918354, 0.8683869222062277, 0.9818961612146867, 0.5630066766420068, 0.6525854694266988, 0.9712587194398842, 0.010569149151600545, 0.8662076989578509, 0.9877926003596393, 0.20238340663339566, 0.37445158978373294, 0.8846669168904193, 0.477393474030258, 0.9814477648684381, 0.49403712407769673, 0.7923543654195513, 0.990115237427553, 0.4060235474405567, 0.9872429847707657, 0.9470354954187618, 0.994516497006348, 0.8885526303745811, 0.9904647199278279, 0.26398343308324046, 0.8466771425383611, 0.762535004655502, 0.935801648959467, 0.8900705109703992, 0.9212982299921131, 0.9790581448916159, 0.9395243161539963, 0.3035906847107808, 0.9798557521464227, 0.98944711997139, 0.9311997985490988, 0.7919659953883736, 0.9476852335198437, 0.9923811743345117, 0.9944360719739543, 0.9607709585087012, 0.8526014283871056, 0.8173304335222639, 0.8665223550556184, 0.9459551449002398, 0.996025076466964, 0.7685116865366564, 0.9931400138470073, 0.9946026940427918, 0.9160848566867251, 0.8056066370190241, 0.8844669574497536, 0.409230041047584, 0.9781866602687473, 0.9793424612049153, 0.306872401090747, 0.8609125205541639, 0.8727158166228012, 0.7809649122631187, 0.8000421289578135, 0.8673916244026302, 0.7230811469722692, 0.9868329526317655, 0.4941443382121909, 0.8694619011866476, 0.9713945427251615, 0.6727349906118514, 0.37323717634330345, 0.708486444245446, 0.8898631854466481, 0.9899432835930726, 0.57744312473294, 0.9708790491003549, 0.9391322616255083, 0.2725364972989963, 0.976708193837582, 0.7944972622563371, 0.8886857605149876, 0.9723081312000401, 0.3828734491010077, 0.9804625680473136, 0.9294372196301315, 0.9903745003871496, 0.4655884796330407, 0.8921451536409156, 0.9371539922527358, 0.7329719506944927, 0.5629992863184593, 0.15902474773245504, 0.8829860756560681, 0.7230382122076318, 0.9342392509061355, 0.08285274152278313, 0.33579263500685125, 0.07690075490543957, 0.9386085003598028, 0.9252124306017515, 0.7527088336312638, 0.636378089102751, 0.3730376622243525, 0.3216567052335376, 0.8882116308619527, 0.07986951214072849, 0.9957939952069518, 0.2587246773787481, 0.7764398990731001, 0.8442961195982305, 0.04967544207687956, 0.30243894231221896, 0.8956546279854442, 0.9952033395871094, 0.780684302283135, 0.8877780209438573, 0.21945416984924968, 0.9931552541024454, 0.9676772005479245, 0.7166573365247416, 0.7570447604722456, 0.19313653346492612, 0.02624181826519572, 0.9818736957588204, 0.49335490594602627, 0.350196071521482, 0.30077119302697586, 0.8608775869089073, 0.00786028487638363, 0.7432998173557166, 0.9802949313297104, 0.825546476691147, 0.9412674866215441, 0.7594677051080473, 0.9495117251753494, 0.642739452187834, 0.06891438324479035, 0.08223877248241317, 0.2933759533206819, 0.6796100514217814, 0.07136154772683623, 0.9892668776500654, 0.8568356555935291, 0.8590473466479751, 0.9824057137410552, 0.9375963939997948, 0.9847679564293956, 0.9135735901761008, 0.9904360066673145, 0.975152425478999, 0.7127897095864932, 0.3724780830718373, 0.302812918911316, 0.29483148485972116, 0.9453823621047776, 0.9533613364749846, 0.955784965849752, 0.5124429742392058, 0.9546769596519937, 0.36246201947097656, 0.1033978557364379, 0.9828350858377697, 0.19337812334235166, 0.4278317730980857, 0.975310762580955, 0.1626388644121368, 0.6928282427010097, 0.9506648408011751, 0.9469806630925249, 0.5498254201048715, 0.73656899016331, 0.22133052119928767, 0.9671272745329228, 0.9884027226048195, 0.04509449856301947, 0.9918537388341622, 0.9880193314817887, 0.9356519605193032, 0.5361745730678751, 0.17046764120838614, 0.958641323851079, 0.6742663928427756, 0.9862064718705651, 0.7090156927993516, 0.9941045038896413, 0.6828357385164342, 0.3151143239979885, 0.2959513092724232, 0.9909239730087952, 0.4016863082697707, 0.8581233916629349, 0.652619964527138, 0.9245233060504872, 0.6502933893969406, 0.6221199925577756, 0.9208818942856255, 0.972994321633957, 0.9955158696000523, 0.07338712070564894, 0.9944154339873098, 0.827362551196656, 0.8370110689029642, 0.9797180820458943, 0.9894664860430399, 0.8587491635698582, 0.9749159230627864, 0.9589950493936675, 0.4170921708862961, 0.9193720911334042, 0.7975196969433669, 0.34950749524929037, 0.08598184079528602, 0.9534830662998733, 0.9692453161826865, 0.981984608230568, 0.3879205274734827, 0.8384419220271045, 0.8885613971635913, 0.5241253402301008, 0.1746177775131486, 0.9660474675721951, 0.35634058473445696, 0.9707087195268712, 0.15910713980275015, 0.873915706764945, 0.8258476383793606, 0.9308207250433721, 0.04480560222598367, 0.700609859668041, 0.6867139617941498, 0.92527497276085, 0.9420317935514794, 0.3062696209763165, 0.7847862146722043, 0.9884284023848546, 0.8901205355464422, 0.18041011194165446, 0.5, 0.026590936695688648, 0.6796405982330258, 0.6985779413742704, 0.2494120905735631, 0.41065635246763965, 0.9085019924990095, 0.0455189962109167, 0.22655079453150934, 0.43800186328613144, 0.187576954248508, 0.32050635759783774, 0.993324059588266, 0.9246051754384101, 0.9513316319741504, 0.9128053733733442, 0.33689258797926097, 0.7560394090714786, 0.4127295771399127, 0.862774122191322, 0.015589886591599161, 0.6941836346291068, 0.9634739273333573, 0.9071722854987435, 0.944572531948024, 0.9769958086807525, 0.9926821738016309, 0.9874035788510167, 0.32127121903678885, 0.9899409962580065, 0.19221613774396787, 0.9974236260845981, 0.9803550840617556, 0.5767679922133321, 0.6605211779212489, 0.9752862694322473, 0.951348569666904, 0.39634135507069096, 0.8075378501430711, 0.9916562829952396, 0.04963454187176344, 0.932775210248366, 0.6238476932533354, 0.5653743018649673, 0.011379842152129692, 0.880644412684151, 0.026062246001574526, 0.9841084285786457, 0.7957111145657939, 0.15174027832229092, 0.3589909211620561, 0.936089463547076, 0.9761308587123074, 0.9904288645465458, 0.9868749980657401, 0.21541820267669606, 0.06730481323400439, 0.5616722384357534, 0.674169487981542, 0.09501485440340761, 0.9999900899030988, 0.38320285571124385, 0.9485721676633487, 0.5659260589955284, 0.9247949850176926, 0.9538042027241682, 0.3764514043417913, 0.9900386920434054, 0.9542219773024433, 0.784378339190872, 0.10725613252039014, 0.046198889115748494, 0.33830200882831574, 0.9441318843476005, 0.6333685998922217, 0.8901054147954401, 0.7119410600646422, 0.20695098266092324, 0.8646166993011895, 0.02091187072523021, 0.07847665854861632, 0.8397850406919006, 0.707078364558449, 0.6320938683592734, 0.9624965499534373, 0.7242481345112634, 0.9068961087739971, 0.04790789144295686, 0.9836800354752107, 0.18585751810942344, 0.8148146437521765, 0.9338630454060484, 0.9827751015945638, 0.9748867434717576, 0.02910368333858927, 0.08219400546273939, 0.22481436480364317, 0.9646511905095514, 0.9512251442039176, 0.8722145091069269, 0.9724077297004077, 0.978794858214156, 0.07919693579792694, 0.9848448977479014, 0.9352772279286762, 0.34881207740929226, 0.48769676383161437, 0.8362469696326524, 0.17102281842043468, 0.9159435206355435, 0.9877784693543963, 0.6827379779147805, 0.8068336963733518, 0.9381144478459272, 0.007406911209244333, 0.022518459842951803, 0.09983718789008669, 0.7162457164072605, 0.7238212244208353, 0.019456088742604325, 0.751600584993526, 0.9756445719646409, 0.574140806653438, 0.07684252023400973, 0.1532015466571592, 0.9167881493359776, 0.9791751148146968, 0.12724162894902163, 0.3978074956657419, 0.23884391738945965, 0.2115423178780698, 0.07413501140216719, 0.3330857919768622, 0.871275862973035, 0.7932146899948073, 0.9765314913675176, 0.55875773283294, 0.423133937418045, 0.03966837395416583, 0.7853736408471003, 0.7172042987908337, 0.8284393069440371, 0.767423135592734, 0.8798912711938682, 0.991361572343134, 0.5797603108063067, 0.8720516609302582, 0.842108158645173, 0.6455225221791158, 0.9913802545426341, 0.44259387684278884, 0.9471298087308961, 0.9879709099389312, 0.828051079119078, 0.9285129433289393, 0.919126992866663, 0.23318619988630995, 0.8788950033584508, 0.8738229226935106, 0.5, 0.7903328895296059, 0.04997800900563481, 0.7224756085907217, 0.9810895000245866, 0.8386468758861635, 0.08510876940420459, 0.6673039815157198, 0.7315172115552758, 0.9821068568441619, 0.4713855496527025, 0.9868401791726167, 0.8819562487044842, 0.979004980356074, 0.2549518879782021, 0.36447768873991737, 0.9326250463054081, 0.8133340678185893, 0.9054277923590981, 0.8362085488331832, 0.9252680079203573, 0.8954043107421709, 0.038531973508038914, 0.9017492862207422, 0.7908194771065481, 0.01938003415648329, 0.869225349949197, 0.9865820363401088, 0.5675831411684481, 0.5477810993539527, 0.10753684587655453, 0.8894372160232997, 0.8109671314406717, 0.6929149481127029, 0.707799143705142, 0.9670337380317612, 0.021528972542600472, 0.3393291615294666, 0.7033666607437402, 0.9893787072572434, 0.9630062402632109, 0.7396911587146615, 0.9101097687384156, 0.758380135234392, 0.8956974678102094, 0.9923186863422918, 0.921325863492512, 0.9656208758084397, 0.13991828593067823, 0.9604549155853742, 0.7205260518452392, 0.9510210059506112, 0.8296867020655412, 0.7030656572787065, 0.9323763193499718, 0.9535018582934185, 0.748759918520265, 0.4305499859981313, 0.9589518092220124, 0.8089913057690402, 0.7697602466223235, 0.44769456064524527, 0.8101736648283735, 0.49003394143036566, 0.9201819538292259, 0.029578313092108656, 0.7633807981838305, 0.6876418577062609, 0.9350209092877417, 0.8620730714376282, 0.1335162097049646, 0.5470787301221696, 0.36621839179754345, 0.05040367632916856, 0.9194777046707154, 0.6544188634193301, 0.8421198222154026, 0.9185985628291433, 0.9863904565219302, 0.7051799470590336, 0.11498215610806617, 0.7862330583393415, 0.9545784817825373, 0.8995802229007022, 0.5114405110832668, 0.7048806080601203, 0.8803520232607775, 0.5862341528062218, 0.882735617723411, 0.1671268845126335, 0.9797730126387398, 0.7885277374930812, 0.7310198101810059, 0.6041636530271376, 0.6925272529815469, 0.5448378534411266, 0.9656335027079708, 0.9034821246007733, 0.019806309635399304, 0.6281332087638833, 0.815941890393508, 0.8516712113123268, 0.40259678070836646, 0.22643297116306094, 0.8903956387620411, 0.4179740647306077, 0.730121950164023, 0.9862840919755809, 0.3339274845879836, 0.8806028413143336, 0.9323495102489099, 0.8435084514212894, 0.8938060013811403, 0.8955425523413051, 0.004674535559523041, 0.7463217296025918, 0.03226965908606155, 0.6105556032753882, 0.6690979447397886, 0.8595480539281269, 0.9142917564734054, 0.24619578195817812, 0.6255185605152955, 0.8871615540259096, 0.038497801474367176, 0.98624799187733, 0.07746208346316405, 0.7801032497084699, 0.2581345891071848, 0.04622720077229573, 0.8109806010963052, 0.6853189947873551, 0.09933377529395071, 0.464574400892792, 0.007787427558693544, 0.9662699569818846, 0.5219978386501046, 0.8524145952826159, 0.9031305571126165, 0.15901410402279534, 0.06259292172696233, 0.00022964348043415993, 0.7008949692079954, 0.14104917801184563, 0.8365572039404683, 0.08285274152278313, 0.0373615380832785, 0.020021169390112455, 0.9447557027864913, 0.9848087474943542, 0.5599819944531504, 0.9338614418115118, 0.4487021340413648, 0.8035098995321801, 0.3896705731191775, 0.9812357265818037, 0.06212400291897608, 0.5202698755808988, 0.03421963645758368, 0.023172308223707232, 0.06435107863835188, 0.08148205607007082, 0.763157084063603, 0.8565761628245824, 0.030736723262074325, 0.86960112426252, 0.39669335341810513, 0.5, 0.15911124496816778, 0.5117992304058874, 0.9948330160968455, 0.10194885543141116, 0.006169300281729358, 0.890386591118454, 0.8196045554097647, 0.9819594866992438, 0.9801815641491359, 0.18466349692857428, 0.08629640523193235, 0.9726569281178634, 0.039589551828329045, 0.792633243982727, 0.9040640823734691, 0.019547475406307337, 0.07228177996839463, 0.14153685574658317, 0.4690805408672433, 0.24239044778486643, 0.8322270866024502, 0.5124409854515413, 0.9831151933009686, 0.9769905641285774, 0.9387878928745771, 0.876023913217903, 0.9496335938835575, 0.07523035908319108, 0.059930572033672004, 0.5992694120979452, 0.09435821116153173, 0.06361024909872445, 0.14465289382554405, 0.042548522074613855, 0.18914472034522578, 0.7525824384391843, 0.9248091679970999, 0.9597338684261711, 0.9143973206064019, 0.9448656729858071, 0.16802560244957263, 0.22798511085038264, 0.8216892435265146, 0.08277243598805745, 0.8614105911647782, 0.20619357240006098, 0.22725405892942732, 0.7505903822876833, 0.6150168497315905, 0.06108463371071703, 0.9672911941068606, 0.9776749392994746, 0.03752736386247084, 0.00894682233028749, 0.8988436652139911, 0.025895638924838975, 0.27754604462558513, 0.8173142271736153, 0.9703510097120612, 0.0969301788640996, 0.9709682018232407, 0.8261975449541171, 0.8504753383857088, 0.9550630598196292, 0.9529759971890366, 0.3666989837281511, 0.98092319214246, 0.01984374820650511, 0.6192654436406358, 0.8581644120695292, 0.007884110697231033, 0.20333463199134097, 0.17287854423404864, 0.8295106601461625, 0.4406981282544943, 0.7062814686417769, 0.7249856126586434, 0.5955745684253043, 0.9400636825814505, 0.9846079228211697, 0.9754298153187106, 0.8746054112662995, 0.8879539588457013, 0.9906467072381762, 0.2145952978573405, 0.5506585033141966, 0.22740454296631327, 0.34108732383388074, 0.8929005561388222, 0.042935374695770405, 0.28281741166309887, 0.5758583367859538, 0.05120643230997457, 0.5327885544288958, 0.38353163562718345, 0.04071684167996667, 0.1205732156939725, 0.08474620477083634, 0.8725514425973205, 0.23453037764936735, 0.9328284147300322, 0.5, 0.9886763692518349, 0.6761543961202356, 0.8022767589438375, 0.5769292828137863, 0.911585166346129, 0.9378890677852532, 0.40080409668548506, 0.8181774066287962, 0.9700304766311577, 0.07318736711600701, 0.7895852265204996, 0.2463519862060237, 0.855469212424729, 0.8975614533931107, 0.8507857617134, 0.9614848687037677, 0.554609054706532, 0.3855421913355811, 0.9803727360343446, 0.9433218594450621, 0.6854805813062366, 0.33515373039533486, 0.9603482035576533, 0.055092647152047106, 0.7080916570752098, 0.810882056300191, 0.7587329817085604, 0.10479966642701229, 0.2443515443042415, 0.3435617575401149, 0.9364923946756272, 0.9253887822923385, 0.00037897078805728264, 0.9590357509871048, 0.46788346952449655, 0.021739782474515714, 0.7143852705652114, 0.9324269160525054, 0.4825267814200594, 0.8728176251992956, 0.44276295522117337, 0.6042495330948066, 0.5771320515657283, 0.6243502300231417, 0.04873707587655128, 0.16984189002673594, 0.7925513455202684, 0.40605581239397465, 0.9893975019232811, 0.9403036258998236, 0.8301586946069424, 0.9461847550452624, 0.9459735160895463, 0.9858646257229465, 0.4813888492039873, 0.8333156708134328, 0.6154410865644965, 0.5614986550203213, 0.0725746432738546, 0.49052074990856376, 0.9732997272609202, 0.8479424984715059, 0.8489987112685248, 0.9480810898410013, 0.34972048720894783, 0.3787782200259547, 0.5464330612161575, 0.23391435346766895, 0.7234386068077795, 0.9792470096539577, 0.2201211314876463, 0.2892095574790848, 0.009967591739976701, 0.8198509198647671, 0.37882101978750854, 0.6422640832194464, 0.9926589075557443, 0.44699401234353137, 0.7953712014333864, 0.1978974106823167, 0.39743517317856736, 0.9818937950177399, 0.49387003602229446, 0.8665841675758233, 0.4286028688808651, 0.002101000102259837, 0.9666242771600442, 0.4354170843507943, 0.9793909859968916, 0.4554083752181137, 0.570233573656431, 0.14969148562666762, 0.004740753476432952, 0.9617810524000032, 0.9239410926750294, 0.6685440881987276, 0.9857718281567198, 0.9746768509475797, 0.2921858026463875, 0.09514479624738499, 0.6583199228111416, 0.07086128845489593, 0.9630036719206323, 0.6159634857787327, 0.10314862672398695, 0.0027641969635127943, 0.4733622088033163, 0.057633553576793964, 0.12092959259028277, 0.6545876703076934, 0.40172629149292, 0.8417868367915388, 0.6336278571128667, 0.0566220748235082, 0.0369358827239302, 0.030412443032922506, 0.08001520136346449, 0.013135405598794999, 0.7322427893839868, 0.0007354757013950102, 0.2508737118058917, 0.4937144218396525, 0.029712482047562758, 0.6946349393182021, 0.13072447934909778, 0.8123540651107534, 0.007782849220146903, 0.31256010336135176, 0.46373565047027654, 0.4743080760076243, 0.0499419783046503, 0.11653384361232604, 0.033245456258725, 0.005173724637929478, 0.20756743731414568, 0.8670081288231725, 0.7300166679363733, 0.5377370735520709, 0.6281028504783513, 0.019074014334627812, 0.7802708731581178, 0.7922548054549613, 0.259626697223581, 0.12169715813308934, 0.3639409054871113, 0.6165521114804895, 0.29835276563611923, 0.010968142954991463, 0.2078505429588108, 0.23255379482275643, 0.12047088103135675, 0.025652739858011423, 0.05403174303449183, 0.003505784175145372, 0.919146950858976, 0.0011795102950402988, 0.06004971863476269, 0.5848742021261637, 0.0336061234546323, 0.44832924373206173, 0.0631173176166866, 0.08670278116170929, 0.16369683865624615, 0.4053029180263302, 0.08383740046869727, 0.12610120502679803, 0.6134314107095817, 0.18313941029484118, 0.005939735649524547, 0.6648379998951346, 0.6041189976846463, 0.682856700511073, 0.36623006554158405, 0.09492823850172798, 0.09940945270750669, 0.04482441018182908, 0.09375987776563358, 0.47173661388152777, 0.2966304603629427, 0.06814119477680057, 0.09461788366063832, 0.32062305525876417, 0.851349481663485, 0.452147994860576, 0.16394585696892114, 0.42547205190629833, 0.17376227688990933, 0.3911917720481909, 0.030274661055827455, 0.2154817670044078, 0.4329642953997576, 0.6554197049488698, 0.053058393164091076, 0.7794145492923881, 0.04490533174426275, 0.5982393603944779, 0.7394009844690309, 0.6622143075272355, 0.5671919378585695, 0.13359709601154998, 0.0321143357542438, 0.03580221673946144, 0.2205944362212321, 0.46928861819251255, 0.027950401243492115, 0.8851408942920226, 0.1291271765130674, 0.19723751211760077, 0.003508289913324639, 0.42482072802477827, 0.06030501576123703, 0.0730468865012327, 0.016727552092746255, 0.5767304587945342, 0.8074402986497206, 0.2359185744511027, 0.020680487557899935, 0.10692130443494158, 0.6708779443687504, 0.8274469309231878, 0.0015835691768008775, 0.339149245438112, 0.4256121966458366, 0.5410084976354386, 0.011222777913698271, 0.040371681891957584, 0.019454839819587514, 0.14718791745600804, 0.10883618534250168, 0.16899522182689233, 0.48034240327522604, 0.42911427626295345, 0.24421590955539707, 0.7043692910445981, 0.41075595527126374, 0.9164625573550681, 0.008285099289177025, 0.10774260622120897, 0.0008553103624678154, 0.11965166299459648, 0.09243214234405901, 0.0020330756084512938, 0.6422109284367711, 0.19212459500488774, 0.07115954434795735, 0.18083845870214638, 0.5814246460676463, 0.31021273347148814, 0.7043185426308322, 0.8627299763995127, 0.2450566774896211, 0.3350562736330753, 0.03607422237774425, 0.5933882187079114, 0.9310093013474695, 0.07034834417049464, 0.14680503733147746, 0.30737424232915567, 0.2109681318354611, 0.06083927228647158, 0.1019995495870766, 0.6451509483715367, 0.5158958929388328, 0.2671571534235663, 0.018443342146160665, 0.26549521982874363, 0.30427555196335204, 0.9926563231676143, 0.04057357850506785, 0.07540050242285032, 0.7642570467379028, 0.63648625843689, 0.25286457237498905, 0.0098192178949174, 0.18403410333642342, 0.008185291928976865, 0.021100934776527462, 0.16159168975114935, 0.06157483276298411, 0.701572472011374, 0.05080258153949787, 0.8215688909080084, 0.26315248810189895, 0.04311408128535533, 0.6940898281804838, 0.6768638302134388, 0.12252811422749688, 0.08354972496563888, 0.04986382566341051, 0.08981066805680135, 0.039515923721758356, 0.002171263728993851, 0.05415306929081587, 0.9863546321154721, 0.012192227682221083, 0.0020610681050020974, 0.2658031240263832, 0.32134872625170324, 0.005219862808160134, 0.44563461557947415, 0.07522103683396521, 0.053673871729359585, 0.4554670128810723, 0.6755011666065867, 0.0520162782832705, 0.9043074657552539, 0.873632299991186, 0.03842577802186724, 0.5790661687726585, 0.7451748045820547, 0.16965651430690995, 0.01299317195782648, 0.25843157696772073, 0.37094543676135633, 0.06274765078680285, 0.04149125768381778, 0.8889194570647828, 0.21194547967034885, 0.5907958685300688, 0</t>
         </is>
       </c>
     </row>
@@ -699,44 +699,44 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>tree</t>
+          <t>Decision tree</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.759919028340081</v>
+        <v>0.7582995951417004</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7597087378640777</v>
+        <v>0.757258064516129</v>
       </c>
       <c r="E4" t="n">
         <v>0.7603238866396761</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7595141700404858</v>
+        <v>0.7562753036437248</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7600161877782274</v>
+        <v>0.7587878787878787</v>
       </c>
       <c r="H4" t="n">
-        <v>0.759919028340081</v>
+        <v>0.7582995951417003</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7130782918149466</v>
+        <v>0.7268683274021353</v>
       </c>
       <c r="J4" t="n">
-        <v>0.7066436583261432</v>
+        <v>0.7236842105263158</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7286476868327402</v>
+        <v>0.7339857651245552</v>
       </c>
       <c r="L4" t="n">
-        <v>0.697508896797153</v>
+        <v>0.7197508896797153</v>
       </c>
       <c r="M4" t="n">
-        <v>0.7174770039421814</v>
+        <v>0.7287985865724382</v>
       </c>
       <c r="N4" t="n">
-        <v>0.759919028340081</v>
+        <v>0.7268683274021353</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -745,7 +745,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>[1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+          <t>[1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -755,17 +755,17 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>[1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+          <t>[1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>[1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+          <t>[1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.5, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.5, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.5, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>[1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+          <t>[1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
     </row>
@@ -781,40 +781,40 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.6692307692307692</v>
+        <v>0.6939271255060728</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6759259259259259</v>
+        <v>0.705932932072227</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6502024291497975</v>
+        <v>0.6647773279352227</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6882591093117408</v>
+        <v>0.7230769230769231</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6628146925299215</v>
+        <v>0.6847372810675563</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6692307692307693</v>
+        <v>0.6939271255060728</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6823843416370107</v>
+        <v>0.6841637010676157</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6959847036328872</v>
+        <v>0.7129629629629629</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6476868327402135</v>
+        <v>0.6165480427046264</v>
       </c>
       <c r="L5" t="n">
-        <v>0.7170818505338078</v>
+        <v>0.751779359430605</v>
       </c>
       <c r="M5" t="n">
-        <v>0.6709677419354839</v>
+        <v>0.6612595419847329</v>
       </c>
       <c r="N5" t="n">
-        <v>0.6692307692307693</v>
+        <v>0.6841637010676157</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -823,7 +823,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>[1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+          <t>[1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0]</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -833,17 +833,17 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>[1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+          <t>[0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>[1.0, 0.2, 0.4, 0.0, 0.4, 1.0, 0.8, 0.6, 0.4, 0.4, 0.6, 0.0, 1.0, 0.2, 1.0, 0.2, 1.0, 1.0, 0.6, 0.0, 1.0, 1.0, 1.0, 0.4, 0.6, 0.4, 1.0, 1.0, 1.0, 0.2, 1.0, 0.2, 0.8, 0.8, 0.8, 0.8, 0.4, 0.6, 0.2, 0.2, 0.4, 0.8, 0.2, 0.8, 1.0, 0.4, 1.0, 0.4, 0.2, 0.8, 1.0, 1.0, 0.0, 0.4, 1.0, 0.4, 0.2, 0.2, 0.4, 0.4, 0.2, 0.4, 0.8, 0.6, 1.0, 0.4, 0.8, 1.0, 0.6, 0.8, 0.4, 0.2, 0.6, 1.0, 0.8, 0.4, 1.0, 1.0, 0.8, 0.0, 0.6, 0.2, 0.4, 0.8, 0.0, 1.0, 0.8, 0.4, 0.2, 1.0, 1.0, 0.2, 0.2, 0.6, 0.4, 0.2, 1.0, 0.2, 1.0, 0.4, 0.4, 0.6, 0.6, 1.0, 0.2, 1.0, 0.0, 1.0, 0.6, 0.8, 0.4, 0.0, 0.2, 1.0, 0.6, 0.0, 1.0, 0.2, 0.8, 0.2, 0.0, 0.4, 1.0, 0.4, 1.0, 0.2, 0.4, 0.4, 0.4, 0.4, 0.6, 0.6, 0.6, 0.4, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.4, 1.0, 0.2, 1.0, 0.6, 0.6, 1.0, 0.0, 1.0, 0.0, 0.8, 1.0, 0.0, 0.0, 0.6, 0.8, 0.4, 0.4, 0.6, 0.0, 0.6, 0.6, 1.0, 0.2, 0.6, 1.0, 0.6, 0.2, 1.0, 1.0, 1.0, 0.6, 0.8, 0.6, 0.6, 0.2, 1.0, 1.0, 1.0, 0.2, 0.2, 0.8, 0.6, 1.0, 1.0, 1.0, 0.2, 0.0, 1.0, 0.8, 0.2, 1.0, 0.8, 0.2, 0.0, 1.0, 0.4, 0.8, 0.8, 0.8, 1.0, 0.8, 1.0, 0.4, 0.4, 1.0, 0.6, 0.4, 1.0, 0.4, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.4, 0.2, 0.2, 0.4, 0.8, 0.2, 1.0, 0.4, 1.0, 0.4, 0.2, 0.6, 1.0, 0.2, 1.0, 0.8, 1.0, 0.6, 0.2, 0.6, 1.0, 0.2, 1.0, 1.0, 1.0, 1.0, 1.0, 0.2, 0.2, 0.2, 0.6, 1.0, 1.0, 0.8, 0.4, 0.4, 0.4, 0.8, 1.0, 0.4, 0.6, 0.8, 1.0, 1.0, 0.2, 0.6, 0.0, 0.4, 1.0, 0.4, 0.8, 0.2, 0.6, 0.0, 0.2, 1.0, 1.0, 1.0, 0.2, 0.8, 1.0, 1.0, 1.0, 0.0, 0.2, 1.0, 1.0, 1.0, 0.4, 0.4, 0.0, 0.4, 1.0, 1.0, 0.2, 0.6, 0.6, 1.0, 1.0, 0.2, 1.0, 0.0, 0.2, 1.0, 0.8, 1.0, 0.4, 0.4, 0.6, 0.0, 0.2, 0.6, 1.0, 1.0, 0.2, 1.0, 0.4, 0.6, 0.4, 1.0, 1.0, 1.0, 0.8, 1.0, 0.4, 1.0, 0.4, 0.0, 1.0, 0.4, 1.0, 1.0, 0.6, 0.0, 0.6, 1.0, 1.0, 0.8, 0.0, 0.8, 0.4, 0.0, 1.0, 1.0, 0.8, 0.4, 0.2, 1.0, 0.6, 0.0, 1.0, 1.0, 0.6, 0.8, 0.4, 0.8, 0.2, 0.6, 0.6, 0.6, 0.2, 0.4, 0.2, 1.0, 1.0, 0.4, 0.4, 0.2, 0.4, 0.6, 1.0, 0.0, 1.0, 1.0, 0.2, 0.8, 0.2, 1.0, 0.4, 0.6, 1.0, 0.2, 0.4, 0.2, 1.0, 0.0, 0.4, 1.0, 1.0, 1.0, 0.0, 0.0, 0.8, 0.0, 1.0, 0.8, 0.4, 0.2, 0.0, 0.8, 0.2, 0.6, 0.2, 0.8, 1.0, 0.0, 0.0, 0.8, 0.8, 0.8, 0.0, 1.0, 1.0, 0.8, 0.4, 0.4, 1.0, 1.0, 0.0, 0.6, 1.0, 0.6, 1.0, 0.4, 0.6, 0.6, 0.4, 0.0, 0.8, 0.4, 0.6, 1.0, 1.0, 1.0, 1.0, 0.8, 1.0, 0.8, 1.0, 1.0, 0.6, 0.6, 0.8, 0.4, 0.6, 1.0, 0.4, 1.0, 0.6, 1.0, 0.8, 0.2, 0.6, 1.0, 0.0, 1.0, 1.0, 0.4, 0.6, 1.0, 1.0, 0.4, 0.0, 1.0, 1.0, 0.0, 0.6, 0.4, 0.6, 0.6, 1.0, 1.0, 0.4, 0.2, 0.0, 0.4, 0.0, 1.0, 0.0, 1.0, 0.2, 1.0, 0.2, 0.2, 0.4, 0.2, 0.0, 1.0, 0.0, 0.2, 0.2, 0.6, 0.4, 1.0, 0.0, 1.0, 1.0, 1.0, 0.8, 0.4, 0.0, 0.4, 0.2, 0.6, 0.4, 0.8, 1.0, 1.0, 1.0, 0.8, 1.0, 0.6, 1.0, 1.0, 0.2, 1.0, 0.8, 0.4, 1.0, 1.0, 1.0, 0.2, 0.8, 1.0, 0.2, 0.2, 1.0, 0.2, 1.0, 1.0, 0.4, 0.8, 0.0, 1.0, 0.8, 0.4, 0.6, 1.0, 1.0, 0.0, 0.0, 0.4, 0.6, 0.2, 0.8, 0.2, 0.8, 0.8, 0.4, 0.6, 1.0, 0.0, 1.0, 0.4, 1.0, 0.2, 0.8, 1.0, 1.0, 0.8, 0.4, 0.0, 0.4, 0.4, 1.0, 1.0, 0.2, 0.8, 0.0, 0.0, 1.0, 1.0, 0.2, 0.0, 0.6, 1.0, 0.8, 1.0, 0.8, 1.0, 1.0, 1.0, 0.6, 1.0, 0.0, 0.4, 1.0, 0.4, 0.8, 1.0, 0.4, 0.2, 0.8, 1.0, 0.8, 0.2, 0.6, 0.2, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.6, 0.0, 0.0, 0.2, 0.2, 0.0, 1.0, 0.0, 1.0, 0.6, 0.0, 1.0, 0.8, 0.0, 0.6, 1.0, 0.2, 0.2, 0.6, 0.2, 0.0, 0.2, 1.0, 0.4, 0.6, 0.8, 0.6, 0.4, 1.0, 1.0, 1.0, 0.0, 0.2, 0.8, 1.0, 1.0, 0.4, 0.2, 0.2, 0.6, 1.0, 0.2, 0.4, 1.0, 0.2, 0.8, 0.8, 1.0, 1.0, 1.0, 1.0, 0.0, 0.2, 0.2, 0.0, 1.0, 1.0, 0.4, 0.8, 1.0, 0.8, 1.0, 0.8, 0.4, 0.8, 1.0, 0.4, 1.0, 0.4, 0.2, 1.0, 0.2, 1.0, 0.2, 0.0, 1.0, 0.4, 0.2, 0.4, 0.6, 1.0, 1.0, 0.2, 0.2, 0.0, 1.0, 1.0, 0.4, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.6, 0.8, 1.0, 0.8, 0.0, 0.2, 0.4, 0.4, 0.0, 1.0, 0.6, 0.4, 1.0, 0.6, 0.6, 1.0, 0.2, 0.6, 0.4, 0.8, 0.2, 0.4, 0.6, 0.6, 0.2, 0.6, 0.6, 1.0, 0.6, 0.6, 1.0, 0.8, 0.8, 1.0, 1.0, 1.0, 0.8, 0.0, 1.0, 1.0, 0.6, 0.4, 0.8, 1.0, 0.6, 0.4, 1.0, 1.0, 0.0, 1.0, 0.6, 1.0, 0.4, 1.0, 1.0, 0.8, 1.0, 0.2, 0.4, 1.0, 0.0, 0.6, 0.0, 1.0, 0.2, 0.2, 1.0, 0.0, 0.4, 0.2, 1.0, 0.8, 0.2, 0.8, 0.6, 1.0, 1.0, 0.6, 0.2, 0.6, 0.6, 0.0, 1.0, 1.0, 1.0, 0.8, 0.6, 0.0, 1.0, 0.2, 0.2, 0.4, 0.0, 0.0, 0.8, 0.4, 0.0, 0.8, 0.6, 0.6, 0.6, 0.8, 0.0, 1.0, 1.0, 0.2, 1.0, 0.6, 0.8, 0.0, 0.8, 0.4, 0.6, 0.6, 1.0, 0.4, 0.4, 1.0, 0.6, 0.6, 0.6, 0.0, 0.8, 0.4, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.8, 0.2, 0.2, 0.4, 0.2, 0.0, 0.4, 0.6, 1.0, 0.4, 0.4, 0.0, 0.0, 1.0, 0.0, 0.4, 0.4, 0.6, 0.0, 0.4, 0.4, 0.4, 0.6, 0.0, 0.2, 0.0, 0.4, 0.0, 0.0, 0.6, 1.0, 1.0, 0.4, 0.8, 0.8, 1.0, 0.4, 1.0, 0.6, 1.0, 0.0, 1.0, 1.0, 0.4, 0.0, 0.2, 1.0, 0.2, 0.4, 0.2, 0.4, 0.8, 0.6, 0.4, 0.4, 0.0, 1.0, 0.2, 0.2, 0.2, 1.0, 0.4, 0.2, 0.0, 0.0, 1.0, 0.8, 0.8, 1.0, 0.2, 0.2, 0.8, 0.6, 0.6, 0.4, 0.6, 0.6, 0.2, 0.6, 0.4, 0.4, 0.6, 0.6, 0.4, 0.8, 0.0, 0.6, 0.4, 0.4, 0.2, 0.4, 1.0, 0.0, 0.8, 1.0, 1.0, 0.0, 0.4, 1.0, 1.0, 0.2, 1.0, 1.0, 1.0, 1.0, 1.0, 0.4, 0.8, 0.2, 0.4, 0.6, 1.0, 0.8, 0.8, 0.0, 0.8, 0.2, 0.0, 0.6, 0.8, 0.6, 1.0, 0.0, 1.0, 0.4, 0.8, 1.0, 0.2, 1.0, 0.8, 0.0, 1.0, 0.0, 0.0, 1.0, 0.6, 1.0, 0.4, 0.4, 0.4, 0.8, 0.6, 1.0, 1.0, 0.6, 0.8, 1.0, 0.6, 0.6, 0.8, 0.6, 0.8, 0.2, 1.0, 0.6, 1.0, 1.0, 1.0, 0.8, 0.4, 0.0, 1.0, 1.0, 0.2, 0.8, 1.0, 0.8, 0.8, 0.0, 0.8, 0.8, 0.8, 0.6, 0.6, 0.0, 0.0, 1.0, 1.0, 0.8, 1.0, 0.6, 0.4, 0.4, 0.2, 0.2, 0.8, 0.2, 0.8, 1.0, 0.4, 0.0, 0.2, 1.0, 0.2, 1.0, 0.6, 0.0, 0.4, 0.6, 0.8, 0.6, 0.4, 1.0, 0.4, 1.0, 1.0, 1.0, 0.2, 1.0, 0.6, 0.6, 1.0, 0.2, 0.0, 0.8, 0.4, 0.4, 0.0, 0.2, 0.6, 0.0, 0.4, 0.6, 0.8, 0.8, 1.0, 1.0, 0.8, 0.2, 1.0, 0.2, 0.2, 1.0, 1.0, 0.2, 1.0, 1.0, 0.4, 0.2, 0.2, 0.6, 0.6, 0.4, 0.4, 1.0, 1.0, 0.2, 1.0, 0.2, 0.0, 1.0, 1.0, 0.8, 0.4, 1.0, 0.4, 1.0, 0.8, 1.0, 0.2, 0.6, 0.6, 0.4, 0.0, 1.0, 1.0, 1.0, 1.0, 0.6, 0.8, 0.0, 0.4, 0.4, 0.8, 1.0, 0.6, 0.4, 0.4, 0.4, 0.0, 0.6, 0.4, 0.8, 1.0, 0.0, 0.2, 1.0, 0.6, 0.8, 0.6, 0.2, 1.0, 0.4, 0.8, 0.4, 0.0, 0.8, 0.2, 0.6, 0.8, 1.0, 0.2, 1.0, 0.8, 0.0, 0.8, 0.8, 0.8, 1.0, 1.0, 1.0, 1.0, 0.8, 1.0, 1.0, 0.4, 1.0, 0.6, 0.2, 0.6, 1.0, 0.4, 0.8, 0.6, 0.2, 0.2, 0.6, 0.2, 0.6, 0.8, 1.0, 0.6, 1.0, 0.0, 1.0, 0.0, 1.0, 0.2, 0.8, 0.0, 0.8, 0.0, 0.6, 0.2, 0.6, 0.4, 1.0, 0.8, 0.8, 1.0, 0.4, 0.0, 0.6, 0.8, 0.4, 0.8, 0.0, 1.0, 1.0, 0.2, 0.0, 1.0, 0.4, 1.0, 0.8, 1.0, 1.0, 0.6, 0.4, 0.0, 0.8, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.4, 0.8, 1.0, 0.6, 0.0, 0.4, 0.0, 1.0, 0.2, 0.2, 0.2, 0.4, 1.0, 0.4, 0.0, 1.0, 0.8, 1.0, 0.0, 1.0, 1.0, 0.0, 0.8, 0.4, 1.0, 0.4, 0.4, 1.0, 0.0, 0.6, 0.8, 1.0, 0.4, 0.6, 0.0, 0.8, 1.0, 1.0, 1.0, 0.4, 0.6, 0.8, 0.6, 0.0, 0.6, 0.6, 0.2, 0.8, 1.0, 1.0, 1.0, 0.2, 1.0, 0.2, 1.0, 0.0, 1.0, 1.0, 0.6, 1.0, 1.0, 0.4, 0.6, 1.0, 0.2, 0.0, 1.0, 0.2, 1.0, 0.2, 0.0, 0.6, 0.0, 0.8, 1.0, 0.2, 0.0, 0.2, 0.8, 0.8, 1.0, 1.0, 1.0, 0.6, 1.0, 1.0, 0.0, 0.2, 0.6, 0.4, 0.2, 1.0, 0.2, 0.6, 0.4, 1.0, 0.4, 0.4, 0.0, 0.4, 0.2, 0.4, 0.8, 0.4, 0.4, 1.0, 1.0, 1.0, 1.0, 0.6, 0.8, 1.0, 0.6, 0.2, 0.6, 0.4, 0.2, 1.0, 0.8, 1.0, 0.2, 1.0, 0.0, 0.0, 0.2, 0.4, 0.0, 0.6, 0.2, 1.0, 0.4, 0.6, 1.0, 1.0, 1.0, 0.6, 0.2, 1.0, 0.8, 0.4, 0.6, 0.2, 1.0, 0.4, 0.6, 0.4, 1.0, 0.4, 1.0, 1.0, 0.0, 1.0, 0.4, 0.6, 0.6, 1.0, 0.4, 0.0, 0.6, 0.2, 0.4, 0.0, 1.0, 0.0, 0.6, 0.6, 0.8, 0.6, 0.6, 0.2, 1.0, 1.0, 1.0, 0.0, 0.4, 0.0, 1.0, 0.8, 0.4, 1.0, 0.8, 0.2, 1.0, 0.6, 0.0, 0.6, 0.0, 1.0, 0.4, 0.2, 0.2, 0.0, 0.4, 1.0, 0.8, 0.4, 1.0, 0.8, 0.4, 0.0, 0.6, 1.0, 1.0, 1.0, 0.6, 0.6, 0.0, 0.2, 0.6, 0.0, 0.0, 0.4, 0.4, 1.0, 0.0, 0.8, 0.8, 1.0, 0.2, 1.0, 0.8, 0.2, 0.6, 0.6, 1.0, 1.0, 1.0, 0.0, 0.2, 0.0, 0.2, 1.0, 1.0, 1.0, 1.0, 0.8, 1.0, 0.8, 0.6, 1.0, 0.6, 0.2, 0.8, 0.8, 0.2, 1.0, 0.4, 0.0, 0.6, 0.4, 1.0, 0.4, 0.2, 0.4, 0.8, 0.4, 0.4, 1.0, 0.2, 0.2, 1.0, 0.0, 0.8, 0.2, 0.4, 0.2, 1.0, 0.0, 0.0, 0.0, 0.6, 0.6, 0.6, 1.0, 0.4, 1.0, 0.8, 1.0, 0.6, 0.4, 1.0, 0.6, 1.0, 0.0, 0.0, 0.2, 0.0, 0.6, 0.8, 0.0, 1.0, 1.0, 0.6, 1.0, 0.0, 1.0, 0.6, 0.8, 1.0, 0.2, 1.0, 0.0, 0.6, 1.0, 0.8, 0.6, 0.8, 0.8, 0.6, 1.0, 0.4, 0.2, 1.0, 0.6, 0.4, 0.2, 1.0, 0.4, 0.2, 0.4, 0.6, 0.4, 0.8, 1.0, 0.6, 0.0, 0.4, 0.0, 0.0, 0.0, 0.2, 0.2, 0.2, 0.6, 0.2, 0.0, 0.0, 0.2, 0.0, 0.2, 0.4, 0.2, 0.2, 0.4, 0.4, 0.2, 0.4, 0.6, 0.6, 0.6, 0.2, 0.0, 0.2, 0.2, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.2, 0.4, 0.2, 1.0, 0.0, 0.0, 0.2, 0.0, 0.0, 0.2, 0.2, 0.6, 0.2, 0.4, 0.2, 0.0, 0.0, 0.6, 1.0, 0.6, 0.0, 0.4, 0.6, 0.2, 0.4, 0.4, 0.8, 0.0, 0.4, 0.2, 0.8, 0.6, 0.4, 0.0, 0.4, 0.0, 0.2, 1.0, 0.0, 0.0, 0.2, 0.0, 0.4, 0.8, 0.0, 0.2, 0.8, 0.0, 0.2, 0.2, 0.2, 0.6, 0.6, 0.0, 0.0, 0.2, 0.4, 0.2, 0.2, 0.0, 1.0, 0.4, 0.4, 0.4, 0.2, 1.0, 0.0, 0.4, 0.2, 0.2, 0.6, 0.2, 0.0, 0.2, 0.2, 0.8, 0.4, 0.6, 0.8, 0.4, 0.0, 0.4, 0.6, 0.6, 0.0, 1.0, 0.4, 1.0, 0.0, 0.6, 1.0, 0.6, 0.0, 0.6, 0.2, 0.0, 0.0, 0.4, 0.4, 0.0, 0.4, 0.4, 0.6, 0.6, 1.0, 0.6, 0.8, 0.0, 0.4, 0.6, 0.6, 0.0, 0.4, 0.8, 0.2, 0.4, 0.0, 0.6, 0.6, 0.0, 0.0, 0.8, 0.4, 0.8, 0.4, 0.6, 0.2, 0.8, 0.0, 1.0, 1.0, 0.0, 0.4, 0.2, 0.0, 0.0, 0.4, 0.2, 0.4, 0.6, 0.6, 0.0, 0.6, 0.0, 0.4, 1.0, 0.2, 0.2, 0.2, 0.4, 0.0, 0.0, 0.4, 0.0, 1.0, 0.2, 0.8, 1.0, 0.4, 0.8, 0.0, 0.8, 0.0, 0.4, 0.6, 1.0, 0.0, 0.2, 0.0, 0.2, 0.6, 0.0, 0.0, 0.0, 0.6, 0.2, 0.6, 1.0, 0.0, 0.8, 0.2, 0.0, 0.0, 0.0, 1.0, 0.0, 0.2, 0.2, 0.0, 0.6, 0.2, 0.0, 0.2, 0.0, 0.6, 0.8, 0.2, 0.2, 0.4, 0.2, 0.4, 0.0, 0.4, 1.0, 0.2, 0.8, 0.0, 0.2, 0.6, 0.0, 0.6, 0.0, 0.4, 0.6, 0.6, 0.4, 0.4, 0.8, 0.2, 0.0, 0.2, 0.0, 0.0, 0.0, 0.2, 0.2, 0.0, 0.0, 0.2, 0.2, 0.8, 0.8, 0.2, 0.6, 0.4, 0.8, 0.0, 0.0, 0.8, 0.0, 0.4, 0.2, 1.0, 0.4, 0.2, 0.2, 0.4, 0.6, 0.4, 0.6, 0.0, 0.2, 0.4, 0.4, 0.0, 0.8, 0.4, 0.2, 0.4, 0.6, 0.0, 0.0, 0.8, 0.4, 0.0, 0.0, 0.4, 0.2, 1.0, 0.6, 0.4, 1.0, 0.2, 0.4, 0.2, 0.4, 0.8, 0.2, 0.0, 0.2, 0.4, 1.0, 0.2, 0.0, 0.2, 0.2, 0.0, 0.2, 0.0, 0.0, 0.2, 1.0, 0.4, 0.0, 1.0, 1.0, 0.0, 0.0, 0.8, 0.0, 0.0, 0.0, 0.6, 1.0, 0.4, 0.0, 0.0, 0.2, 0.2, 0.4, 0.2, 0.4, 0.2, 0.2, 0.6, 0.6, 0.2, 0.2, 0.6, 0.2, 1.0, 0.4, 0.0, 0.2, 0.6, 0.4, 0.8, 1.0, 0.0, 0.2, 0.0, 0.6, 0.0, 0.0, 0.4, 0.6, 1.0, 0.0, 0.6, 0.0, 0.6, 0.0, 0.0, 0.0, 0.4, 0.6, 0.0, 0.2, 0.4, 0.8, 0.2, 0.0, 0.8, 0.6, 0.0, 0.2, 0.2, 0.4, 0.8, 1.0, 0.6, 0.8, 0.2, 0.0, 1.0, 0.6, 0.4, 0.8, 0.2, 0.0, 0.6, 0.4, 0.0, 1.0, 0.6, 0.2, 0.0, 0.8, 0.0, 0.0, 0.6, 1.0, 0.6, 0.4, 0.0, 0.6, 0.2, 0.2, 0.6, 0.6, 0.0, 0.0, 0.8, 0.0, 0.2, 0.2, 0.2, 0.2, 0.2, 0.4, 0.2, 0.0, 0.0, 0.0, 0.2, 0.0, 0.2, 0.4, 0.0, 1.0, 0.4, 0.2, 0.4, 0.4, 1.0, 0.0, 0.2, 1.0, 0.0, 0.4, 0.0, 0.2, 0.8, 1.0, 0.2, 0.4, 0.4, 0.4, 0.2, 0.6, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.8, 0.4, 0.4, 0.6, 0.2, 0.2, 0.0, 0.2, 0.6, 0.0, 0.0, 0.6, 0.2, 0.6, 0.2, 0.6, 0.2, 0.6, 0.4, 1.0, 0.0, 0.2, 0.4, 1.0, 0.8, 1.0, 0.2, 1.0, 0.0, 0.2, 0.0, 0.2, 0.0, 0.6, 0.2, 0.0, 0.8, 1.0, 0.0, 0.4, 0.2, 0.8, 0.8, 0.0, 0.2, 1.0, 0.4, 0.4, 0.0, 0.2, 0.4, 0.4, 0.0, 0.0, 0.0, 0.6, 0.4, 1.0, 0.6, 0.2, 0.0, 0.0, 0.8, 0.0, 0.0, 0.0, 0.2, 0.8, 0.6, 0.8, 0.2, 0.2, 0.0, 0.0, 0.0, 0.2, 0.4, 0.6, 0.2, 0.0, 0.2, 0.2, 0.0, 0.2, 0.6, 0.6, 0.6, 0.0, 0.2, 0.2, 0.0, 0.6, 0.2, 0.8, 0.0, 0.0, 1.0, 0.0, 0.2, 0.0, 0.8, 0.2, 0.8, 0.0, 0.6, 1.0, 0.6, 0.2, 0.4, 1.0, 0.4, 0.0, 0.4, 0.6, 0.4, 0.4, 0.0, 0.0, 0.0, 0.0, 0.6, 1.0, 0.2, 0.2, 0.8, 0.2, 0.2, 0.6, 0.8, 0.0, 0.6, 0.4, 0.0, 0.4, 0.4, 0.0, 0.4, 0.0, 0.4, 0.2, 0.0, 1.0, 0.4, 0.6, 0.4, 0.0, 0.2, 0.2, 0.0, 0.8, 0.8, 0.6, 0.4, 0.8, 0.6, 0.4, 0.6, 0.4, 0.2, 0.0, 0.4, 0.2, 0.4, 0.0, 0.0, 1.0, 0.2, 0.2, 0.4, 0.6, 0.8, 0.4, 0.4, 0.0, 0.0, 0.8, 0.0, 0.6, 0.0, 0.0, 0.2, 0.8, 0.0, 0.6, 0.0, 0.0, 0.0, 0.0, 0.8, 0.4, 0.2, 0.0, 0.4, 0.6, 0.2, 0.6, 0.0, 0.2, 0.4, 1.0, 0.8, 0.0, 0.4, 0.2, 0.0, 0.4, 0.2, 0.2, 0.0, 0.8, 0.4, 0.6, 0.2, 0.0, 0.2, 0.6, 0.6, 0.0, 0.6, 0.0, 0.6, 0.2, 0.0, 0.0, 0.6, 1.0, 0.8, 0.4, 0.2, 0.8, 1.0, 0.6, 0.4, 0.4, 0.6, 0.0, 0.0, 0.2, 0.0, 0.4, 0.4, 1.0, 0.4, 0.8, 0.2, 1.0, 0.0, 1.0, 0.6, 0.2, 0.0, 0.2, 0.0, 0.6, 0.6, 0.0, 1.0, 0.4, 0.6, 0.6, 0.2, 0.2, 0.6, 1.0, 0.2, 1.0, 0.2, 0.6, 0.6, 0.6, 0.2, 0.0, 0.0, 0.0, 0.4, 0.4, 0.0, 0.0, 0.2, 0.0, 0.8, 0.6, 1.0, 1.0, 0.4, 0.4, 0.2, 1.0, 0.8, 0.4, 0.4, 0.8, 0.0, 0.2, 0.6, 0.6, 0.8, 0.0, 0.0, 0.0, 1.0, 1.0, 0.6, 0.8, 1.0, 0.6, 1.0, 0.2, 1.0, 0.0, 0.6, 0.2, 1.0, 0.2, 0.4, 0.0, 0.6, 0.6, 0.0, 0.0, 0.2, 0.0, 0.8, 0.2, 0.4, 0.4, 0.2, 0.0, 0.6, 0.0, 0.0, 0.2, 0.6, 0.0, 0.4, 0.2, 0.4, 1.0, 0.6, 0.2, 0.4, 0.2, 0.6, 0.0, 0.8, 0.6, 0.0, 0.2, 0.8, 0.0, 1.0, 0.2, 0.0, 0.6, 1.0, 1.0, 0.2, 0.0, 0.4, 0.2, 0.4, 0.0, 0.0, 1.0, 0.0, 0.2, 0.8, 0.8, 0.6, 0.2, 0.2, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.4, 0.4, 0.6, 0.2, 0.6, 0.6, 0.0, 0.0, 0.0, 0.2, 0.0, 0.0, 0.2, 0.0, 0.0, 0.2, 0.2, 0.6, 0.0, 0.0, 1.0, 1.0, 0.2, 0.4, 0.2, 0.6, 0.8, 0.0, 0.0, 0.0, 0.0, 0.2, 0.0, 0.0, 0.0, 0.6, 0.4, 0.6, 0.4, 0.8, 0.0, 0.0, 0.6, 0.8, 0.0, 0.4, 0.2, 0.0, 0.0, 1.0, 0.2, 0.2, 0.0, 0.0, 0.2, 1.0, 0.0, 0.0, 0.4, 0.0, 1.0, 0.0, 0.6, 0.0, 0.2, 0.2, 0.0, 0.0, 0.2, 0.2, 1.0, 0.0, 0.0, 0.6, 0.0, 0.6, 0.8, 0.4, 0.2, 0.6, 0.6, 0.6, 0.0, 0.2, 0.2, 0.0, 0.2]</t>
+          <t>[1.0, 0.2, 0.6, 0.0, 0.4, 1.0, 1.0, 0.2, 0.6, 0.6, 0.4, 0.0, 0.6, 0.2, 1.0, 0.0, 1.0, 0.8, 0.6, 0.0, 1.0, 1.0, 1.0, 0.4, 0.8, 0.2, 1.0, 1.0, 1.0, 0.2, 1.0, 0.4, 0.6, 0.2, 0.8, 0.4, 0.4, 0.8, 0.2, 0.4, 0.4, 0.8, 0.0, 0.8, 1.0, 0.2, 1.0, 0.4, 0.2, 1.0, 1.0, 1.0, 0.0, 0.6, 0.8, 0.4, 0.0, 0.2, 1.0, 0.6, 0.4, 0.4, 1.0, 0.6, 1.0, 0.4, 0.4, 0.8, 0.2, 1.0, 0.2, 0.2, 0.8, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.8, 0.4, 0.4, 0.6, 0.0, 0.8, 1.0, 0.2, 0.2, 0.4, 1.0, 0.4, 0.2, 0.8, 0.0, 0.2, 1.0, 0.2, 1.0, 0.6, 0.2, 0.6, 0.6, 1.0, 0.0, 1.0, 0.0, 1.0, 0.6, 0.6, 0.4, 0.0, 0.4, 0.8, 0.6, 0.0, 1.0, 0.4, 0.8, 0.6, 0.4, 0.6, 0.8, 0.6, 0.4, 0.2, 0.4, 0.4, 1.0, 0.2, 1.0, 1.0, 0.6, 0.4, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.8, 0.0, 0.8, 0.6, 1.0, 0.2, 1.0, 0.2, 0.4, 0.6, 0.0, 1.0, 0.2, 1.0, 0.8, 0.2, 0.0, 0.4, 0.8, 0.2, 1.0, 0.0, 0.2, 1.0, 1.0, 0.8, 0.8, 0.4, 1.0, 0.6, 0.0, 1.0, 1.0, 1.0, 0.4, 1.0, 1.0, 1.0, 0.0, 0.8, 1.0, 1.0, 0.2, 0.6, 0.8, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.4, 1.0, 0.2, 1.0, 0.2, 1.0, 0.6, 0.8, 0.8, 0.6, 0.8, 0.8, 0.8, 0.0, 0.2, 0.8, 0.8, 0.2, 1.0, 0.6, 1.0, 1.0, 1.0, 1.0, 0.6, 0.4, 0.2, 0.4, 0.6, 0.4, 0.6, 0.0, 1.0, 0.4, 1.0, 0.8, 0.2, 0.6, 1.0, 0.4, 1.0, 0.2, 1.0, 0.2, 0.2, 0.6, 0.8, 0.2, 1.0, 1.0, 1.0, 1.0, 1.0, 0.2, 0.0, 0.8, 0.8, 1.0, 0.8, 0.2, 0.2, 0.4, 0.4, 0.6, 0.8, 0.4, 0.6, 0.0, 0.8, 1.0, 0.0, 0.8, 0.0, 0.6, 1.0, 0.4, 0.6, 0.6, 0.6, 0.2, 0.4, 0.6, 1.0, 1.0, 0.6, 0.4, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.4, 0.4, 0.2, 1.0, 1.0, 1.0, 0.2, 0.8, 1.0, 0.8, 0.8, 0.0, 0.8, 0.2, 0.2, 1.0, 1.0, 1.0, 0.4, 0.8, 0.4, 0.4, 0.4, 0.6, 1.0, 1.0, 0.2, 0.2, 0.0, 0.8, 0.4, 1.0, 1.0, 1.0, 0.2, 1.0, 0.4, 1.0, 0.2, 0.0, 1.0, 0.4, 1.0, 1.0, 0.8, 0.4, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.4, 0.0, 1.0, 1.0, 0.6, 0.8, 0.4, 1.0, 0.4, 0.0, 1.0, 0.6, 1.0, 1.0, 0.8, 1.0, 0.2, 0.6, 1.0, 0.8, 0.2, 0.6, 0.4, 1.0, 1.0, 0.2, 0.0, 0.2, 1.0, 0.6, 1.0, 0.0, 1.0, 1.0, 0.4, 1.0, 0.0, 1.0, 0.2, 1.0, 1.0, 0.0, 0.4, 0.2, 1.0, 0.2, 0.8, 1.0, 1.0, 1.0, 0.0, 0.6, 1.0, 0.2, 1.0, 0.4, 1.0, 0.2, 0.0, 0.8, 0.4, 0.4, 0.2, 0.6, 0.8, 0.0, 0.2, 1.0, 0.6, 0.6, 0.0, 0.6, 1.0, 0.6, 0.8, 0.2, 1.0, 1.0, 0.0, 0.2, 1.0, 0.8, 1.0, 0.2, 0.8, 0.6, 0.4, 0.0, 0.8, 0.4, 0.8, 1.0, 1.0, 1.0, 0.8, 0.8, 1.0, 0.8, 1.0, 1.0, 0.8, 0.8, 1.0, 1.0, 0.8, 0.6, 0.4, 1.0, 0.4, 1.0, 1.0, 0.2, 0.2, 1.0, 0.0, 1.0, 0.8, 0.6, 0.8, 1.0, 1.0, 0.4, 0.0, 1.0, 0.8, 0.0, 0.6, 0.6, 1.0, 0.6, 1.0, 0.6, 0.6, 0.4, 0.0, 0.6, 0.0, 1.0, 0.0, 0.6, 0.2, 1.0, 0.0, 0.0, 0.4, 0.4, 0.0, 1.0, 0.4, 0.4, 0.2, 0.4, 0.8, 0.6, 0.0, 1.0, 1.0, 1.0, 0.4, 0.6, 0.0, 0.2, 0.2, 0.6, 0.8, 1.0, 0.8, 1.0, 1.0, 1.0, 1.0, 0.8, 1.0, 1.0, 0.2, 1.0, 0.4, 0.4, 1.0, 0.8, 1.0, 0.6, 0.6, 1.0, 0.0, 0.8, 1.0, 0.4, 0.8, 1.0, 1.0, 0.6, 0.0, 1.0, 0.8, 0.2, 0.6, 1.0, 1.0, 0.0, 0.2, 0.0, 0.6, 0.8, 0.6, 0.0, 1.0, 0.8, 0.8, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.2, 0.8, 1.0, 1.0, 0.8, 0.8, 0.0, 0.2, 0.2, 1.0, 1.0, 0.2, 0.8, 0.2, 0.0, 1.0, 1.0, 0.2, 0.6, 0.6, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.4, 1.0, 0.0, 0.6, 1.0, 0.2, 0.8, 1.0, 0.8, 0.2, 0.4, 1.0, 1.0, 0.0, 0.6, 0.0, 1.0, 0.8, 1.0, 1.0, 0.0, 1.0, 0.6, 0.0, 0.6, 0.0, 0.4, 0.0, 1.0, 0.2, 1.0, 0.8, 0.2, 1.0, 1.0, 0.2, 0.6, 1.0, 0.2, 0.4, 0.6, 0.4, 0.4, 0.2, 1.0, 0.4, 0.8, 0.6, 0.8, 0.2, 1.0, 1.0, 1.0, 0.0, 0.2, 0.2, 1.0, 0.8, 0.8, 0.2, 0.2, 0.4, 0.8, 0.4, 0.2, 1.0, 0.2, 1.0, 0.8, 1.0, 1.0, 1.0, 0.8, 0.0, 0.2, 0.2, 0.2, 1.0, 0.8, 0.8, 0.6, 1.0, 0.8, 1.0, 0.4, 0.4, 0.4, 0.8, 0.4, 1.0, 0.0, 0.4, 0.8, 0.0, 1.0, 0.2, 0.0, 1.0, 1.0, 0.2, 0.4, 0.6, 1.0, 1.0, 0.2, 0.0, 0.2, 1.0, 1.0, 0.0, 0.4, 0.2, 1.0, 0.2, 0.8, 1.0, 0.6, 0.6, 0.8, 1.0, 0.0, 0.4, 0.2, 0.6, 0.0, 1.0, 0.6, 0.4, 0.8, 0.6, 1.0, 1.0, 0.2, 1.0, 0.2, 0.6, 0.0, 0.4, 0.6, 0.6, 0.2, 0.6, 0.4, 1.0, 0.2, 0.8, 1.0, 0.6, 1.0, 1.0, 1.0, 1.0, 1.0, 0.2, 1.0, 1.0, 0.8, 0.4, 0.2, 1.0, 0.6, 0.2, 1.0, 0.8, 0.2, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.8, 1.0, 0.4, 0.2, 0.8, 0.4, 0.6, 0.4, 1.0, 0.8, 0.6, 1.0, 0.0, 0.4, 0.2, 1.0, 0.4, 0.2, 1.0, 0.8, 1.0, 1.0, 0.6, 0.2, 0.4, 0.6, 0.4, 1.0, 1.0, 1.0, 0.6, 0.6, 0.0, 0.8, 0.4, 0.6, 0.4, 0.0, 0.0, 0.6, 0.8, 0.0, 0.8, 1.0, 0.6, 0.2, 0.4, 0.4, 0.8, 1.0, 0.4, 0.8, 0.4, 1.0, 0.4, 0.8, 0.4, 0.4, 0.8, 0.8, 0.6, 0.6, 1.0, 0.8, 1.0, 0.4, 0.0, 0.6, 0.2, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.8, 0.4, 0.4, 0.2, 0.0, 0.2, 0.6, 0.8, 0.4, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.2, 0.4, 0.2, 0.4, 0.4, 0.0, 0.2, 0.0, 0.4, 0.6, 0.0, 0.4, 1.0, 1.0, 0.4, 0.6, 1.0, 1.0, 0.8, 1.0, 0.4, 1.0, 0.2, 0.8, 1.0, 0.6, 0.0, 0.2, 1.0, 0.2, 0.0, 0.0, 1.0, 1.0, 0.4, 0.0, 0.2, 0.0, 1.0, 0.2, 0.2, 0.8, 0.6, 0.8, 0.4, 0.0, 0.0, 1.0, 0.6, 0.8, 1.0, 0.2, 0.2, 0.8, 0.8, 0.8, 0.2, 0.8, 0.4, 0.2, 0.6, 0.4, 0.8, 0.8, 1.0, 0.6, 1.0, 0.4, 0.6, 0.4, 0.4, 0.8, 0.6, 0.8, 0.0, 0.8, 1.0, 1.0, 0.0, 0.2, 1.0, 1.0, 0.2, 1.0, 1.0, 0.4, 1.0, 0.8, 0.2, 0.8, 0.4, 0.4, 1.0, 1.0, 0.6, 0.8, 0.0, 0.8, 0.2, 0.0, 0.6, 0.2, 0.6, 1.0, 0.0, 1.0, 0.4, 0.6, 1.0, 0.2, 0.8, 1.0, 0.0, 0.8, 0.0, 0.0, 1.0, 0.6, 0.6, 0.4, 0.0, 0.6, 0.8, 0.6, 1.0, 1.0, 0.0, 1.0, 1.0, 0.6, 0.8, 0.6, 0.8, 1.0, 0.2, 1.0, 0.2, 0.8, 1.0, 1.0, 1.0, 0.4, 0.0, 0.0, 1.0, 0.6, 1.0, 1.0, 0.6, 0.6, 0.0, 0.8, 0.6, 0.8, 0.4, 0.6, 0.0, 0.0, 1.0, 1.0, 0.8, 1.0, 0.2, 0.2, 0.6, 0.2, 0.4, 0.6, 0.0, 0.8, 1.0, 0.2, 0.0, 1.0, 1.0, 0.0, 1.0, 0.6, 0.0, 0.6, 0.6, 0.6, 0.8, 0.4, 0.8, 0.6, 0.4, 0.8, 1.0, 0.0, 1.0, 0.8, 0.6, 1.0, 0.2, 0.2, 1.0, 0.6, 0.4, 0.0, 0.2, 0.4, 0.0, 0.8, 0.2, 0.6, 1.0, 1.0, 1.0, 0.6, 0.0, 0.8, 0.0, 0.2, 0.6, 1.0, 0.2, 1.0, 0.4, 0.2, 0.0, 0.2, 0.8, 0.6, 0.4, 0.4, 1.0, 1.0, 0.4, 1.0, 0.2, 0.0, 1.0, 1.0, 0.8, 0.0, 1.0, 0.4, 1.0, 1.0, 1.0, 0.0, 1.0, 0.6, 0.6, 0.0, 1.0, 0.8, 1.0, 1.0, 0.4, 0.6, 0.4, 0.6, 0.4, 1.0, 1.0, 0.8, 0.2, 0.6, 0.2, 0.2, 0.4, 0.8, 0.4, 1.0, 0.0, 0.2, 1.0, 0.6, 0.2, 0.2, 0.8, 1.0, 1.0, 0.8, 0.4, 0.4, 0.8, 0.4, 0.8, 0.8, 0.8, 0.2, 1.0, 1.0, 0.0, 0.8, 1.0, 0.8, 1.0, 1.0, 1.0, 1.0, 0.6, 1.0, 1.0, 0.4, 1.0, 0.6, 0.0, 0.4, 1.0, 0.4, 0.8, 0.6, 0.0, 0.4, 0.8, 0.2, 0.4, 0.4, 0.8, 1.0, 1.0, 0.0, 1.0, 0.6, 1.0, 0.0, 0.6, 0.2, 1.0, 0.0, 0.8, 0.4, 0.4, 0.4, 0.8, 0.8, 1.0, 0.6, 0.6, 0.0, 0.8, 1.0, 0.2, 0.2, 0.4, 1.0, 0.6, 0.8, 0.0, 1.0, 0.6, 1.0, 0.8, 1.0, 1.0, 1.0, 0.6, 0.2, 0.8, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.2, 0.8, 1.0, 1.0, 0.2, 0.2, 0.0, 1.0, 0.4, 0.4, 0.2, 0.2, 1.0, 1.0, 0.0, 1.0, 0.8, 1.0, 0.0, 1.0, 0.8, 0.0, 0.8, 0.4, 1.0, 0.4, 0.4, 1.0, 0.0, 0.8, 0.4, 1.0, 0.0, 0.6, 0.0, 0.4, 1.0, 1.0, 1.0, 0.4, 0.2, 0.8, 0.8, 0.0, 0.6, 0.4, 0.2, 1.0, 1.0, 1.0, 1.0, 0.2, 0.8, 0.2, 1.0, 0.0, 1.0, 1.0, 0.8, 0.8, 1.0, 0.4, 0.0, 0.6, 0.4, 0.0, 1.0, 0.2, 1.0, 0.0, 0.0, 0.6, 0.2, 1.0, 1.0, 0.4, 0.4, 0.0, 1.0, 0.8, 1.0, 0.8, 1.0, 0.4, 1.0, 1.0, 0.0, 0.6, 0.8, 0.6, 0.2, 1.0, 0.2, 0.2, 0.4, 1.0, 0.2, 0.2, 0.0, 0.0, 0.2, 0.6, 0.4, 0.6, 1.0, 1.0, 1.0, 1.0, 1.0, 0.8, 0.6, 1.0, 0.6, 0.4, 1.0, 0.4, 0.2, 1.0, 1.0, 1.0, 0.0, 0.6, 0.0, 0.4, 0.4, 0.4, 0.0, 0.6, 0.0, 1.0, 0.4, 1.0, 0.8, 0.8, 1.0, 0.8, 0.8, 0.8, 0.8, 0.4, 0.8, 0.2, 1.0, 0.4, 0.4, 0.8, 0.8, 0.2, 1.0, 1.0, 0.2, 1.0, 0.2, 0.8, 0.4, 1.0, 0.6, 0.0, 1.0, 0.2, 0.6, 0.0, 0.8, 0.0, 0.6, 0.4, 0.8, 0.4, 0.6, 0.8, 1.0, 1.0, 1.0, 0.2, 0.6, 0.0, 1.0, 0.8, 0.0, 1.0, 0.4, 0.2, 1.0, 0.2, 0.0, 0.6, 0.0, 0.8, 0.2, 0.2, 0.2, 0.0, 0.6, 1.0, 0.6, 0.6, 1.0, 0.8, 0.4, 0.0, 0.6, 1.0, 1.0, 1.0, 0.6, 0.6, 0.2, 0.6, 0.6, 0.0, 0.2, 0.4, 0.4, 1.0, 0.0, 0.8, 0.8, 1.0, 0.2, 1.0, 0.8, 0.4, 0.8, 0.2, 1.0, 1.0, 1.0, 0.6, 0.4, 0.0, 0.4, 1.0, 1.0, 1.0, 1.0, 0.4, 0.8, 1.0, 0.6, 0.8, 0.8, 0.0, 0.8, 0.6, 0.4, 1.0, 0.2, 0.0, 1.0, 0.2, 1.0, 0.6, 0.2, 0.6, 1.0, 0.8, 0.4, 1.0, 0.2, 0.2, 1.0, 0.4, 0.8, 0.2, 0.0, 0.2, 1.0, 0.0, 0.0, 0.4, 0.8, 0.8, 1.0, 1.0, 0.6, 1.0, 0.4, 1.0, 1.0, 0.2, 1.0, 0.2, 1.0, 0.0, 0.0, 0.2, 0.4, 0.4, 1.0, 0.2, 1.0, 1.0, 0.6, 0.8, 0.2, 1.0, 0.6, 0.8, 0.8, 0.0, 0.8, 0.0, 0.6, 1.0, 1.0, 0.4, 1.0, 0.8, 0.2, 1.0, 0.6, 0.4, 1.0, 0.0, 0.4, 0.2, 1.0, 0.4, 0.0, 0.2, 0.2, 0.4, 0.8, 1.0, 0.0, 0.2, 0.4, 0.2, 0.2, 0.2, 0.2, 0.2, 0.2, 0.4, 0.2, 0.2, 1.0, 0.2, 0.8, 0.0, 0.8, 0.0, 0.0, 0.0, 0.0, 0.4, 0.0, 0.2, 0.2, 0.0, 0.4, 0.4, 0.8, 0.2, 0.0, 0.4, 0.0, 0.2, 0.0, 0.2, 0.8, 0.0, 0.8, 0.8, 0.0, 0.0, 0.0, 0.0, 0.4, 0.4, 0.0, 0.0, 0.0, 0.2, 0.2, 0.6, 0.0, 0.0, 0.0, 0.2, 1.0, 1.0, 0.0, 0.4, 0.0, 0.2, 0.6, 0.2, 0.0, 0.0, 0.2, 0.8, 1.0, 0.4, 0.2, 0.4, 0.2, 0.0, 0.2, 0.0, 1.0, 0.2, 0.0, 1.0, 0.0, 0.0, 0.2, 0.4, 0.0, 0.0, 0.6, 0.4, 0.4, 0.0, 0.8, 0.8, 1.0, 1.0, 1.0, 0.0, 0.2, 0.8, 0.8, 0.2, 0.0, 0.0, 0.4, 0.2, 1.0, 0.0, 0.0, 0.0, 1.0, 0.2, 0.2, 0.4, 0.6, 0.4, 0.0, 0.2, 0.4, 0.0, 0.2, 0.4, 0.0, 0.8, 0.0, 0.2, 0.0, 0.2, 0.4, 0.0, 0.2, 0.2, 0.0, 0.4, 0.4, 1.0, 0.6, 0.4, 0.2, 0.2, 0.4, 0.0, 0.0, 0.2, 0.2, 0.0, 0.6, 0.0, 0.2, 0.0, 0.0, 0.2, 0.8, 0.0, 0.0, 0.0, 1.0, 0.2, 0.2, 0.4, 0.4, 0.2, 0.6, 0.2, 0.0, 0.0, 0.4, 0.8, 0.0, 0.6, 0.0, 0.4, 0.6, 1.0, 0.8, 0.2, 0.4, 0.0, 0.0, 0.4, 0.2, 0.0, 0.0, 0.4, 0.4, 0.0, 0.4, 0.4, 0.0, 0.0, 0.6, 0.2, 0.6, 0.0, 0.4, 0.4, 0.0, 0.4, 0.6, 0.4, 0.4, 0.0, 0.4, 0.8, 0.8, 1.0, 0.6, 0.2, 0.0, 1.0, 0.4, 0.2, 1.0, 0.2, 0.0, 0.8, 1.0, 0.0, 0.2, 0.0, 0.0, 0.2, 0.2, 0.0, 0.6, 0.2, 0.2, 0.0, 0.6, 0.0, 0.2, 0.4, 0.0, 0.4, 0.2, 0.6, 0.6, 0.2, 1.0, 0.0, 0.4, 0.8, 0.6, 0.8, 0.0, 0.0, 0.2, 0.2, 0.0, 0.4, 0.0, 0.2, 0.4, 0.8, 0.0, 0.0, 0.0, 0.0, 0.0, 0.2, 0.2, 1.0, 0.0, 0.6, 0.0, 0.6, 0.4, 0.4, 0.0, 0.2, 0.8, 0.4, 0.6, 0.0, 1.0, 0.6, 0.0, 0.2, 0.8, 0.8, 0.6, 0.4, 0.0, 0.2, 0.4, 0.8, 0.4, 0.0, 0.2, 1.0, 0.4, 0.0, 0.0, 0.6, 0.0, 0.8, 0.0, 0.0, 1.0, 0.2, 0.6, 0.0, 0.4, 0.0, 1.0, 0.6, 0.0, 0.0, 0.0, 0.0, 0.2, 0.4, 0.2, 0.4, 0.4, 0.0, 0.2, 0.0, 0.6, 0.0, 0.4, 0.0, 0.0, 0.4, 0.0, 0.2, 0.2, 0.2, 0.0, 0.6, 0.6, 0.4, 0.2, 0.8, 0.0, 0.0, 0.8, 0.4, 1.0, 0.0, 0.2, 0.0, 0.0, 0.2, 0.8, 0.8, 0.0, 0.2, 0.2, 0.2, 0.0, 0.0, 0.2, 0.6, 0.0, 0.2, 0.2, 0.6, 0.0, 0.6, 0.8, 0.6, 0.2, 0.6, 0.0, 0.2, 0.4, 0.6, 0.2, 0.0, 0.2, 0.4, 0.8, 0.4, 0.0, 0.4, 0.0, 0.2, 0.0, 0.6, 0.6, 0.2, 0.4, 0.4, 0.4, 0.0, 1.0, 0.6, 0.0, 0.6, 0.0, 0.4, 1.0, 0.4, 0.0, 0.2, 0.0, 0.0, 1.0, 0.2, 0.6, 0.6, 0.2, 0.4, 0.4, 0.6, 0.4, 0.4, 1.0, 1.0, 0.6, 1.0, 1.0, 0.4, 1.0, 0.2, 0.0, 0.2, 0.2, 0.6, 0.2, 0.0, 0.2, 0.6, 0.2, 0.0, 1.0, 0.0, 0.0, 0.8, 0.0, 0.0, 0.2, 0.0, 0.6, 0.0, 0.0, 0.0, 0.0, 0.0, 0.2, 0.2, 0.6, 0.4, 0.6, 0.0, 1.0, 0.4, 0.4, 0.4, 0.2, 0.8, 0.8, 0.0, 0.6, 0.4, 0.2, 0.2, 0.6, 0.8, 0.2, 0.4, 0.0, 0.4, 0.0, 0.0, 0.2, 1.0, 0.2, 0.0, 0.6, 0.4, 0.0, 0.0, 0.6, 0.4, 0.6, 0.8, 0.8, 0.4, 0.6, 1.0, 0.2, 0.0, 1.0, 0.4, 0.0, 0.2, 0.2, 0.2, 0.0, 0.2, 0.2, 0.2, 0.0, 0.2, 0.2, 0.4, 0.0, 0.0, 0.4, 0.4, 0.4, 1.0, 0.4, 0.0, 0.0, 0.4, 0.0, 0.0, 0.2, 0.6, 0.4, 0.2, 0.6, 0.4, 0.4, 0.0, 0.0, 0.2, 0.2, 0.0, 0.4, 0.0, 0.2, 0.0, 0.2, 0.6, 0.2, 0.2, 0.2, 0.6, 0.2, 0.4, 0.2, 0.2, 0.8, 0.4, 0.0, 0.4, 0.0, 0.4, 0.2, 0.0, 0.2, 0.4, 0.4, 0.2, 0.2, 0.0, 0.0, 0.2, 0.6, 0.2, 1.0, 0.0, 0.0, 0.8, 0.4, 0.6, 0.0, 0.4, 0.2, 0.2, 0.8, 0.0, 0.8, 0.6, 0.4, 0.4, 0.0, 0.4, 0.2, 0.6, 0.6, 0.2, 0.4, 0.0, 0.0, 0.2, 0.4, 0.0, 0.2, 0.6, 0.0, 1.0, 0.0, 0.0, 0.2, 0.8, 0.4, 0.6, 1.0, 0.0, 0.2, 0.8, 0.0, 0.0, 0.0, 0.6, 0.2, 0.0, 0.8, 0.2, 0.6, 0.2, 0.8, 0.0, 1.0, 0.0, 0.8, 0.0, 0.4, 0.0, 1.0, 0.0, 0.8, 0.0, 0.6, 0.0, 0.0, 0.0, 0.0, 0.4, 0.0, 0.2, 0.4, 0.0, 0.2, 0.2, 0.6, 0.6, 0.4, 0.0, 0.6, 0.2, 0.8, 0.2, 0.0, 0.0, 0.0, 0.2, 0.4, 0.6, 0.0, 1.0, 0.4, 0.0, 0.4, 0.2, 0.4, 0.4, 0.4, 0.4, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.4, 0.4, 0.0, 0.0, 0.2, 0.6, 0.6, 0.0, 0.2, 0.0, 0.0, 0.6, 0.8, 1.0, 0.6, 0.2, 0.0, 0.0, 0.6, 0.0, 0.6, 0.0, 0.0, 0.4, 0.2, 0.4, 0.4, 0.4, 0.8, 0.2, 0.6, 0.8, 0.2, 0.0, 0.6, 0.2, 0.0, 0.6, 1.0, 0.2, 0.0, 0.0, 0.4, 0.4, 0.2, 0.2, 0.4, 1.0, 0.8, 0.6, 0.0, 0.4, 0.6, 0.0, 0.8, 0.0, 0.6, 0.2, 0.2, 1.0, 0.4, 0.6, 0.6, 0.4, 0.2, 0.0, 1.0, 0.8, 0.4, 0.4, 0.0, 0.2, 0.0, 0.2, 0.0, 0.0, 0.4, 0.8, 1.0, 1.0, 0.0, 1.0, 0.0, 0.2, 0.4, 0.2, 1.0, 0.2, 0.8, 0.0, 1.0, 0.2, 0.8, 0.8, 0.2, 1.0, 0.8, 0.2, 0.6, 0.2, 0.8, 0.2, 0.0, 0.8, 0.4, 0.8, 0.0, 0.4, 0.4, 0.2, 0.8, 0.0, 0.4, 0.2, 0.4, 0.0, 0.4, 0.2, 0.0, 0.2, 0.2, 0.0, 0.4, 0.0, 0.4, 0.2, 0.0, 0.0, 0.0, 0.2, 1.0, 0.2, 0.8, 0.2, 0.0, 0.8, 0.0, 0.2, 0.0, 0.2, 0.0, 0.0, 0.6, 0.0, 0.6, 0.8, 0.4, 0.8, 0.2, 0.6, 0.2, 0.0, 0.0, 0.2, 0.4, 0.2, 0.0, 0.2, 0.0, 0.8, 0.0, 0.4, 0.0, 0.0, 0.2, 0.8, 1.0, 0.2, 0.2, 0.4, 1.0, 0.4, 0.2, 0.2, 0.6, 1.0, 0.0, 0.0, 1.0, 0.0, 0.4, 0.4, 0.0, 0.0, 0.4, 1.0, 0.6, 0.2, 0.2, 0.6, 1.0, 0.6, 0.6, 0.4, 0.4, 0.4, 0.0, 0.2, 0.6, 0.6, 0.2, 0.0, 0.0, 0.6, 0.6, 0.0, 1.0, 0.0, 0.6, 0.0, 0.8, 0.2, 0.4, 0.2, 1.0, 1.0, 0.0, 0.4, 0.2, 0.4, 0.8, 0.6, 0.4, 1.0, 0.2, 0.0, 0.0, 0.4, 0.6, 0.4, 0.4, 0.6, 0.4, 0.2, 0.4, 0.0, 0.8, 0.0, 0.2, 1.0, 0.2, 0.0, 0.0, 0.0, 0.2, 1.0, 0.2, 0.4, 0.4, 0.2, 0.2, 0.0, 0.6, 0.2, 0.2, 0.0, 0.8, 0.2, 0.0, 0.2, 1.0, 0.2, 0.6, 0.4, 0.2, 0.2, 0.8, 0.0, 0.0, 0.2, 0.0, 0.2, 0.6, 0.4, 0.0, 0.4, 0.2, 0.0, 0.6, 0.0, 0.2, 0.6]</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>[0.6, 0.8, 0.0, 1.0, 0.6, 0.4, 0.8, 1.0, 0.6, 0.4, 0.4, 1.0, 0.6, 0.8, 1.0, 0.2, 0.4, 0.6, 0.6, 0.6, 1.0, 0.0, 0.4, 0.2, 0.4, 0.2, 0.2, 1.0, 0.2, 1.0, 0.4, 1.0, 0.8, 1.0, 0.0, 1.0, 0.6, 0.0, 1.0, 0.8, 1.0, 1.0, 1.0, 0.2, 0.0, 0.8, 1.0, 0.8, 0.8, 0.6, 1.0, 0.4, 0.8, 0.2, 1.0, 0.0, 0.2, 0.6, 1.0, 0.6, 0.4, 0.6, 0.8, 0.8, 1.0, 1.0, 0.8, 0.0, 1.0, 1.0, 0.6, 1.0, 1.0, 1.0, 1.0, 0.2, 1.0, 1.0, 1.0, 1.0, 0.4, 1.0, 0.4, 0.4, 1.0, 0.0, 1.0, 0.6, 1.0, 1.0, 1.0, 0.4, 1.0, 1.0, 1.0, 0.6, 0.4, 0.2, 1.0, 0.6, 1.0, 0.6, 0.6, 0.6, 0.4, 0.0, 0.2, 0.2, 0.2, 0.8, 0.0, 1.0, 0.8, 0.6, 0.4, 1.0, 0.8, 0.0, 0.8, 0.6, 0.6, 0.4, 0.8, 0.6, 1.0, 1.0, 0.4, 0.6, 0.8, 0.4, 0.0, 0.4, 0.0, 1.0, 0.6, 1.0, 1.0, 1.0, 0.8, 1.0, 1.0, 1.0, 0.8, 0.6, 1.0, 0.0, 0.2, 1.0, 1.0, 0.6, 0.2, 0.2, 0.8, 1.0, 0.8, 0.2, 0.4, 1.0, 0.8, 0.4, 0.4, 0.4, 0.0, 0.6, 0.4, 1.0, 0.0, 0.8, 0.4, 1.0, 0.2, 0.6, 0.0, 0.0, 0.6, 1.0, 0.4, 0.4, 0.8, 1.0, 1.0, 0.2, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.6, 1.0, 0.2, 0.0, 0.8, 0.8, 0.8, 0.6, 0.0, 0.6, 0.2, 0.8, 1.0, 0.0, 0.4, 0.2, 0.0, 0.2, 0.8, 0.8, 0.0, 0.8, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.2, 1.0, 1.0, 0.0, 1.0, 0.6, 0.2, 0.2, 0.6, 0.4, 0.4, 0.0, 0.8, 0.0, 1.0, 0.8, 0.2, 0.0, 0.0, 0.6, 0.0, 0.4, 0.2, 0.0, 0.0, 0.2, 0.4, 0.6, 1.0, 1.0, 0.8, 0.8, 0.4, 1.0, 0.6, 0.4, 0.2, 0.4, 0.2, 0.8, 1.0, 1.0, 0.0, 0.2, 1.0, 0.4, 0.4, 0.0, 0.8, 0.6, 0.2, 0.2, 0.2, 0.4, 0.4, 1.0, 1.0, 0.4, 0.0, 1.0, 0.2, 1.0, 0.2, 0.0, 1.0, 0.6, 0.8, 0.6, 0.0, 1.0, 0.0, 1.0, 0.6, 0.2, 0.0, 1.0, 1.0, 0.0, 1.0, 0.6, 0.0, 0.6, 0.2, 0.0, 1.0, 0.2, 0.2, 1.0, 0.6, 0.4, 0.6, 0.8, 0.0, 0.4, 0.0, 1.0, 0.0, 1.0, 0.4, 0.6, 0.6, 0.8, 0.0, 0.2, 0.8, 0.8, 0.0, 0.2, 0.0, 0.8, 0.8, 0.8, 0.2, 0.6, 1.0, 0.2, 0.2, 0.2, 0.6, 0.2, 1.0, 0.2, 0.0, 0.8, 1.0, 0.8, 0.6, 0.6, 0.8, 1.0, 0.6, 0.6, 1.0, 0.6, 0.0, 0.2, 1.0, 0.2, 0.8, 0.0, 0.4, 1.0, 0.2, 0.6, 0.6, 1.0, 1.0, 1.0, 0.0, 0.8, 1.0, 0.6, 1.0, 1.0, 1.0, 0.2, 0.4, 1.0, 0.0, 1.0, 0.8, 0.0, 1.0, 0.8, 1.0, 0.8, 0.2, 1.0, 0.4, 0.8, 1.0, 0.8, 0.2, 1.0, 1.0, 1.0, 1.0, 0.6, 0.8, 0.4, 1.0, 1.0, 0.8, 0.8, 1.0, 0.8, 1.0, 0.2, 0.0, 0.4, 0.6, 0.4, 1.0, 0.4, 0.6, 0.6, 0.6, 1.0, 0.0, 0.4, 0.2, 0.6, 1.0, 0.2, 1.0, 0.2, 0.0, 0.0, 0.4, 0.0, 0.0, 0.0, 0.8, 0.2, 0.6, 0.4, 0.6, 0.8, 0.0, 0.6, 0.4, 0.0, 1.0, 0.0, 1.0, 0.6, 0.8, 1.0, 0.6, 0.6, 0.0, 1.0, 0.0, 0.2, 0.0, 1.0, 0.0, 0.0, 0.6, 0.0, 0.2, 1.0, 1.0, 0.0, 0.2, 0.6, 0.0, 0.4, 0.8, 0.6, 0.6, 0.8, 1.0, 0.4, 0.0, 0.6, 0.2, 0.0, 0.8, 0.2, 1.0, 0.6, 0.2, 1.0, 0.0, 0.4, 0.6, 0.6, 0.2, 0.4, 0.8, 0.2, 1.0, 0.4, 0.6, 0.6, 1.0, 1.0, 0.6, 0.8, 0.0, 0.8, 0.0, 1.0, 0.6, 0.4, 0.0, 0.0, 0.2, 0.8, 0.2, 0.6, 0.8, 0.0, 1.0, 0.4, 0.0, 0.6, 0.2, 0.0, 0.2, 0.8, 0.6, 1.0, 1.0, 0.0, 0.6, 0.0, 1.0, 0.4, 0.4, 1.0, 0.2, 0.0, 0.6, 0.2, 0.6, 0.2, 0.2, 1.0, 1.0, 0.4, 0.2, 0.6, 1.0, 0.0, 0.0, 0.2, 0.6, 1.0, 0.0, 0.2, 0.4, 0.2, 0.2, 0.2, 0.8, 1.0, 0.8, 0.2, 0.6, 0.6, 0.6, 0.2, 1.0, 0.4, 0.2, 0.2, 1.0, 0.8, 0.8, 0.2, 0.6, 0.8, 0.6, 0.6, 0.4, 0.4, 1.0, 0.8, 0.8, 0.6, 1.0, 0.0, 0.8, 0.8, 1.0, 1.0, 1.0, 1.0, 0.4, 0.8, 1.0, 0.0, 1.0, 0.4, 1.0, 0.8, 0.8, 0.4, 0.2, 0.4, 0.6, 0.0, 0.0, 0.0, 1.0, 0.8, 1.0, 0.6, 1.0, 1.0, 0.8, 0.6, 1.0, 0.0, 0.4, 0.2, 0.2, 1.0, 0.2, 0.4, 0.6, 0.2, 0.8, 0.2, 0.8, 1.0, 1.0, 0.2, 1.0, 0.6, 1.0, 0.6, 0.2, 0.4, 0.2, 1.0, 1.0, 1.0, 0.4, 1.0, 0.0, 0.2, 1.0, 0.0, 1.0, 0.6, 1.0, 0.0, 0.8, 0.0, 0.4, 1.0, 0.0, 0.2, 1.0, 0.4, 0.0, 1.0, 1.0, 1.0, 0.2, 0.2, 1.0, 0.6, 1.0, 1.0, 0.8, 1.0, 0.4, 0.4, 0.2, 0.8, 0.8, 1.0, 0.2, 1.0, 1.0, 0.6, 1.0, 1.0, 1.0, 0.2, 0.8, 1.0, 0.6, 1.0, 0.2, 0.6, 0.2, 0.8, 1.0, 0.4, 1.0, 1.0, 0.8, 1.0, 0.4, 0.8, 1.0, 1.0, 0.0, 1.0, 0.8, 0.8, 0.8, 1.0, 0.0, 1.0, 0.2, 1.0, 1.0, 0.0, 0.2, 0.0, 1.0, 1.0, 0.4, 0.6, 1.0, 0.0, 1.0, 0.2, 0.6, 0.8, 0.4, 0.4, 1.0, 1.0, 0.6, 1.0, 0.6, 0.6, 0.4, 0.4, 0.6, 0.2, 0.4, 0.2, 0.0, 0.0, 0.6, 0.6, 0.2, 0.0, 0.2, 0.8, 0.4, 0.6, 0.6, 0.6, 0.2, 0.6, 0.2, 0.6, 0.4, 1.0, 0.8, 0.4, 0.0, 0.8, 0.4, 0.4, 1.0, 0.6, 0.8, 0.6, 0.6, 1.0, 1.0, 0.2, 0.0, 1.0, 1.0, 1.0, 0.8, 0.6, 0.4, 0.4, 0.2, 0.8, 0.0, 0.8, 0.2, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.6, 0.8, 1.0, 1.0, 0.8, 0.4, 0.8, 0.4, 1.0, 1.0, 1.0, 1.0, 0.6, 0.2, 1.0, 1.0, 0.2, 1.0, 0.8, 0.8, 1.0, 0.8, 1.0, 0.8, 0.0, 1.0, 1.0, 0.0, 0.8, 1.0, 1.0, 0.2, 0.0, 1.0, 0.4, 0.6, 0.6, 0.8, 0.4, 0.4, 0.0, 1.0, 0.2, 0.6, 0.0, 1.0, 0.8, 0.6, 0.8, 1.0, 0.6, 0.2, 0.6, 0.2, 0.6, 1.0, 1.0, 0.4, 0.8, 0.6, 0.8, 1.0, 1.0, 1.0, 0.0, 0.2, 0.6, 1.0, 0.4, 0.2, 0.2, 1.0, 0.0, 1.0, 1.0, 0.8, 0.4, 0.4, 0.8, 0.2, 0.0, 0.8, 0.6, 1.0, 0.2, 0.4, 1.0, 0.8, 1.0, 0.2, 0.4, 0.0, 0.6, 0.0, 0.6, 0.0, 0.2, 0.6, 0.4, 0.2, 0.2, 0.6, 1.0, 0.8, 0.8, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.4, 1.0, 1.0, 1.0, 1.0, 0.6, 0.8, 0.0, 1.0, 0.2, 1.0, 1.0, 0.2, 1.0, 0.8, 1.0, 0.4, 0.6, 0.8, 0.0, 0.0, 0.6, 0.2, 0.4, 1.0, 0.6, 0.8, 0.4, 0.4, 1.0, 1.0, 1.0, 1.0, 0.0, 0.4, 0.0, 0.4, 1.0, 0.8, 1.0, 0.4, 0.8, 0.0, 1.0, 0.8, 0.4, 0.6, 0.8, 1.0, 0.2, 0.0, 1.0, 1.0, 1.0, 0.6, 0.8, 0.4, 1.0, 0.4, 0.4, 1.0, 0.6, 0.4, 0.8, 0.4, 1.0, 0.0, 0.6, 0.2, 1.0, 0.6, 0.6, 0.4, 0.0, 0.2, 0.6, 1.0, 1.0, 0.8, 0.2, 0.8, 0.0, 0.6, 0.8, 0.0, 0.8, 0.8, 0.8, 0.6, 0.8, 0.8, 0.6, 1.0, 0.2, 0.0, 0.0, 0.6, 0.8, 0.0, 0.4, 0.8, 0.2, 0.2, 0.6, 0.8, 1.0, 0.0, 0.4, 0.4, 0.0, 0.2, 0.0, 0.2, 1.0, 0.6, 1.0, 0.8, 1.0, 0.8, 0.2, 1.0, 0.8, 0.8, 0.4, 0.2, 0.0, 1.0, 0.6, 0.8, 0.6, 1.0, 1.0, 0.2, 0.8, 0.0, 0.4, 0.2, 1.0, 0.4, 0.2, 0.0, 0.6, 1.0, 0.4, 0.2, 1.0, 0.8, 1.0, 0.0, 1.0, 1.0, 1.0, 0.6, 0.0, 1.0, 1.0, 0.8, 0.8, 0.6, 1.0, 0.0, 1.0, 0.8, 0.0, 1.0, 1.0, 0.2, 0.4, 0.4, 0.4, 0.8, 0.2, 0.2, 0.6, 0.6, 0.4, 1.0, 0.8, 1.0, 0.2, 1.0, 0.6, 1.0, 1.0, 1.0, 0.8, 0.2, 1.0, 1.0, 0.6, 0.8, 0.0, 1.0, 1.0, 1.0, 0.6, 0.6, 0.6, 0.4, 1.0, 1.0, 0.4, 0.8, 0.0, 1.0, 0.6, 0.2, 1.0, 1.0, 0.4, 1.0, 0.0, 0.8, 1.0, 1.0, 0.4, 0.2, 0.6, 0.8, 0.2, 1.0, 0.6, 0.6, 1.0, 0.4, 0.8, 1.0, 0.0, 0.8, 0.2, 0.8, 0.4, 0.2, 1.0, 0.8, 1.0, 0.6, 0.4, 0.8, 1.0, 0.2, 0.2, 1.0, 0.2, 1.0, 0.6, 0.0, 0.8, 0.8, 1.0, 1.0, 0.8, 0.0, 0.2, 0.4, 1.0, 0.0, 1.0, 1.0, 0.8, 1.0, 1.0, 0.4, 1.0, 0.2, 1.0, 0.8, 0.0, 1.0, 1.0, 0.2, 0.6, 0.0, 1.0, 0.4, 1.0, 0.4, 0.2, 0.0, 0.2, 1.0, 0.2, 0.8, 0.2, 0.0, 0.2, 0.8, 1.0, 0.4, 1.0, 0.0, 0.2, 0.6, 0.8, 0.6, 0.0, 0.0, 0.0, 0.2, 0.8, 0.8, 0.4, 0.0, 0.2, 0.2, 0.2, 0.4, 0.4, 1.0, 0.6, 0.0, 0.2, 1.0, 1.0, 1.0, 0.2, 0.2, 1.0, 0.0, 0.8, 0.4, 0.0, 0.2, 0.0, 0.4, 0.2, 0.0, 0.2, 0.0, 0.8, 1.0, 0.2, 0.4, 0.6, 0.0, 0.4, 0.0, 0.0, 0.6, 0.2, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.2, 0.8, 0.0, 1.0, 1.0, 0.2, 0.2, 1.0, 0.6, 1.0, 0.4, 0.2, 0.2, 0.8, 0.4, 1.0, 1.0, 0.0, 0.4, 0.6, 0.0, 0.0, 1.0, 0.8, 0.8, 0.4, 0.6, 1.0, 1.0, 0.6, 0.2, 0.2, 1.0, 0.2, 0.8, 0.4, 0.4, 0.4, 1.0, 1.0, 0.8, 0.8, 1.0, 1.0, 0.6, 0.4, 0.2, 0.2, 0.0, 0.0, 0.2, 0.0, 0.2, 0.6, 0.2, 1.0, 0.6, 1.0, 0.4, 1.0, 1.0, 1.0, 0.6, 0.2, 1.0, 0.6, 0.8, 0.8, 1.0, 0.8, 0.0, 0.0, 0.6, 0.2, 1.0, 1.0, 1.0, 0.4, 0.6, 0.8, 1.0, 0.6, 1.0, 1.0, 0.2, 0.0, 1.0, 0.2, 0.2, 0.6, 0.4, 1.0, 0.6, 0.2, 0.2, 0.2, 0.0, 0.6, 1.0, 0.0, 1.0, 0.8, 0.2, 0.8, 0.8, 0.0, 0.0, 0.4, 0.0, 0.6, 1.0, 1.0, 0.4, 1.0, 0.8, 0.4, 0.6, 1.0, 0.4, 0.0, 0.6, 1.0, 1.0, 1.0, 0.8, 0.8, 1.0, 0.2, 0.2, 0.0, 1.0, 0.4, 0.4, 0.0, 0.8, 0.4, 0.4, 1.0, 0.2, 0.4, 0.6, 0.4, 1.0, 0.4, 0.4, 0.8, 0.0, 0.6, 0.2, 1.0, 0.8, 1.0, 0.2, 0.0, 1.0, 0.4, 0.6, 1.0, 0.8, 0.8, 0.0, 0.6, 0.2, 0.0, 0.2, 0.0, 0.2, 0.2, 0.0, 0.0, 0.4, 0.6, 0.4, 0.0, 0.2, 0.2, 0.8, 0.6, 0.2, 0.6, 0.0, 0.6, 0.8, 0.2, 0.6, 0.2, 0.6, 0.2, 0.8, 0.2, 0.6, 0.2, 0.2, 0.6, 1.0, 0.6, 0.2, 0.0, 0.2, 1.0, 0.4, 0.8, 0.4, 0.0, 0.2, 0.0, 0.0, 0.2, 0.6, 0.0, 0.8, 0.0, 0.0, 0.6, 0.2, 0.2, 0.8, 0.0, 0.2, 0.0, 0.2, 0.2, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.8, 0.6, 0.6, 0.4, 0.6, 1.0, 0.6, 0.8, 0.4, 0.0, 0.2, 0.2, 1.0, 0.2, 0.0, 1.0, 0.4, 0.4, 0.0, 0.2, 0.4, 0.0, 0.2, 0.2, 0.2, 0.6, 0.0, 0.0, 0.0, 0.4, 0.0, 0.0, 0.8, 0.6, 0.2, 1.0, 0.6, 0.2, 0.4, 0.4, 1.0, 0.0, 0.0, 0.2, 0.4, 0.0, 0.2, 0.8, 0.0, 0.8, 0.2, 0.2, 0.2, 0.8, 0.2, 0.0, 0.2, 0.2, 0.0, 0.2, 0.6, 0.2, 0.2, 0.8, 1.0, 0.0, 0.0, 0.6, 0.8, 0.4, 0.6, 0.8, 0.0, 0.4, 0.2, 0.4, 0.0, 0.6, 0.8, 0.6, 0.0, 0.2, 0.4, 1.0, 0.8, 0.0, 0.0, 0.0, 0.6, 1.0, 0.4, 0.4, 1.0, 0.4, 0.6, 0.0, 0.2, 1.0, 0.0, 0.8, 0.4, 0.6, 0.2, 1.0, 0.2, 0.8, 0.2, 1.0, 0.0, 0.2, 0.4, 0.2, 0.4, 0.0, 0.6, 0.2, 0.2, 0.2, 0.4, 0.0, 0.0, 0.0, 1.0, 0.2, 1.0, 0.2, 0.4, 0.2, 0.2, 0.6, 0.4, 0.0, 0.2, 0.2, 0.2, 0.0, 0.4, 0.2, 0.8, 0.0, 0.6, 0.0, 1.0, 0.2, 0.2, 0.0, 0.2, 0.0, 0.0, 0.0, 0.2, 0.2, 0.2, 0.2, 0.6, 0.4, 0.0, 0.2, 0.6, 0.0, 0.0, 0.2, 0.6, 0.2, 0.2, 0.0, 0.2, 0.8, 0.8, 0.4, 0.0, 0.0, 0.2, 0.4, 1.0, 0.6, 0.8, 0.4, 0.4, 0.0, 0.2, 0.0, 0.8, 0.0, 0.4, 0.4, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.8, 0.0, 1.0, 0.2, 0.2, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.4, 0.0, 0.2, 0.4, 0.4, 0.0, 1.0, 0.2, 0.4, 0.0, 0.0, 0.0, 0.0, 0.0, 0.4, 0.0, 0.0, 0.8, 0.0, 0.8, 0.2, 0.4, 1.0, 0.4, 0.0, 0.2, 0.2, 0.0, 0.0, 0.0, 0.6, 0.0, 1.0, 0.0, 0.0, 0.6, 0.0, 0.4, 0.6, 0.2, 0.2, 0.6, 0.4, 0.8, 1.0, 0.0, 0.4, 0.4, 0.6, 0.2, 0.6, 0.2, 1.0, 0.2, 0.0, 0.4, 0.6, 0.0, 0.2, 0.0, 0.0, 0.8, 0.2, 0.4, 0.4, 0.4, 0.4, 1.0, 0.2, 0.8, 1.0, 0.2, 0.4, 0.2, 0.2, 0.0, 0.0, 0.2, 0.0, 0.6, 0.0, 0.0, 0.4, 0.2, 0.2, 0.2, 0.0, 0.4, 0.0, 0.8, 0.4, 0.0, 0.6, 0.2, 0.0, 0.4, 0.0, 1.0, 0.0, 0.4, 0.0, 0.2, 0.0, 0.2, 0.4, 0.0, 0.2, 1.0, 0.4, 0.4, 0.6, 0.4, 0.2, 0.2, 0.8, 0.0, 0.2, 0.4, 0.4, 0.6, 0.0, 0.8, 0.0, 0.4, 0.4, 0.4, 0.2, 0.2, 0.0, 0.6, 0.0, 0.2, 1.0, 0.2, 1.0, 0.4, 1.0, 0.0, 0.2, 0.0, 0.0, 0.2, 0.4, 0.2, 0.0, 0.2, 0.0, 0.0, 0.0, 0.0, 0.2, 0.2, 0.2, 0.0, 0.8, 0.6, 0.2, 0.8, 0.0, 1.0, 0.2, 0.0, 1.0, 0.0, 0.0, 0.0, 0.6, 0.8, 0.0, 0.6, 0.4, 0.0, 0.4, 0.0, 0.0, 0.0, 0.0, 0.4, 0.6, 0.8, 0.0, 0.4, 0.2, 0.4, 0.0, 0.4, 0.2, 0.0, 0.6, 0.4, 0.2, 0.6, 0.8, 0.8, 0.8, 0.0, 0.8, 0.0, 0.8, 0.6, 0.6, 0.2, 0.4, 0.0, 0.2, 0.4, 0.2, 0.0, 0.0, 1.0, 0.2, 0.2, 1.0, 0.8, 0.6, 0.2, 0.4, 0.0, 0.2, 0.0, 0.0, 0.2, 0.0, 1.0, 1.0, 0.0, 0.2, 0.8, 0.0, 0.6, 0.2, 0.2, 0.2, 0.0, 0.4, 0.6, 0.8, 0.4, 0.4, 0.0, 0.4, 0.0, 0.6, 0.6, 0.4, 0.0, 0.2, 0.0, 0.0, 0.2, 0.0, 0.2, 0.2, 0.6, 0.0, 0.4, 0.2, 0.4, 0.2, 0.8, 0.2, 1.0, 0.8, 0.6, 0.4, 1.0, 0.0, 0.4, 0.4, 0.2, 0.0, 0.4, 0.8, 0.2, 0.4, 0.2, 0.0, 0.0, 0.0, 0.4, 0.0, 0.2, 0.4, 0.6, 0.2, 1.0, 0.2, 0.4, 0.0, 0.0, 0.2, 0.0, 0.6, 0.2, 0.2, 0.2, 0.0, 0.4, 0.0, 0.4, 1.0, 0.4, 0.2, 0.0, 0.4, 0.4, 1.0, 0.2, 0.8, 1.0, 0.6, 0.4, 0.6, 0.2, 0.0, 0.2, 0.6, 0.2, 0.0, 0.4, 0.8, 0.6, 0.4, 0.0, 0.2, 0.0, 1.0, 1.0, 0.8, 0.2, 0.4, 0.0, 0.6, 0.0, 0.6, 0.0, 0.8, 0.0, 0.0, 1.0, 0.0, 0.4, 0.4, 0.6, 0.4, 0.2, 0.2, 0.4, 0.2, 1.0, 0.2, 0.0, 0.4, 1.0, 0.4, 0.0, 0.6, 0.0, 0.2, 0.0, 0.6, 0.6, 0.0, 0.2, 0.2, 1.0, 0.2, 0.2, 0.2, 0.8, 0.8, 0.8, 0.2, 0.0, 0.4, 0.2, 1.0, 0.8, 0.2, 0.8, 0.2, 0.4, 0.6, 0.6, 1.0, 0.0, 0.2, 0.2, 1.0, 0.0, 0.2, 0.0, 0.4, 0.0, 0.4, 1.0, 0.0, 0.8, 0.2, 0.2, 0.2, 0.4, 0.0, 0.4, 0.2, 0.6, 0.2, 0.4, 1.0, 0.4, 0.4, 0.2, 0.0, 0.4, 0.0, 0.4, 0.0, 0.2, 0.6, 0.2, 0.4, 0.2, 0.8, 0.8, 1.0, 0.4, 0.2, 0.0, 0.0, 0.8, 1.0, 0.4, 0.2, 0.0, 0.0, 0.0, 0.0, 0.2, 0.0, 0.0, 0.2, 0.2, 0.2, 0.0, 0.2, 0.2, 0.2, 0.2, 0.0, 0.0, 0.2, 0.4, 0.4, 0.0, 1.0, 0.4, 0.0, 0.4, 0.4, 0.0, 0.2, 0.2, 0.8, 0.0, 0.2, 0.0, 0.0, 0.0, 0.2, 0.0, 0.0, 0.0, 0.6, 0.0, 0.6, 0.0, 0.0, 0.4, 0.6, 0.4, 0.0, 1.0, 0.6, 0.2, 0.0, 0.2, 0.0, 0.0, 0.0, 1.0, 0.2, 0.0, 0.0, 0.6, 0.0, 0.6, 0.0, 0.6, 0.0, 0.0, 0.0, 0.0, 0.4, 0.0, 0.0, 0.2, 0.2, 0.2, 1.0, 0.0, 0.2, 0.6, 0.4, 0.2, 0.8, 0.0, 0.0, 0.2, 0.4, 0.6, 0.8, 1.0, 0.0, 0.2, 0.4, 0.4, 0.6, 0.0, 0.0, 0.2, 0.2, 0.2, 1.0, 0.0, 0.2, 0.0, 0.6, 0.2, 0.0, 0.2, 0.2, 0.4, 0.6, 0.8, 0.8, 0.2, 0.6, 0.0, 0.4, 0.2, 0.6, 0.4, 0.6, 0.4, 0.8, 0.6, 0.4, 0.0, 0.2, 1.0, 0.4, 0.2, 0.4, 0.4, 0.0, 0.2, 0.4]</t>
+          <t>[0.2, 1.0, 0.2, 1.0, 0.4, 1.0, 0.4, 1.0, 0.8, 0.4, 0.4, 1.0, 1.0, 0.8, 0.8, 0.4, 0.4, 0.8, 0.6, 0.8, 1.0, 0.0, 0.4, 0.0, 0.4, 0.4, 0.4, 1.0, 1.0, 0.2, 0.0, 0.8, 0.6, 1.0, 0.6, 0.8, 1.0, 0.0, 1.0, 0.8, 1.0, 1.0, 1.0, 0.2, 0.8, 0.8, 1.0, 1.0, 0.4, 0.4, 1.0, 0.4, 1.0, 0.4, 1.0, 0.2, 0.0, 0.8, 1.0, 0.8, 1.0, 0.4, 0.8, 0.6, 1.0, 1.0, 0.4, 0.0, 0.6, 0.8, 0.6, 1.0, 1.0, 0.4, 1.0, 0.8, 1.0, 1.0, 0.6, 1.0, 0.6, 1.0, 0.2, 0.4, 1.0, 0.2, 0.2, 1.0, 1.0, 1.0, 1.0, 0.6, 0.8, 1.0, 1.0, 0.8, 1.0, 0.4, 0.8, 0.4, 1.0, 0.0, 0.8, 0.2, 0.4, 0.2, 0.6, 0.0, 0.2, 0.8, 0.0, 1.0, 0.8, 0.8, 0.6, 1.0, 0.4, 0.0, 0.4, 0.6, 1.0, 0.4, 0.8, 0.8, 1.0, 1.0, 0.6, 0.4, 0.6, 0.4, 0.0, 0.4, 0.2, 1.0, 0.6, 0.4, 1.0, 1.0, 1.0, 0.8, 1.0, 1.0, 1.0, 0.6, 1.0, 0.2, 0.4, 1.0, 1.0, 0.6, 0.6, 0.2, 0.8, 1.0, 0.6, 0.6, 0.2, 1.0, 0.8, 0.2, 0.8, 0.6, 0.4, 0.6, 0.6, 0.8, 0.2, 0.8, 0.4, 1.0, 0.2, 0.8, 0.2, 0.0, 0.4, 1.0, 0.4, 0.2, 1.0, 0.2, 1.0, 0.8, 0.6, 0.8, 1.0, 0.0, 1.0, 1.0, 0.0, 0.8, 0.4, 1.0, 0.2, 0.0, 0.8, 0.6, 1.0, 0.4, 0.2, 1.0, 0.2, 1.0, 0.8, 0.0, 0.4, 0.2, 0.0, 0.4, 0.6, 1.0, 0.2, 0.6, 0.6, 0.2, 1.0, 1.0, 1.0, 1.0, 0.2, 1.0, 1.0, 0.0, 1.0, 0.8, 0.0, 0.6, 0.4, 0.4, 0.2, 0.0, 0.6, 0.0, 1.0, 0.8, 0.2, 0.4, 0.4, 0.6, 0.0, 0.0, 0.6, 0.0, 0.0, 0.4, 0.6, 0.8, 1.0, 1.0, 0.6, 0.6, 0.4, 1.0, 0.4, 0.0, 0.8, 0.6, 0.4, 0.4, 1.0, 0.8, 0.4, 0.4, 1.0, 0.4, 0.2, 0.0, 0.4, 0.4, 0.4, 0.4, 0.2, 0.2, 1.0, 1.0, 1.0, 0.4, 0.0, 1.0, 0.4, 1.0, 0.2, 0.0, 0.8, 0.0, 0.6, 1.0, 0.0, 1.0, 0.6, 1.0, 0.8, 0.0, 0.0, 1.0, 1.0, 0.0, 0.8, 0.6, 0.0, 0.6, 0.2, 0.0, 0.8, 0.2, 0.2, 1.0, 0.6, 0.4, 0.4, 1.0, 0.4, 0.4, 0.0, 1.0, 0.2, 1.0, 0.0, 0.6, 0.2, 0.6, 0.2, 0.4, 1.0, 1.0, 0.0, 0.2, 0.0, 0.8, 0.6, 0.8, 0.4, 0.8, 1.0, 0.4, 0.4, 0.2, 0.4, 0.2, 1.0, 0.4, 0.2, 0.6, 0.6, 1.0, 0.8, 0.6, 0.6, 1.0, 0.0, 1.0, 0.6, 0.2, 0.0, 0.4, 1.0, 0.0, 0.6, 0.0, 0.2, 1.0, 0.2, 0.0, 0.4, 0.8, 0.8, 0.8, 0.4, 0.6, 0.6, 0.2, 0.6, 0.8, 1.0, 0.0, 0.6, 0.2, 0.6, 1.0, 0.4, 0.2, 1.0, 0.8, 1.0, 0.8, 1.0, 1.0, 0.2, 0.8, 1.0, 0.6, 0.2, 1.0, 1.0, 1.0, 1.0, 0.6, 1.0, 0.8, 1.0, 1.0, 0.2, 0.8, 1.0, 0.2, 1.0, 0.2, 0.0, 0.0, 0.6, 0.0, 1.0, 0.4, 1.0, 0.4, 0.2, 0.8, 0.2, 0.2, 0.2, 0.4, 0.6, 0.4, 1.0, 0.2, 0.0, 0.4, 0.4, 0.0, 0.0, 0.0, 0.8, 0.0, 0.6, 0.0, 0.6, 0.6, 0.0, 0.2, 0.4, 0.2, 1.0, 0.0, 1.0, 0.8, 1.0, 1.0, 1.0, 0.4, 0.0, 0.8, 0.0, 0.0, 0.4, 1.0, 0.2, 0.2, 0.8, 0.0, 0.0, 1.0, 1.0, 0.0, 0.6, 1.0, 0.0, 0.4, 0.8, 0.4, 0.4, 0.8, 1.0, 0.6, 0.4, 1.0, 0.6, 0.2, 0.8, 0.2, 0.6, 0.6, 0.6, 0.4, 0.2, 0.4, 0.8, 0.6, 0.0, 1.0, 0.4, 0.2, 1.0, 0.6, 0.4, 0.4, 0.4, 1.0, 0.4, 1.0, 0.0, 1.0, 0.0, 0.8, 0.6, 0.8, 0.0, 0.2, 0.2, 0.6, 0.2, 0.6, 0.8, 0.2, 1.0, 0.4, 0.4, 0.6, 0.2, 0.0, 0.2, 1.0, 1.0, 1.0, 0.6, 0.0, 0.6, 0.8, 1.0, 0.6, 0.6, 0.8, 0.2, 0.2, 0.6, 0.2, 0.8, 0.0, 0.4, 1.0, 1.0, 0.2, 0.2, 0.4, 0.4, 0.0, 0.0, 0.4, 0.4, 0.8, 0.0, 0.6, 0.8, 0.6, 0.4, 0.4, 1.0, 1.0, 1.0, 0.6, 0.4, 1.0, 0.4, 0.2, 1.0, 0.4, 0.6, 0.2, 1.0, 0.4, 0.6, 0.4, 0.8, 0.6, 0.4, 0.8, 0.4, 0.8, 1.0, 0.4, 0.8, 1.0, 1.0, 0.2, 0.6, 1.0, 1.0, 1.0, 0.8, 1.0, 0.4, 1.0, 1.0, 0.0, 0.4, 0.0, 0.6, 0.4, 0.6, 0.2, 0.6, 0.2, 0.6, 0.0, 0.0, 1.0, 1.0, 0.8, 1.0, 0.4, 0.8, 0.4, 0.6, 0.2, 0.8, 0.0, 0.4, 0.2, 0.4, 1.0, 0.2, 1.0, 0.8, 1.0, 0.4, 1.0, 0.6, 1.0, 1.0, 0.6, 0.8, 0.6, 0.8, 0.6, 0.4, 0.4, 0.2, 1.0, 1.0, 1.0, 0.2, 1.0, 0.0, 0.2, 1.0, 0.0, 1.0, 0.6, 0.6, 0.2, 0.4, 0.0, 0.4, 1.0, 0.0, 0.6, 0.6, 0.2, 0.0, 0.8, 1.0, 1.0, 0.4, 0.2, 0.8, 0.8, 1.0, 1.0, 1.0, 0.8, 1.0, 0.2, 0.2, 0.6, 0.8, 1.0, 1.0, 1.0, 1.0, 0.6, 1.0, 1.0, 1.0, 0.4, 1.0, 1.0, 0.4, 1.0, 0.2, 0.6, 0.4, 0.8, 1.0, 0.6, 1.0, 0.6, 0.6, 0.6, 0.0, 0.8, 0.8, 1.0, 0.0, 0.8, 0.6, 0.6, 0.8, 1.0, 0.0, 1.0, 0.2, 0.6, 0.6, 0.0, 0.2, 0.0, 1.0, 0.8, 0.4, 1.0, 1.0, 0.0, 0.6, 0.2, 0.8, 0.6, 0.8, 0.2, 0.6, 1.0, 0.2, 0.8, 0.4, 0.2, 0.6, 0.2, 1.0, 0.2, 1.0, 0.2, 0.2, 0.0, 0.6, 0.4, 0.2, 0.2, 0.2, 1.0, 0.2, 0.6, 0.4, 0.8, 0.2, 0.4, 0.0, 0.6, 0.8, 0.8, 0.6, 0.4, 0.0, 1.0, 0.4, 0.4, 1.0, 0.6, 0.8, 0.4, 0.6, 1.0, 1.0, 0.6, 0.0, 0.8, 0.8, 1.0, 0.8, 0.6, 0.2, 0.4, 0.2, 0.4, 0.0, 1.0, 0.2, 0.4, 0.6, 1.0, 1.0, 0.8, 1.0, 0.6, 1.0, 0.8, 1.0, 1.0, 0.6, 0.8, 0.6, 1.0, 1.0, 1.0, 1.0, 0.6, 0.2, 0.8, 1.0, 0.2, 1.0, 0.8, 0.6, 1.0, 0.6, 1.0, 1.0, 0.0, 0.8, 1.0, 0.0, 0.6, 1.0, 1.0, 0.2, 0.0, 0.8, 0.4, 0.4, 0.4, 0.4, 0.2, 0.4, 0.0, 1.0, 0.4, 0.8, 0.0, 1.0, 0.8, 0.4, 0.8, 1.0, 0.8, 0.2, 0.6, 0.4, 0.8, 0.6, 1.0, 0.6, 1.0, 1.0, 0.6, 1.0, 0.8, 1.0, 0.0, 0.4, 0.8, 1.0, 0.4, 0.4, 0.4, 1.0, 0.2, 1.0, 1.0, 0.6, 0.4, 0.8, 0.8, 0.6, 0.0, 0.8, 0.8, 1.0, 0.2, 0.0, 1.0, 0.6, 1.0, 0.2, 0.2, 0.2, 0.2, 0.0, 0.4, 0.0, 0.0, 0.6, 0.4, 0.2, 0.0, 0.6, 1.0, 0.8, 0.6, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.8, 1.0, 1.0, 1.0, 1.0, 0.6, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.2, 0.4, 1.0, 1.0, 0.8, 0.6, 0.4, 0.0, 0.2, 0.8, 0.0, 0.4, 1.0, 0.4, 0.4, 0.4, 0.4, 1.0, 1.0, 1.0, 0.6, 0.4, 0.2, 0.0, 0.4, 1.0, 0.2, 1.0, 0.4, 0.4, 0.0, 1.0, 0.8, 0.2, 0.4, 0.6, 1.0, 0.2, 0.0, 0.8, 1.0, 1.0, 0.4, 1.0, 0.4, 1.0, 0.4, 0.4, 1.0, 0.6, 0.2, 0.4, 0.4, 1.0, 0.2, 0.4, 0.2, 0.8, 0.8, 1.0, 0.2, 0.0, 0.0, 0.0, 1.0, 1.0, 0.8, 0.8, 0.8, 0.0, 1.0, 0.8, 0.0, 0.4, 0.4, 0.8, 0.8, 0.4, 0.8, 0.4, 1.0, 0.2, 0.0, 0.0, 0.8, 0.6, 0.0, 0.6, 0.8, 0.2, 0.2, 0.8, 1.0, 1.0, 0.0, 0.4, 0.4, 0.0, 0.2, 0.2, 0.2, 0.8, 0.6, 1.0, 1.0, 0.8, 0.4, 0.2, 0.8, 0.6, 1.0, 0.4, 0.0, 0.2, 1.0, 1.0, 0.4, 0.4, 1.0, 1.0, 0.0, 0.8, 0.0, 0.2, 0.6, 0.8, 0.4, 0.4, 0.0, 0.6, 1.0, 0.6, 0.2, 1.0, 0.8, 1.0, 0.0, 1.0, 1.0, 0.8, 0.4, 0.0, 1.0, 1.0, 1.0, 0.8, 0.6, 0.8, 0.0, 1.0, 0.8, 0.0, 1.0, 0.4, 0.2, 0.0, 0.0, 0.8, 0.8, 0.6, 0.4, 0.8, 0.4, 0.4, 0.8, 0.4, 1.0, 0.4, 0.6, 0.6, 0.8, 1.0, 0.8, 0.6, 0.2, 0.4, 1.0, 0.8, 1.0, 0.0, 0.8, 1.0, 0.6, 0.4, 0.6, 0.6, 0.6, 1.0, 1.0, 0.6, 0.8, 0.0, 1.0, 0.8, 0.2, 1.0, 1.0, 0.4, 0.8, 0.0, 0.8, 1.0, 0.4, 0.8, 0.2, 0.6, 0.6, 0.4, 0.8, 0.6, 0.4, 0.8, 0.2, 1.0, 1.0, 0.0, 0.8, 0.4, 0.6, 0.4, 0.2, 1.0, 0.8, 1.0, 0.6, 0.6, 0.8, 1.0, 0.2, 0.2, 1.0, 0.2, 1.0, 0.4, 0.2, 0.8, 0.4, 0.8, 0.8, 1.0, 0.0, 0.2, 0.4, 1.0, 0.0, 1.0, 1.0, 0.8, 1.0, 0.6, 0.4, 0.8, 0.2, 1.0, 1.0, 0.0, 0.6, 0.8, 0.4, 0.6, 0.0, 0.8, 0.6, 0.8, 0.4, 0.2, 0.0, 0.2, 0.6, 0.4, 0.8, 0.2, 0.0, 0.2, 0.8, 0.8, 0.4, 1.0, 0.0, 0.4, 0.6, 0.4, 0.6, 0.0, 0.0, 0.0, 0.0, 0.8, 1.0, 0.0, 0.0, 0.6, 0.2, 0.4, 0.2, 0.6, 1.0, 0.0, 0.0, 0.4, 1.0, 1.0, 1.0, 0.4, 0.2, 1.0, 0.0, 0.6, 0.4, 0.0, 0.0, 0.0, 0.4, 0.0, 0.2, 0.2, 0.2, 0.2, 1.0, 0.0, 0.2, 0.6, 0.0, 0.4, 0.0, 0.0, 0.4, 0.2, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.6, 0.2, 0.0, 0.6, 0.6, 0.2, 0.4, 0.6, 0.6, 1.0, 0.8, 0.0, 0.4, 0.6, 0.4, 1.0, 1.0, 0.4, 0.4, 0.6, 0.2, 0.2, 1.0, 0.4, 0.4, 0.2, 1.0, 0.8, 0.8, 0.2, 0.6, 0.2, 1.0, 0.0, 0.6, 0.4, 0.6, 0.8, 0.8, 0.8, 0.8, 0.8, 1.0, 1.0, 0.2, 0.0, 0.0, 0.2, 0.0, 0.0, 0.0, 0.0, 0.4, 0.8, 0.4, 0.4, 0.4, 1.0, 0.6, 1.0, 0.8, 0.8, 0.4, 0.4, 0.8, 1.0, 0.8, 0.2, 1.0, 0.8, 0.0, 0.0, 0.2, 0.0, 1.0, 1.0, 1.0, 0.2, 0.4, 1.0, 0.8, 0.6, 1.0, 1.0, 0.2, 0.2, 1.0, 0.2, 0.2, 0.4, 0.4, 1.0, 0.8, 0.4, 0.4, 0.2, 0.0, 0.6, 1.0, 0.0, 1.0, 0.8, 0.0, 0.4, 0.0, 0.2, 0.0, 0.4, 0.2, 0.8, 1.0, 1.0, 0.4, 0.6, 0.4, 0.4, 0.4, 1.0, 0.8, 0.0, 0.4, 1.0, 1.0, 1.0, 0.6, 0.4, 1.0, 0.4, 0.2, 0.0, 0.8, 0.8, 0.4, 0.0, 1.0, 0.4, 0.4, 1.0, 0.2, 0.4, 1.0, 0.8, 1.0, 0.8, 0.4, 0.8, 0.0, 0.6, 0.2, 1.0, 0.6, 1.0, 0.4, 0.0, 1.0, 0.6, 0.4, 1.0, 0.8, 0.8, 0.0, 1.0, 0.0, 0.4, 0.2, 0.4, 0.0, 0.4, 0.2, 0.4, 0.8, 0.6, 0.2, 0.8, 0.2, 0.0, 0.2, 0.0, 0.4, 0.8, 0.0, 0.0, 0.0, 0.2, 0.6, 0.2, 0.4, 0.0, 0.6, 0.4, 0.4, 0.0, 0.0, 0.0, 0.2, 0.2, 0.2, 0.4, 0.2, 0.0, 0.0, 1.0, 1.0, 1.0, 0.2, 0.4, 0.2, 0.0, 0.2, 0.6, 0.6, 0.0, 0.0, 0.2, 0.2, 1.0, 0.2, 0.2, 0.0, 0.0, 0.6, 0.2, 0.4, 0.4, 0.6, 0.2, 0.2, 0.0, 0.0, 0.0, 0.0, 0.0, 0.2, 0.8, 0.2, 0.2, 0.2, 0.2, 1.0, 0.2, 0.0, 0.0, 0.2, 0.4, 0.0, 0.6, 0.2, 0.8, 0.4, 0.0, 0.4, 0.0, 0.6, 0.2, 0.4, 0.0, 0.8, 0.2, 0.4, 0.8, 0.0, 0.4, 0.4, 0.8, 0.4, 0.4, 0.6, 0.0, 0.8, 0.0, 0.6, 0.2, 0.0, 0.0, 0.4, 0.2, 0.4, 0.0, 0.0, 1.0, 0.2, 0.0, 0.2, 0.2, 0.6, 0.0, 0.4, 0.0, 0.6, 0.0, 0.0, 0.0, 0.6, 0.6, 0.2, 0.0, 0.8, 0.0, 0.2, 0.0, 0.8, 0.8, 0.0, 0.4, 0.2, 0.0, 0.4, 0.8, 0.4, 0.4, 0.4, 0.0, 0.4, 0.0, 0.4, 0.4, 0.0, 0.2, 0.4, 0.4, 0.0, 0.2, 1.0, 0.0, 0.6, 0.0, 0.0, 0.0, 0.6, 0.2, 0.0, 0.4, 0.4, 0.2, 0.2, 0.2, 0.0, 0.0, 0.4, 0.0, 0.0, 0.2, 0.8, 0.2, 0.2, 0.6, 0.4, 0.2, 0.2, 0.0, 0.0, 0.0, 0.4, 0.0, 1.0, 0.0, 0.0, 1.0, 0.4, 0.0, 0.0, 0.2, 0.2, 0.0, 0.4, 0.2, 0.8, 0.8, 0.2, 0.4, 1.0, 0.8, 0.2, 0.8, 0.2, 0.2, 0.2, 0.2, 0.0, 0.2, 0.2, 0.0, 0.0, 1.0, 0.8, 0.6, 0.8, 0.0, 0.0, 0.6, 0.2, 0.0, 0.0, 0.0, 0.2, 0.0, 0.4, 1.0, 0.2, 0.0, 0.2, 0.0, 0.8, 0.0, 0.2, 0.6, 0.0, 0.2, 0.2, 0.0, 0.0, 0.4, 0.2, 0.0, 0.6, 0.2, 0.0, 0.6, 0.6, 0.0, 0.2, 0.0, 0.0, 0.0, 0.2, 0.2, 0.2, 0.4, 0.2, 0.4, 0.0, 0.8, 0.4, 0.0, 1.0, 0.4, 0.8, 0.0, 0.4, 0.6, 0.0, 0.6, 1.0, 0.6, 1.0, 0.0, 0.0, 0.6, 0.6, 0.8, 0.4, 1.0, 0.0, 0.2, 0.6, 0.2, 0.6, 0.8, 0.8, 0.0, 0.8, 0.0, 0.2, 0.2, 0.6, 0.2, 0.0, 0.4, 0.6, 0.6, 0.2, 0.2, 1.0, 0.4, 0.0, 0.6, 0.2, 0.4, 0.2, 1.0, 0.0, 0.0, 0.6, 1.0, 0.0, 0.2, 1.0, 0.2, 0.0, 0.2, 0.2, 0.0, 0.2, 0.0, 0.4, 0.2, 0.2, 0.0, 0.0, 0.4, 0.0, 0.0, 0.2, 0.2, 0.2, 0.8, 0.0, 1.0, 0.4, 0.0, 1.0, 0.6, 1.0, 0.2, 0.0, 0.6, 0.0, 0.2, 0.0, 0.6, 0.0, 0.6, 0.8, 0.8, 0.0, 0.4, 1.0, 0.4, 0.0, 0.2, 0.4, 0.0, 0.2, 0.8, 0.4, 1.0, 0.0, 0.2, 0.0, 0.2, 0.2, 0.0, 0.0, 0.2, 0.2, 0.0, 0.4, 0.2, 0.0, 0.4, 0.2, 0.2, 0.4, 0.2, 0.0, 0.0, 0.2, 0.4, 0.4, 0.0, 0.2, 0.8, 0.4, 0.2, 0.4, 0.2, 0.0, 0.2, 0.0, 0.6, 0.0, 0.0, 0.2, 0.2, 0.2, 1.0, 0.0, 0.4, 0.0, 0.0, 0.6, 0.2, 0.0, 0.4, 0.6, 1.0, 0.2, 0.4, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.4, 0.2, 0.2, 0.4, 0.0, 0.8, 0.0, 0.0, 0.2, 0.0, 0.2, 0.2, 0.0, 1.0, 0.0, 0.0, 0.4, 0.0, 0.0, 0.2, 0.0, 0.0, 1.0, 0.2, 0.2, 0.2, 0.4, 0.8, 0.0, 1.0, 0.0, 0.0, 0.4, 0.0, 0.0, 0.2, 0.2, 0.4, 0.0, 0.0, 0.4, 0.2, 0.2, 0.8, 0.2, 0.0, 0.2, 0.0, 0.2, 0.4, 0.8, 1.0, 0.2, 0.2, 0.8, 0.0, 0.0, 0.0, 0.6, 0.0, 0.4, 0.8, 0.6, 0.4, 0.6, 0.0, 0.6, 0.0, 0.6, 0.6, 0.4, 0.0, 1.0, 0.2, 0.2, 0.2, 0.0, 0.2, 1.0, 1.0, 0.4, 0.0, 0.2, 0.4, 0.0, 0.2, 0.4, 0.2, 0.8, 0.0, 0.4, 0.2, 0.0, 0.2, 0.8, 0.0, 0.4, 0.0, 0.0, 0.0, 0.8, 0.8, 1.0, 0.6, 0.0, 0.8, 0.4, 0.4, 0.4, 0.4, 0.4, 1.0, 0.0, 0.6, 0.4, 0.2, 0.8, 0.0, 0.6, 0.0, 0.2, 0.0, 0.0, 0.0, 0.8, 0.2, 0.4, 0.0, 0.6, 0.0, 0.4, 0.2, 0.4, 0.8, 0.2, 0.4, 0.0, 0.0, 1.0, 0.0, 0.4, 0.2, 0.0, 0.2, 0.0, 0.0, 0.4, 0.4, 0.4, 0.0, 0.2, 0.4, 0.2, 0.6, 0.2, 0.2, 0.4, 0.0, 0.2, 0.0, 0.8, 0.0, 0.6, 0.0, 0.4, 0.2, 0.4, 0.4, 0.0, 0.2, 0.2, 1.0, 0.2, 0.2, 0.0, 0.4, 0.4, 0.2, 0.4, 0.6, 0.8, 0.4, 0.2, 0.0, 0.2, 1.0, 0.6, 0.2, 0.0, 0.8, 0.2, 0.2, 0.0, 0.0, 0.0, 0.2, 0.0, 0.2, 0.2, 0.2, 0.2, 0.0, 0.4, 0.4, 0.2, 0.0, 0.2, 0.0, 1.0, 0.2, 0.6, 1.0, 0.0, 0.2, 0.6, 0.0, 0.4, 0.0, 0.2, 0.0, 0.0, 0.6, 0.6, 0.0, 0.8, 0.4, 0.0, 0.2, 0.0, 0.0, 0.2, 0.0, 0.2, 0.0, 0.0, 0.2, 1.0, 0.2, 0.2, 0.4, 0.4, 0.0, 0.4, 0.6, 0.2, 0.0, 0.0, 0.0, 0.2, 0.4, 0.8, 1.0, 0.2, 0.6, 0.4, 0.2, 0.2, 0.2, 0.0, 0.2, 0.0, 0.0, 0.2, 1.0, 0.2, 0.2, 0.0, 0.4, 0.0, 0.2, 0.0, 1.0, 0.0, 1.0, 0.0, 0.4, 0.0, 0.6, 0.4, 0.0, 0.8, 0.0, 1.0, 0.6, 0.2, 0.4, 0.0, 0.0, 0.2, 0.0, 0.4, 0.4, 0.8, 0.2, 0.2, 0.0, 0.2, 0.6, 0.4, 0.0, 0.2, 0.6, 0.4, 0.0, 0.2, 0.4, 0.2, 0.0, 1.0, 0.0, 1.0, 0.8, 0.4, 0.4, 0.4, 1.0, 0.0, 0.4, 0.0, 0.8, 0.4, 0.0, 0.2, 0.2, 0.2, 0.2, 0.0, 0.0, 0.6, 0.4, 0.0, 0.0, 0.4, 0.6, 0.2, 0.8, 0.2, 0.2, 1.0, 0.2, 0.0, 0.2, 0.2, 0.4, 0.8, 0.0, 0.8, 0.0, 0.0, 1.0, 0.2, 0.4, 0.0, 0.0, 0.0, 0.8, 0.6, 0.2, 0.0, 0.0, 0.2, 0.0, 0.4, 1.0, 1.0, 0.2, 0.2, 0.2, 0.6, 1.0, 0.0, 0.8, 0.4, 0.2, 0.4, 0.2, 1.0, 0.2, 0.0, 0.4, 0.2, 0.0, 0.6, 0.2, 0.0, 0.0, 0.4, 0.2, 0.2, 0.2, 0.0, 0.6, 0.0, 1.0, 0.0, 0.2, 0.4, 0.0, 0.4, 0.4, 0.0, 0.0, 0.2, 0.2, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
     </row>
@@ -855,44 +855,44 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>Random forest</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.868421052631579</v>
+        <v>0.862753036437247</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8521671826625387</v>
+        <v>0.8419847328244274</v>
       </c>
       <c r="E6" t="n">
-        <v>0.891497975708502</v>
+        <v>0.8931174089068826</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8453441295546559</v>
+        <v>0.8323886639676114</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8713889988128214</v>
+        <v>0.8667976424361492</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8684210526315789</v>
+        <v>0.8627530364372471</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8149466192170819</v>
+        <v>0.8171708185053381</v>
       </c>
       <c r="J6" t="n">
-        <v>0.7813990461049285</v>
+        <v>0.790073230268511</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8745551601423488</v>
+        <v>0.8638790035587188</v>
       </c>
       <c r="L6" t="n">
-        <v>0.755338078291815</v>
+        <v>0.7704626334519573</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8253568429890848</v>
+        <v>0.8253293667658308</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8684210526315789</v>
+        <v>0.8171708185053381</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>[1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+          <t>[1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -911,17 +911,17 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>[1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+          <t>[1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>[0.95, 0.13, 0.48, 0.75, 0.84, 0.94, 0.8, 0.25, 0.57, 0.89, 0.79, 0.67, 0.92, 0.49, 0.88, 0.41, 0.94, 0.84, 0.84, 0.51, 0.73, 0.75, 0.76, 0.41, 0.84, 0.24, 0.88, 0.9, 0.77, 0.61, 0.96, 0.56, 0.73, 0.92, 0.77, 0.99, 0.59, 0.62, 0.78, 0.79, 0.59, 0.68, 0.34, 0.62, 0.96, 0.38, 0.835, 0.79, 0.17, 0.73, 0.9, 0.93, 0.51, 0.7, 0.85, 0.43, 0.6, 0.84, 0.95, 0.87, 0.65, 0.83, 0.75, 0.58, 0.94, 0.39, 0.73, 0.83, 0.73, 0.66, 0.6, 0.72, 0.68, 0.945, 0.92, 0.75, 0.88, 0.8810714285714286, 0.83, 0.35, 0.76, 0.67, 0.8, 0.84, 0.81, 0.67, 0.77, 0.89, 0.58, 0.75, 0.9, 0.34, 0.65, 0.61, 0.51, 0.81, 0.59, 0.59, 0.94, 0.59, 0.72, 0.63, 0.73, 0.78, 0.47, 0.7925, 0.34, 0.91, 0.64, 0.66, 0.4, 0.1, 0.77, 0.855, 0.72, 0.75, 0.87, 0.58, 0.8, 0.69, 0.62, 0.71, 0.87, 0.76, 0.6, 0.63, 0.74, 0.77, 0.71, 0.44, 0.65, 0.76, 0.7, 0.68, 0.73, 0.9, 0.3, 0.9, 0.91, 0.82, 0.83, 0.94, 0.85, 0.45, 0.8, 0.8, 0.94, 0.61, 0.92, 0.57, 0.44, 0.94, 0.24, 0.82, 0.33, 0.89, 0.78, 0.39, 0.42, 0.62, 0.54, 0.54, 0.83, 0.81, 0.76, 0.67, 0.86, 0.94, 0.85, 0.67, 0.91, 0.73, 0.68, 0.8, 0.8025, 0.63, 0.64, 0.7025, 0.76, 0.72, 0.72, 0.56, 0.805, 0.86, 0.31, 0.44, 0.79, 0.85, 0.66, 0.83, 0.89, 0.76, 0.56, 0.8075, 0.53, 0.55, 0.885, 0.76, 0.86, 0.33, 0.795, 0.62, 0.78, 0.77, 0.75, 0.7, 0.81, 0.82, 0.3, 0.78, 0.73, 0.55, 0.73, 0.93, 0.89, 0.95, 0.8, 0.86, 0.89, 0.8, 0.64, 0.39, 0.65, 0.77, 0.616, 0.83, 0.39, 0.88, 0.64, 0.92, 0.89, 0.56, 0.9, 1.0, 0.61, 0.89, 0.51, 0.65, 0.73, 0.74, 0.6, 0.54, 0.4333333333333333, 0.96, 0.95, 0.64, 0.57, 0.8810714285714286, 0.35, 0.27, 0.85, 0.91, 0.97, 0.9, 0.91, 0.55, 0.86, 0.78, 0.59, 0.6, 0.55, 0.46, 0.84, 0.82, 0.63, 0.365, 0.84, 0.22, 0.76, 0.92, 0.73, 0.41, 0.4, 0.26, 0.78, 0.78, 0.7, 0.81, 0.94, 0.74, 0.41, 0.97, 0.91, 0.83, 0.81, 0.36, 0.89, 0.91, 0.63, 0.38, 0.8, 0.55, 0.93, 0.8635714285714287, 0.8275, 0.74, 0.84, 0.83, 0.66, 0.6, 0.31, 0.82, 0.29, 0.44, 0.61, 0.79, 0.75, 0.84, 0.58, 0.6, 0.41, 0.41, 0.57, 0.805, 0.83, 0.44, 0.29, 0.6, 0.79, 0.77, 0.89, 0.94, 0.98, 0.75, 0.89, 0.83, 0.95, 0.57, 0.58, 0.85, 0.63, 0.75, 0.78, 0.95, 0.56, 0.65, 0.97, 0.87, 0.85, 0.62, 0.55, 0.59, 0.62, 0.89, 0.87, 0.92, 0.77, 0.61, 0.55, 0.84, 0.57, 0.99, 0.85, 0.92, 0.91, 0.93, 0.98, 0.34, 0.69, 0.91, 0.59, 0.38, 0.63, 0.86, 0.9125, 0.51, 0.78, 0.77, 0.58, 0.63, 0.91, 0.96, 0.38, 0.93, 0.785, 0.71, 0.81, 0.6, 0.8820714285714285, 0.65, 0.87, 0.9075, 0.78, 0.29, 0.65, 0.96, 0.5, 0.5, 0.9060714285714286, 0.92, 0.98, 0.44, 0.74, 0.84, 0.59, 0.85, 0.69, 0.91, 0.52, 0.53, 0.49, 0.66, 0.58, 0.7, 0.72, 0.56, 0.93, 0.51, 0.9, 0.64, 0.67, 0.37, 0.62, 0.84, 0.97, 0.83, 0.49, 0.56, 0.96, 0.59, 0.41, 0.94, 0.87, 0.78, 0.44, 0.6, 0.63, 0.75, 0.26, 0.72, 0.69, 0.73, 0.75, 0.94, 0.87, 0.83, 0.87, 0.85, 0.59, 0.7, 0.9, 0.81, 0.5, 0.76, 0.77, 0.92, 0.84, 0.83, 0.86, 0.63, 0.94, 0.84, 0.4, 0.67, 0.9, 0.39, 0.97, 0.42, 0.69, 0.87, 0.86, 0.99, 0.8, 0.36, 0.88, 0.77, 0.33, 0.68, 0.53, 0.88, 0.856, 0.97, 0.72, 0.59, 0.33, 0.295, 0.6, 0.53, 0.9, 0.27, 0.77, 0.48, 0.93, 0.57, 0.49, 0.86, 0.8, 0.23, 0.94, 0.44, 0.514, 0.33, 0.42, 0.62, 0.72, 0.76, 0.93, 0.75, 0.98, 0.69, 0.46, 0.43, 0.56, 0.37, 0.26, 0.65, 0.92, 0.81, 0.68, 0.88, 0.79, 0.95, 0.56, 0.98, 0.64, 0.42, 0.89, 0.53, 0.58, 0.89, 0.57, 0.8975, 0.65, 0.71, 0.8510714285714286, 0.51, 0.58, 0.64, 0.73, 0.77, 0.89, 0.85, 0.73, 0.34, 0.91, 0.78, 0.64, 0.98, 0.75, 0.88, 0.11, 0.21, 0.66, 0.73, 0.42, 0.95, 0.35, 0.74, 0.87, 0.55, 0.77, 0.92, 0.58, 0.85, 0.54, 0.97, 0.48, 0.86, 0.89, 0.68, 0.8, 0.5, 0.49, 0.62, 0.62, 0.97, 0.91, 0.7, 0.87, 0.29, 0.38, 0.97, 0.79, 0.3, 0.8, 0.71, 0.97, 0.84, 0.79, 0.96, 0.92, 0.815, 0.87, 0.87, 0.57, 0.54, 0.72, 0.78, 0.18, 0.82, 0.83, 0.61, 0.93, 0.6, 0.95, 0.33, 0.81, 0.75, 0.49, 0.95, 0.8, 0.97, 0.65, 0.12, 0.48, 0.64, 0.24, 0.8, 0.46, 0.17, 0.45, 0.88, 0.4, 0.87, 0.43, 0.62, 0.95, 0.92, 0.4, 0.72, 0.91, 0.42, 0.35, 0.81, 0.66, 0.45, 0.58, 0.53, 0.46, 0.88, 0.87, 0.8, 0.8, 0.93, 0.87, 0.85, 0.34, 0.77, 0.52, 0.96, 0.88, 0.78, 0.62, 0.37, 0.92, 0.88, 0.62, 0.09, 0.82, 0.23, 0.89, 0.56, 0.98, 0.54, 0.72, 0.67, 0.33, 0.6, 0.92, 0.67, 0.73, 0.86, 0.59, 0.66, 0.72, 0.52, 0.91, 0.39, 0.79, 0.77, 0.85, 0.77, 0.825, 0.65, 0.58, 0.75, 0.65, 0.8710714285714286, 0.65, 0.45, 0.86, 0.39, 0.43, 0.64, 0.71, 0.99, 0.97, 0.21, 0.43, 0.59, 0.93, 0.97, 0.63, 0.45, 0.34, 0.46, 0.32, 0.86, 0.67, 0.83, 0.61, 0.76, 0.81, 0.55, 0.61, 0.74, 0.88, 0.33, 0.96, 0.3775, 0.45, 0.89, 0.39, 0.86, 0.86, 0.54, 0.85, 0.6, 0.43, 0.42, 0.61, 0.87, 0.64, 0.31, 0.92, 0.78, 0.89, 0.64, 0.7, 0.7, 0.61, 0.76, 0.74, 0.94, 0.64, 0.79, 0.38, 0.71, 0.94, 0.9, 0.81, 0.62, 0.83, 0.53, 0.42, 0.62, 0.92, 0.76, 0.41, 0.87, 0.81, 0.29, 0.83, 0.93, 0.79, 0.81, 0.71, 0.63, 0.98, 0.67, 0.86, 0.56, 1.0, 0.46, 0.52, 0.82, 0.4, 0.55, 0.56, 0.93, 0.87, 0.53, 0.64, 0.79, 0.96, 0.84, 0.3775, 0.23, 0.97, 0.75, 0.57, 0.805, 0.74, 0.73, 0.76, 0.38, 0.24, 0.76, 0.76, 0.56, 0.8, 0.53, 0.5, 0.35, 0.53, 0.42, 0.82, 0.64, 0.63, 0.57, 0.62, 0.56, 0.91, 0.95, 0.57, 0.74, 0.67, 0.81, 0.21, 0.94, 0.56, 0.25, 0.71, 0.94, 0.88, 0.51, 0.89, 0.64, 0.46, 0.7, 0.65, 0.8025, 0.62, 0.35, 0.97, 0.68, 0.91, 0.36, 0.95, 0.89, 0.46, 0.72, 0.78, 0.53, 0.26, 0.52, 0.34, 0.89, 0.44, 0.76, 0.43, 0.44, 0.98, 0.32, 0.43, 0.59, 0.63, 0.56, 0.36, 0.27, 0.7, 0.39, 0.31, 0.49, 0.64, 0.79, 0.51, 0.11, 0.36, 0.84, 0.86, 0.6, 0.57, 0.64, 0.96, 0.58, 0.93, 0.78, 0.99, 0.43, 0.89, 0.86, 0.86, 0.32, 0.5, 0.94, 0.72, 0.68, 0.53, 0.61, 0.84, 0.72, 0.54, 0.43, 0.41, 0.45, 0.37, 0.54, 0.54, 0.43, 0.82, 0.46, 0.34, 0.72, 0.8025, 0.45, 0.8, 0.92, 0.3, 0.71, 0.43, 0.92, 0.69, 0.74, 0.46, 0.83, 0.48, 0.81, 0.51, 0.76, 0.99, 0.75, 0.73, 0.61, 0.73, 0.64, 0.63, 0.8766666666666666, 0.5, 0.72, 0.77, 0.32, 0.83, 0.89, 0.68, 0.48, 0.65, 0.96, 0.74, 0.69, 0.83, 0.97, 0.82, 0.96, 0.8, 0.77, 0.76, 0.62, 0.49, 0.91, 0.8, 0.62, 0.83, 0.5, 0.79, 0.52, 0.17, 0.55, 0.9, 0.79, 0.96, 0.32, 0.9075, 0.25, 0.63, 0.51, 0.63, 0.85, 0.65, 0.79, 0.9, 0.43, 0.21666666666666665, 0.88, 0.92, 0.86, 0.49, 0.46, 0.65, 0.81, 0.45, 0.88, 0.73, 0.88, 0.91, 0.91, 0.84, 0.69, 0.79, 0.69, 0.94, 0.55, 0.91, 0.66, 0.93, 0.91, 0.91, 0.77, 0.31, 0.63, 0.84, 0.72, 0.72, 0.85, 0.85, 0.88, 0.69, 0.53, 0.47, 0.93, 0.78, 0.86, 0.84, 0.33, 0.22, 0.88, 0.93, 0.89, 0.81, 0.53, 0.83, 0.69, 0.44, 0.36, 0.87, 0.41, 0.57, 0.85, 0.63, 0.65, 0.92, 0.82, 0.51, 0.82, 0.37, 0.24, 0.62, 0.91, 0.77, 0.58, 0.455, 0.67, 0.63, 0.87, 0.59, 0.63, 0.29, 0.8425, 0.44, 0.87, 0.66, 0.55, 0.55, 0.86, 0.66, 0.84, 0.62, 0.67, 0.89, 0.72, 0.82, 0.52, 0.87, 0.77, 0.97, 0.64, 0.59, 0.61, 0.67, 0.23, 0.75, 0.83, 0.98, 0.69, 0.5, 0.82, 0.49, 0.77, 0.35, 0.84, 0.49, 0.67, 0.52, 0.95, 0.83, 0.77, 0.97, 0.46, 0.71, 0.7, 0.81, 0.99, 0.28, 0.8025, 0.87, 0.85, 0.78, 0.9, 0.25, 0.86, 0.85, 0.64, 0.57, 0.88, 0.83, 0.89, 0.94, 0.42, 0.73, 0.71, 0.83, 0.69, 0.79, 0.95, 0.54, 0.35, 0.49, 0.54, 0.34, 0.61, 0.92, 0.7, 0.98, 0.92, 0.64, 0.96, 0.67, 0.57, 0.76, 0.63, 0.95, 0.8, 0.93, 0.77, 0.36, 0.97, 0.8, 0.61, 0.78, 0.61, 0.57, 0.95, 0.61, 0.25, 0.78, 0.72, 0.82, 0.87, 0.49, 0.75, 0.89, 0.64, 0.91, 0.93, 0.84, 0.75, 0.86, 0.47, 0.45, 0.93, 0.88, 0.78, 0.63, 0.7, 0.51, 0.83, 0.49, 0.58, 0.56, 0.85, 0.88, 0.91, 0.91, 0.81, 0.59, 0.97, 0.67, 0.64, 0.46, 0.72, 0.77, 0.56, 0.64, 0.63, 0.49, 1.0, 0.63, 0.88, 0.84, 0.64, 0.52, 0.67, 0.69, 0.44, 0.9, 0.64, 0.9, 0.68, 0.73, 0.64, 0.87, 0.61, 0.98, 0.97, 0.95, 0.9, 0.96, 0.61, 0.76, 0.8, 0.4, 0.52, 0.99, 0.8075, 0.93, 0.76, 0.65, 0.72, 0.8871428571428571, 0.77, 0.39, 0.38, 0.51, 0.79, 0.56, 0.64, 0.28, 0.52, 0.94, 0.66, 0.4, 0.84, 0.92, 0.94, 0.62, 0.65, 0.68, 0.38, 0.65, 0.75, 0.98, 0.48, 0.525, 0.52, 0.52, 0.69, 0.62, 0.96, 0.74, 0.61, 0.6, 0.62, 0.83, 0.95, 0.96, 0.48, 0.78, 0.88, 0.96, 0.25, 0.79, 0.5, 0.32, 0.63, 0.8885714285714286, 0.88, 0.8075, 0.62, 0.5, 0.59, 0.94, 0.29, 0.85, 0.87, 0.77, 0.845, 0.95, 0.56, 0.7, 0.77, 0.41, 0.44, 0.88, 0.77, 0.82, 0.77, 0.64, 0.9, 0.5, 0.82, 0.87, 0.48, 0.36, 0.28, 0.69, 0.67, 0.815, 0.77, 0.85, 0.45, 0.91, 0.85, 0.68, 0.77, 0.77, 0.75, 0.55, 0.7, 0.44, 0.81, 0.75, 0.97, 0.55, 0.45, 0.22, 0.44, 0.69, 0.82, 0.64, 0.47, 0.81, 0.95, 0.92, 0.68, 0.95, 0.54, 0.65, 0.96, 0.67, 0.63, 0.9, 0.65, 0.54, 0.93, 0.69, 0.86, 0.14, 0.88, 0.35, 0.73, 0.77, 0.22, 0.56, 0.8, 0.34, 0.68, 0.53, 0.63, 0.49, 0.735, 0.83, 0.89, 0.47, 0.8, 0.68, 0.76, 0.89, 0.49, 0.85, 0.69, 0.73, 0.8, 0.87, 0.67, 0.95, 0.82, 0.29, 0.98, 0.49, 0.89, 0.39, 0.88, 0.95, 0.51, 0.53, 0.89, 0.53, 0.5, 0.61, 0.5, 0.32, 0.73, 0.21, 0.91, 0.76, 0.73, 0.85, 0.66, 0.94, 0.71, 0.82, 0.74, 0.98, 0.78, 0.69, 0.86, 0.72, 0.91, 0.71, 0.62, 0.74, 0.54, 0.31, 0.84, 0.76, 0.69, 0.77, 0.25, 0.47, 0.94, 0.84, 0.75, 0.96, 0.87, 0.59, 0.61, 0.96, 0.8635714285714287, 0.91, 0.94, 0.62, 0.72, 0.61, 0.7, 0.48, 0.31, 0.41, 0.45, 0.53, 0.83, 0.25, 0.81, 0.93, 0.62, 0.61, 0.73, 0.89, 0.67, 0.69, 0.44, 0.9, 0.86, 0.83, 0.27, 0.53, 0.37, 0.5, 0.73, 0.94, 0.87, 0.695, 0.33, 0.91, 0.97, 0.58, 0.89, 0.43, 0.37, 0.65, 0.75, 0.54, 0.71, 0.6, 0.51, 0.81, 0.61, 0.95, 0.71, 0.46, 0.53, 0.85, 0.61, 0.71, 0.74, 0.6, 0.48, 0.67, 0.77, 0.93, 0.26, 0.69, 0.48, 0.88, 0.46, 0.16, 0.57, 0.78, 0.83, 0.35, 0.35, 0.55, 0.5526666666666666, 0.87, 0.7, 0.78, 0.74, 0.73, 0.45, 0.54, 0.42, 0.73, 0.64, 0.77, 0.88, 0.9, 0.6, 0.94, 0.8885714285714286, 0.31, 0.88, 0.21, 0.98, 0.48, 0.71, 0.65, 0.55, 0.94, 0.62, 0.97, 0.37, 0.7, 0.71, 0.64, 0.83, 0.52, 0.97, 0.73, 0.78, 0.82, 0.52, 0.4, 0.68, 0.88, 0.62, 0.51, 0.52, 0.3, 0.7, 0.87, 0.97, 0.05, 0.07, 0.22, 0.34, 0.49, 0.21, 0.65, 0.3, 0.23, 0.25, 0.36, 0.03, 0.16, 0.04, 0.09, 0.28, 0.38, 0.08, 0.27, 0.11, 0.12, 0.09, 0.61, 0.1, 0.68, 0.32, 0.36, 0.05, 0.34, 0.13, 0.17, 0.41, 0.2, 0.02, 0.32, 0.33, 0.37, 0.04, 0.06, 0.19, 0.26, 0.2, 0.06, 0.05, 0.01, 0.2, 0.12, 0.26, 0.04, 0.27, 0.02, 0.28, 0.05, 0.54, 0.24, 0.23, 0.03, 0.45, 0.08, 0.14, 0.24, 0.54, 0.09, 0.28, 0.49, 0.11, 0.22, 0.23, 0.04, 0.2, 0.25, 0.2, 0.21, 0.68, 0.08, 0.09, 0.09, 0.05, 0.32, 0.07, 0.13, 0.28, 0.14, 0.09, 0.12, 0.21, 0.31, 0.41, 0.57, 0.15, 0.37, 0.26, 0.17, 0.15, 0.15, 0.06, 0.41, 0.33, 0.25, 0.46, 0.2, 0.51, 0.28, 0.1, 0.05, 0.02, 0.23, 0.39, 0.0, 0.15, 0.49, 0.38, 0.02, 0.39, 0.3, 0.09, 0.18, 0.23, 0.12, 0.27, 0.42, 0.53, 0.16, 0.37, 0.13, 0.08, 0.09, 0.16, 0.11, 0.18, 0.25, 0.15, 0.18, 0.62, 0.23, 0.03, 0.41, 0.25, 0.1, 0.2, 0.05, 0.29, 0.2, 0.06, 0.04, 0.51, 0.53, 0.08, 0.24, 0.34, 0.245, 0.1, 0.08, 0.31, 0.13, 0.03, 0.14, 0.42, 0.32, 0.43, 0.33, 0.23, 0.02, 0.28, 0.42, 0.26, 0.33, 0.04, 0.13, 0.11, 0.21, 0.09, 0.23, 0.22, 0.2, 0.37, 0.15, 0.44, 0.18, 0.53, 0.18, 0.03, 0.0, 0.08, 0.13, 0.24, 0.11, 0.1, 0.37, 0.29, 0.75, 0.31, 0.47, 0.34, 0.41, 0.08, 0.03, 0.33, 0.12, 0.34, 0.06, 0.67, 0.08, 0.53, 0.28, 0.11, 0.17, 0.05, 0.08, 0.39, 0.48, 0.09, 0.21, 0.36, 0.03, 0.57, 0.34, 0.02, 0.01, 0.04, 0.5, 0.26, 0.07, 0.22, 0.04, 0.45, 0.09, 0.2, 0.23, 0.06, 0.23, 0.35, 0.21, 0.05, 0.25, 0.25, 0.18, 0.24, 0.09, 0.45, 0.09, 0.15, 0.26, 0.27, 0.16, 0.06, 0.29, 0.19, 0.49, 0.22, 0.27, 0.53, 0.52, 0.29, 0.32, 0.05, 0.19, 0.03, 0.22, 0.02, 0.35, 0.14, 0.11, 0.21, 0.255, 0.16, 0.24, 0.35, 0.16, 0.34, 0.05, 0.25, 0.1, 0.12, 0.57, 0.04, 0.23, 0.04, 0.86, 0.35, 0.24, 0.27, 0.31, 0.24, 0.47, 0.47, 0.04, 0.22, 0.3, 0.08, 0.03, 0.28, 0.09, 0.05, 0.32, 0.11, 0.28, 0.28, 0.4, 0.2, 0.13, 0.24, 0.21, 0.14, 0.11, 0.24, 0.1, 0.31, 0.18, 0.1, 0.07, 0.09, 0.305, 0.27, 0.41, 0.19, 0.68, 0.37, 0.26, 0.17, 0.26, 0.26, 0.15, 0.05, 0.03, 0.22, 0.41, 0.53, 0.11, 0.17, 0.41, 0.38, 0.13, 0.24, 0.35, 0.04, 0.09, 0.32, 0.05, 0.41, 0.05, 0.04, 0.17, 0.13, 0.05, 0.27, 0.35, 0.28, 0.14, 0.19, 0.04, 0.08, 0.26, 0.11, 0.19, 0.39, 0.08, 0.12, 0.25, 0.16, 0.29, 0.17, 0.24, 0.33, 0.17, 0.21, 0.14, 0.32, 0.08, 0.04, 0.37, 0.18, 0.39, 0.06, 0.36, 0.17, 0.19, 0.15, 0.4, 0.16, 0.25, 0.22, 0.09, 0.06, 0.39, 0.08, 0.06, 0.32, 0.15, 0.23, 0.26, 0.3, 0.17, 0.32, 0.42, 0.22, 0.28, 0.4, 0.12, 0.19, 0.18, 0.23, 0.25, 0.22, 0.2, 0.17, 0.11, 0.07, 0.03, 0.4, 0.21, 0.18, 0.02, 0.27, 0.12, 0.11, 0.21, 0.32, 0.31, 0.13, 0.15, 0.59, 0.28, 0.21, 0.39, 0.45, 0.25, 0.51, 0.51, 0.05, 0.35, 0.27, 0.19, 0.12, 0.33, 0.43, 0.06, 0.49, 0.19, 0.06, 0.15, 0.04, 0.07, 0.06, 0.06, 0.28, 0.15, 0.12, 0.25, 0.19, 0.41, 0.11, 0.05, 0.04, 0.29, 0.11, 0.02, 0.4, 0.27, 0.38, 0.25, 0.56, 0.28, 0.29, 0.29, 0.3, 0.15, 0.28, 0.36, 0.04, 0.15, 0.05, 0.04, 0.03, 0.35, 0.31, 0.37, 0.02, 0.46, 0.27, 0.18, 0.15, 0.37, 0.38, 0.39, 0.25, 0.26, 0.08, 0.33, 0.03, 0.17, 0.06, 0.32, 0.2, 0.28, 0.09, 0.14, 0.35, 0.39, 0.55, 0.31, 0.7, 0.53, 0.34, 0.03, 0.11, 0.07, 0.5, 0.07, 0.5, 0.05, 0.8, 0.4, 0.12, 0.25, 0.5, 0.09, 0.04, 0.18, 0.1, 0.22, 0.55, 0.21, 0.13, 0.38, 0.49, 0.0, 0.12, 0.27, 0.34, 0.28, 0.235, 0.24, 0.17, 0.41, 0.59, 0.05, 0.12, 0.07, 0.07, 0.16, 0.07, 0.27, 0.23, 0.11, 0.24, 0.32, 0.14, 0.02, 0.05, 0.25, 0.14, 0.15, 0.16, 0.39, 0.09, 0.5, 0.11, 0.13, 0.25, 0.18, 0.48, 0.36, 0.31, 0.35, 0.06, 0.15, 0.09, 0.14, 0.06, 0.33, 0.37, 0.14, 0.3, 0.05, 0.29, 0.25, 0.47, 0.05, 0.36, 0.24, 0.35, 0.21, 0.22, 0.12, 0.28, 0.04, 0.01, 0.29, 0.21, 0.2, 0.07, 0.24, 0.15, 0.01, 0.12, 0.42, 0.31, 0.08, 0.21, 0.31, 0.19, 0.59, 0.25, 0.45, 0.04, 0.23, 0.01, 0.41, 0.27, 0.15, 0.59, 0.16, 0.32, 0.36, 0.22, 0.18, 0.41, 0.29, 0.15, 0.2, 0.28, 0.13, 0.12, 0.48, 0.45, 0.6, 0.53, 0.46, 0.56, 0.31, 0.18, 0.07, 0.18, 0.03, 0.47, 0.34, 0.04, 0.11, 0.62, 0.27, 0.24, 0.16, 0.41, 0.23, 0.28, 0.19, 0.22, 0.32, 0.18, 0.54, 0.28, 0.28, 0.05, 0.1, 0.32, 0.23, 0.14, 0.03, 0.01, 0.09, 0.07, 0.11, 0.13, 0.08, 0.05, 0.01, 0.17, 0.44, 0.38, 0.13, 0.04, 0.04, 0.36, 0.32, 0.13, 0.04, 0.47, 0.1, 0.09, 0.23, 0.28, 0.39, 0.27, 0.25, 0.25, 0.59, 0.12, 0.06, 0.1, 0.2, 0.27, 0.08, 0.21, 0.07, 0.45, 0.06, 0.3, 0.05, 0.42, 0.72, 0.12, 0.27, 0.05, 0.12, 0.52, 0.2, 0.05, 0.23, 0.16, 0.41, 0.17, 0.28, 0.05, 0.39, 0.02, 0.05, 0.13, 0.41, 0.25, 0.17, 0.1, 0.49, 0.48, 0.37, 0.01, 0.28, 0.01, 0.16, 0.34, 0.26, 0.26, 0.26, 0.43, 0.48, 0.12, 0.22, 0.38, 0.48, 0.08, 0.38, 0.17, 0.35, 0.17, 0.52, 0.14, 0.36, 0.11, 0.48, 0.23, 0.05, 0.19, 0.04, 0.33, 0.07, 0.36, 0.22, 0.56, 0.48, 0.2, 0.76, 0.2, 0.53, 0.26, 0.23, 0.18, 0.43, 0.1, 0.45, 0.58, 0.24, 0.31, 0.32, 0.14, 0.01, 0.496, 0.29, 0.44, 0.43, 0.16, 0.27, 0.43, 0.24, 0.06, 0.34, 0.41, 0.47, 0.48, 0.28, 0.56, 0.0, 0.28, 0.21, 0.24, 0.23, 0.4, 0.13, 0.42, 0.17, 0.1, 0.22, 0.14, 0.52, 0.03, 0.07, 0.09, 0.26, 0.16, 0.09, 0.28, 0.15, 0.16, 0.27, 0.14, 0.62, 0.3, 0.58, 0.12, 0.09, 0.08, 0.08, 0.14, 0.24, 0.31, 0.1, 0.69, 0.02, 0.13, 0.55, 0.13, 0.57, 0.08, 0.34, 0.17, 0.14, 0.41, 0.07, 0.2, 0.55, 0.26, 0.2, 0.18, 0.17, 0.63, 0.04, 0.12, 0.16, 0.07, 0.04, 0.23, 0.25, 0.28, 0.1, 0.22, 0.09, 0.17, 0.04, 0.26, 0.16, 0.08, 0.07, 0.29, 0.01, 0.13, 0.34, 0.11, 0.22, 0.15, 0.45, 0.37, 0.28, 0.19, 0.28, 0.46, 0.32, 0.14, 0.33, 0.54, 0.23, 0.18, 0.02, 0.15, 0.41, 0.17, 0.05, 0.15, 0.07, 0.2, 0.19, 0.18, 0.24, 0.2, 0.35, 0.05, 0.18, 0.04, 0.4, 0.05, 0.23, 0.26, 0.08, 0.24, 0.35, 0.02, 0.22, 0.13, 0.15, 0.19, 0.29, 0.46, 0.07, 0.8, 0.09, 0.3, 0.14, 0.4, 0.05, 0.16, 0.05, 0.15, 0.4, 0.18, 0.26666666666666666, 0.26, 0.19, 0.04, 0.27, 0.1, 0.29, 0.03, 0.2, 0.16, 0.16, 0.37, 0.45, 0.34, 0.1, 0.09, 0.06, 0.14]</t>
+          <t>[0.93, 0.15, 0.47, 0.7, 0.8, 0.99, 0.69, 0.35, 0.61, 0.87, 0.77, 0.74, 0.87, 0.53, 0.98, 0.29, 0.9, 0.92, 0.79, 0.47, 0.84, 0.83, 0.77, 0.44, 0.83, 0.31, 0.93, 0.9, 0.83, 0.62, 0.93, 0.57, 0.6866666666666668, 0.9, 0.83, 0.97, 0.63, 0.63, 0.76, 0.78, 0.67, 0.58, 0.28, 0.56, 0.88, 0.31, 0.93, 0.74, 0.2, 0.82, 0.8966666666666667, 0.9, 0.5, 0.76, 0.8, 0.41, 0.48, 0.86, 0.95, 0.79, 0.57, 0.74, 0.73, 0.66, 0.95, 0.46, 0.75, 0.78, 0.73, 0.6, 0.63, 0.63, 0.75, 0.98, 0.92, 0.84, 0.83, 0.8666666666666666, 0.78, 0.25, 0.8, 0.74, 0.88, 0.8, 0.81, 0.62, 0.76, 0.93, 0.6, 0.78, 0.88, 0.38, 0.75, 0.73, 0.38, 0.83, 0.8, 0.55, 0.92, 0.69, 0.56, 0.63, 0.72, 0.9, 0.45, 0.8566666666666666, 0.32, 0.9179999999999999, 0.55, 0.64, 0.33, 0.1, 0.73, 0.94, 0.76, 0.74, 0.82, 0.62, 0.8, 0.57, 0.67, 0.69, 0.83, 0.66, 0.53, 0.63, 0.75, 0.77, 0.72, 0.55, 0.69, 0.7, 0.66, 0.69, 0.77, 0.84, 0.3875, 0.85, 0.88, 0.83, 0.92, 0.9366666666666668, 0.86, 0.39, 0.75, 0.93, 0.93, 0.72, 0.96, 0.49, 0.48, 0.84, 0.35, 0.71, 0.31, 0.92, 0.8, 0.35, 0.48, 0.59, 0.53, 0.51, 0.74, 0.81, 0.81, 0.79, 0.87, 0.89, 0.83, 0.74, 0.89, 0.77, 0.63, 0.77, 0.8366666666666666, 0.59, 0.54, 0.7016666666666665, 0.84, 0.65, 0.69, 0.5, 0.8566666666666666, 0.82, 0.23, 0.59, 0.83, 0.78, 0.79, 0.8, 0.92, 0.72, 0.6666666666666665, 0.86, 0.51, 0.46, 0.89, 0.8, 0.85, 0.39, 0.8466666666666666, 0.6, 0.7866666666666666, 0.88, 0.66, 0.59, 0.83, 0.83, 0.34, 0.82, 0.75, 0.6, 0.77, 0.95, 0.92, 0.92, 0.89, 0.79, 0.89, 0.78, 0.66, 0.4, 0.71, 0.81, 0.74, 0.73, 0.3, 0.95, 0.58, 0.9, 0.81, 0.5, 0.87, 0.97, 0.62, 0.89, 0.58, 0.6, 0.78, 0.71, 0.64, 0.55, 0.59, 0.91, 0.93, 0.66, 0.61, 0.8666666666666666, 0.31, 0.39, 0.85, 0.91, 0.95, 0.85, 0.93, 0.54, 0.91, 0.81, 0.61, 0.55, 0.59, 0.45, 0.83, 0.75, 0.69, 0.45, 0.86, 0.34, 0.74, 0.9, 0.69, 0.36, 0.55, 0.31, 0.75, 0.84, 0.81, 0.85, 0.98, 0.79, 0.53, 0.94, 0.83, 0.77, 0.74, 0.41, 0.89, 0.92, 0.43, 0.36, 0.85, 0.52, 0.91, 0.7816666666666666, 0.86, 0.72, 0.85, 0.82, 0.55, 0.54, 0.3, 0.76, 0.28, 0.36, 0.67, 0.81, 0.79, 0.88, 0.61, 0.61, 0.43, 0.31, 0.48, 0.88, 0.81, 0.43, 0.33, 0.46, 0.84, 0.72, 0.94, 0.91, 0.99, 0.75, 0.88, 0.79, 0.99, 0.47, 0.43, 0.82, 0.64, 0.78, 0.85, 0.86, 0.55, 0.62, 0.96, 0.84, 0.91, 0.68, 0.52, 0.57, 0.69, 0.94, 0.87, 0.92, 0.86, 0.6, 0.73, 0.86, 0.53, 0.89, 0.76, 0.97, 0.93, 0.95, 0.99, 0.5, 0.72, 0.97, 0.56, 0.3875, 0.66, 0.83, 0.84, 0.59, 0.74, 0.62, 0.58, 0.68, 0.91, 0.92, 0.45, 0.95, 0.86, 0.69, 0.75, 0.67, 0.9266666666666667, 0.62, 0.87, 0.9166666666666667, 0.82, 0.26, 0.63, 0.94, 0.35, 0.62, 0.9166666666666667, 0.93, 0.95, 0.41, 0.85, 0.85, 0.56, 0.88, 0.75, 0.88, 0.35, 0.44, 0.45, 0.7, 0.49, 0.91, 0.68, 0.62, 0.92, 0.51, 0.84, 0.65, 0.52, 0.46, 0.66, 0.83, 0.9471428571428572, 0.88, 0.52, 0.51, 0.9566666666666666, 0.59, 0.42, 0.94, 0.87, 0.85, 0.53, 0.76, 0.56, 0.74, 0.26, 0.74, 0.69, 0.87, 0.73, 0.96, 0.91, 0.86, 0.86, 0.82, 0.68, 0.6, 0.94, 0.77, 0.58, 0.79, 0.76, 0.9, 0.84, 0.75, 0.88, 0.62, 0.88, 0.76, 0.43, 0.61, 0.92, 0.52, 0.97, 0.59, 0.7, 0.85, 0.92, 0.94, 0.82, 0.26, 0.85, 0.83, 0.27, 0.72, 0.53, 0.9, 0.84, 0.92, 0.81, 0.52, 0.33, 0.25, 0.51, 0.7, 0.88, 0.36, 0.76, 0.47, 0.86, 0.54, 0.43, 0.87, 0.78, 0.18, 0.92, 0.42, 0.53, 0.34, 0.58, 0.57, 0.69, 0.72, 0.94, 0.77, 0.98, 0.84, 0.57, 0.43, 0.45, 0.4175, 0.24, 0.59, 0.87, 0.8, 0.61, 0.89, 0.89, 0.99, 0.62, 0.92, 0.67, 0.49, 0.91, 0.55, 0.49, 0.8666666666666666, 0.58, 0.93, 0.635, 0.82, 0.8216666666666668, 0.6, 0.6, 0.68, 0.62, 0.7, 0.9, 0.82, 0.75, 0.37, 0.89, 0.7866666666666666, 0.73, 0.95, 0.81, 0.81, 0.12, 0.22, 0.69, 0.7, 0.47, 0.91, 0.35, 0.76, 0.9, 0.58, 0.81, 0.86, 0.61, 0.85, 0.52, 0.94, 0.39, 0.94, 0.96, 0.76, 0.85, 0.53, 0.52, 0.74, 0.61, 1.0, 0.87, 0.62, 0.88, 0.3975, 0.54, 0.95, 0.73, 0.26, 0.81, 0.79, 0.96, 0.96, 0.78, 0.96, 0.91, 0.7866666666666666, 0.84, 0.84, 0.6, 0.46, 0.67, 0.78, 0.27, 0.82, 0.89, 0.64, 0.88, 0.57, 0.95, 0.34, 0.79, 0.79, 0.58, 0.93, 0.69, 0.98, 0.67, 0.14, 0.46, 0.71, 0.34, 0.77, 0.4, 0.19, 0.515, 0.84, 0.43, 0.88, 0.37, 0.5, 0.94, 0.92, 0.3, 0.68, 0.9066666666666667, 0.51, 0.36, 0.89, 0.63, 0.53, 0.65, 0.56, 0.48, 0.9, 0.89, 0.88, 0.68, 0.96, 0.88, 0.9, 0.34, 0.74, 0.53, 0.98, 0.9, 0.84, 0.64, 0.36, 0.95, 0.9, 0.78, 0.12, 0.84, 0.14, 0.86, 0.59, 1.0, 0.53, 0.68, 0.59, 0.32, 0.65, 0.94, 0.64, 0.72, 0.79, 0.54, 0.71, 0.76, 0.53, 0.96, 0.4, 0.72, 0.77, 0.87, 0.67, 0.8666666666666666, 0.665, 0.61, 0.8, 0.72, 0.8766666666666667, 0.7, 0.4, 0.88, 0.29, 0.4, 0.73, 0.64, 0.96, 0.97, 0.28, 0.39, 0.5, 0.94, 0.94, 0.61, 0.47, 0.44, 0.63, 0.18, 0.85, 0.67, 0.84, 0.66, 0.8, 0.92, 0.64, 0.73, 0.61, 0.83, 0.21, 0.96, 0.5316666666666667, 0.4075, 0.92, 0.29, 0.95, 0.93, 0.51, 0.81, 0.55, 0.44, 0.45, 0.62, 0.86, 0.7, 0.21, 0.91, 0.88, 0.84, 0.66, 0.79, 0.8, 0.51, 0.78, 0.73, 0.85, 0.72, 0.79, 0.45, 0.86, 0.91, 0.85, 0.8, 0.63, 0.74, 0.56, 0.44, 0.77, 0.87, 0.78, 0.44, 0.8, 0.87, 0.31, 0.84, 0.88, 0.77, 0.83, 0.79, 0.62, 0.95, 0.69, 0.86, 0.67, 1.0, 0.41, 0.55, 0.77, 0.37, 0.69, 0.51, 0.87, 0.89, 0.46, 0.66, 0.84, 0.93, 0.8, 0.5316666666666667, 0.28, 0.94, 0.73, 0.63, 0.87, 0.73, 0.74, 0.74, 0.47, 0.22, 0.85, 0.87, 0.58, 0.77, 0.49, 0.53, 0.34, 0.53, 0.53, 0.76, 0.68, 0.64, 0.55, 0.67, 0.55, 0.96, 0.93, 0.51, 0.73, 0.63, 0.81, 0.16, 0.92, 0.64, 0.26, 0.74, 0.92, 0.85, 0.55, 0.95, 0.62, 0.48, 0.615, 0.74, 0.8266666666666665, 0.68, 0.46, 0.98, 0.62, 0.83, 0.36, 0.91, 0.85, 0.52, 0.67, 0.85, 0.48, 0.18, 0.53, 0.38, 0.74, 0.44, 0.77, 0.34, 0.46, 0.95, 0.3, 0.38, 0.62, 0.6, 0.52, 0.37, 0.21, 0.57, 0.41, 0.33, 0.62, 0.64, 0.78, 0.53, 0.11, 0.48, 0.87, 0.88, 0.61, 0.47, 0.68, 0.95, 0.59, 0.95, 0.83, 0.95, 0.46, 0.87, 0.88, 0.92, 0.3, 0.51, 0.93, 0.67, 0.78, 0.51, 0.65, 0.86, 0.76, 0.5, 0.36, 0.61, 0.43, 0.42, 0.51, 0.55, 0.46, 0.84, 0.51, 0.35, 0.72, 0.8366666666666666, 0.43, 0.75, 0.86, 0.3975, 0.82, 0.51, 0.83, 0.61, 0.72, 0.59, 0.82, 0.45, 0.9, 0.55, 0.8, 0.92, 0.59, 0.77, 0.62, 0.81, 0.55, 0.65, 0.77, 0.57, 0.76, 0.86, 0.36, 0.8, 0.95, 0.78, 0.29, 0.73, 0.91, 0.71, 0.6, 0.8066666666666665, 0.87, 0.83, 0.94, 0.82, 0.8, 0.79, 0.72, 0.6, 0.86, 0.89, 0.55, 0.76, 0.63, 0.89, 0.54, 0.11, 0.5, 0.9, 0.74, 1.0, 0.37, 0.9166666666666667, 0.23, 0.67, 0.63, 0.6, 0.9, 0.68, 0.77, 0.86, 0.48, 0.3, 0.828, 0.93, 0.74, 0.42, 0.38, 0.7, 0.84, 0.4, 0.82, 0.7, 0.83, 0.89, 0.9, 0.78, 0.65, 0.72, 0.69, 0.94, 0.47, 0.95, 0.52, 0.93, 0.86, 0.89, 0.82, 0.45, 0.56, 0.75, 0.58, 0.79, 0.81, 0.9, 0.89, 0.7, 0.5, 0.48, 0.95, 0.69, 0.9, 0.84, 0.26, 0.16, 0.9, 0.94, 0.88, 0.74, 0.53, 0.84, 0.6, 0.55, 0.31, 0.91, 0.47, 0.53, 0.84, 0.65, 0.71, 0.87, 0.85, 0.46, 0.77, 0.26, 0.46, 0.67, 0.9, 0.75, 0.52, 0.5066666666666666, 0.69, 0.72, 0.89, 0.65, 0.52, 0.26, 0.8666666666666666, 0.42, 0.91, 0.69, 0.57, 0.55, 0.91, 0.7, 0.83, 0.63, 0.74, 0.96, 0.68, 0.8, 0.45, 0.85, 0.76, 0.94, 0.54, 0.58, 0.67, 0.65, 0.42, 0.83, 0.78, 0.96, 0.67, 0.44, 0.83, 0.51, 0.7, 0.5, 0.78, 0.47, 0.74, 0.46, 0.99, 0.89, 0.76, 0.91, 0.53, 0.71, 0.73, 0.88, 0.96, 0.23, 0.8166666666666665, 0.84, 0.83, 0.82, 0.87, 0.2, 0.87, 0.87, 0.7, 0.41, 0.94, 0.79, 0.83, 0.88, 0.5, 0.66, 0.77, 0.75, 0.71, 0.76, 0.87, 0.53, 0.38, 0.52, 0.55, 0.4, 0.56, 0.9, 0.68, 0.99, 0.8, 0.57, 0.91, 0.62, 0.57, 0.72, 0.62, 0.89, 0.71, 0.86, 0.73, 0.35, 0.94, 0.64, 0.6466666666666666, 0.86, 0.67, 0.67, 0.9, 0.58, 0.11, 0.7866666666666666, 0.75, 0.85, 0.89, 0.47, 0.69, 0.93, 0.77, 0.88, 0.91, 0.81, 0.77, 0.73, 0.49, 0.5, 0.94, 0.88, 0.89, 0.58, 0.78, 0.38, 0.85, 0.46, 0.57, 0.53, 0.89, 0.76, 0.92, 0.93, 0.78, 0.51, 1.0, 0.63, 0.73, 0.51, 0.74, 0.68, 0.57, 0.67, 0.64, 0.51, 0.96, 0.61, 0.88, 0.85, 0.67, 0.43, 0.74, 0.71, 0.45, 0.82, 0.63, 0.91, 0.64, 0.76, 0.65, 0.83, 0.65, 0.97, 0.95, 0.938, 0.89, 0.94, 0.53, 0.66, 0.83, 0.45, 0.41, 0.96, 0.86, 0.94, 0.76, 0.58, 0.83, 0.88, 0.8, 0.39, 0.39, 0.54, 0.74, 0.57, 0.69, 0.34, 0.51, 0.94, 0.61, 0.3, 0.89, 0.95, 0.96, 0.61, 0.66, 0.78, 0.31, 0.52, 0.8, 0.96, 0.47, 0.64, 0.45, 0.66, 0.74, 0.58, 0.97, 0.85, 0.61, 0.65, 0.65, 0.83, 0.93, 0.96, 0.53, 0.67, 0.82, 0.99, 0.15, 0.79, 0.49, 0.39, 0.65, 0.8666666666666667, 0.88, 0.86, 0.71, 0.57, 0.63, 0.94, 0.26, 0.83, 0.91, 0.74, 0.79, 0.95, 0.61, 0.68, 0.74, 0.38, 0.47, 0.9, 0.83, 0.91, 0.67, 0.76, 0.86, 0.56, 0.71, 0.9, 0.51, 0.3, 0.33, 0.79, 0.57, 0.7866666666666666, 0.79, 0.81, 0.48, 0.92, 0.85, 0.63, 0.77, 0.72, 0.74, 0.52, 0.72, 0.45, 0.72, 0.78, 0.99, 0.56, 0.46, 0.31, 0.27, 0.66, 0.86, 0.66, 0.57, 0.79, 0.93, 0.94, 0.765, 0.96, 0.58, 0.61, 0.97, 0.69, 0.54, 0.89, 0.57, 0.5066666666666666, 0.93, 0.74, 0.88, 0.27, 0.88, 0.49, 0.81, 0.79, 0.31, 0.59, 0.84, 0.46, 0.69, 0.51, 0.59, 0.47, 0.85, 0.87, 0.89, 0.4, 0.81, 0.68, 0.75, 0.87, 0.55, 0.89, 0.64, 0.71, 0.88, 0.78, 0.66, 0.94, 0.81, 0.31, 0.88, 0.56, 0.95, 0.33, 0.87, 0.9, 0.56, 0.61, 0.91, 0.5, 0.65, 0.6, 0.57, 0.43, 0.74, 0.34, 0.85, 0.66, 0.74, 0.87, 0.68, 0.8, 0.59, 0.78, 0.68, 0.97, 0.7866666666666666, 0.59, 0.84, 0.71, 0.95, 0.73, 0.54, 0.76, 0.6, 0.41, 0.87, 0.89, 0.65, 0.82, 0.32, 0.59, 0.93, 0.81, 0.67, 0.94, 0.81, 0.59, 0.61, 0.92, 0.7816666666666666, 0.85, 0.82, 0.68, 0.72, 0.7, 0.6, 0.49, 0.31, 0.41, 0.44, 0.61, 0.91, 0.26, 0.8, 0.95, 0.66, 0.62, 0.73, 0.85, 0.62, 0.65, 0.48, 0.82, 0.88, 0.9, 0.32, 0.59, 0.46, 0.58, 0.74, 1.0, 0.84, 0.635, 0.35, 0.95, 0.96, 0.59, 0.86, 0.36, 0.34, 0.56, 0.82, 0.62, 0.76, 0.61, 0.61, 0.77, 0.52, 0.93, 0.72, 0.51, 0.53, 0.83, 0.64, 0.68, 0.74, 0.5, 0.48, 0.7166666666666666, 0.84, 0.97, 0.18, 0.71, 0.57, 0.91, 0.46, 0.21, 0.59, 0.88, 0.84, 0.48, 0.24, 0.43, 0.5833333333333333, 0.82, 0.64, 0.89, 0.8, 0.75, 0.57, 0.46, 0.55, 0.75, 0.7, 0.82, 0.8, 0.91, 0.81, 0.94, 0.8666666666666667, 0.32, 0.89, 0.28, 0.99, 0.49, 0.69, 0.64, 0.56, 0.94, 0.66, 0.91, 0.37, 0.66, 0.79, 0.57, 0.82, 0.46, 0.95, 0.77, 0.73, 0.9, 0.52, 0.39, 0.78, 0.82, 0.63, 0.61, 0.56, 0.36, 0.62, 0.91, 0.94, 0.17, 0.16, 0.33, 0.14, 0.16, 0.14, 0.53, 0.17, 0.06, 0.24, 0.05, 0.17, 0.29, 0.3, 0.2, 0.08, 0.33, 0.21, 0.19, 0.16, 0.19, 0.54, 0.0, 0.05, 0.18, 0.03, 0.3133333333333333, 0.12, 0.56, 0.23, 0.05, 0.17, 0.05, 0.68, 0.1, 0.07, 0.04, 0.11, 0.22, 0.38, 0.23, 0.3175, 0.58, 0.43, 0.13, 0.37, 0.34, 0.11, 0.16, 0.12, 0.34, 0.1, 0.07, 0.03, 0.07, 0.16, 0.48, 0.61, 0.36, 0.36, 0.07, 0.15, 0.33, 0.06, 0.04, 0.09, 0.48, 0.27, 0.46, 0.16, 0.51, 0.14, 0.57, 0.1, 0.04, 0.12, 0.4, 0.28, 0.17, 0.11, 0.33, 0.23, 0.23, 0.61, 0.13, 0.19, 0.16, 0.25, 0.23, 0.06, 0.5, 0.4, 0.25, 0.59, 0.635, 0.55, 0.09, 0.41, 0.27, 0.23, 0.05, 0.04, 0.1, 0.09, 0.75, 0.03, 0.14, 0.22, 0.865, 0.15, 0.18, 0.45, 0.21, 0.09, 0.1, 0.3975, 0.31, 0.04, 0.32, 0.29, 0.1, 0.39, 0.14, 0.3, 0.52, 0.23, 0.27, 0.08, 0.04, 0.19, 0.3175, 0.44, 0.05, 0.43, 0.19, 0.06, 0.13, 0.33, 0.08, 0.16, 0.16, 0.27, 0.03, 0.25, 0.2, 0.03, 0.05, 0.41, 0.29, 0.07, 0.23, 0.24, 0.49, 0.11, 0.66, 0.1, 0.14, 0.06, 0.18, 0.28, 0.16, 0.22, 0.11, 0.15, 0.37, 0.21, 0.21, 0.17, 0.04, 0.39, 0.24916666666666665, 0.43, 0.39666666666666667, 0.01, 0.21, 0.2, 0.13, 0.29, 0.2, 0.08, 0.1, 0.3466666666666666, 0.25, 0.12, 0.17, 0.15, 0.13, 0.17, 0.08, 0.08, 0.13, 0.51, 0.54, 0.26, 0.23, 0.29, 0.33, 0.48, 0.11, 0.07, 0.33, 0.23, 0.2, 0.5, 0.11666666666666668, 0.38, 0.41, 0.41, 0.6, 0.18, 0.39, 0.14, 0.08, 0.35, 0.39, 0.01, 0.48, 0.0, 0.13, 0.29, 0.12, 0.11, 0.44, 0.19, 0.35, 0.2075, 0.23, 0.48, 0.18, 0.46, 0.0, 0.14, 0.42, 0.07, 0.45, 0.16, 0.65, 0.17, 0.4, 0.25, 0.28, 0.08, 0.12, 0.04, 0.19, 0.14, 0.29, 0.04, 0.02, 0.31, 0.17, 0.55, 0.04, 0.07, 0.06, 0.07, 0.11, 0.24, 0.09, 0.19, 0.43, 0.22, 0.02, 0.42, 0.1, 0.32, 0.23, 0.32, 0.22, 0.01, 0.17, 0.09, 0.45, 0.05, 0.17, 0.39, 0.54, 0.55, 0.31, 0.51, 0.09, 0.23, 0.13, 0.19, 0.22, 0.24, 0.26, 0.23, 0.21, 0.2, 0.04, 0.23, 0.05, 0.03, 0.37, 0.09, 0.23, 0.39, 0.21, 0.14, 0.3575, 0.09, 0.28, 0.25, 0.17, 0.1, 0.03, 0.07, 0.11, 0.16, 0.13, 0.57, 0.33, 0.18, 0.15, 0.03, 0.34, 0.09, 0.23, 0.09, 0.17, 0.27, 0.05, 0.21, 0.41, 0.34, 0.24, 0.62, 0.18, 0.32, 0.21, 0.4, 0.04, 0.19, 0.36, 0.09, 0.87, 0.16, 0.16, 0.21, 0.19, 0.65, 0.29, 0.47, 0.06, 0.22, 0.34, 0.15, 0.04, 0.03, 0.11, 0.28, 0.09, 0.26, 0.04, 0.18, 0.02, 0.22, 0.43, 0.24, 0.35, 0.37666666666666665, 0.12, 0.28, 0.27, 0.04, 0.1, 0.13, 0.19, 0.32, 0.21, 0.17, 0.03, 0.29, 0.03, 0.23, 0.15, 0.28, 0.56, 0.45, 0.36, 0.22, 0.32, 0.07, 0.43, 0.22, 0.12, 0.67, 0.31, 0.37, 0.09, 0.06, 0.12, 0.44, 0.05, 0.38, 0.34, 0.43, 0.55, 0.08, 0.68, 0.11, 0.12, 0.24, 0.08, 0.15, 0.49, 0.36, 0.56, 0.53, 0.28, 0.07, 0.49, 0.09, 0.55, 0.43, 0.27, 0.49, 0.18, 0.1, 0.13, 0.11, 0.13, 0.03, 0.41, 0.38, 0.5, 0.43, 0.29, 0.52, 0.13, 0.19, 0.19, 0.05, 0.11, 0.42, 0.18, 0.31, 0.24, 0.11, 0.29, 0.27, 0.25, 0.09, 0.13, 0.04, 0.365, 0.27, 0.05, 0.4, 0.19, 0.15, 0.2, 0.03, 0.15, 0.12, 0.3, 0.33, 0.18, 0.47, 0.19, 0.17, 0.2, 0.2, 0.31, 0.31, 0.08, 0.26, 0.24, 0.3, 0.11, 0.42, 0.39, 0.29, 0.16, 0.47, 0.23, 0.12, 0.18, 0.39, 0.15, 0.1475, 0.72, 0.39, 0.04, 0.18, 0.53, 0.48, 0.22, 0.6, 0.31, 0.21, 0.15, 0.14, 0.33, 0.33, 0.12, 0.11, 0.3, 0.37, 0.44, 0.26, 0.1, 0.13, 0.05, 0.14, 0.05, 0.08, 0.16, 0.29, 0.18, 0.22, 0.24, 0.27, 0.31, 0.22, 0.04, 0.5, 0.19, 0.36, 0.14, 0.24, 0.04, 0.07, 0.06, 0.23, 0.13, 0.15, 0.23, 0.3, 0.08, 0.14, 0.19, 0.34, 0.22, 0.21, 0.3, 0.21, 0.12, 0.07, 0.19, 0.03, 0.29, 0.08, 0.04, 0.33, 0.0975, 0.37, 0.01, 0.03, 0.61, 0.05, 0.28, 0.26, 0.01, 0.05, 0.12, 0.31, 0.21, 0.34, 0.12, 0.3, 0.21, 0.21, 0.21, 0.4, 0.3275, 0.16, 0.02, 0.265, 0.27, 0.12, 0.21, 0.23, 0.31, 0.05, 0.01, 0.23, 0.5366666666666666, 0.26, 0.58, 0.41, 0.36, 0.42, 0.2, 0.02, 0.17, 0.18, 0.32, 0.24, 0.15, 0.11, 0.56, 0.26, 0.34, 0.03, 0.1, 0.36, 0.08, 0.1, 0.14, 0.45, 0.59, 0.18, 0.18, 0.21, 0.37, 0.03, 0.21, 0.05, 0.38, 0.43, 0.35, 0.19, 0.34, 0.41, 0.3, 0.09, 0.16, 0.08, 0.15, 0.4, 0.16, 0.38, 0.06, 0.05, 0.2, 0.13, 0.28, 0.24, 0.23, 0.15, 0.3, 0.27, 0.35, 0.31, 0.21, 0.08, 0.15, 0.09, 0.29, 0.46, 0.14, 0.3, 0.2, 0.21, 0.05, 0.13, 0.24, 0.02, 0.18, 0.6, 0.12, 0.09, 0.45, 0.08, 0.1, 0.31, 0.14, 0.21, 0.25, 0.25, 0.3, 0.2, 0.44, 0.26, 0.23, 0.16, 0.18, 0.28, 0.37, 0.65, 0.36, 0.45, 0.11, 0.2, 0.25, 0.1, 0.36, 0.19, 0.05, 0.18, 0.02, 0.35, 0.31, 0.13, 0.44, 0.16, 0.24, 0.51, 0.03, 0.12, 0.26, 0.28, 0.05, 0.39, 0.58, 0.05, 0.04, 0.22, 0.4, 0.1, 0.05, 0.14, 0.07, 0.42, 0.68, 0.23, 0.08, 0.22, 0.2575, 0.09, 0.24, 0.06, 0.71, 0.28, 0.02, 0.36, 0.15, 0.62, 0.29, 0.29, 0.36, 0.53, 0.39, 0.35, 0.37, 0.25, 0.09, 0.29, 0.05, 0.18, 0.25, 0.27, 0.14, 0.22, 0.45, 0.41, 0.25, 0.19, 0.18, 0.06, 0.18, 0.11, 0.55, 0.37, 0.08, 0.29, 0.1, 0.33, 0.16, 0.1, 0.04, 0.45, 0.26, 0.24, 0.33, 0.13, 0.15, 0.29, 0.17, 0.29, 0.18, 0.27, 0.02, 0.22, 0.33, 0.04, 0.09, 0.13, 0.43, 0.16, 0.29, 0.19, 0.02, 0.04, 0.01, 0.21, 0.16, 0.4075, 0.34, 0.16, 0.03, 0.14, 0.28, 0.18, 0.07, 0.29, 0.67, 0.1, 0.21, 0.03, 0.02, 0.48, 0.27, 0.17, 0.08, 0.36, 0.08, 0.1, 0.5, 0.14, 0.04, 0.45, 0.32, 0.31, 0.26, 0.05, 0.45, 0.19, 0.05, 0.1, 0.23, 0.17, 0.17, 0.17, 0.18, 0.17, 0.16, 0.18, 0.04, 0.07, 0.14, 0.45, 0.5, 0.05, 0.09, 0.22, 0.17, 0.19, 0.56, 0.22, 0.23, 0.42, 0.2, 0.15, 0.1, 0.05, 0.37, 0.21, 0.19, 0.09, 0.14, 0.1, 0.35, 0.41, 0.05, 0.17, 0.09, 0.15, 0.2633333333333333, 0.04, 0.29, 0.49, 0.1, 0.11, 0.1, 0.19, 0.29, 0.07, 0.02, 0.12, 0.18, 0.1, 0.36, 0.02, 0.36, 0.21, 0.57, 0.44, 0.18, 0.16, 0.62, 0.07, 0.06, 0.18, 0.49, 0.31, 0.44, 0.235, 0.3, 0.66, 0.13, 0.05, 0.07, 0.25, 0.18, 0.04, 0.16, 0.42, 0.25, 0.13, 0.08, 0.13, 0.44666666666666666, 0.07, 0.18, 0.41, 0.11, 0.08, 0.08, 0.25, 0.03, 0.54, 0.08, 0.23, 0.62, 0.03, 0.2, 0.24, 0.31, 0.11, 0.11, 0.03, 0.4, 0.3, 0.31, 0.4, 0.54, 0.45, 0.42, 0.41, 0.12, 0.11, 0.26, 0.21, 0.38, 0.13, 0.03, 0.36, 0.22, 0.13, 0.01, 0.15, 0.2, 0.21, 0.06, 0.04, 0.19, 0.25]</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>[0.54, 0.58, 0.2, 0.87, 0.81, 0.65, 0.66, 0.63, 0.76, 0.28, 0.62, 0.78, 0.63, 0.85, 0.93, 0.48, 0.67, 0.59, 0.39, 0.87, 0.9, 0.64, 0.97, 0.39, 0.49, 0.58, 0.73, 0.45, 0.58, 0.5, 0.42, 0.6, 0.94, 0.93, 0.68, 0.87, 0.94, 0.44, 0.93, 0.84, 0.95, 0.94, 0.83, 0.35, 0.61, 0.65, 0.97, 0.95, 0.68, 0.78, 0.73, 0.56, 0.77, 0.63, 0.88, 0.51, 0.69, 0.64, 0.86, 0.67, 0.66, 0.76, 0.83, 0.64, 0.9, 0.89, 0.87, 0.42, 0.88, 0.76, 0.66, 0.85, 0.76, 0.73, 0.88, 0.85, 0.83, 0.95, 0.87, 0.53, 0.51, 0.94, 0.5, 0.94, 0.92, 0.71, 0.46, 0.5, 0.85, 0.8, 0.72, 0.85, 0.78, 0.99, 0.84, 0.69, 0.52, 0.72, 0.64, 0.96, 0.7, 0.58, 0.62, 0.62, 0.85, 0.66, 0.92, 0.53, 0.51, 0.9, 0.41, 0.9, 0.73, 0.81, 0.73, 0.89, 0.61, 0.59, 0.73, 0.44, 0.83, 0.53, 0.68, 0.88, 0.75, 0.81, 0.48, 0.85, 0.66, 0.9, 0.31, 0.53, 0.26, 0.72, 0.79, 0.86, 0.84, 0.49, 0.78, 0.63, 0.85, 0.75, 0.84, 0.51, 0.74, 0.65, 0.49, 0.67, 0.89, 0.81, 0.76, 0.47, 0.62, 0.63, 0.8, 0.8, 0.49, 0.75, 0.83, 0.64, 0.46, 0.49, 0.42, 0.61, 0.57, 0.7, 0.6, 0.61, 0.59, 0.89, 0.44, 0.76, 0.7, 0.59, 0.6, 0.55, 0.52, 0.59, 0.83, 0.72, 0.72, 0.83, 0.42, 0.89, 0.67, 0.65, 0.7, 0.83, 0.33, 0.86, 0.9, 0.76, 0.57, 0.49, 0.72, 0.62, 0.81, 0.63, 0.58, 0.95, 0.66, 0.73, 0.64, 0.74, 0.6, 0.67, 0.69, 0.4, 0.76, 0.91, 0.5, 0.94, 0.83, 0.43, 0.78, 0.82, 0.87, 0.77, 0.56, 0.6, 0.67, 0.59, 0.54, 0.68, 0.23, 0.72, 0.6, 0.39, 0.44, 0.36, 0.95, 0.66, 0.86, 0.65, 0.65, 0.49, 0.37, 0.42, 0.28, 0.33, 0.7, 0.35, 0.23, 0.32, 0.61, 0.69, 0.8, 0.6, 0.66, 0.76, 0.35, 0.92, 0.85, 0.54, 0.58, 0.61, 0.5, 0.72, 0.9, 0.92, 0.51, 0.48, 0.94, 0.69, 0.48, 0.53, 0.56, 0.39, 0.6, 0.28, 0.51, 0.63, 0.72, 0.79, 0.62, 0.46, 0.43, 0.97, 0.82, 0.67, 0.53, 0.48, 0.92, 0.78, 0.48, 0.61, 0.53, 0.86, 0.38, 0.71, 0.8, 0.6, 0.55, 0.77, 0.84, 0.85, 0.65, 0.51, 0.54, 0.44, 0.44, 0.55, 0.87, 0.52, 0.41, 0.74, 0.54, 0.57, 0.93, 0.94, 0.37, 0.6, 0.35, 0.89, 0.53, 0.79, 0.62, 0.67, 0.63, 0.93, 0.43, 0.56, 0.93, 0.82, 0.42, 0.84, 0.53, 0.67, 0.77, 0.67, 0.6, 0.68, 0.87, 0.72, 0.66, 0.44, 0.63, 0.78, 0.75, 0.32, 0.44, 0.61, 0.7, 0.43, 0.48, 0.65, 0.73, 0.84, 0.69, 0.78, 0.72, 0.75, 0.45, 0.78, 0.86, 0.67, 0.83, 0.51, 0.66, 0.86, 0.61, 0.52, 0.36, 0.58, 0.62, 0.96, 0.456, 0.73, 0.63, 0.66, 0.64, 0.6, 0.68, 0.41, 0.76, 0.75, 0.46, 0.82, 0.8, 0.63, 0.93, 0.8, 0.93, 0.68, 0.74, 0.705, 0.42, 0.61, 0.59, 0.53, 0.27, 0.91, 0.6, 0.88, 0.63, 0.82, 0.9, 0.54, 0.97, 0.61, 0.43, 0.77, 0.66, 0.71, 0.56, 0.52, 0.54, 0.53, 0.63, 0.59, 0.91, 0.71, 0.89, 0.68, 0.57, 0.89, 0.5, 0.66, 0.35, 0.64, 0.53, 0.46, 0.85, 0.46, 0.41, 0.44, 0.55, 0.39, 0.37, 0.29, 0.68, 0.43, 0.71, 0.52, 0.6, 0.8, 0.24, 0.59, 0.39, 0.65, 0.72, 0.37, 0.98, 0.62, 0.82, 0.72, 0.79, 0.9, 0.69, 0.71, 0.56, 0.43, 0.35, 0.91, 0.63, 0.31, 0.83, 0.4, 0.7, 0.82, 0.79, 0.24, 0.56, 0.72, 0.45, 0.62, 0.48, 0.51, 0.6, 0.66, 0.85, 0.83, 0.58, 0.76, 0.53, 0.41, 0.71, 0.46, 0.71, 0.55, 0.26, 0.84, 0.39, 0.44, 0.7766666666666667, 0.58, 0.56, 0.64, 0.62, 0.28, 0.78, 0.61, 0.74, 0.67, 0.8466666666666667, 0.58, 0.51, 0.66, 0.39, 0.66, 0.44, 0.77, 0.33, 0.72, 0.56, 0.44, 0.45, 0.84, 0.49, 0.66, 0.64, 0.66, 0.86, 0.3766666666666667, 0.64, 0.56, 0.4, 0.62, 0.75, 0.57, 0.7, 0.86, 0.85, 0.27, 0.81, 0.73, 0.55, 0.7, 0.55, 0.59, 0.44, 0.78, 0.79, 0.67, 0.65, 0.57, 0.55, 0.8, 0.91, 0.36, 0.43, 0.43, 0.83, 0.42, 0.46, 0.41, 0.81, 0.52, 0.54, 0.66, 0.7, 0.47, 0.67, 0.34, 0.5, 0.64, 0.63, 0.62, 0.43, 0.51, 0.69, 0.54, 0.88, 0.9, 0.98, 0.59, 0.78, 0.92, 0.49, 0.56, 0.62, 0.6233333333333334, 0.62, 0.36, 0.6, 0.75, 0.99, 0.77, 0.96, 0.59, 0.76, 0.16, 0.96, 0.59, 0.78, 0.93, 0.72, 0.84, 0.33, 0.59, 0.65, 0.61, 0.62, 0.6, 0.74, 0.82, 0.91, 0.72, 0.43, 0.71, 0.68, 0.35, 0.57, 0.73, 0.72, 0.67, 0.8, 0.94, 0.7, 0.71, 0.97, 0.95, 0.87, 0.23, 0.37, 0.41, 0.65, 0.7, 0.35, 0.51, 0.82, 0.72, 0.7, 0.54, 0.94, 0.72, 0.81, 0.69, 0.96, 0.78, 0.7, 0.69, 0.75, 0.26, 0.71, 0.84, 0.85, 0.87, 0.71, 0.92, 0.53, 0.68, 0.77, 0.37, 0.69, 0.71, 0.7, 0.73, 0.9, 0.49, 0.49, 0.91, 0.39, 0.7, 0.95, 0.58, 0.52, 0.65, 0.48, 0.84, 0.49, 0.58, 0.95, 0.38, 0.81, 0.68, 0.91, 0.68, 0.89, 0.46, 0.66, 0.46, 0.9, 0.67, 0.83, 0.92, 0.76, 0.58, 0.72, 0.86, 0.86, 0.59, 0.64, 0.99, 0.94, 0.94, 0.64, 0.66, 0.75, 0.88, 0.91, 0.7, 0.9, 0.835, 0.71, 0.77, 0.65, 0.66, 0.73, 0.93, 0.48, 0.68, 0.72, 0.75, 0.74, 0.34, 0.59, 0.86, 0.56, 0.65, 0.89, 0.58, 0.5, 0.44, 0.78, 0.83, 0.42, 0.76, 0.88, 0.6, 0.74, 0.6, 0.57, 0.66, 0.57, 0.81, 0.73, 0.94, 0.74, 0.84, 0.82, 0.61, 0.57, 0.34, 0.62, 0.61, 0.75, 0.54, 0.44, 0.37, 0.76, 0.78, 0.72, 0.54, 0.5, 0.53, 0.72, 0.38, 0.9, 0.6, 0.8, 0.92, 0.38, 0.59, 0.88, 0.98, 0.65, 0.78, 0.38, 0.95, 0.89, 0.7, 0.81, 0.54, 0.53, 0.93, 0.51, 0.55, 0.66, 0.94, 0.39, 0.7, 0.96, 0.98, 0.95, 0.76, 0.97, 0.74, 0.37, 0.45, 0.67, 0.78, 0.31, 0.96, 0.75, 0.87, 0.96, 0.94, 0.98, 0.86, 0.96, 0.97, 0.85, 0.67, 0.59, 0.72, 0.97, 0.94, 0.96, 0.81, 0.975, 0.62, 0.45, 0.98, 0.63, 0.67, 0.97, 0.53, 0.8, 0.96, 0.96, 0.85, 0.76, 0.66, 0.97, 0.92, 0.39, 0.93, 0.97, 0.98, 0.7, 0.5, 0.93, 0.69, 0.89, 0.67, 0.93, 0.86, 0.49, 0.65, 0.95, 0.68, 0.83, 0.58, 0.83, 0.68, 0.6, 0.96, 0.99, 0.76, 0.25, 0.96, 0.84, 0.75, 0.96, 0.99, 0.9, 0.95, 0.96, 0.75, 0.78, 0.79, 0.44, 0.5, 0.79, 0.9, 0.95, 0.76, 0.76, 0.78, 0.77, 0.5, 0.8, 0.67, 0.98, 0.61, 0.8, 0.98, 0.83, 0.56, 0.68, 0.83, 0.98, 0.85, 0.66, 0.85, 0.97, 0.95, 0.6, 0.64, 0.57, 0.78, 0.73, 0.6, 0.7, 0.83, 0.43, 0.47, 0.61, 0.5, 0.53, 0.97, 0.66, 0.99, 0.94, 0.56, 0.92, 0.67, 0.95, 0.33, 0.57, 0.89, 0.9, 0.9, 0.9, 0.91, 0.9, 0.43, 0.91, 0.48, 0.91, 0.97, 0.82, 0.77, 0.99, 0.8375, 0.76, 0.78, 0.99, 0.67, 0.78, 0.79, 0.37, 0.2, 0.76, 0.41, 0.98, 0.84, 0.25, 0.75, 0.96, 0.96, 0.89, 0.98, 0.54, 0.4, 0.7, 0.74, 0.52, 0.97, 0.61, 0.97, 0.555, 0.63, 0.69, 0.56, 0.97, 0.99, 0.88, 0.41, 0.26, 0.54, 0.83, 0.84, 0.99, 0.74, 0.46, 0.93, 0.47, 0.52, 0.88, 0.6, 0.48, 0.99, 0.65, 0.92, 0.5, 0.93, 0.74, 0.81, 0.91, 0.88, 0.77, 0.38, 0.59, 0.44, 0.93, 0.97, 0.79, 0.51, 0.94, 0.63, 0.84, 0.77, 0.53, 0.55, 0.92, 0.47, 0.81, 0.9, 0.79, 0.68, 0.91, 0.23, 0.48, 0.48, 0.56, 0.71, 0.44, 0.75, 0.96, 0.61, 0.44, 0.64, 0.82, 0.98, 0.57, 0.58, 0.54, 0.61, 0.52, 0.64, 0.91, 0.7, 0.94, 0.6, 0.77, 0.46, 0.68, 0.69, 0.83, 0.87, 0.94, 0.82, 0.585, 0.82, 0.8175, 0.8, 0.98, 0.7, 0.99, 0.99, 0.78, 0.83, 0.72, 0.58, 0.77, 0.86, 0.54, 0.99, 0.34, 0.6, 0.96, 0.81, 0.38, 0.79, 0.57, 0.96, 0.52, 0.98, 0.81, 0.93, 0.58, 0.72, 0.995, 0.83, 0.93, 0.8, 0.92, 0.72, 0.23, 0.97, 0.81, 0.46, 0.74, 0.97, 0.6, 0.71, 0.58, 0.79, 0.94, 0.73, 0.76, 0.93, 0.54, 0.7, 0.73, 0.88, 0.78, 0.8, 0.81, 0.71, 0.67, 0.89, 0.84, 0.98, 0.41, 0.93, 0.68, 0.93, 0.64, 0.6, 0.93, 0.85, 0.79, 0.7, 0.94, 0.88, 0.48, 0.49, 0.87, 0.56, 0.86, 0.36, 0.74, 0.6, 0.63, 0.66, 0.51, 0.61, 0.81, 0.42, 0.89, 0.92, 0.74, 0.73, 0.84, 0.86, 0.45, 0.7, 0.85, 0.88, 0.69, 0.85, 0.59, 0.67, 0.97, 0.61, 0.91, 0.67, 0.84, 0.75, 0.635, 0.76, 0.81, 0.88, 0.41, 0.59, 0.65, 0.87, 0.73, 0.56, 0.76, 0.8, 0.93, 0.83, 0.62, 0.72, 0.99, 0.93, 0.8, 0.7, 0.4, 0.53, 0.18, 0.63, 0.75, 0.72, 0.93, 0.5033333333333334, 0.61, 0.91, 0.31, 0.95, 0.24, 0.81, 0.5, 0.22, 0.9, 0.61, 0.46, 0.79, 0.12, 0.94, 0.68, 0.8, 0.84, 0.45, 0.47, 0.09, 0.77, 0.26, 0.9, 0.54, 0.4, 0.34, 0.94, 0.76, 0.655, 0.82, 0.52, 0.75, 0.67, 0.98, 0.41, 0.73, 0.47, 0.56, 0.32, 0.44, 0.73, 0.78, 0.35, 0.75, 0.43, 0.66, 0.47, 0.68, 0.94, 0.46, 0.35, 0.83, 0.97, 0.78, 0.97, 0.7, 0.51, 0.98, 0.29, 0.64, 0.6, 0.37, 0.4, 0.55, 0.6, 0.46, 0.645, 0.75, 1.0, 0.89, 0.9, 0.73, 0.82, 0.33, 0.38, 0.55, 0.57, 0.55, 0.37, 0.58, 0.57, 0.83, 0.93, 0.84, 0.99, 0.98, 0.5, 0.47, 0.88, 0.6, 0.84, 0.5, 0.48, 0.55, 0.66, 0.44, 0.86, 0.93, 0.39, 0.3, 0.67, 0.39, 0.61, 0.67, 0.88, 0.21, 0.98, 0.65, 0.73, 0.82, 0.99, 0.57, 0.83, 0.23, 0.62, 0.76, 0.14, 0.49, 0.41, 0.79, 0.58, 0.79, 0.64, 0.59, 0.86, 0.92, 0.86, 0.8, 0.86, 0.95, 0.54, 0.46, 0.37, 0.68, 0.76, 0.37, 0.65, 0.69, 0.375, 0.74, 0.78, 0.38, 0.56, 0.48, 0.86, 0.34, 0.82, 0.54, 0.98, 0.66, 0.53, 0.72, 0.91, 0.94, 0.71, 0.88, 0.88, 0.53, 0.83, 0.39, 0.67, 0.98, 0.76, 0.9, 0.61, 0.7, 0.85, 0.84, 0.54, 0.74, 0.76, 0.36, 0.72, 0.74, 0.76, 0.44, 0.53, 0.58, 0.98, 0.78, 0.12, 0.86, 0.51, 0.23, 0.62, 0.98, 0.7, 0.47, 0.72, 0.8, 0.77, 0.54, 0.32, 0.56, 0.64, 0.59, 0.97, 0.9, 0.68, 0.86, 0.91, 0.88, 0.48, 0.69, 0.63, 0.63, 0.22, 0.78, 0.96, 0.77, 0.86, 0.97, 0.55, 0.62, 0.68, 0.62, 0.66, 0.99, 0.52, 0.61, 0.37, 0.7, 0.65, 0.59, 0.9, 0.51, 0.7, 0.47, 0.57, 0.82, 0.6, 0.69, 0.68, 0.24, 0.82, 0.77, 0.91, 0.8, 0.77, 0.48, 0.37, 0.93, 0.88, 0.78, 0.96, 0.94, 0.66, 0.27, 0.74, 0.13, 0.06, 0.45, 0.12, 0.06, 0.31, 0.08, 0.21, 0.14, 0.44, 0.44, 0.21, 0.09, 0.08, 0.52, 0.13, 0.4, 0.32, 0.34, 0.5, 0.41, 0.53, 0.49, 0.34, 0.24, 0.26, 0.26, 0.13, 0.36, 0.44, 0.43, 0.24, 0.63, 0.61, 0.34, 0.06, 0.39, 0.47, 0.53, 0.35, 0.28, 0.13, 0.09, 0.29, 0.11, 0.34, 0.78, 0.07, 0.2, 0.32, 0.19, 0.3, 0.24, 0.27, 0.44, 0.04, 0.44, 0.3, 0.06, 0.69, 0.09, 0.47, 0.14, 0.29, 0.24, 0.39, 0.22, 0.36, 0.61, 0.56, 0.4, 0.92, 0.27, 0.42, 0.16, 0.24, 0.18, 0.07, 0.23, 0.31, 0.18, 0.67, 0.7, 0.55, 0.29, 0.1, 0.59, 0.43, 0.14, 0.21, 0.2, 0.53, 0.29, 0.53, 0.2, 0.43, 0.44, 0.47, 0.43, 0.69, 0.09, 0.58, 0.77, 0.62, 0.43, 0.2, 0.53, 0.39, 0.33, 0.17, 0.43, 0.11, 0.31, 0.68, 0.24, 0.33, 0.12, 0.22, 0.45, 0.67, 0.2, 0.07, 0.2, 0.35, 0.22, 0.1, 0.22, 0.32, 0.14, 0.55, 0.45, 0.21, 0.11, 0.11, 0.41, 0.15, 0.34, 0.27, 0.43, 0.54, 0.22, 0.32, 0.15, 0.58, 0.66, 0.59, 0.67, 0.1, 0.05, 0.07, 0.61, 0.2, 0.06, 0.26, 0.18, 0.3, 0.33, 0.24, 0.2, 0.13, 0.45, 0.05, 0.47, 0.26, 0.55, 0.21, 0.17, 0.28, 0.03, 0.41, 0.35, 0.33, 0.18, 0.23, 0.21, 0.18, 0.11, 0.81, 0.03, 0.09, 0.49, 0.11, 0.34, 0.26, 0.4, 0.29, 0.15, 0.32, 0.69, 0.4, 0.16, 0.17, 0.37, 0.49, 0.1, 0.3, 0.26, 0.05, 0.44, 0.14, 0.5, 0.31, 0.19, 0.32, 0.24, 0.07, 0.2, 0.03, 0.67, 0.17, 0.14, 0.25, 0.44, 0.13, 0.28, 0.24, 0.19, 0.16, 0.46, 0.12, 0.44, 0.74, 0.1, 0.28, 0.3, 0.25, 0.05, 0.33, 0.11, 0.39, 0.33, 0.285, 0.19, 0.54, 0.34, 0.36, 0.25, 0.35, 0.43, 0.3, 0.3, 0.36, 0.46, 0.32, 0.47, 0.31, 0.41, 0.19, 0.3, 0.0, 0.4, 0.32, 0.03, 0.43, 0.16, 0.39, 0.3, 0.25, 0.34, 0.16, 0.37, 0.29, 0.38, 0.4, 0.4, 0.52, 0.01, 0.15, 0.13, 0.13, 0.34, 0.11, 0.17, 0.26, 0.15, 0.18, 0.06, 0.3, 0.61, 0.36, 0.12, 0.25, 0.15, 0.19, 0.13, 0.24, 0.19, 0.09, 0.08, 0.4, 0.26, 0.26, 0.15, 0.39, 0.26, 0.52, 0.45, 0.06, 0.32, 0.29, 0.28, 0.29, 0.73, 0.0, 0.5, 0.28, 0.07, 0.64, 0.33, 0.25, 0.46, 0.15, 0.3, 0.14, 0.11, 0.27, 0.09, 0.16, 0.32, 0.27, 0.08, 0.16, 0.15, 0.49, 0.65, 0.54, 0.04, 0.07, 0.36, 0.26, 0.07, 0.08, 0.12, 0.22, 0.04, 0.31, 0.56, 0.22, 0.15, 0.24, 0.26, 0.4, 0.47, 0.26, 0.1, 0.09, 0.32, 0.04, 0.14, 0.19, 0.3, 0.54, 0.33, 0.08, 0.41, 0.3, 0.03, 0.22, 0.43, 0.18, 0.23, 0.59, 0.25, 0.23, 0.27, 0.18, 0.32, 0.74, 0.2, 0.08, 0.2, 0.39, 0.27, 0.15, 0.66, 0.0, 0.21, 0.235, 0.49, 0.48, 0.18, 0.3, 0.44, 0.3, 0.11, 0.42, 0.28, 0.44, 0.38, 0.49, 0.26, 0.72, 0.41, 0.43, 0.09, 0.23, 0.39, 0.37, 0.18, 0.44, 0.46, 0.36, 0.41, 0.54, 0.83, 0.13, 0.32, 0.46, 0.4, 0.12, 0.21, 0.63, 0.11, 0.46, 0.19, 0.1, 0.22, 0.1, 0.27, 0.06, 0.24, 0.35, 0.33, 0.0, 0.47, 0.16, 0.39, 0.51, 0.27, 0.14, 0.14, 0.3575, 0.51, 0.48, 0.27, 0.47, 0.21, 0.27, 0.51, 0.33, 0.44, 0.43, 0.18, 0.22, 0.25, 0.41, 0.24, 0.39, 0.39, 0.69, 0.47, 0.38, 0.17, 0.13, 0.53, 0.2, 0.43, 0.26, 0.22, 0.29, 0.45, 0.26, 0.04, 0.42, 0.23, 0.6, 0.57, 0.26, 0.34, 0.23, 0.37, 0.5, 0.17, 0.57, 0.75, 0.36, 0.12, 0.27, 0.23, 0.23, 0.11, 0.35, 0.31, 0.11, 0.73, 0.75, 0.51, 0.25, 0.41, 0.04, 0.32, 0.39, 0.13, 0.16, 0.06, 0.45, 0.23, 0.37, 0.32, 0.18, 0.35, 0.58, 0.32, 0.08, 0.52, 0.22, 0.39, 0.43, 0.44, 0.23, 0.33, 0.24, 0.2, 0.455, 0.26, 0.63, 0.15, 0.64, 0.09, 0.1, 0.34, 0.07, 0.11, 0.47, 0.35, 0.22, 0.15, 0.22, 0.77, 0.18, 0.19, 0.66, 0.55, 0.34, 0.13, 0.56, 0.14, 0.25, 0.33, 0.26, 0.57, 0.2, 0.25, 0.26, 0.44, 0.29, 0.01, 0.13, 0.04, 0.24, 0.29, 0.36, 0.06, 0.21, 0.21, 0.68, 0.18, 0.57, 0.6, 0.41, 0.22, 0.17, 0.07, 0.24, 0.89, 0.24, 0.48, 0.27, 0.16, 0.29, 0.51, 0.5, 0.565, 0.33, 0.37, 0.63, 0.11, 0.25, 0.41, 0.15, 0.76, 0.51, 0.14, 0.13, 0.49, 0.07, 0.26, 0.21, 0.37, 0.19, 0.25, 0.65, 0.28, 0.29, 0.3, 0.15, 0.07, 0.09, 0.51, 0.17, 0.67, 0.32, 0.45, 0.17, 0.18, 0.17, 0.18, 0.04, 0.53, 0.29, 0.52, 0.31, 0.27, 0.33, 0.17, 0.28, 0.47, 0.64, 0.55, 0.44, 0.73, 0.33, 0.54, 0.19, 0.33, 0.06, 0.37, 0.06, 0.43, 0.25, 0.15, 0.06, 0.21, 0.14, 0.25, 0.25, 0.54, 0.05, 0.36, 0.29, 0.35, 0.45, 0.45, 0.27, 0.18, 0.12, 0.24, 0.35, 0.2, 0.46, 0.01, 0.31, 0.13, 0.22, 0.38, 0.12, 0.34, 0.08, 0.43, 0.55, 0.4, 0.19, 0.6, 0.15, 0.14, 0.14, 0.12, 0.48, 0.11, 0.28, 0.15, 0.13, 0.35, 0.39, 0.38, 0.14, 0.2, 0.4, 0.13, 0.3066666666666667, 0.67, 0.31, 0.14, 0.23, 0.2, 0.26, 0.08, 0.45, 0.14, 0.17, 0.53, 0.19, 0.33, 0.26, 0.47, 0.54, 0.29, 0.68, 0.62, 0.35, 0.24, 0.69, 0.43, 0.21, 0.53, 0.08, 0.39, 0.15, 0.1, 0.06, 0.13, 0.65, 0.17, 0.58, 0.43, 0.56, 0.13, 0.23, 0.26, 0.12, 0.09, 0.16, 0.21, 0.21, 0.13, 0.01, 0.46, 0.32, 0.24, 0.41, 0.52, 0.06, 0.29, 0.28, 0.36, 0.555, 0.14, 0.22, 0.19, 0.18, 0.33, 0.28, 0.32, 0.37, 0.15, 0.45, 0.23, 0.37, 0.07, 0.51, 0.32, 0.08, 0.06, 0.49, 0.2, 0.71, 0.29, 0.32, 0.28, 0.15, 0.27, 0.41, 0.17, 0.25, 0.09, 0.34, 0.27, 0.24, 0.16, 0.26, 0.08, 0.51, 0.28, 0.82, 0.28, 0.33, 0.17, 0.52, 0.27, 0.08, 0.44, 0.21, 0.35, 0.18, 0.1, 0.21, 0.52, 0.465, 0.11, 0.14, 0.7, 0.34, 0.64, 0.49, 0.09, 0.19, 0.29, 0.56, 0.4, 0.08, 0.12, 0.41, 0.59, 0.49, 0.25, 0.22, 0.07, 0.31, 0.32, 0.04, 0.44, 0.0, 0.53, 0.13, 0.3, 0.31, 0.14, 0.19, 0.3, 0.06, 0.31, 0.26, 0.16, 0.4, 0.25, 0.12, 0.25, 0.09, 0.21, 0.13, 0.34, 0.54, 0.38, 0.16, 0.41, 0.34, 0.27, 0.04, 0.05]</t>
+          <t>[0.58, 0.55, 0.21, 0.9, 0.77, 0.64, 0.68, 0.62, 0.71, 0.35, 0.66, 0.82, 0.59, 0.87, 0.91, 0.5, 0.62, 0.65, 0.46, 0.87, 0.92, 0.48, 0.93, 0.39, 0.57, 0.68, 0.75, 0.4, 0.59, 0.47, 0.35, 0.56, 0.94, 0.92, 0.64, 0.82, 0.92, 0.5, 0.93, 0.84, 0.99, 0.88, 0.85, 0.32, 0.68, 0.58, 0.98, 0.91, 0.76, 0.79, 0.82, 0.55, 0.76, 0.78, 0.95, 0.55, 0.7, 0.69, 0.83, 0.66, 0.55, 0.89, 0.76, 0.67, 0.9, 0.92, 0.83, 0.42, 0.89, 0.8, 0.54, 0.82, 0.71, 0.77, 0.86, 0.94, 0.84, 0.95, 0.88, 0.64, 0.62, 0.95, 0.43, 0.87, 0.93, 0.73, 0.63, 0.54, 0.86, 0.85, 0.77, 0.82, 0.76, 0.92, 0.89, 0.65, 0.49, 0.71, 0.79, 0.95, 0.74, 0.39, 0.66, 0.63, 0.85, 0.68, 0.99, 0.59, 0.58, 0.93, 0.44, 0.93, 0.77, 0.78, 0.79, 0.87, 0.59, 0.59, 0.58, 0.46, 0.79, 0.73, 0.7, 0.96, 0.75, 0.79, 0.58, 0.89, 0.61, 0.86, 0.36, 0.61, 0.33, 0.74, 0.69, 0.78, 0.85, 0.71, 0.65, 0.61, 0.85, 0.66, 0.85, 0.66, 0.69, 0.65, 0.6, 0.81, 0.89, 0.8, 0.79, 0.42, 0.5, 0.58, 0.8, 0.74, 0.56, 0.74, 0.82, 0.69, 0.3, 0.54, 0.35, 0.58, 0.63, 0.67, 0.69, 0.63, 0.47, 0.91, 0.32, 0.69, 0.78, 0.5, 0.61, 0.6, 0.44, 0.69, 0.79, 0.75, 0.65, 0.82, 0.51, 0.85, 0.61, 0.61, 0.69, 0.77, 0.32, 0.86, 0.88, 0.79, 0.58, 0.45, 0.64, 0.72, 0.92, 0.7, 0.52, 0.88, 0.65, 0.67, 0.74, 0.65, 0.61, 0.65, 0.76, 0.34, 0.81, 0.84, 0.4, 0.91, 0.89, 0.36, 0.8, 0.88, 0.86, 0.77, 0.49, 0.58, 0.62, 0.52, 0.49, 0.71, 0.21, 0.7, 0.59, 0.44, 0.43, 0.39, 0.93, 0.62, 0.86, 0.8, 0.59, 0.55, 0.41, 0.37, 0.29, 0.28, 0.66, 0.24, 0.33, 0.3, 0.54, 0.63, 0.73, 0.63, 0.63, 0.64, 0.38, 0.94, 0.87, 0.53, 0.71, 0.72, 0.57, 0.72, 0.88, 0.96, 0.54, 0.44, 0.9, 0.55, 0.4, 0.43, 0.55, 0.59, 0.53, 0.505, 0.51, 0.59, 0.79, 0.69, 0.69, 0.37, 0.49, 0.97, 0.62, 0.78, 0.68, 0.48, 0.86, 0.78, 0.49, 0.51, 0.46, 0.88, 0.43, 0.78, 0.9, 0.53, 0.52, 0.83, 0.87, 0.87, 0.66, 0.49, 0.39, 0.48, 0.41, 0.5, 0.88, 0.49, 0.46, 0.79, 0.58, 0.43, 0.9, 0.89, 0.38, 0.52, 0.3, 0.9, 0.55, 0.71, 0.66, 0.76, 0.62, 0.95, 0.55, 0.51, 0.98, 0.85, 0.41, 0.86, 0.57, 0.78, 0.77, 0.7, 0.58, 0.66, 0.97, 0.71, 0.66, 0.52, 0.62, 0.75, 0.8, 0.26, 0.49, 0.55, 0.58, 0.45, 0.47, 0.68, 0.69, 0.83, 0.74, 0.7, 0.79, 0.86, 0.42, 0.78, 0.88, 0.6, 0.82, 0.52, 0.57, 0.8, 0.69, 0.5, 0.35, 0.61, 0.72, 0.99, 0.52, 0.72, 0.6, 0.7, 0.54, 0.51, 0.66, 0.38, 0.9, 0.71, 0.53, 0.77, 0.72, 0.69, 0.91, 0.76, 0.93, 0.68, 0.78, 0.74, 0.46, 0.7, 0.66, 0.62, 0.37, 0.94, 0.61, 0.91, 0.64, 0.8, 0.92, 0.53, 0.94, 0.67, 0.33, 0.74, 0.71, 0.78, 0.59, 0.35, 0.54, 0.55, 0.63, 0.52, 0.92, 0.65, 0.88, 0.7, 0.51, 0.84, 0.51, 0.64, 0.47, 0.78, 0.59, 0.44, 0.84, 0.49, 0.44, 0.36, 0.58, 0.36, 0.24, 0.31, 0.53, 0.39, 0.65, 0.44, 0.59, 0.67, 0.23, 0.67, 0.33, 0.65, 0.66, 0.32, 0.96, 0.77, 0.81, 0.84, 0.78, 0.96, 0.65, 0.76, 0.51, 0.31, 0.41, 0.93, 0.63, 0.33, 0.73, 0.39, 0.68, 0.775, 0.7, 0.15, 0.7, 0.73, 0.47, 0.55, 0.54, 0.45, 0.57, 0.69, 0.86, 0.89, 0.48, 0.73, 0.57, 0.46, 0.76, 0.64, 0.62, 0.42, 0.28, 0.89, 0.39, 0.35, 0.81, 0.57, 0.65, 0.66, 0.67, 0.14, 0.78, 0.57, 0.77, 0.7, 0.93, 0.48, 0.59, 0.68, 0.23, 0.8, 0.35, 0.76, 0.35, 0.74, 0.62, 0.37, 0.53, 0.79, 0.41, 0.66, 0.68, 0.73, 0.82, 0.39, 0.76, 0.61, 0.39, 0.52, 0.74, 0.64, 0.6, 0.82, 0.86, 0.33, 0.74, 0.74, 0.6, 0.73, 0.58, 0.58, 0.42, 0.79, 0.78, 0.62, 0.55, 0.64, 0.52, 0.83, 0.96, 0.32, 0.49, 0.52, 0.71, 0.41, 0.45, 0.26, 0.76, 0.5, 0.5, 0.67, 0.78, 0.48, 0.69, 0.39, 0.62, 0.75, 0.56, 0.53, 0.44, 0.61, 0.71, 0.47, 0.89, 0.85, 0.99, 0.49, 0.87, 0.94, 0.5, 0.58, 0.68, 0.54, 0.56, 0.38, 0.58, 0.76, 0.96, 0.85, 0.91, 0.64, 0.76, 0.24, 0.9, 0.53, 0.74, 0.94, 0.72, 0.74, 0.27, 0.58, 0.57, 0.56, 0.74, 0.62, 0.69, 0.8, 0.89, 0.64, 0.42, 0.68, 0.66, 0.35, 0.44, 0.78, 0.69, 0.53, 0.78, 0.95, 0.6, 0.73, 0.98, 0.93, 0.84, 0.21, 0.26, 0.36, 0.66, 0.65, 0.39, 0.44, 0.82, 0.74, 0.69, 0.57, 0.96, 0.79, 0.82, 0.85, 0.99, 0.76, 0.68, 0.71, 0.66, 0.29, 0.75, 0.82, 0.82, 0.87, 0.69, 0.94, 0.42, 0.58, 0.89, 0.45, 0.64, 0.71, 0.67, 0.77, 0.85, 0.48, 0.4, 0.93, 0.27, 0.72, 0.92, 0.59, 0.49, 0.59, 0.36, 0.94, 0.46, 0.58, 0.95, 0.48, 0.81, 0.67, 0.94, 0.72, 0.91, 0.46, 0.73, 0.39, 0.89, 0.67, 0.84, 0.94, 0.7, 0.48, 0.88, 0.87, 0.96, 0.52, 0.6, 0.98, 0.94, 0.95, 0.69, 0.71, 0.78, 0.87, 0.91, 0.64, 0.87, 0.88, 0.77, 0.87, 0.63, 0.55, 0.83, 0.94, 0.43, 0.76, 0.74, 0.69, 0.54, 0.45, 0.63, 0.88, 0.51, 0.59, 0.92, 0.63, 0.59, 0.5, 0.77, 0.83, 0.54, 0.7, 0.85, 0.55, 0.74, 0.53, 0.72, 0.68, 0.6, 0.73, 0.75, 0.95, 0.65, 0.8, 0.83, 0.62, 0.7, 0.41, 0.64, 0.53, 0.75, 0.645, 0.4, 0.37, 0.83, 0.87, 0.75, 0.67, 0.48, 0.54, 0.74, 0.31, 0.92, 0.58, 0.88, 0.93, 0.42, 0.7, 0.89, 0.97, 0.67, 0.82, 0.35, 0.98, 0.84, 0.74, 0.88, 0.59, 0.49, 0.91, 0.51, 0.54, 0.65, 0.97, 0.36, 0.73, 1.0, 0.9466666666666665, 0.96, 0.65, 0.95, 0.68, 0.41, 0.59, 0.45, 0.79, 0.23, 0.97, 0.67, 0.82, 0.95, 0.9, 0.98, 0.87, 0.98, 0.93, 0.91, 0.73, 0.48, 0.74, 0.86, 0.93, 0.91, 0.86, 0.93, 0.69, 0.5, 0.98, 0.59, 0.68, 0.98, 0.53, 0.78, 0.94, 0.92, 0.86, 0.72, 0.57, 0.95, 0.95, 0.55, 0.91, 0.98, 0.97, 0.6, 0.49, 0.93, 0.65, 0.89, 0.78, 0.95, 0.79, 0.5466666666666666, 0.66, 0.88, 0.66, 0.75, 0.56, 0.86, 0.69, 0.64, 0.96, 0.96, 0.8, 0.22, 0.96, 0.88, 0.78, 0.94, 0.99, 0.85, 0.97, 0.95, 0.71, 0.84, 0.78, 0.48, 0.42, 0.74, 0.87, 0.95, 0.76, 0.85, 0.8, 0.73, 0.53, 0.91, 0.5, 0.96, 0.66, 0.87, 0.92, 0.92, 0.34, 0.65, 0.84, 0.96, 0.78, 0.75, 0.75, 0.95, 0.94, 0.65, 0.58, 0.51, 0.78, 0.61, 0.66, 0.72, 0.85, 0.38, 0.44, 0.58, 0.48, 0.56, 0.97, 0.81, 0.94, 0.86, 0.57, 0.94, 0.64, 0.99, 0.42, 0.48, 0.9, 0.86, 0.86, 0.9, 0.98, 0.99, 0.45, 0.93, 0.53, 0.96, 0.99, 0.81, 0.68, 0.96, 0.86, 0.74, 0.76, 1.0, 0.58, 0.76, 0.82, 0.41, 0.2, 0.74, 0.41, 0.97, 0.84, 0.22, 0.8, 0.99, 0.97, 0.95, 0.97, 0.44, 0.43, 0.73, 0.84, 0.6, 0.97, 0.67, 0.95, 0.56, 0.81, 0.72, 0.62, 0.97, 0.96, 0.86, 0.31, 0.25, 0.6, 0.89, 0.8, 0.93, 0.84, 0.42, 0.89, 0.5, 0.55, 0.93, 0.6, 0.45, 0.97, 0.63, 0.87, 0.46, 0.99, 0.76, 0.75, 0.89, 0.85, 0.92, 0.41, 0.59, 0.39, 0.92, 0.9, 0.87, 0.56, 0.89, 0.66, 0.77, 0.73, 0.6, 0.67, 0.87, 0.4, 0.86, 0.93, 0.84, 0.6066666666666667, 0.86, 0.21, 0.41, 0.5, 0.69, 0.7, 0.42, 0.8, 0.92, 0.51, 0.48, 0.69, 0.81, 0.95, 0.62, 0.62, 0.63, 0.54, 0.46, 0.56, 0.84, 0.69, 0.95, 0.68, 0.83, 0.47, 0.655, 0.68, 0.82, 0.83, 0.97, 0.87, 0.64, 0.89, 0.8, 0.91, 0.95, 0.78, 0.97, 0.99, 0.8, 0.9, 0.65, 0.5, 0.74, 0.89, 0.65, 0.88, 0.28, 0.68, 0.98, 0.84, 0.4, 0.77, 0.7, 1.0, 0.45, 0.95, 0.87, 0.96, 0.61, 0.7, 0.94, 0.81, 0.92, 0.84, 0.92, 0.81, 0.21, 0.93, 0.79, 0.31, 0.61, 0.98, 0.58, 0.65, 0.71, 0.83, 0.89, 0.7, 0.73, 0.94, 0.55, 0.7, 0.79, 0.89, 0.84, 0.81, 0.81, 0.68, 0.69, 0.94, 0.89, 0.99, 0.43, 0.95, 0.76, 0.95, 0.55, 0.62, 0.96, 0.83, 0.82, 0.82, 0.88, 0.83, 0.37, 0.54, 0.84, 0.62, 0.9, 0.4, 0.67, 0.62, 0.62, 0.72, 0.51, 0.53, 0.73, 0.26, 0.9, 0.92, 0.7, 0.83, 0.9, 0.77, 0.48, 0.72, 0.92, 0.86, 0.71, 0.78, 0.66, 0.68, 0.93, 0.55, 0.95, 0.73, 0.83, 0.69, 0.58, 0.78, 0.87, 0.88, 0.43, 0.64, 0.67, 0.86, 0.73, 0.52, 0.78, 0.68, 0.88, 0.88, 0.64, 0.76, 0.94, 0.86, 0.8, 0.74, 0.41, 0.63, 0.19, 0.71, 0.78, 0.66, 0.88, 0.49, 0.59, 0.94, 0.37, 0.99, 0.28, 0.67, 0.48, 0.22, 0.87, 0.59, 0.34, 0.72, 0.21, 0.94, 0.68, 0.85, 0.86, 0.44, 0.46, 0.13, 0.79, 0.19, 0.91, 0.645, 0.35, 0.27, 0.89, 0.82, 0.54, 0.79, 0.54, 0.67, 0.58, 0.98, 0.41, 0.72, 0.34, 0.515, 0.35, 0.4, 0.78, 0.75, 0.3, 0.78, 0.37, 0.76, 0.515, 0.72, 0.9, 0.39, 0.29, 0.84, 0.99, 0.78, 0.98, 0.64, 0.63, 0.99, 0.32, 0.57, 0.58, 0.32, 0.52, 0.53, 0.62, 0.33, 0.6, 0.68, 0.93, 0.89, 0.87, 0.78, 0.88, 0.36, 0.43, 0.62, 0.48, 0.49, 0.34, 0.47, 0.58, 0.81, 0.9, 0.92, 0.91, 0.97, 0.445, 0.44, 0.81, 0.45, 0.86, 0.55, 0.44, 0.58, 0.63, 0.28, 0.88, 0.93, 0.44, 0.23, 0.75, 0.38, 0.57, 0.65, 0.93, 0.24, 0.98, 0.6, 0.72, 0.8566666666666667, 0.95, 0.55, 0.8, 0.24, 0.73, 0.75, 0.16, 0.67, 0.33, 0.81, 0.62, 0.76, 0.73, 0.6, 0.9, 0.91, 0.84, 0.8766666666666666, 0.8, 0.96, 0.56, 0.43, 0.47, 0.64, 0.75, 0.37, 0.52, 0.61, 0.33, 0.76, 0.73, 0.32, 0.52, 0.53, 0.8, 0.29, 0.8, 0.41, 0.97, 0.625, 0.44, 0.7, 0.95, 0.93, 0.76, 0.84, 0.94, 0.58, 0.75, 0.36, 0.56, 0.9666666666666666, 0.72, 0.94, 0.51, 0.68, 0.84, 0.86, 0.62, 0.67, 0.76, 0.52, 0.73, 0.68, 0.7, 0.45, 0.59, 0.56, 0.99, 0.87, 0.12, 0.82, 0.45, 0.37, 0.64, 0.88, 0.64, 0.52, 0.61, 0.73, 0.75, 0.5, 0.45, 0.58, 0.71, 0.61, 0.94, 0.84, 0.76, 0.88, 0.93, 0.92, 0.5, 0.65, 0.66, 0.59, 0.32, 0.71, 0.94, 0.7, 0.81, 0.91, 0.6, 0.65, 0.72, 0.62, 0.62, 1.0, 0.45, 0.61, 0.31, 0.67, 0.59, 0.65, 0.94, 0.6, 0.78, 0.59, 0.54, 0.86, 0.5, 0.59, 0.65, 0.23, 0.9, 0.68, 0.93, 0.86, 0.85, 0.58, 0.34, 0.96, 0.81, 0.84, 0.94, 0.86, 0.68, 0.33, 0.77, 0.12, 0.7, 0.35, 0.25, 0.08, 0.16, 0.35, 0.07, 0.8, 0.57, 0.51, 0.21, 0.28, 0.35, 0.37, 0.3, 0.22, 0.51, 0.07, 0.52, 0.1, 0.12, 0.2, 0.3, 0.38, 0.09, 0.41, 0.27, 0.43, 0.17, 0.1, 0.05, 0.17, 0.31, 0.7, 0.5, 0.19, 0.12, 0.43, 0.45, 0.39, 0.3, 0.07, 0.48, 0.56, 0.25, 0.07, 0.13, 0.54, 0.17, 0.01, 0.24, 0.1, 0.59, 0.01, 0.44, 0.41, 0.14, 0.25, 0.33, 0.13, 0.21, 0.5, 0.08, 0.13, 0.36, 0.48, 0.13, 0.46, 0.27, 0.4, 0.32, 0.22, 0.47, 0.2, 0.13, 0.5, 0.34, 0.12, 0.32, 0.33666666666666667, 0.42, 0.34, 0.4, 0.51, 0.28, 0.23, 0.03, 0.13, 0.17, 0.38, 0.39, 0.14, 0.04, 0.32, 0.47, 0.4, 0.34, 0.21, 0.07, 0.3, 0.46, 0.14, 0.05, 0.21, 0.18, 0.17, 0.16, 0.45, 0.06, 0.14, 0.2, 0.23, 0.17, 0.4, 0.02, 0.64, 0.3, 0.35, 0.1, 0.45, 0.19, 0.23, 0.05, 0.15, 0.21, 0.15, 0.53, 0.02, 0.09, 0.12, 0.35, 0.1, 0.37, 0.73, 0.21, 0.06, 0.04, 0.355, 0.42, 0.01, 0.44, 0.34, 0.27, 0.4466666666666667, 0.55, 0.51, 0.56, 0.48, 0.61, 0.31, 0.11, 0.3, 0.47, 0.16, 0.4, 0.27, 0.14, 0.21, 0.35, 0.42, 0.3, 0.34, 0.48, 0.06, 0.04, 0.55, 0.26, 0.2, 0.58, 0.43, 0.3, 0.08, 0.07, 0.04, 0.09, 0.11, 0.29, 0.22, 0.25, 0.23, 0.22, 0.28, 0.37, 0.21, 0.2, 0.29, 0.12, 0.12, 0.26, 0.03, 0.31, 0.73, 0.13, 0.07, 0.34666666666666673, 0.15, 0.05, 0.15, 0.26, 0.11, 0.56, 0.41, 0.23, 0.8, 0.81, 0.24, 0.45, 0.33, 0.29, 0.29, 0.32, 0.16, 0.265, 0.15, 0.33, 0.16, 0.24, 0.22, 0.39, 0.26, 0.24, 0.33, 0.39, 0.17, 0.2, 0.02, 0.14, 0.61, 0.54, 0.43, 0.16, 0.08, 0.66, 0.46, 0.22, 0.17, 0.01, 0.08, 0.09, 0.64, 0.06, 0.46, 0.31, 0.21, 0.18, 0.21, 0.33, 0.14, 0.23, 0.4, 0.22, 0.34, 0.07, 0.17, 0.39, 0.36, 0.05, 0.51, 0.18, 0.15, 0.06, 0.26, 0.21, 0.1, 0.38, 0.18, 0.05, 0.18, 0.17, 0.15, 0.16, 0.47, 0.43, 0.32, 0.36, 0.74, 0.21, 0.04, 0.36, 0.39, 0.14, 0.48, 0.37, 0.1, 0.365, 0.69, 0.91, 0.12, 0.17, 0.05, 0.37, 0.22, 0.15, 0.19, 0.46, 0.53, 0.07, 0.48, 0.07, 0.24, 0.43, 0.41, 0.52, 0.36, 0.5, 0.14, 0.15, 0.1, 0.07, 0.55, 0.46, 0.07, 0.6, 0.35, 0.16, 0.21, 0.91, 0.05, 0.25, 0.58, 0.33, 0.135, 0.24, 0.5, 0.02, 0.31, 0.49666666666666665, 0.15, 0.23, 0.67, 0.06, 0.13, 0.29, 0.2, 0.24, 0.16, 0.29, 0.08, 0.18, 0.18, 0.4, 0.21, 0.58, 0.1, 0.53, 0.3, 0.16, 0.23, 0.35, 0.3, 0.18, 0.27, 0.39, 0.12, 0.41, 0.15, 0.21, 0.46, 0.16, 0.38, 0.45, 0.19, 0.39, 0.3, 0.52, 0.16, 0.17, 0.46, 0.29, 0.15, 0.21, 0.32, 0.32, 0.27, 0.48, 0.34, 0.29, 0.09, 0.07, 0.2, 0.37, 0.575, 0.51, 0.54, 0.12, 0.06, 0.32, 0.31, 0.19, 0.13, 0.28, 0.11, 0.24, 0.71, 0.33, 0.095, 0.32, 0.1, 0.25, 0.74, 0.45, 0.51, 0.17, 0.5, 0.09, 0.25, 0.17, 0.53, 0.36, 0.2, 0.01, 0.36, 0.49, 0.04, 0.28, 0.25, 0.2, 0.51, 0.08, 0.2, 0.09, 0.49, 0.63, 0.52, 0.09, 0.52, 0.37, 0.09, 0.56, 0.36, 0.09, 0.11, 0.39, 0.17, 0.11, 0.11, 0.52, 0.09, 0.1, 0.25, 0.13, 0.42, 0.06, 0.27, 0.22, 0.19, 0.12, 0.68, 0.54, 0.21, 0.06, 0.53, 0.12, 0.69, 0.07, 0.33, 0.1, 0.26, 0.22, 0.08, 0.43, 0.12, 0.05, 0.26, 0.12, 0.03, 0.09, 0.42, 0.33, 0.2, 0.14, 0.47, 0.645, 0.43, 0.14, 0.26, 0.35, 0.16, 0.16, 0.89, 0.46, 0.77, 0.32, 0.51, 0.31, 0.46, 0.06, 0.3, 0.13, 0.3, 0.31, 0.29, 0.38, 0.49, 0.5, 0.24, 0.38, 0.26, 0.26, 0.28, 0.13, 0.25, 0.2, 0.41, 0.09, 0.485, 0.49, 0.34, 0.11, 0.43, 0.43, 0.15, 0.25, 0.06, 0.3, 0.43, 0.3, 0.17, 0.36, 0.15, 0.24, 0.32, 0.21, 0.16, 0.16, 0.41, 0.16, 0.08, 0.16, 0.24, 0.27, 0.49, 0.6, 0.16, 0.18, 0.2, 0.72, 0.24, 0.52, 0.39, 0.11, 0.11, 0.46, 0.22, 0.19, 0.18, 0.26, 0.53, 0.29, 0.18, 0.24, 0.18, 0.19, 0.06, 0.46, 0.3266666666666667, 0.36, 0.27, 0.19, 0.16, 0.16, 0.29, 0.37, 0.05, 0.16, 0.18, 0.34, 0.23, 0.16, 0.28, 0.29, 0.37, 0.62, 0.13, 0.23, 0.19, 0.33, 0.17, 0.11, 0.08, 0.45, 0.39, 0.31, 0.24, 0.49, 0.62, 0.02, 0.13, 0.02, 0.1, 0.3, 0.53, 0.19, 0.5, 0.17, 0.49, 0.08, 0.355, 0.15, 0.64, 0.36, 0.23, 0.37, 0.41, 0.51, 0.27, 0.11, 0.04, 0.08, 0.35, 0.35, 0.38, 0.25, 0.27, 0.2, 0.46, 0.34, 0.25, 0.18, 0.15, 0.77, 0.21, 0.68, 0.31, 0.04, 0.02, 0.14, 0.1, 0.47, 0.645, 0.17, 0.15, 0.5, 0.22, 0.18, 0.61, 0.09, 0.01, 0.56, 0.37, 0.15, 0.15, 0.43, 0.28, 0.11, 0.22, 0.36, 0.08, 0.24, 0.26, 0.32, 0.31, 0.48, 0.24, 0.23, 0.37, 0.47, 0.4, 0.36, 0.14, 0.12, 0.36, 0.12, 0.04, 0.27, 0.11, 0.19, 0.48, 0.06, 0.16, 0.27666666666666667, 0.29, 0.09, 0.16, 0.34, 0.2, 0.14, 0.13, 0.45, 0.31, 0.3, 0.66, 0.74, 0.11, 0.52, 0.27, 0.69, 0.07, 0.08, 0.22, 0.47, 0.16, 0.34, 0.06, 0.39, 0.37, 0.04, 0.26, 0.52, 0.08, 0.77, 0.04, 0.47, 0.24, 0.62, 0.38, 0.2, 0.41, 0.33, 0.38, 0.32, 0.16, 0.1, 0.59, 0.08, 0.41, 0.33, 0.37, 0.13, 0.59, 0.07, 0.14, 0.46, 0.34, 0.45, 0.19, 0.24, 0.16, 0.28, 0.25, 0.3, 0.34, 0.21, 0.47, 0.18, 0.34, 0.24, 0.51, 0.32, 0.22, 0.22, 0.48, 0.32, 0.39, 0.17, 0.29, 0.64, 0.27, 0.42, 0.15, 0.51, 0.64, 0.27, 0.18, 0.16, 0.66, 0.18, 0.39, 0.11, 0.52, 0.16, 0.12, 0.23, 0.66, 0.17, 0.4, 0.53, 0.15, 0.27, 0.75, 0.02, 0.14, 0.17, 0.36, 0.42, 0.18, 0.49, 0.25, 0.09, 0.0, 0.22, 0.59, 0.49, 0.32, 0.18, 0.12, 0.76, 0.27, 0.12, 0.14, 0.06, 0.29, 0.25, 0.08, 0.81, 0.53, 0.27, 0.11, 0.21, 0.47, 0.47, 0.14, 0.19, 0.5, 0.19, 0.23, 0.15, 0.7, 0.31, 0.07, 0.14, 0.1, 0.09, 0.27, 0.29, 0.24, 0.28, 0.05, 0.44, 0.15, 0.285, 0.18, 0.61, 0.2, 0.42, 0.12, 0.36, 0.08, 0.12, 0.12, 0.6, 0.08, 0.13, 0.15, 0.5, 0.04, 0.19, 0.1]</t>
         </is>
       </c>
     </row>
@@ -933,44 +933,44 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>boost</t>
+          <t>XGboost</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.8643724696356275</v>
+        <v>0.8651821862348178</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8879310344827587</v>
+        <v>0.8822033898305085</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8340080971659919</v>
+        <v>0.8429149797570851</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8947368421052632</v>
+        <v>0.8874493927125506</v>
       </c>
       <c r="G7" t="n">
-        <v>0.860125260960334</v>
+        <v>0.8621118012422361</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8643724696356275</v>
+        <v>0.8651821862348179</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8296263345195729</v>
+        <v>0.8229537366548043</v>
       </c>
       <c r="J7" t="n">
-        <v>0.8572806171648988</v>
+        <v>0.8497109826589595</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7909252669039146</v>
+        <v>0.7846975088967971</v>
       </c>
       <c r="L7" t="n">
-        <v>0.8683274021352313</v>
+        <v>0.8612099644128114</v>
       </c>
       <c r="M7" t="n">
-        <v>0.8227672373900972</v>
+        <v>0.8159111933395005</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8643724696356275</v>
+        <v>0.8229537366548042</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -979,7 +979,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>[1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0]</t>
+          <t>[1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -989,17 +989,95 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>[1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t xml:space="preserve">[0.998526930809021, 0.008006488904356956, 0.6199756860733032, 0.8576450347900391, 0.7519584894180298, 0.9989830851554871, 0.951845645904541, 0.3642059862613678, 0.46263328194618225, 0.9563536047935486, 0.32268956303596497, 0.19866140186786652, 0.9751399159431458, 0.12134958058595657, 0.9780811667442322, 0.16884185373783112, 0.9301396608352661, 0.985620379447937, 0.8404721617698669, 0.45169973373413086, 0.9316103458404541, 0.8844826817512512, 0.979582667350769, 0.17952388525009155, 0.8586946129798889, 0.14056357741355896, 0.9931095838546753, 0.9884340167045593, 0.9556376338005066, 0.5704813599586487, 0.995280921459198, 0.10882444679737091, 0.9208772778511047, 0.9484657645225525, 0.9185715913772583, 0.9724497199058533, 0.4196736514568329, 0.5244002342224121, 0.9739282727241516, 0.9947933554649353, 0.731198787689209, 0.6563571095466614, 0.0039040555711835623, 0.31754547357559204, 0.9884825348854065, 0.013907099142670631, 0.9445057511329651, 0.9707757234573364, 0.024353796616196632, 0.9831146001815796, 0.9906542897224426, 0.9891766905784607, 0.7568895816802979, 0.9797055125236511, 0.9773114323616028, 0.49231860041618347, 0.4282839596271515, 0.9965813755989075, 0.9441718459129333, 0.995924711227417, 0.720745325088501, 0.9238927364349365, 0.21725201606750488, 0.7535576820373535, 0.9931665062904358, 0.016988225281238556, 0.7379817962646484, 0.940687358379364, 0.8708305358886719, 0.028381405398249626, 0.7733451724052429, 0.8526796102523804, 0.7756836414337158, 0.9834358096122742, 0.9942929744720459, 0.9686281085014343, 0.995235025882721, 0.9445919990539551, 0.9991039633750916, 0.36511629819869995, 0.49024662375450134, 0.9109629988670349, 0.997186005115509, 0.9586304426193237, 0.9651314616203308, 0.4999016225337982, 0.7678440809249878, 0.9982755184173584, 0.4326270520687103, 0.8837200403213501, 0.9775663018226624, 0.011761204339563847, 0.8909776210784912, 0.7622057795524597, 0.04110423102974892, 0.7046711444854736, 0.8793110251426697, 0.617159366607666, 0.9843565821647644, 0.9074959754943848, 0.8228102326393127, 0.6146418452262878, 0.9909014701843262, 0.9630349278450012, 0.11713104695081711, 0.9719424843788147, 0.25961488485336304, 0.9974773526191711, 0.4745776653289795, 0.7159531712532043, 0.11599753797054291, 0.021239599213004112, 0.9302296042442322, 0.9867336750030518, 0.2255622148513794, 0.794438362121582, 0.9143007397651672, 0.36741605401039124, 0.9591233730316162, 0.7686542272567749, 0.553856372833252, 0.9156985282897949, 0.9509745240211487, 0.9549890756607056, 0.6334947943687439, 0.28077125549316406, 0.9733002185821533, 0.8772337436676025, 0.6745821237564087, 0.34284910559654236, 0.4901735186576843, 0.9649804830551147, 0.9596859216690063, 0.9518855810165405, 0.6057384014129639, 0.9231528639793396, 0.3777349889278412, 0.9942209720611572, 0.9920452833175659, 0.9444281458854675, 0.9968861937522888, 0.9969798922538757, 0.9683588743209839, 0.8644319176673889, 0.9005723595619202, 0.9731225371360779, 0.9988802075386047, 0.9236276745796204, 0.9897913336753845, 0.2142326533794403, 0.07930414378643036, 0.986425518989563, 0.01265196967869997, 0.943326473236084, 0.11189991980791092, 0.9955493211746216, 0.9515304565429688, 0.09529461711645126, 0.7361759543418884, 0.5682411789894104, 0.4783359467983246, 0.17973627150058746, 0.948538601398468, 0.986922025680542, 0.4148033857345581, 0.9247761964797974, 0.9886283278465271, 0.9996824264526367, 0.9743255972862244, 0.9146973490715027, 0.9860754609107971, 0.9563755393028259, 0.6200323700904846, 0.9969040751457214, 0.9732681512832642, 0.9494219422340393, 0.46360817551612854, 0.7919914126396179, 0.978919506072998, 0.9742209911346436, 0.9490369558334351, 0.7855402231216431, 0.9571678042411804, 0.9870696067810059, 0.027845920994877815, 0.6961493492126465, 0.8506582379341125, 0.9803282618522644, 0.9381762146949768, 0.9086208939552307, 0.9853604435920715, 0.19967088103294373, 0.694295346736908, 0.9762755036354065, 0.5690494179725647, 0.31125712394714355, 0.9879152774810791, 0.9702306985855103, 0.8321141600608826, 0.01675332523882389, 0.9617725610733032, 0.35788390040397644, 0.9583032131195068, 0.9293495416641235, 0.8462575078010559, 0.8835316300392151, 0.8635134100914001, 0.9825575947761536, 0.020101159811019897, 0.9363881349563599, 0.8584482669830322, 0.8303680419921875, 0.6089319586753845, 0.9923684000968933, 0.8629839420318604, 0.9978373646736145, 0.9792495369911194, 0.9698857665061951, 0.7987656593322754, 0.8772385120391846, 0.9150393009185791, 0.39025014638900757, 0.6976618766784668, 0.9587413668632507, 0.8061020970344543, 0.9815552830696106, 0.19032305479049683, 0.9826975464820862, 0.5253180861473083, 0.9826664924621582, 0.6508769989013672, 0.585433840751648, 0.9749503135681152, 0.9901806116104126, 0.4541008174419403, 0.9853480458259583, 0.3061354458332062, 0.7959557771682739, 0.8336437940597534, 0.393784761428833, 0.8476393818855286, 0.27139633893966675, 0.7610223889350891, 0.9956108927726746, 0.995280921459198, 0.7432374358177185, 0.47141629457473755, 0.9445919990539551, 0.07361824810504913, 0.05123734846711159, 0.9740936160087585, 0.9960997104644775, 0.9794268608093262, 0.9028266072273254, 0.9850760102272034, 0.2681085467338562, 0.970176637172699, 0.9746940732002258, 0.883310854434967, 0.5084721446037292, 0.5991206169128418, 0.799507200717926, 0.9932481050491333, 0.9549416899681091, 0.7711754441261292, 0.20563627779483795, 0.9915533661842346, 0.10898540169000626, 0.9607940316200256, 0.9783552885055542, 0.8223560452461243, 0.15377125144004822, 0.7468610405921936, 0.15138483047485352, 0.8158121705055237, 0.9020155072212219, 0.8553998470306396, 0.9889189600944519, 0.995784342288971, 0.7824140191078186, 0.06585442274808884, 0.9946913123130798, 0.9833651185035706, 0.8420755863189697, 0.9904019236564636, 0.30313006043434143, 0.7932738661766052, 0.9948592185974121, 0.5265234112739563, 0.7908101677894592, 0.9838283061981201, 0.4979439079761505, 0.9465367197990417, 0.9392083287239075, 0.95844566822052, 0.9000155925750732, 0.9629408121109009, 0.9820672273635864, 0.7471083402633667, 0.7109394073486328, 0.334568589925766, 0.9500256776809692, 0.041939835995435715, 0.1492646038532257, 0.8607518672943115, 0.9348015189170837, 0.9689105749130249, 0.9895213842391968, 0.6227598190307617, 0.8597603440284729, 0.584470808506012, 0.1729278862476349, 0.2403353750705719, 0.9772787690162659, 0.9961613416671753, 0.13336648046970367, 0.07692401111125946, 0.6506515145301819, 0.961545467376709, 0.8244872689247131, 0.920478105545044, 0.9809256196022034, 0.9970687031745911, 0.9359044432640076, 0.9690304398536682, 0.9834387898445129, 0.9801151752471924, 0.2299063801765442, 0.6051825881004333, 0.9934934973716736, 0.7948077321052551, 0.9205997586250305, 0.9574424624443054, 0.9980008006095886, 0.8506299257278442, 0.20736680924892426, 0.999459445476532, 0.9862818121910095, 0.9885302186012268, 0.4355766475200653, 0.8697993159294128, 0.39268532395362854, 0.9238360524177551, 0.9977364540100098, 0.9793170094490051, 0.9696509838104248, 0.9507379531860352, 0.8611047863960266, 0.9069439768791199, 0.9269040822982788, 0.03874211758375168, 0.9947121143341064, 0.9957039952278137, 0.9955871105194092, 0.9887977242469788, 0.9907704591751099, 0.9851552844047546, 0.5198867917060852, 0.9663158059120178, 0.9946410655975342, 0.7330164313316345, 0.37816011905670166, 0.9118947386741638, 0.7953010201454163, 0.796502947807312, 0.7032272219657898, 0.8360123634338379, 0.8924682140350342, 0.12521719932556152, 0.9910253286361694, 0.9976106882095337, 0.9972706437110901, 0.6890231370925903, 0.9951660633087158, 0.9737928509712219, 0.6833493709564209, 0.9603989124298096, 0.16967788338661194, 0.9475627541542053, 0.4647717773914337, 0.9557754397392273, 0.9896973967552185, 0.8072430491447449, 0.11669463664293289, 0.6325255632400513, 0.9956108927726746, 0.06378799676895142, 0.5888030529022217, 0.9669252038002014, 0.9937753677368164, 0.996647298336029, 0.20995500683784485, 0.9772911667823792, 0.8162042498588562, 0.6342872977256775, 0.9780161380767822, 0.9755606651306152, 0.9934180974960327, 0.15459105372428894, 0.456108957529068, 0.7755449414253235, 0.23109503090381622, 0.14528658986091614, 0.9422007203102112, 0.7955235242843628, 0.9566287994384766, 0.9719198346138, 0.3964967131614685, 0.9946065545082092, 0.8575652241706848, 0.30837282538414, 0.28484588861465454, 0.36373141407966614, 0.9908279180526733, 0.9567537307739258, 0.8917481303215027, 0.5466174483299255, 0.6522965431213379, 0.9937684535980225, 0.012557857669889927, 0.03601986914873123, 0.9870131611824036, 0.935384213924408, 0.9175109267234802, 0.2464834302663803, 0.9317176342010498, 0.8813368082046509, 0.8979925513267517, 0.5127856135368347, 0.7867025136947632, 0.5528168082237244, 0.9076966047286987, 0.9278642535209656, 0.9833574891090393, 0.9882329106330872, 0.9989296793937683, 0.9455702900886536, 0.9940872192382812, 0.5508586764335632, 0.7908241748809814, 0.9965294003486633, 0.9494753479957581, 0.5821385383605957, 0.9239006042480469, 0.7781022787094116, 0.9011713862419128, 0.9932395219802856, 0.9492458701133728, 0.9658633470535278, 0.7335704565048218, 0.9966930150985718, 0.929006814956665, 0.3330672085285187, 0.45841002464294434, 0.995158851146698, 0.2000207006931305, 0.9927167296409607, 0.264744371175766, 0.8862616419792175, 0.8482232093811035, 0.9763177633285522, 0.996356725692749, 0.9481830596923828, 0.09144091606140137, 0.992520809173584, 0.9493903517723083, 0.0025623927358537912, 0.7069977521896362, 0.36728233098983765, 0.9479259252548218, 0.9985431432723999, 0.9996228218078613, 0.8790472149848938, 0.3687676787376404, 0.08066758513450623, 0.054689135402441025, 0.41078057885169983, 0.4982009530067444, 0.9359535574913025, 0.09387277811765671, 0.9638703465461731, 0.30588415265083313, 0.9831226468086243, 0.5601475238800049, 0.14312507212162018, 0.9759924411773682, 0.9175431728363037, 0.026852864772081375, 0.9874652624130249, 0.48690077662467957, 0.18949094414710999, 0.8829016089439392, 0.23749753832817078, 0.13946346938610077, 0.8730817437171936, 0.9938163757324219, 0.9919875860214233, 0.8750396370887756, 0.9949476718902588, 0.1266917586326599, 0.2582545280456543, 0.4805580675601959, 0.37684428691864014, 0.5849263072013855, 0.004482489079236984, 0.5973634123802185, 0.8449146151542664, 0.9506954550743103, 0.9404137134552002, 0.9882867932319641, 0.9757677316665649, 0.9979579448699951, 0.4105542302131653, 0.999029278755188, 0.9484147429466248, 0.14761361479759216, 0.977965772151947, 0.10052601248025894, 0.8489600419998169, 0.9838608503341675, 0.7154281735420227, 0.9955896139144897, 0.6385427713394165, 0.9273326992988586, 0.9408426880836487, 0.8346089124679565, 0.9092434048652649, 0.5959387421607971, 0.6141153573989868, 0.7309935092926025, 0.9934399724006653, 0.8889120817184448, 0.7401462197303772, 0.0780239999294281, 0.9979689717292786, 0.9583032131195068, 0.769821286201477, 0.9909470081329346, 0.8098627924919128, 0.971433699131012, 0.019739476963877678, 0.044127121567726135, 0.4686175286769867, 0.9059315323829651, 0.5587682723999023, 0.9776443839073181, 0.02423645555973053, 0.879243016242981, 0.9916292428970337, 0.7096334099769592, 0.934719979763031, 0.9970393776893616, 0.11625537276268005, 0.9971268773078918, 0.5697351098060608, 0.9953097701072693, 0.35435399413108826, 0.9967767596244812, 0.9928385615348816, 0.9599819183349609, 0.9592767953872681, 0.8519822359085083, 0.5977573990821838, 0.945910632610321, 0.7691452503204346, 0.9962764382362366, 0.9557403922080994, 0.8936429023742676, 0.9593830108642578, 0.4674381613731384, 0.6886148452758789, 0.994576096534729, 0.8855868577957153, 0.03277700021862984, 0.9368550777435303, 0.7758939266204834, 0.9995457530021667, 0.9920422434806824, 0.9763327240943909, 0.9853543043136597, 0.9989323019981384, 0.943732500076294, 0.9663153886795044, 0.9643862843513489, 0.8916419148445129, 0.22401966154575348, 0.4406539797782898, 0.9830656051635742, 0.09302271902561188, 0.9647581577301025, 0.7218954563140869, 0.7872082591056824, 0.9823871850967407, 0.9796634316444397, 0.9971959590911865, 0.2184244841337204, 0.7619406580924988, 0.9521320462226868, 0.2155161201953888, 0.995116114616394, 0.9746755957603455, 0.9980286955833435, 0.8807359933853149, 0.055442217737436295, 0.19312430918216705, 0.2613491415977478, 0.16493305563926697, 0.9878517389297485, 0.20092368125915527, 0.28195902705192566, 0.7769461870193481, 0.6840618252754211, 0.05198581889271736, 0.9946569204330444, 0.19031834602355957, 0.2254989594221115, 0.9964743256568909, 0.9930517673492432, 0.01951844058930874, 0.6833094954490662, 0.9880254864692688, 0.7261382937431335, 0.23597964644432068, 0.9882644414901733, 0.8767651915550232, 0.6211978197097778, 0.9269705414772034, 0.5793116092681885, 0.05324200913310051, 0.987176239490509, 0.9996461868286133, 0.6597223877906799, 0.889424204826355, 0.8807631134986877, 0.9983230233192444, 0.9733238220214844, 0.29974332451820374, 0.939869225025177, 0.774570107460022, 0.9972688555717468, 0.9976069927215576, 0.8408096432685852, 0.5888198018074036, 0.01623418740928173, 0.998514711856842, 0.9982700347900391, 0.45599761605262756, 0.0033446724992245436, 0.9563020467758179, 0.028580695390701294, 0.9960930943489075, 0.5918881297111511, 0.9996474981307983, 0.6094881892204285, 0.859132707118988, 0.394973486661911, 0.07711320370435715, 0.6704792380332947, 0.9901629686355591, 0.8812929391860962, 0.9796426892280579, 0.975679337978363, 0.5581629276275635, 0.771400511264801, 0.9883193969726562, 0.4039102792739868, 0.9973230957984924, 0.2241833209991455, 0.8456805944442749, 0.9727334380149841, 0.9789302349090576, 0.8184707164764404, 0.9772787690162659, 0.841289758682251, 0.4286523461341858, 0.7188706398010254, 0.9138607978820801, 0.9408426880836487, 0.9122403264045715, 0.03869931772351265, 0.939647912979126, 0.028408532962203026, 0.03488197922706604, 0.725770890712738, 0.6761052012443542, 0.9879576563835144, 0.9978430271148682, 0.020486924797296524, 0.023963652551174164, 0.26755088567733765, 0.9981766939163208, 0.9972960352897644, 0.6167887449264526, 0.3009084463119507, 0.4680720865726471, 0.7057644724845886, 0.04768453538417816, 0.988250732421875, 0.8292984962463379, 0.9120059609413147, 0.3488019108772278, 0.9919141530990601, 0.9773863554000854, 0.2701372802257538, 0.9171773791313171, 0.468973308801651, 0.9398728609085083, 0.01667824201285839, 0.996758759021759, 0.48035529255867004, 0.43174418807029724, 0.9734165668487549, 0.23193678259849548, 0.9812023639678955, 0.9870517253875732, 0.12449745833873749, 0.9682083129882812, 0.7134559154510498, 0.11927606165409088, 0.09121417254209518, 0.8179028630256653, 0.9795922636985779, 0.7067403197288513, 0.020208965986967087, 0.9248113036155701, 0.978948175907135, 0.9977784752845764, 0.6477826833724976, 0.821483850479126, 0.9827739000320435, 0.6863961219787598, 0.7599558234214783, 0.397391140460968, 0.996344268321991, 0.8542912006378174, 0.9869736433029175, 0.15631398558616638, 0.9130206108093262, 0.9980239868164062, 0.9741026759147644, 0.9221874475479126, 0.967901885509491, 0.9607703685760498, 0.24966350197792053, 0.023203158751130104, 0.7810027003288269, 0.9661240577697754, 0.904326319694519, 0.4730378985404968, 0.9878098964691162, 0.659167468547821, 0.7432596683502197, 0.9988610744476318, 0.9958513975143433, 0.9714254140853882, 0.9820319414138794, 0.934735894203186, 0.46563756465911865, 0.9920692443847656, 0.663214385509491, 0.9820632934570312, 0.5763397812843323, 0.9987534284591675, 0.20507489144802094, 0.6610907316207886, 0.990013599395752, 0.10404044389724731, 0.719093382358551, 0.24416255950927734, 0.9977666139602661, 0.989284336566925, 0.022384921088814735, 0.4596801698207855, 0.9070278406143188, 0.9956108927726746, 0.8433053493499756, 0.48035529255867004, 0.002408715896308422, 0.9685958623886108, 0.9267629981040955, 0.8089584112167358, 0.9772787690162659, 0.6754471659660339, 0.9807991981506348, 0.9463365077972412, 0.5926535725593567, 0.012855376116931438, 0.9653406143188477, 0.9379358887672424, 0.8233180642127991, 0.8526890277862549, 0.03674162179231644, 0.6563295125961304, 0.1468351036310196, 0.524989128112793, 0.03200685232877731, 0.915490984916687, 0.8938029408454895, 0.8974940180778503, 0.6770734190940857, 0.9062970280647278, 0.9615235924720764, 0.981840193271637, 0.9977452158927917, 0.5523650050163269, 0.9511818885803223, 0.7184154391288757, 0.944007158279419, 0.007901394739747047, 0.9921505451202393, 0.9100775718688965, 0.03787298873066902, 0.935409665107727, 0.8940707445144653, 0.9885988235473633, 0.5160381197929382, 0.9931429624557495, 0.20015545189380646, 0.5070532560348511, 0.7668159604072571, 0.7108235359191895, 0.9579840302467346, 0.8400142192840576, 0.08613062649965286, 0.9934084415435791, 0.7906638383865356, 0.9393986463546753, 0.19723351299762726, 0.9899769425392151, 0.9921795129776001, 0.5753846168518066, 0.7236573100090027, 0.9470799565315247, 0.6519771814346313, 0.016304917633533478, 0.7769388556480408, 0.030449887737631798, 0.9963605999946594, 0.0789075493812561, 0.9261353611946106, 0.351010799407959, 0.046036478132009506, 0.9950101375579834, 0.02371763251721859, 0.5301079154014587, 0.623532772064209, 0.8042645454406738, 0.861981987953186, 0.037417683750391006, 0.04873020201921463, 0.9243233799934387, 0.18365122377872467, 0.0655154213309288, 0.26860085129737854, 0.7952229380607605, 0.9006449580192566, 0.2901500463485718, 0.016033796593546867, 0.040129516273736954, 0.9333754181861877, 0.9463320374488831, 0.8118469715118408, 0.8685543537139893, 0.9209610819816589, 0.9951589703559875, 0.2291213721036911, 0.9947540760040283, 0.8407315015792847, 0.9793316125869751, 0.0992085188627243, 0.9591131806373596, 0.9783397912979126, 0.9777416586875916, 0.1871977299451828, 0.08083336055278778, 0.9958454966545105, 0.8591439127922058, 0.9278731346130371, 0.2466408908367157, 0.9484578371047974, 0.9953519105911255, 0.8521589040756226, 0.9323821067810059, 0.7484338879585266, 0.23599280416965485, 0.3321477174758911, 0.24113820493221283, 0.3780330717563629, 0.5541442036628723, 0.14718149602413177, 0.9724108576774597, 0.3158091604709625, 0.4530808925628662, 0.8918148875236511, 0.9732681512832642, 0.3681003749370575, 0.8244183659553528, 0.989164412021637, 0.41773927211761475, 0.6936197876930237, 0.6434202194213867, 0.879800021648407, 0.9599875211715698, 0.9505149126052856, 0.43621140718460083, 0.9049737453460693, 0.32433104515075684, 0.978300154209137, 0.5898805260658264, 0.5941751599311829, 0.9181671142578125, 0.6538336277008057, 0.9455079436302185, 0.7391985654830933, 0.9360976815223694, 0.40995725989341736, 0.9137030243873596, 0.9407122731208801, 0.8475980162620544, 0.9290475249290466, 0.7578081488609314, 0.37516698241233826, 0.9804601073265076, 0.9951840043067932, 0.8592514395713806, 0.3062931001186371, 0.8368738889694214, 0.9934458136558533, 0.9888812899589539, 0.9707059860229492, 0.9605709910392761, 0.8212306499481201, 0.9762861728668213, 0.9965567588806152, 0.9044092297554016, 0.9271063208580017, 0.9626120924949646, 0.8487532138824463, 0.5348130464553833, 0.9894527196884155, 0.9792495369911194, 0.43232402205467224, 0.9276036024093628, 0.5116202235221863, 0.859614908695221, 0.1902974396944046, 0.002563254442065954, 0.39865198731422424, 0.9966956377029419, 0.9532456994056702, 0.9979402422904968, 0.19500009715557098, 0.9896973967552185, 0.005096207372844219, 0.23834344744682312, 0.7082774043083191, 0.3612500727176666, 0.9845505356788635, 0.4309147000312805, 0.9423635005950928, 0.9453776478767395, 0.5572000741958618, 0.007903061807155609, 0.9700273275375366, 0.9785155057907104, 0.9040440917015076, 0.1997734159231186, 0.012790688313543797, 0.9478046894073486, 0.9589115381240845, 0.07454541325569153, 0.9962445497512817, 0.885345995426178, 0.9360541105270386, 0.9821138978004456, 0.9916273355484009, 0.8878018260002136, 0.9158573746681213, 0.968025267124176, 0.7487123012542725, 0.998202919960022, 0.5561414957046509, 0.9899425506591797, 0.5690465569496155, 0.9860610961914062, 0.9346920847892761, 0.994951605796814, 0.9302964806556702, 0.10472827404737473, 0.8979502320289612, 0.986281156539917, 0.7799366116523743, 0.9419248104095459, 0.9996084570884705, 0.8020842671394348, 0.9856752753257751, 0.8639543652534485, 0.7661508321762085, 0.02112109400331974, 0.9920382499694824, 0.6877598762512207, 0.9324900507926941, 0.9945430755615234, 0.0053711566142737865, 0.014282820746302605, 0.9921842217445374, 0.9724158048629761, 0.97491055727005, 0.9832836389541626, 0.2954709231853485, 0.8723277449607849, 0.4765251576900482, 0.12627138197422028, 0.07540632039308548, 0.9935845732688904, 0.2555026113986969, 0.037835389375686646, 0.6721163988113403, 0.5834064483642578, 0.8981212377548218, 0.9942846894264221, 0.9932564496994019, 0.1506364345550537, 0.9732785224914551, 0.19644157588481903, 0.006431398913264275, 0.36024340987205505, 0.9931975603103638, 0.9926121830940247, 0.24607695639133453, 0.5326393246650696, 0.9787821173667908, 0.9050144553184509, 0.9780681729316711, 0.9927700161933899, 0.6162410378456116, 0.007310051470994949, 0.948737382888794, 0.0510229729115963, 0.9574018716812134, 0.5444238781929016, 0.8149135708808899, 0.392757385969162, 0.9921607375144958, 0.26073718070983887, 0.9896335601806641, 0.8112678527832031, 0.9686791896820068, 0.9928842782974243, 0.9545571208000183, 0.4160379469394684, 0.4442371428012848, 0.9802342057228088, 0.9786742925643921, 0.9985520243644714, 0.8610363006591797, 0.8312523365020752, 0.6186659932136536, 0.7291699051856995, 0.0756717398762703, 0.9527800679206848, 0.9622560739517212, 0.9942097663879395, 0.7911401987075806, 0.15003618597984314, 0.9406474232673645, 0.5041968822479248, 0.7798526287078857, 0.09391062706708908, 0.9822027683258057, 0.6370486617088318, 0.9335439205169678, 0.9396305084228516, 0.9992536902427673, 0.9459269642829895, 0.9908545017242432, 0.9968758821487427, 0.2363007813692093, 0.8471894264221191, 0.9245802164077759, 0.9946322441101074, 0.983786404132843, 0.10320523381233215, 0.9749869108200073, 0.935104250907898, 0.9732985496520996, 0.9454354643821716, 0.9870295524597168, 0.04745049029588699, 0.9434076547622681, 0.9639233946800232, 0.946252703666687, 0.7811360955238342, 0.9948150515556335, 0.957273006439209, 0.9938867688179016, 0.9886876344680786, 0.43468359112739563, 0.9360878467559814, 0.4312306344509125, 0.941606342792511, 0.44979241490364075, 0.9758244752883911, 0.9853795170783997, 0.11650927364826202, 0.10215864330530167, 0.09862376749515533, 0.2860226631164551, 0.006702152080833912, 0.5048648715019226, 0.9804450869560242, 0.9287784695625305, 0.9967173933982849, 0.9332676529884338, 0.9404782652854919, 0.9859472513198853, 0.9846420884132385, 0.6027734875679016, 0.928713858127594, 0.7336559295654297, 0.9854397177696228, 0.996729850769043, 0.9896495342254639, 0.7887588143348694, 0.08270995318889618, 0.9972718358039856, 0.8777162432670593, 0.504175066947937, 0.9389289617538452, 0.4958306550979614, 0.6279814839363098, 0.9995434880256653, 0.8083388805389404, 0.1187388077378273, 0.9583032131195068, 0.7300398945808411, 0.9750081300735474, 0.9529631733894348, 0.36796072125434875, 0.9340035319328308, 0.9776396751403809, 0.9580965042114258, 0.9973676800727844, 0.9959063529968262, 0.9925345182418823, 0.9990684390068054, 0.9755874276161194, 0.05080551654100418, 0.4644802510738373, 0.9915862083435059, 0.9226804375648499, 0.9788515567779541, 0.892825186252594, 0.7139742970466614, 0.23661960661411285, 0.9068188071250916, 0.18579833209514618, 0.016493821516633034, 0.24478472769260406, 0.9947795867919922, 0.9446076154708862, 0.9000498056411743, 0.9969229102134705, 0.9891479015350342, 0.5533437132835388, 0.9957885146141052, 0.6209042072296143, 0.902904748916626, 0.2525518834590912, 0.9793766736984253, 0.6086386442184448, 0.7440532445907593, 0.7347118854522705, 0.8589136004447937, 0.2501246929168701, 0.9963749051094055, 0.9382060170173645, 0.9908181428909302, 0.9971563816070557, 0.38651320338249207, 0.05886248126626015, 0.9677084684371948, 0.9098921418190002, 0.1399603635072708, 0.9801577925682068, 0.6667771935462952, 0.9900615215301514, 0.7031421065330505, 0.9413970112800598, 0.8118955492973328, 0.8433890342712402, 0.8699214458465576, 0.989463210105896, 0.9976471066474915, 0.991761326789856, 0.9604548811912537, 0.9897933006286621, 0.29080596566200256, 0.3831765353679657, 0.9882547855377197, 0.2166597545146942, 0.7020418047904968, 0.9984265565872192, 0.9762755036354065, 0.9860721230506897, 0.9606993794441223, 0.490742951631546, 0.9520611763000488, 0.994658887386322, 0.9899300932884216, 0.26864519715309143, 0.0020825585816055536, 0.595500111579895, 0.789684534072876, 0.6864007115364075, 0.5170230269432068, 0.0018951675156131387, 0.43188172578811646, 0.9971750974655151, 0.2029903084039688, 0.0031412900425493717, 0.9930958151817322, 0.9745371341705322, 0.9971150159835815, 0.730553925037384, 0.6863966584205627, 0.771490752696991, 0.2852780222892761, 0.3548697829246521, 0.8405064940452576, 0.9995850920677185, 0.3216294050216675, 0.23993666470050812, 0.9517965912818909, 0.5159502625465393, 0.9710981249809265, 0.9619091749191284, 0.9990529417991638, 0.8512237071990967, 0.5177646279335022, 0.6411021947860718, 0.8987575769424438, 0.790109395980835, 0.995280921459198, 0.9988136291503906, 0.24918414652347565, 0.8711663484573364, 0.9931420683860779, 0.9928433299064636, 0.010965770110487938, 0.9602900743484497, 0.3695230484008789, 0.07126916944980621, 0.7559566497802734, 0.9460898637771606, 0.9861524105072021, 0.9762755036354065, 0.8816911578178406, 0.6559614539146423, 0.9516937136650085, 0.9963418841362, 0.04556024819612503, 0.969399094581604, 0.9779797792434692, 0.9695461392402649, 0.8408519625663757, 0.9949916005134583, 0.515305757522583, 0.3283190429210663, 0.9741239547729492, 0.1632208377122879, 0.2653709650039673, 0.9654526710510254, 0.8852890729904175, 0.9724830985069275, 0.9575132727622986, 0.6260009407997131, 0.9586807489395142, 0.7576599717140198, 0.9869731068611145, 0.9964447617530823, 0.21070481836795807, 0.01807710900902748, 0.0693884938955307, 0.7308176755905151, 0.40638941526412964, 0.943732500076294, 0.974563479423523, 0.9974710941314697, 0.2779543101787567, 0.962805986404419, 0.989696741104126, 0.6033627390861511, 0.7161954045295715, 0.868262767791748, 0.9572101831436157, 0.41906848549842834, 0.9083382487297058, 0.21040089428424835, 0.9338202476501465, 0.9896795749664307, 0.9979240894317627, 0.25682908296585083, 0.09903492033481598, 0.005777052138000727, 0.0385441929101944, 0.8697311878204346, 0.9971795082092285, 0.7524128556251526, 0.1921689212322235, 0.9199193120002747, 0.995280921459198, 0.9898932576179504, 0.7736051082611084, 0.9962041974067688, 0.814268171787262, 0.7379520535469055, 0.9906861186027527, 0.45316019654273987, 0.25593864917755127, 0.9955316781997681, 0.552035391330719, 0.7458405494689941, 0.9634202718734741, 0.8011532425880432, 0.8848419785499573, 0.019076330587267876, 0.9966418743133545, 0.1684400886297226, 0.8043206930160522, 0.9456180334091187, 0.358651340007782, 0.5221218466758728, 0.6593882441520691, 0.32944610714912415, 0.18805953860282898, 0.7974326014518738, 0.8815513253211975, 0.12174750864505768, 0.9645466208457947, 0.9866679906845093, 0.9953922033309937, 0.6066443920135498, 0.8971342444419861, 0.89484041929245, 0.8176574110984802, 0.9858647584915161, 0.05830992013216019, 0.41007575392723083, 0.8463868498802185, 0.9416731595993042, 0.9440120458602905, 0.9924423694610596, 0.5661749839782715, 0.9784340262413025, 0.5258408188819885, 0.5532066226005554, 0.9971597194671631, 0.49274787306785583, 0.998005211353302, 0.10682179778814316, 0.9830784201622009, 0.9753587245941162, 0.026030924171209335, 0.608883261680603, 0.9593194723129272, 0.17699067294597626, 0.2912544310092926, 0.6283280253410339, 0.5355455875396729, 0.15946096181869507, 0.9356657266616821, 0.3089979588985443, 0.9486156105995178, 0.2903149425983429, 0.7695504426956177, 0.9456415176391602, 0.7153473496437073, 0.9964902997016907, 0.7931966781616211, 0.9311845898628235, 0.7581582069396973, 0.9976922273635864, 0.9583032131195068, 0.10576926916837692, 0.9038003087043762, 0.961688220500946, 0.9972720742225647, 0.8827564120292664, 0.654585599899292, 0.9534147381782532, 0.34026458859443665, 0.06034744903445244, 0.9533053040504456, 0.9816786646842957, 0.455172061920166, 0.7366945743560791, 0.01889260858297348, 0.5333504676818848, 0.9701560139656067, 0.9935235977172852, 0.9478129148483276, 0.9915558099746704, 0.9181537628173828, 0.6529127955436707, 0.3836110830307007, 0.9939362406730652, 0.9392083287239075, 0.8404679298400879, 0.9733670949935913, 0.8877794146537781, 0.44263333082199097, 0.8445965647697449, 0.7796828150749207, 0.8628440499305725, 0.002984536811709404, 0.17178571224212646, 0.31941670179367065, 0.6730457544326782, 0.9875965118408203, 0.06098524481058121, 0.9371446967124939, 0.9737192392349243, 0.7537380456924438, 0.9530390501022339, 0.8098489046096802, 0.9972074627876282, 0.7966221570968628, 0.8595910668373108, 0.20434999465942383, 0.7100142240524292, 0.9753738045692444, 0.9720962047576904, 0.1392718255519867, 0.6858499646186829, 0.2518611252307892, 0.20200379192829132, 0.8591424822807312, 0.9973512887954712, 0.7312912344932556, 0.8162137866020203, 0.04729190096259117, 0.9952465891838074, 0.9943893551826477, 0.5878841280937195, 0.8994389772415161, 0.04182882979512215, 0.04525799676775932, 0.9200770258903503, 0.8753031492233276, 0.5350865721702576, 0.5481545925140381, 0.4605739414691925, 0.5996890068054199, 0.7720050811767578, 0.43390199542045593, 0.9942328333854675, 0.8717629909515381, 0.7769297361373901, 0.5326749682426453, 0.9833112955093384, 0.7359158396720886, 0.9243955612182617, 0.7884485721588135, 0.3028756082057953, 0.7336849570274353, 0.8041427135467529, 0.3079110383987427, 0.9957712292671204, 0.021620837971568108, 0.9917852878570557, 0.8718017339706421, 0.9984172582626343, 0.09856055676937103, 0.0316319614648819, 0.7279795408248901, 0.9716358184814453, 0.9608365893363953, 0.47836753726005554, 0.0963967964053154, 0.7059119939804077, 0.810169517993927, 0.9951949715614319, 0.28986358642578125, 0.9416447281837463, 0.9871992468833923, 0.5910126566886902, 0.29956069588661194, 0.9709686636924744, 0.48461011052131653, 0.6242040395736694, 0.31393760442733765, 0.6772602796554565, 0.8958966135978699, 0.9987862706184387, 0.9186893701553345, 0.9925965070724487, 0.9460898637771606, 0.1489972472190857, 0.9897623658180237, 0.039817675948143005, 0.9966251850128174, 0.5017363429069519, 0.23031671345233917, 0.764031708240509, 0.4431356191635132, 0.9819129705429077, 0.5417917966842651, 0.9962379932403564, 0.567531168460846, 0.765811026096344, 0.7851242423057556, 0.8933643102645874, 0.9606329202651978, 0.1978570520877838, 0.9998494386672974, 0.9695386290550232, 0.9868692755699158, 0.975581169128418, 0.2728795111179352, 0.31948938965797424, 0.6808249354362488, 0.933961033821106, 0.9139543771743774, 0.7677172422409058, 0.7395981550216675, 0.049659229815006256, 0.8229801058769226, 0.7534475922584534, 0.9976928234100342, 0.00010996586934197694, 0.0018539282027631998, 0.002182472264394164, 0.007273105904459953, 0.005778615828603506, 0.007941716350615025, 0.18395718932151794, 0.003341830102726817, 0.003371460596099496, 0.00352132273837924, 0.0001909782731672749, 3.432689936744282e-06, 0.0001142795299529098, 9.620235505281016e-05, 0.00011454266496002674, 0.0005367923877201974, 0.0017316302983090281, 2.7772513931267895e-05, 0.004580256063491106, 0.0002149262436432764, 8.56752012623474e-05, 0.00012276071356609464, 0.5834064483642578, 0.0002079149999190122, 0.2536951005458832, 0.027279578149318695, 0.0013215923681855202, 0.001850742963142693, 0.012657290324568748, 7.694662781432271e-05, 0.0007947709527797997, 0.06785266101360321, 0.001623781630769372, 0.00012939174484927207, 0.015016079880297184, 0.0027239008340984583, 0.312801718711853, 3.726782961166464e-05, 0.0006381590501405299, 0.001880161464214325, 0.00025494370493106544, 0.0005219600861892104, 0.0012496933341026306, 4.329685907578096e-05, 0.0006953281699679792, 0.0018643687944859266, 0.012391951866447926, 0.003446254413574934, 0.0013469067635014653, 0.0007695448002777994, 0.00012496457202360034, 0.020077360793948174, 0.004028884693980217, 0.03910740837454796, 0.0022779384162276983, 0.00042114147800020874, 0.00014534803631249815, 0.006698632147163153, 7.02730321791023e-05, 9.037358540808782e-05, 0.00012688818969763815, 0.4280914068222046, 0.0032026402186602354, 0.0020130483899265528, 0.06305525451898575, 0.00012235797476023436, 0.0001086382326320745, 0.0001599312963662669, 0.0007007438107393682, 0.006191933527588844, 0.0005413223407231271, 0.00017457894864492118, 0.002697551157325506, 0.5686152577400208, 8.477902156300843e-05, 0.0002492819621693343, 2.6256937417201698e-05, 0.0009725754498504102, 0.0014908065786585212, 0.00016230529581662267, 0.001298114424571395, 0.00403937790542841, 3.5691157336259494e-06, 0.000645194377284497, 8.742209502088372e-06, 0.00028536145691759884, 0.0002608645590953529, 0.0014110114425420761, </t>
+          <t>[0.9985532164573669, 0.0024600320030003786, 0.5815272331237793, 0.9857592582702637, 0.7664432525634766, 0.9998401403427124, 0.6780804395675659, 0.4190571904182434, 0.5959131121635437, 0.9804060459136963, 0.8288048505783081, 0.7487971186637878, 0.9927406907081604, 0.24705132842063904, 0.9761378765106201, 0.12222568690776825, 0.9084178805351257, 0.985954225063324, 0.9875192642211914, 0.4171377718448639, 0.9936532974243164, 0.834425151348114, 0.9683954119682312, 0.6499385833740234, 0.9413300156593323, 0.18433061242103577, 0.983309805393219, 0.9964156150817871, 0.9873177409172058, 0.7999793887138367, 0.9972501397132874, 0.1667850762605667, 0.9802361130714417, 0.943857729434967, 0.7079623937606812, 0.9909570217132568, 0.5693665146827698, 0.3793337643146515, 0.9824312329292297, 0.9853692650794983, 0.958964467048645, 0.46890148520469666, 0.0006393498042598367, 0.4331783652305603, 0.994906485080719, 0.052546724677085876, 0.9585148692131042, 0.7388119101524353, 0.010104203596711159, 0.9936090707778931, 0.9885181784629822, 0.9869338274002075, 0.7100855112075806, 0.9931569695472717, 0.9365357756614685, 0.41379451751708984, 0.16771969199180603, 0.9985257983207703, 0.9879064559936523, 0.9936074018478394, 0.5597737431526184, 0.8842511177062988, 0.7000027298927307, 0.6357495784759521, 0.9728574156761169, 0.21925438940525055, 0.9088466167449951, 0.9762012958526611, 0.7899736166000366, 0.1437142938375473, 0.5379302501678467, 0.6813741326332092, 0.6993384957313538, 0.9964893460273743, 0.9892944097518921, 0.9506336450576782, 0.9986562728881836, 0.9579495191574097, 0.9993312358856201, 0.14426584541797638, 0.6261774301528931, 0.8010526299476624, 0.9991717338562012, 0.9795467257499695, 0.9567281603813171, 0.8781101107597351, 0.6883324980735779, 0.9989827275276184, 0.17692340910434723, 0.9102756381034851, 0.9947454929351807, 0.08224386721849442, 0.953718364238739, 0.8817424774169922, 0.24517574906349182, 0.92433762550354, 0.924837589263916, 0.41304707527160645, 0.9821583032608032, 0.900942325592041, 0.23841513693332672, 0.9296842813491821, 0.994598388671875, 0.9480744004249573, 0.281089723110199, 0.9599699378013611, 0.12032438814640045, 0.9736985564231873, 0.17724278569221497, 0.9075780510902405, 0.0444476380944252, 0.006470880005508661, 0.851415753364563, 0.9908796548843384, 0.656000554561615, 0.9030721187591553, 0.991200864315033, 0.5623018145561218, 0.95647794008255, 0.7412790656089783, 0.35127899050712585, 0.8820492029190063, 0.8152647614479065, 0.9397000074386597, 0.7939254641532898, 0.6170525550842285, 0.9425733685493469, 0.6502039432525635, 0.8122058510780334, 0.8194001913070679, 0.8633902072906494, 0.9676373600959778, 0.9719609618186951, 0.8535578846931458, 0.8380745053291321, 0.957882285118103, 0.4096823036670685, 0.9808263778686523, 0.9985976815223694, 0.821480393409729, 0.9841120839118958, 0.9969825148582458, 0.9806780219078064, 0.6168326735496521, 0.9454169273376465, 0.9561020731925964, 0.99974125623703, 0.30194130539894104, 0.963478684425354, 0.6639825105667114, 0.3867390751838684, 0.9974159002304077, 0.18997806310653687, 0.8820484280586243, 0.5570837259292603, 0.9969366788864136, 0.8240322470664978, 0.09840013086795807, 0.6608174443244934, 0.6291516423225403, 0.8051145672798157, 0.8169763088226318, 0.9778386354446411, 0.9930744171142578, 0.44654321670532227, 0.9205619692802429, 0.9987238049507141, 0.9990344047546387, 0.9883804321289062, 0.4329196512699127, 0.9890228509902954, 0.9791371822357178, 0.7764338850975037, 0.9766880869865417, 0.9705116748809814, 0.9178494811058044, 0.881355881690979, 0.944058895111084, 0.9407246112823486, 0.9899875521659851, 0.9460278749465942, 0.6607576608657837, 0.928358256816864, 0.9797936081886292, 0.005414873361587524, 0.37625735998153687, 0.9297432899475098, 0.9273752570152283, 0.9284757971763611, 0.8206589221954346, 0.9932172894477844, 0.8131911158561707, 0.9376021027565002, 0.993243396282196, 0.6917340755462646, 0.6527082920074463, 0.9103895425796509, 0.9130222201347351, 0.8535633683204651, 0.007737233303487301, 0.966508686542511, 0.3796149492263794, 0.7951850891113281, 0.9815046191215515, 0.7412134408950806, 0.9630120396614075, 0.9697511196136475, 0.9686384797096252, 0.008397446013987064, 0.7075650095939636, 0.9348068237304688, 0.7503004670143127, 0.9066916704177856, 0.9836000204086304, 0.940395712852478, 0.994707465171814, 0.9705128073692322, 0.9924047589302063, 0.9092211723327637, 0.9096001386642456, 0.4601461589336395, 0.7737534642219543, 0.7423220276832581, 0.9507256746292114, 0.8545087575912476, 0.9321130514144897, 0.2910490334033966, 0.9848884344100952, 0.5357344150543213, 0.9848659038543701, 0.9234825372695923, 0.6073473691940308, 0.9419844746589661, 0.9967417120933533, 0.19265902042388916, 0.9952685236930847, 0.4650738537311554, 0.8319204449653625, 0.9338228106498718, 0.7648672461509705, 0.6066710352897644, 0.9574277997016907, 0.30795422196388245, 0.9934866428375244, 0.9969925880432129, 0.9318151473999023, 0.698322594165802, 0.9579495191574097, 0.05465676262974739, 0.013457952067255974, 0.93473881483078, 0.9980136156082153, 0.9952321648597717, 0.9130125641822815, 0.9941931366920471, 0.5573915839195251, 0.9945958256721497, 0.9916862845420837, 0.9019092917442322, 0.4665030837059021, 0.7084961533546448, 0.7229700088500977, 0.9799045324325562, 0.9412298798561096, 0.768875241279602, 0.6650318503379822, 0.989018976688385, 0.05666711926460266, 0.9483373165130615, 0.9628646969795227, 0.5548142790794373, 0.6927697658538818, 0.8400364518165588, 0.5749186277389526, 0.9443158507347107, 0.8808827996253967, 0.9398927092552185, 0.9837942719459534, 0.9981119632720947, 0.5594986081123352, 0.08901189267635345, 0.9969736337661743, 0.9935112595558167, 0.9178814888000488, 0.9274052977561951, 0.11546287685632706, 0.9793974757194519, 0.973800539970398, 0.29536354541778564, 0.29493439197540283, 0.9729310870170593, 0.4490449130535126, 0.9796591997146606, 0.9153572916984558, 0.869580090045929, 0.9795224666595459, 0.9744405746459961, 0.996695876121521, 0.6629499793052673, 0.4312388300895691, 0.5269824862480164, 0.9145193696022034, 0.026719603687524796, 0.17848673462867737, 0.9139032959938049, 0.8501843810081482, 0.9590506553649902, 0.969370424747467, 0.9331716895103455, 0.8783934116363525, 0.5128002762794495, 0.08761295676231384, 0.27603569626808167, 0.9772369861602783, 0.9824032783508301, 0.6389697194099426, 0.26744505763053894, 0.3516973555088043, 0.9740803837776184, 0.6891961693763733, 0.8770363330841064, 0.9739013910293579, 0.9994587302207947, 0.9769392609596252, 0.975907027721405, 0.9939099550247192, 0.9957833290100098, 0.5551252365112305, 0.5342066287994385, 0.9653887152671814, 0.878438413143158, 0.9446478486061096, 0.9507579803466797, 0.9784365296363831, 0.683377742767334, 0.26022520661354065, 0.9987384676933289, 0.9866581559181213, 0.9791057705879211, 0.8805477023124695, 0.771995484828949, 0.1684170961380005, 0.9655374884605408, 0.9578366875648499, 0.9938568472862244, 0.9608547687530518, 0.9469270706176758, 0.5064145922660828, 0.9614290595054626, 0.9077778458595276, 0.40639787912368774, 0.996753990650177, 0.9908808469772339, 0.9988484382629395, 0.9915001392364502, 0.9949159622192383, 0.9972798824310303, 0.8273154497146606, 0.9738754630088806, 0.9974862337112427, 0.6553558111190796, 0.3445066213607788, 0.9398453235626221, 0.8836826682090759, 0.9824020266532898, 0.8990691900253296, 0.7481216192245483, 0.8492286801338196, 0.47041448950767517, 0.9428079128265381, 0.9981182813644409, 0.9894019961357117, 0.6862677931785583, 0.9986586570739746, 0.9830136299133301, 0.917004406452179, 0.9861068725585938, 0.6224700808525085, 0.9654170274734497, 0.8335650563240051, 0.9692912697792053, 0.9823278188705444, 0.901178777217865, 0.5221182107925415, 0.4282573461532593, 0.9975735545158386, 0.01226898655295372, 0.595048725605011, 0.9636124968528748, 0.9910495281219482, 0.9980055689811707, 0.01613042689859867, 0.9442518949508667, 0.9857051372528076, 0.813032329082489, 0.9882466197013855, 0.9784567356109619, 0.9874513745307922, 0.7535447478294373, 0.4738401770591736, 0.5211235880851746, 0.41754746437072754, 0.19358520209789276, 0.9592651724815369, 0.6506320238113403, 0.901671290397644, 0.9853398203849792, 0.4856772720813751, 0.9996709823608398, 0.7927892804145813, 0.6417845487594604, 0.04373585060238838, 0.8087294697761536, 0.9906022548675537, 0.9666842818260193, 0.9590754508972168, 0.30241814255714417, 0.5765788555145264, 0.9982231259346008, 0.153760626912117, 0.2183963656425476, 0.9926003813743591, 0.9897242784500122, 0.9094917178153992, 0.3215668201446533, 0.9703715443611145, 0.9404934644699097, 0.9255279898643494, 0.35345879197120667, 0.6659704446792603, 0.2956278324127197, 0.9887939095497131, 0.940853476524353, 0.9764202237129211, 0.9983139038085938, 0.9980611205101013, 0.9425973296165466, 0.966321587562561, 0.7770953178405762, 0.8706656694412231, 0.986265242099762, 0.9196435809135437, 0.4518200159072876, 0.788436770439148, 0.5805513858795166, 0.9268434643745422, 0.988573431968689, 0.9812801480293274, 0.9784279465675354, 0.7982644438743591, 0.9980674386024475, 0.7730599045753479, 0.32991281151771545, 0.83091139793396, 0.9968740940093994, 0.47032734751701355, 0.9844247102737427, 0.2687091529369354, 0.9177564978599548, 0.9673352837562561, 0.9951558113098145, 0.9834111332893372, 0.9966747760772705, 0.01957111433148384, 0.9860671162605286, 0.9231426119804382, 0.0005862971884198487, 0.9386641979217529, 0.8906784057617188, 0.9692552089691162, 0.993865430355072, 0.9936398863792419, 0.6968774199485779, 0.337502121925354, 0.07502609491348267, 0.007134816609323025, 0.2330021858215332, 0.5722793340682983, 0.983235776424408, 0.021354036405682564, 0.972350537776947, 0.14345890283584595, 0.9775634407997131, 0.6930622458457947, 0.6917284727096558, 0.9850473403930664, 0.8978856205940247, 0.007538124453276396, 0.9990983009338379, 0.30700230598449707, 0.22684700787067413, 0.2891864776611328, 0.1870977282524109, 0.07030394673347473, 0.8719989657402039, 0.9563415050506592, 0.9887211918830872, 0.6654859185218811, 0.998772919178009, 0.8740546703338623, 0.17664766311645508, 0.7785922884941101, 0.32791027426719666, 0.48608461022377014, 0.0026258956640958786, 0.44940412044525146, 0.992975115776062, 0.9518415331840515, 0.9730691313743591, 0.9986660480499268, 0.9779016971588135, 0.9998384714126587, 0.4216235280036926, 0.9973669648170471, 0.9665337204933167, 0.05010807514190674, 0.9967071413993835, 0.2236620932817459, 0.966559112071991, 0.9514940977096558, 0.5860856771469116, 0.9826772809028625, 0.8966357111930847, 0.9065434336662292, 0.9609196782112122, 0.6345281004905701, 0.951073944568634, 0.8576294183731079, 0.5330058336257935, 0.6032609939575195, 0.9988850951194763, 0.9542285799980164, 0.843881368637085, 0.006630683783441782, 0.9922089576721191, 0.7951850891113281, 0.5253504514694214, 0.9727492332458496, 0.4857267141342163, 0.9838634729385376, 0.08598362654447556, 0.011065583676099777, 0.5659988522529602, 0.9529051780700684, 0.5531187653541565, 0.9939694404602051, 0.0446704737842083, 0.8526580929756165, 0.9974410533905029, 0.6253976821899414, 0.8773815631866455, 0.9947100877761841, 0.2742832899093628, 0.938247799873352, 0.45562422275543213, 0.9933549165725708, 0.7655498385429382, 0.9975691437721252, 0.998596727848053, 0.965121328830719, 0.972159743309021, 0.9543009400367737, 0.6527758240699768, 0.9490371942520142, 0.8299598097801208, 0.9984874725341797, 0.9499807357788086, 0.7725426554679871, 0.9372259378433228, 0.38599830865859985, 0.16014447808265686, 0.9899457097053528, 0.9154567122459412, 0.04578114673495293, 0.8936397433280945, 0.9624803066253662, 0.9983240962028503, 0.9980766773223877, 0.9971327781677246, 0.9814157485961914, 0.9914532899856567, 0.9023695588111877, 0.8818538188934326, 0.7539752721786499, 0.8967117071151733, 0.08964237570762634, 0.4373530447483063, 0.9546641111373901, 0.2609042823314667, 0.9753583073616028, 0.9860295653343201, 0.8417996168136597, 0.9779466390609741, 0.9533863067626953, 0.9959259033203125, 0.4298430383205414, 0.9758510589599609, 0.9206268191337585, 0.3693711459636688, 0.9959618449211121, 0.9933043122291565, 0.9988440275192261, 0.8086785078048706, 0.05576422065496445, 0.059975918382406235, 0.6892368793487549, 0.19136403501033783, 0.9880008101463318, 0.5990692377090454, 0.2527942359447479, 0.505906879901886, 0.6233533024787903, 0.20743565261363983, 0.9944593906402588, 0.2042326182126999, 0.05976894125342369, 0.9991632699966431, 0.996679425239563, 0.04348886013031006, 0.9507125020027161, 0.986117422580719, 0.5920567512512207, 0.5308560132980347, 0.9686372876167297, 0.6683585047721863, 0.46944260597229004, 0.8680856823921204, 0.7599563002586365, 0.025189055129885674, 0.9971123933792114, 0.9993189573287964, 0.9392575621604919, 0.4417344033718109, 0.9941180944442749, 0.999354898929596, 0.98773592710495, 0.3227840065956116, 0.7041524648666382, 0.2754579484462738, 0.999117910861969, 0.9597443342208862, 0.9810417294502258, 0.642725944519043, 0.020888272672891617, 0.9987829327583313, 0.9963555335998535, 0.8044866323471069, 0.0019883380737155676, 0.9850937128067017, 0.02223227359354496, 0.9966371059417725, 0.48227459192276, 0.9997643828392029, 0.5488190650939941, 0.8530238270759583, 0.5220593214035034, 0.16220055520534515, 0.615576982498169, 0.989388644695282, 0.764922559261322, 0.9856845140457153, 0.9735706448554993, 0.28357309103012085, 0.9359332919120789, 0.9228044152259827, 0.3080821931362152, 0.9970473647117615, 0.6678170561790466, 0.9396681189537048, 0.9005346298217773, 0.9699171781539917, 0.3635939955711365, 0.9789575338363647, 0.7026480436325073, 0.6936818957328796, 0.8877640962600708, 0.947307288646698, 0.9549272656440735, 0.950534999370575, 0.01960570178925991, 0.9440309405326843, 0.04115212708711624, 0.29959818720817566, 0.4813072085380554, 0.6697543263435364, 0.9963306784629822, 0.9882981181144714, 0.04042799770832062, 0.09497308731079102, 0.5362598896026611, 0.9961265921592712, 0.9988582134246826, 0.45011216402053833, 0.18548078835010529, 0.31582972407341003, 0.17212852835655212, 0.01240795198827982, 0.9513109922409058, 0.8700941205024719, 0.9560604095458984, 0.08197790384292603, 0.994426965713501, 0.9940555095672607, 0.5942882895469666, 0.549546480178833, 0.701510488986969, 0.9973561763763428, 0.008954930119216442, 0.9989718198776245, 0.5854236483573914, 0.391924113035202, 0.9792576432228088, 0.15611755847930908, 0.9902964234352112, 0.9991759657859802, 0.07467237859964371, 0.9913569688796997, 0.9235582947731018, 0.15173698961734772, 0.008874869905412197, 0.8595216274261475, 0.9913449287414551, 0.5642044544219971, 0.02050415799021721, 0.9829135537147522, 0.9567322134971619, 0.9926736950874329, 0.7486538290977478, 0.97664475440979, 0.9846820831298828, 0.7042732834815979, 0.8305447101593018, 0.3300189971923828, 0.9935398697853088, 0.9186210632324219, 0.931816577911377, 0.3064384162425995, 0.8119581937789917, 0.9999313354492188, 0.9781944155693054, 0.9125611782073975, 0.557380735874176, 0.9578924179077148, 0.4305150806903839, 0.23155327141284943, 0.3993588387966156, 0.9920349717140198, 0.9191266894340515, 0.5845504999160767, 0.9900367259979248, 0.9818516969680786, 0.6545377373695374, 0.9967400431632996, 0.9472785592079163, 0.9977433681488037, 0.9964487552642822, 0.9210978746414185, 0.5624222755432129, 0.995489776134491, 0.5854459404945374, 0.9730966687202454, 0.9650747179985046, 0.9992369413375854, 0.32999083399772644, 0.5000941753387451, 0.9723618030548096, 0.13350236415863037, 0.48187151551246643, 0.5145434737205505, 0.968858540058136, 0.9549724459648132, 0.12503477931022644, 0.9119357466697693, 0.8382216691970825, 0.9968356490135193, 0.9892433881759644, 0.5854236483573914, 0.0026772371493279934, 0.9760977029800415, 0.968778669834137, 0.8987495303153992, 0.9803724884986877, 0.9435940980911255, 0.9920245409011841, 0.9366077184677124, 0.8385621905326843, 0.011167189106345177, 0.9673857092857361, 0.9250141978263855, 0.8693589568138123, 0.9115378856658936, 0.07458381354808807, 0.4952945113182068, 0.09280286729335785, 0.6603403687477112, 0.20166151225566864, 0.9407690167427063, 0.5157508850097656, 0.7647470235824585, 0.7548287510871887, 0.761614203453064, 0.9255875945091248, 0.9907236695289612, 0.9985343217849731, 0.8367365598678589, 0.8085262179374695, 0.7501696944236755, 0.9063543677330017, 0.006424814462661743, 0.9873119592666626, 0.7979468703269958, 0.060423173010349274, 0.7974393963813782, 0.958258330821991, 0.9915667176246643, 0.9479737281799316, 0.9607837796211243, 0.6896482110023499, 0.25642144680023193, 0.9537651538848877, 0.8139685988426208, 0.8914441466331482, 0.8692888617515564, 0.21728608012199402, 0.9983276724815369, 0.41029486060142517, 0.9708160758018494, 0.03583331033587456, 0.9852743148803711, 0.9938958287239075, 0.9471649527549744, 0.8132357597351074, 0.8685823082923889, 0.6513539552688599, 0.015808425843715668, 0.6751893758773804, 0.03767755627632141, 0.9425904154777527, 0.640260636806488, 0.9832952618598938, 0.4646579623222351, 0.2271725982427597, 0.998077392578125, 0.07268718630075455, 0.2676474153995514, 0.38204097747802734, 0.44613325595855713, 0.5981445908546448, 0.02902059629559517, 0.06493594497442245, 0.8885394930839539, 0.04337001591920853, 0.24474558234214783, 0.37057945132255554, 0.7815269827842712, 0.9886143207550049, 0.5854968428611755, 0.012483936734497547, 0.02418414130806923, 0.9834889769554138, 0.9915503263473511, 0.7027407288551331, 0.7411542534828186, 0.9611611366271973, 0.9961634874343872, 0.5352779030799866, 0.9987049102783203, 0.9265378713607788, 0.9945966005325317, 0.02439182624220848, 0.9937386512756348, 0.9946790933609009, 0.9444323778152466, 0.05496445298194885, 0.08486808091402054, 0.9964498281478882, 0.8015795946121216, 0.8495533466339111, 0.24460428953170776, 0.6196408867835999, 0.9685219526290894, 0.917891263961792, 0.5887399315834045, 0.37302955985069275, 0.8096532225608826, 0.44154757261276245, 0.27607107162475586, 0.3419008255004883, 0.5530602931976318, 0.26236405968666077, 0.9953881502151489, 0.5173713564872742, 0.44136881828308105, 0.8662906885147095, 0.9705116748809814, 0.0754527598619461, 0.5596344470977783, 0.919364869594574, 0.3445066213607788, 0.8811659216880798, 0.36442282795906067, 0.9739313721656799, 0.8978416323661804, 0.9256531000137329, 0.177820086479187, 0.9650776982307434, 0.6939864158630371, 0.9667872786521912, 0.6015257835388184, 0.8741201758384705, 0.9531043767929077, 0.4273436963558197, 0.891124427318573, 0.6747703552246094, 0.9246975183486938, 0.5754970908164978, 0.9616057276725769, 0.9781593084335327, 0.7597650289535522, 0.8283488750457764, 0.9348510503768921, 0.045023363083601, 0.9898417592048645, 0.9859573841094971, 0.9581739902496338, 0.10289032757282257, 0.653958797454834, 0.9835900664329529, 0.9623756408691406, 0.9389752745628357, 0.8845234513282776, 0.9066808223724365, 0.8995940089225769, 0.9991602897644043, 0.8127323985099792, 0.8100916147232056, 0.9603562355041504, 0.9014710187911987, 0.4292674958705902, 0.9996849298477173, 0.9705128073692322, 0.5141856074333191, 0.9781011343002319, 0.6951702237129211, 0.911496102809906, 0.7788583040237427, 0.0008420972735621035, 0.21090789139270782, 0.984303891658783, 0.9934604167938232, 0.9983622431755066, 0.3925340473651886, 0.9823278188705444, 0.01894846186041832, 0.6819589734077454, 0.923454999923706, 0.7972986698150635, 0.9952947497367859, 0.9168553948402405, 0.9514302015304565, 0.995036780834198, 0.8928358554840088, 0.007374752778559923, 0.9893504977226257, 0.9834110140800476, 0.9636942744255066, 0.06226424127817154, 0.03790014609694481, 0.7813555598258972, 0.9798727035522461, 0.21341857314109802, 0.9989596605300903, 0.9837355613708496, 0.9405770897865295, 0.9756238460540771, 0.9929787516593933, 0.9852576851844788, 0.8266848921775818, 0.983667254447937, 0.7244665622711182, 0.9919565916061401, 0.21983246505260468, 0.9959579110145569, 0.3760819137096405, 0.9960325360298157, 0.9381615519523621, 0.994975209236145, 0.9907448887825012, 0.7409222722053528, 0.39391887187957764, 0.994551956653595, 0.6653039455413818, 0.7755096554756165, 0.9994615912437439, 0.9722887873649597, 0.9977232813835144, 0.5547745227813721, 0.13762520253658295, 0.03207356855273247, 0.9990659356117249, 0.9190082550048828, 0.8757391571998596, 0.9891889095306396, 0.015276025980710983, 0.008938474580645561, 0.9971580505371094, 0.9874159693717957, 0.9462890028953552, 0.9743120074272156, 0.2410389631986618, 0.9492202997207642, 0.911835253238678, 0.5790074467658997, 0.03800935670733452, 0.9881805181503296, 0.2328570932149887, 0.09113012999296188, 0.9263020753860474, 0.5798683166503906, 0.8735141754150391, 0.9993433356285095, 0.9906700849533081, 0.2776433229446411, 0.9817095398902893, 0.7555016875267029, 0.013918816111981869, 0.34330078959465027, 0.9850655198097229, 0.9827356338500977, 0.06036471948027611, 0.7254949808120728, 0.9939870834350586, 0.7929141521453857, 0.9799360036849976, 0.9618671536445618, 0.10969529300928116, 0.023131273686885834, 0.9441679120063782, 0.46731868386268616, 0.9833225011825562, 0.7931649684906006, 0.5914651155471802, 0.4368860423564911, 0.9909002780914307, 0.6349833011627197, 0.9621129631996155, 0.8645930886268616, 0.9670370221138, 0.9924801588058472, 0.6672034859657288, 0.8186864256858826, 0.18924476206302643, 0.9285297393798828, 0.8244255185127258, 0.9994093179702759, 0.9476616382598877, 0.9236848950386047, 0.9420300722122192, 0.3618485927581787, 0.6648811101913452, 0.858654797077179, 0.9476063847541809, 0.9889662861824036, 0.5456767082214355, 0.5872538685798645, 0.990475594997406, 0.4785621762275696, 0.7589584589004517, 0.6154853105545044, 0.9867026805877686, 0.7095418572425842, 0.7975983023643494, 0.5585012435913086, 0.9950124621391296, 0.940568208694458, 0.9974205493927002, 0.9931429624557495, 0.12031149119138718, 0.851578950881958, 0.9506256580352783, 0.9946704506874084, 0.9973984956741333, 0.05567188933491707, 0.9705116748809814, 0.9413573741912842, 0.910816490650177, 0.926218569278717, 0.9807372689247131, 0.1109495609998703, 0.9941177368164062, 0.9892086386680603, 0.9757497310638428, 0.5621298551559448, 0.9976348876953125, 0.9576438665390015, 0.9989920258522034, 0.9910231828689575, 0.6250658631324768, 0.9221673607826233, 0.8405681848526001, 0.9404264688491821, 0.6775735020637512, 0.5823289155960083, 0.9797679781913757, 0.4773868918418884, 0.1458149254322052, 0.28970158100128174, 0.18233096599578857, 0.006922835484147072, 0.380787193775177, 0.9726126194000244, 0.9927998781204224, 0.993928074836731, 0.9187065958976746, 0.8734461069107056, 0.9925714135169983, 0.9382336139678955, 0.8923838138580322, 0.887067973613739, 0.8103741407394409, 0.9720433950424194, 0.9824602603912354, 0.9508566856384277, 0.8558446764945984, 0.12034233659505844, 0.9983757734298706, 0.8829941749572754, 0.8681986331939697, 0.9200712442398071, 0.3899385631084442, 0.5492120385169983, 0.9969064593315125, 0.8717560768127441, 0.058064378798007965, 0.7951850891113281, 0.6402096152305603, 0.8539508581161499, 0.9707575440406799, 0.17610061168670654, 0.8601969480514526, 0.9857915639877319, 0.9515424370765686, 0.997340977191925, 0.9777721166610718, 0.978478193283081, 0.8784366846084595, 0.9176496267318726, 0.4438727796077728, 0.4209534823894501, 0.949148416519165, 0.9872592091560364, 0.9784772992134094, 0.9013773798942566, 0.7430291771888733, 0.32494351267814636, 0.9512048363685608, 0.2252362072467804, 0.15981999039649963, 0.47748813033103943, 0.9974718689918518, 0.9245046973228455, 0.9599219560623169, 0.9881389737129211, 0.9388758540153503, 0.3302609920501709, 0.997307300567627, 0.9652425050735474, 0.8462450504302979, 0.03527839854359627, 0.9842563271522522, 0.42788052558898926, 0.49024903774261475, 0.6428437232971191, 0.7205427885055542, 0.15173162519931793, 0.9860568046569824, 0.9686592817306519, 0.9966685175895691, 0.9972692131996155, 0.34446796774864197, 0.06300101429224014, 0.9837661981582642, 0.9699541926383972, 0.16284045577049255, 0.9622181057929993, 0.7082157135009766, 0.999528169631958, 0.8044850826263428, 0.8746593594551086, 0.8009595274925232, 0.9594832062721252, 0.7449780702590942, 0.9845332503318787, 0.9750638604164124, 0.9976993203163147, 0.9752892255783081, 0.9676007628440857, 0.3863363564014435, 0.6144047379493713, 0.9823877215385437, 0.40793606638908386, 0.5828808546066284, 0.9986820816993713, 0.993243396282196, 0.9921489953994751, 0.49796199798583984, 0.8023678064346313, 0.9432666301727295, 0.9899281859397888, 0.9832778573036194, 0.3935084342956543, 0.01174147892743349, 0.5344058275222778, 0.9239993691444397, 0.4713084101676941, 0.8497317433357239, 0.010272707790136337, 0.3313722610473633, 0.9987574815750122, 0.28586727380752563, 0.0060975332744419575, 0.9898009896278381, 0.9962366223335266, 0.9757726192474365, 0.5114423632621765, 0.4242423176765442, 0.9513193964958191, 0.0290168896317482, 0.1523829847574234, 0.9842240810394287, 0.9952207207679749, 0.22972047328948975, 0.7505649328231812, 0.7846077680587769, 0.42752960324287415, 0.9255679845809937, 0.9659098982810974, 0.9993957281112671, 0.8099245429039001, 0.7688215970993042, 0.4013250172138214, 0.7214651703834534, 0.9806566834449768, 0.9969925880432129, 0.9910078644752502, 0.4748585522174835, 0.9668498635292053, 0.998446524143219, 0.9917873740196228, 0.014803818427026272, 0.8041158318519592, 0.6343415975570679, 0.2531659007072449, 0.9107608199119568, 0.9704267978668213, 0.9820441007614136, 0.993243396282196, 0.9788589477539062, 0.5540791153907776, 0.5037540197372437, 0.9991958737373352, 0.0921778753399849, 0.8833572864532471, 0.9988359808921814, 0.9896200299263, 0.9385634660720825, 0.9960136413574219, 0.6723534464836121, 0.7439351081848145, 0.9716639518737793, 0.24669183790683746, 0.013635963201522827, 0.9790598154067993, 0.7512791752815247, 0.9836836457252502, 0.8594288229942322, 0.5544410943984985, 0.8784700632095337, 0.36959385871887207, 0.968384325504303, 0.9306312799453735, 0.20120207965373993, 0.015681399032473564, 0.3171435594558716, 0.9845518469810486, 0.773962140083313, 0.9023695588111877, 0.9857656955718994, 0.9989688396453857, 0.10316149890422821, 0.9905000329017639, 0.9895638823509216, 0.3761061131954193, 0.9386657476425171, 0.9341903328895569, 0.9068198800086975, 0.22537221014499664, 0.6260768175125122, 0.2431928962469101, 0.7228581309318542, 0.9957143664360046, 0.9818364977836609, 0.6483690738677979, 0.2399340271949768, 0.0026115693617612123, 0.038858991116285324, 0.9734659194946289, 0.9737111330032349, 0.6118398308753967, 0.43142861127853394, 0.8742785453796387, 0.9969925880432129, 0.9953805208206177, 0.9373370409011841, 0.9924265146255493, 0.8850606083869934, 0.8442361950874329, 0.9549303650856018, 0.1494191437959671, 0.7823352813720703, 0.9858982563018799, 0.739035964012146, 0.27333909273147583, 0.978752851486206, 0.9975100755691528, 0.9330624938011169, 0.004233562853187323, 0.993170976638794, 0.8654258251190186, 0.9890005588531494, 0.9324013590812683, 0.3056928813457489, 0.8019742965698242, 0.8788988590240479, 0.10237718373537064, 0.274037629365921, 0.6553797721862793, 0.6405326724052429, 0.5444270372390747, 0.9924894571304321, 0.9850338101387024, 0.9982061386108398, 0.36057111620903015, 0.7675729393959045, 0.8909173607826233, 0.9911660552024841, 0.9205971956253052, 0.34324878454208374, 0.6528837084770203, 0.8623392581939697, 0.8512662053108215, 0.9945530891418457, 0.9922468662261963, 0.42069628834724426, 0.9854786396026611, 0.9128924608230591, 0.323026180267334, 0.9955440163612366, 0.7339340448379517, 0.9961373209953308, 0.2796002924442291, 0.9876236915588379, 0.9923908114433289, 0.2830573618412018, 0.5865927338600159, 0.9914002418518066, 0.2816859185695648, 0.3578691780567169, 0.8665764331817627, 0.84193354845047, 0.07101540267467499, 0.9830054640769958, 0.19731631875038147, 0.9789131283760071, 0.8390598893165588, 0.9841761589050293, 0.9689317345619202, 0.9430919885635376, 0.994492769241333, 0.7704597115516663, 0.9786514639854431, 0.6699280738830566, 0.9964073300361633, 0.7951850891113281, 0.3335072994232178, 0.8422820568084717, 0.9786362051963806, 0.9905905723571777, 0.9563823938369751, 0.5212886333465576, 0.7256263494491577, 0.3017064929008484, 0.07279612123966217, 0.9158753156661987, 0.9529077410697937, 0.9652532935142517, 0.9317557215690613, 0.02944202348589897, 0.6024186611175537, 0.9630869626998901, 0.8842855095863342, 0.9350447654724121, 0.9995211362838745, 0.9282506108283997, 0.44113874435424805, 0.4047529399394989, 0.9669829607009888, 0.9153572916984558, 0.9768909811973572, 0.9642884135246277, 0.8986209034919739, 0.5367034077644348, 0.8770514726638794, 0.9899566769599915, 0.6994703412055969, 0.005770414136350155, 0.2986266613006592, 0.13452723622322083, 0.622550904750824, 0.9402359127998352, 0.053088199347257614, 0.9658063650131226, 0.9966856837272644, 0.7179176807403564, 0.9684938788414001, 0.9322054386138916, 0.9881173968315125, 0.7276153564453125, 0.9084798097610474, 0.4460271894931793, 0.9200423955917358, 0.959703266620636, 0.9739938974380493, 0.2599220275878906, 0.9570222496986389, 0.2847885191440582, 0.18715953826904297, 0.9773135781288147, 0.9986979961395264, 0.758866012096405, 0.7699778079986572, 0.294778972864151, 0.9994392991065979, 0.9934892654418945, 0.28626179695129395, 0.9487022161483765, 0.2721982002258301, 0.03023224137723446, 0.838028073310852, 0.9413907527923584, 0.5464020371437073, 0.6673110723495483, 0.8225800395011902, 0.7313168048858643, 0.7920523285865784, 0.28204870223999023, 0.9964321851730347, 0.7558972835540771, 0.09900008141994476, 0.35190463066101074, 0.996188223361969, 0.7898651957511902, 0.9825002551078796, 0.9332041144371033, 0.24684184789657593, 0.1961173117160797, 0.899573564529419, 0.9397791624069214, 0.9881338477134705, 0.010920406319200993, 0.9621502757072449, 0.7236875295639038, 0.9963731169700623, 0.06699717044830322, 0.0464656800031662, 0.7357111573219299, 0.908492386341095, 0.963513195514679, 0.7383712530136108, 0.03451652452349663, 0.7027528882026672, 0.5213262438774109, 0.99137282371521, 0.3622557818889618, 0.9807970523834229, 0.986626923084259, 0.9817368984222412, 0.06386994570493698, 0.9161461591720581, 0.3230213522911072, 0.8492628335952759, 0.5186278223991394, 0.921164333820343, 0.9174544215202332, 0.9891688823699951, 0.9517308473587036, 0.9944478273391724, 0.9704267978668213, 0.18022340536117554, 0.9944131970405579, 0.04308644309639931, 0.9997912049293518, 0.2777339816093445, 0.6510738134384155, 0.7568379640579224, 0.455008327960968, 0.9575544595718384, 0.25612157583236694, 0.9917379021644592, 0.778778076171875, 0.8434798717498779, 0.8307616114616394, 0.979831874370575, 0.9209159016609192, 0.13653281331062317, 0.9992600083351135, 0.9541128873825073, 0.9886730313301086, 0.9975481629371643, 0.28928181529045105, 0.32595497369766235, 0.8001657724380493, 0.9095774292945862, 0.8644430637359619, 0.7795047760009766, 0.5247917175292969, 0.08066326379776001, 0.6832678318023682, 0.8205306529998779, 0.9984903335571289, 0.0691002607345581, 0.0033998405560851097, 0.0004496370384003967, 0.004269012715667486, 0.0005753978621214628, 0.017659371718764305, 0.45241084694862366, 6.879809370730072e-05, 2.6811512725544162e-05, 0.003321434836834669, 0.00010927127004833892, 0.0001935825275722891, 0.0014338345499709249, 0.0007558304932899773, 0.0018776424694806337, 6.6912225520354696e-06, 0.0027697812765836716, 0.0010327572235837579, 0.002577309962362051, 0.010656697675585747, 0.0013002624036744237, 0.1712609827518463, 0.00012323113332968205, 0.00022174025070853531, 2.686013795027975e-05, 0.00030940494616515934, 0.006843093782663345, 0.00032863346859812737, 0.032857298851013184, 0.00010669967741705477, 0.00021605219808407128, 0.00033493730006739497, 0.0006476027774624527, 0.009053248912096024, 0.0007375845452770591, 0.00010098914208356291, 0.0003263800754211843, 0.0005735756130889058, 0.0007500387146137655, 0.004580579698085785, 0.0192201416939497, 0.12683290243148804, 0.16435831785202026, 0.033365968614816666, 6.523928459500894e-05, 0.06862349808216095, 0.048629242926836014, 0.0002868447918444872, 3.159737752866931e-05, 0.0013159741647541523, 0.019148731604218483, 0.0012625608360394835, 0.0010082421358674765, 0.0018710641888901591, 2.041122570517473e-05, 0.00032768392702564597, 0.025480637326836586, 0.010062575340270996, 0.006800387520343065, 0.006402662489563227, 6.601663335459307e-05, 0.010606606490910053, 0.00867496058344841, 8.892102778190747e-05, 0.0007799203158356249, 0.008008947595953941, 0.004057236481457949, 0.0001877898903330788, 0.006079008802771568, 7.500820356654003e-05, 0.0034590584691613913, 0.00020426818809937686, 0.7481216192245483, 0.00013988168211653829, 0.00011173957318533212, 0.0059638130478560925, 0.0006957875448279083, 0.003679804038256407, 4.165858626947738e-05, 4.062621883349493e-05, 0.001079327194020152, 0.004876611288636923, 0.0010136733762919903, 0.10003547370433807, 0.0002829670556820929, 0.0009511123644188046, 0.0003851526998914778, 0.0005109831690788269, 0.000389331195037812, 0.00018036011897493</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>[0.6512571573257446, 0.518426775932312, 0.22227220237255096, 0.9985502362251282, 0.9362854957580566, 0.5282945036888123, 0.9398465752601624, 0.5585426688194275, 0.9669273495674133, 0.07476592063903809, 0.765052080154419, 0.8527607917785645, 0.9185080528259277, 0.992219865322113, 0.9990798234939575, 0.10202254354953766, 0.7853681445121765, 0.556739091873169, 0.08099322766065598, 0.9615274667739868, 0.9738321900367737, 0.30111536383628845, 0.9833923578262329, 0.13840438425540924, 0.191274955868721, 0.4250219762325287, 0.93863844871521, 0.7623707056045532, 0.6486994028091431, 0.5581556558609009, 0.079678013920784, 0.7681796550750732, 0.833859920501709, 0.9711730480194092, 0.7417529225349426, 0.8091307282447815, 0.9957096576690674, 0.2405744045972824, 0.9162002801895142, 0.904982328414917, 0.9831603169441223, 0.9565339088439941, 0.9908016324043274, 0.10032864660024643, 0.9640955328941345, 0.3803219199180603, 0.9997143149375916, 0.9305363893508911, 0.7285496592521667, 0.6662929058074951, 0.9780821800231934, 0.8559299111366272, 0.8361693620681763, 0.8828379511833191, 0.9733238220214844, 0.8503140211105347, 0.9618774056434631, 0.681114912033081, 0.9861735105514526, 0.9449528455734253, 0.722863495349884, 0.9761084914207458, 0.7450305819511414, 0.9990622401237488, 0.9964994192123413, 0.9939054846763611, 0.9702099561691284, 0.17186038196086884, 0.9975743889808655, 0.8756104111671448, 0.6869242787361145, 0.9486330151557922, 0.7216919660568237, 0.9102966785430908, 0.9678005576133728, 0.9993187189102173, 0.8778086304664612, 0.9981231093406677, 0.9806532859802246, 0.425595760345459, 0.3751675486564636, 0.9511232972145081, 0.10596910864114761, 0.9062920808792114, 0.9864630103111267, 0.7430832982063293, 0.714270293712616, 0.03948388621211052, 0.9857550859451294, 0.9957108497619629, 0.9221832156181335, 0.9936448335647583, 0.8662382364273071, 0.999723494052887, 0.9822589159011841, 0.169439896941185, 0.16883598268032074, 0.5074711441993713, 0.820205807685852, 0.9929603934288025, 0.9243271350860596, 0.881843090057373, 0.9929714798927307, 0.5450389981269836, 0.9848782420158386, 0.932835578918457, 0.9964069724082947, 0.8976343870162964, 0.09109512716531754, 0.7890782952308655, 0.1428348571062088, 0.9526308178901672, 0.9447462558746338, 0.32367345690727234, 0.9789313673973083, 0.8417170643806458, 0.9056951999664307, 0.5776114463806152, 0.4588130712509155, 0.07447893917560577, 0.9590006470680237, 0.9187953472137451, 0.9635715484619141, 0.9995274543762207, 0.966691792011261, 0.9979039430618286, 0.19755984842777252, 0.9598163962364197, 0.9175357222557068, 0.993939995765686, 0.5192770957946777, 0.42353907227516174, 0.008220003917813301, 0.9047062993049622, 0.6482336521148682, 0.9359466433525085, 0.9913690686225891, 0.6391226053237915, 0.7291821837425232, 0.8753369450569153, 0.9988663196563721, 0.9577194452285767, 0.9970894455909729, 0.6951255798339844, 0.7070851922035217, 0.6884894371032715, 0.49490657448768616, 0.7163532376289368, 0.9969990253448486, 0.9737101197242737, 0.5252626538276672, 0.01837526634335518, 0.5514037609100342, 0.7426304221153259, 0.9714042544364929, 0.9560266733169556, 0.37309107184410095, 0.9321025609970093, 0.9827720522880554, 0.7774613499641418, 0.855898380279541, 0.06495892256498337, 0.07221732288599014, 0.9265150427818298, 0.6774342060089111, 0.8031933307647705, 0.6179938912391663, 0.7835070490837097, 0.5529961585998535, 0.9885224103927612, 0.4310832619667053, 0.9917014241218567, 0.986332356929779, 0.4334675669670105, 0.8190314769744873, 0.6763724088668823, 0.20324856042861938, 0.9123324155807495, 0.9271252751350403, 0.9718974232673645, 0.8051564693450928, 0.9629839658737183, 0.22285054624080658, 0.9212075471878052, 0.8300297856330872, 0.5384545922279358, 0.9845982789993286, 0.9923337697982788, 0.048732511699199677, 0.9347934126853943, 0.9087194204330444, 0.9069881439208984, 0.1762661635875702, 0.13057301938533783, 0.5372846722602844, 0.9953393936157227, 0.9854803681373596, 0.7155485153198242, 0.4610605835914612, 0.9979709982872009, 0.49657490849494934, 0.9316466450691223, 0.8333669304847717, 0.39235353469848633, 0.4253517985343933, 0.3170502781867981, 0.9933011531829834, 0.03700101003050804, 0.803722620010376, 0.994224488735199, 0.12880872189998627, 0.9843637347221375, 0.9878778457641602, 0.2341766357421875, 0.9756075143814087, 0.9966551065444946, 0.9515031576156616, 0.5802290439605713, 0.041263602674007416, 0.2319430112838745, 0.6034703850746155, 0.05385761708021164, 0.43071305751800537, 0.9500155448913574, 0.008664182387292385, 0.7524522542953491, 0.620481014251709, 0.0809868574142456, 0.14224421977996826, 0.01817925088107586, 0.9871852993965149, 0.8039527535438538, 0.9190122485160828, 0.9251624345779419, 0.22754211723804474, 0.4869769215583801, 0.02587013505399227, 0.3161148726940155, 0.026973340660333633, 0.3439420759677887, 0.9153242707252502, 0.002642405452206731, 0.07518759369850159, 0.06555638462305069, 0.7272091507911682, 0.9779089093208313, 0.9757971167564392, 0.9093983769416809, 0.8772199749946594, 0.9955253005027771, 0.1719094067811966, 0.9997077584266663, 0.969357430934906, 0.4339848756790161, 0.4942176938056946, 0.6230172514915466, 0.5627833008766174, 0.9114827513694763, 0.9997089505195618, 0.983648419380188, 0.08974535018205643, 0.052967991679906845, 0.98453289270401, 0.9209370017051697, 0.12303955107927322, 0.05357404053211212, 0.2099156677722931, 0.12758222222328186, 0.7122294306755066, 0.1404525190591812, 0.06772756576538086, 0.3185434639453888, 0.3564470112323761, 0.7253332138061523, 0.9065332412719727, 0.6346002817153931, 0.047815319150686264, 0.9982407093048096, 0.7641740441322327, 0.9080988168716431, 0.36762335896492004, 0.29411494731903076, 0.9989633560180664, 0.9836898446083069, 0.22736835479736328, 0.8073091506958008, 0.16970744729042053, 0.9994589686393738, 0.08255907148122787, 0.5533125400543213, 0.997017502784729, 0.6465768814086914, 0.583067774772644, 0.9973128437995911, 0.9046960473060608, 0.7907698750495911, 0.866157054901123, 0.794342041015625, 0.4124578535556793, 0.870092511177063, 0.27864712476730347, 0.7822328805923462, 0.998501181602478, 0.2610933780670166, 0.12463013082742691, 0.7554392218589783, 0.5356745719909668, 0.3721742331981659, 0.9853886961936951, 0.9911858439445496, 0.05298677086830139, 0.10733781009912491, 0.024631943553686142, 0.9984911680221558, 0.7671975493431091, 0.9864646196365356, 0.7824406027793884, 0.9618517160415649, 0.9787275195121765, 0.9601679444313049, 0.13614362478256226, 0.7503744959831238, 0.9976204037666321, 0.9905155897140503, 0.5139713287353516, 0.9703916907310486, 0.19452548027038574, 0.7042257785797119, 0.7411351203918457, 0.4918130338191986, 0.49350884556770325, 0.9490985870361328, 0.9897835850715637, 0.963596761226654, 0.48418769240379333, 0.2905718684196472, 0.328792005777359, 0.5719773173332214, 0.8318625092506409, 0.05934625864028931, 0.2928553819656372, 0.33418288826942444, 0.6327018737792969, 0.8976081609725952, 0.5993242859840393, 0.9205042719841003, 0.9258983731269836, 0.9936216473579407, 0.962873101234436, 0.9029180407524109, 0.9544017314910889, 0.9940104484558105, 0.1453799456357956, 0.9688751101493835, 0.9712628722190857, 0.21572978794574738, 0.9994511008262634, 0.018904363736510277, 0.931069552898407, 0.8028702735900879, 0.4289977252483368, 0.874337911605835, 0.05045977979898453, 0.08631011098623276, 0.867753267288208, 0.9895405173301697, 0.25794684886932373, 0.9142261147499084, 0.3121986985206604, 0.9682195782661438, 0.9377551674842834, 0.5034753084182739, 0.2169695347547531, 0.42493921518325806, 0.9806159138679504, 0.9584185481071472, 0.7628780007362366, 0.9934656023979187, 0.9870583415031433, 0.8756349086761475, 0.9667899012565613, 0.9206182360649109, 0.9993940591812134, 0.938376247882843, 0.7541171908378601, 0.9922837615013123, 0.15558721125125885, 0.24963250756263733, 0.7824823260307312, 0.24290528893470764, 0.18085837364196777, 0.9884603023529053, 0.18189555406570435, 0.9824784398078918, 0.9613032341003418, 0.6787847280502319, 0.9012942910194397, 0.6083488464355469, 0.9979281425476074, 0.5945268869400024, 0.08835087716579437, 0.9768978357315063, 0.950288712978363, 0.6953337788581848, 0.9009280800819397, 0.19770480692386627, 0.831581711769104, 0.4337669312953949, 0.4625530540943146, 0.19418494403362274, 0.9958699345588684, 0.6470316648483276, 0.9895589351654053, 0.849080502986908, 0.3723938465118408, 0.9892599582672119, 0.6604897379875183, 0.8712994456291199, 0.02058165706694126, 0.9912729859352112, 0.4390576481819153, 0.6783226132392883, 0.9634803533554077, 0.9223085045814514, 0.10502883046865463, 0.04959603399038315, 0.725435733795166, 0.6619167923927307, 0.0009631751454435289, 0.0012328915763646364, 0.4962753653526306, 0.026295334100723267, 0.9632030129432678, 0.32639071345329285, 0.27382081747055054, 0.9051783084869385, 0.04672598838806152, 0.8826666474342346, 0.3085727393627167, 0.19169820845127106, 0.9350095391273499, 0.05782696604728699, 0.9928560256958008, 0.9771623015403748, 0.7840681076049805, 0.9837237596511841, 0.926688015460968, 0.9958891272544861, 0.5959017872810364, 0.9980137348175049, 0.31540438532829285, 0.40144479274749756, 0.02430778741836548, 0.993040919303894, 0.5809909701347351, 0.07416614145040512, 0.9967039227485657, 0.06621073931455612, 0.5685225129127502, 0.8966236114501953, 0.8727556467056274, 0.012456614524126053, 0.7437984347343445, 0.8743252754211426, 0.1393572837114334, 0.6447620987892151, 0.5780600309371948, 0.39625194668769836, 0.37077265977859497, 0.8717848062515259, 0.9815480709075928, 0.9855323433876038, 0.5001399517059326, 0.9658806920051575, 0.05619267001748085, 0.13876354694366455, 0.9193719625473022, 0.08739753067493439, 0.6245774030685425, 0.1683845818042755, 0.24486218392848969, 0.993030846118927, 0.013818459585309029, 0.1261858493089676, 0.929803192615509, 0.2650083899497986, 0.5476788878440857, 0.85308438539505, 0.8575186133384705, 0.035554468631744385, 0.8997693061828613, 0.8612374067306519, 0.9099698662757874, 0.8867401480674744, 0.9868905544281006, 0.7557446360588074, 0.8888197541236877, 0.8539718389511108, 0.29151058197021484, 0.8547508120536804, 0.21586808562278748, 0.6580604910850525, 0.01486668735742569, 0.9130491614341736, 0.40265610814094543, 0.5369542241096497, 0.056401558220386505, 0.94525545835495, 0.14846950769424438, 0.7825788259506226, 0.7574517130851746, 0.9291399121284485, 0.9981231093406677, 0.23995433747768402, 0.8911120295524597, 0.7011715173721313, 0.132513165473938, 0.2959626615047455, 0.9504964351654053, 0.26822951436042786, 0.8230996131896973, 0.990199863910675, 0.7752562761306763, 0.03590814396739006, 0.8903619050979614, 0.46173807978630066, 0.5271720886230469, 0.8813889622688293, 0.5226043462753296, 0.8043303489685059, 0.4357260763645172, 0.9227012395858765, 0.6636005640029907, 0.8255089521408081, 0.43874630331993103, 0.9076326489448547, 0.27742165327072144, 0.9438736438751221, 0.994383692741394, 0.007358842063695192, 0.05956196412444115, 0.4675462245941162, 0.9329714179039001, 0.32134249806404114, 0.010903602465987206, 0.25394493341445923, 0.9457733631134033, 0.9595866799354553, 0.09009282290935516, 0.9764149188995361, 0.897528350353241, 0.4172387421131134, 0.9833395481109619, 0.01089509017765522, 0.6371890902519226, 0.42901554703712463, 0.6842336058616638, 0.7407204508781433, 0.16817951202392578, 0.16621637344360352, 0.2202669084072113, 0.4430294334888458, 0.9862850904464722, 0.9901751279830933, 0.9977236390113831, 0.7578659653663635, 0.7854273915290833, 0.9742603898048401, 0.320650577545166, 0.39458799362182617, 0.8461278676986694, 0.9171788692474365, 0.8993771076202393, 0.3837953209877014, 0.34664905071258545, 0.969325840473175, 0.995313286781311, 0.6242190599441528, 0.9940356016159058, 0.8077689409255981, 0.937167227268219, 0.027238691225647926, 0.989970862865448, 0.6569364070892334, 0.9300483465194702, 0.9964019060134888, 0.9885353446006775, 0.9916349649429321, 0.014801711775362492, 0.4125308692455292, 0.9514164328575134, 0.21067914366722107, 0.5069707632064819, 0.5811070799827576, 0.9429579973220825, 0.9201115965843201, 0.9675893783569336, 0.6407871842384338, 0.7395608425140381, 0.8112863302230835, 0.8075715899467468, 0.5341680645942688, 0.015332486480474472, 0.6628244519233704, 0.3568510413169861, 0.7228512167930603, 0.9593660831451416, 0.993283748626709, 0.5972910523414612, 0.8837361335754395, 0.9706827998161316, 0.9893430471420288, 0.7885507941246033, 0.02328081801533699, 0.004145227838307619, 0.05427746847271919, 0.9257082343101501, 0.9645837545394897, 0.2606758177280426, 0.07482124119997025, 0.9055373072624207, 0.4776025712490082, 0.7824678421020508, 0.8277809619903564, 0.9672117233276367, 0.9737014174461365, 0.753180742263794, 0.9271449446678162, 0.9895502924919128, 0.37354037165641785, 0.964874804019928, 0.8495491743087769, 0.2946929335594177, 0.0046744514256715775, 0.8905777335166931, 0.9978941082954407, 0.8561726212501526, 0.9494701623916626, 0.8127632737159729, 0.9980151653289795, 0.03018270432949066, 0.04792073741555214, 0.9770324230194092, 0.11778222024440765, 0.8822886347770691, 0.9884492754936218, 0.7469292879104614, 0.9054311513900757, 0.9917054176330566, 0.21223898231983185, 0.3523050844669342, 0.9457386136054993, 0.030223676934838295, 0.9218060374259949, 0.9476221203804016, 0.22496242821216583, 0.3065854609012604, 0.8137949109077454, 0.237552210688591, 0.9898287057876587, 0.48921844363212585, 0.8813170194625854, 0.9946771860122681, 0.3997940719127655, 0.9796914458274841, 0.9478545784950256, 0.9947116374969482, 0.9111369252204895, 0.9940449595451355, 0.019950635731220245, 0.974900484085083, 0.4977380931377411, 0.956165611743927, 0.9828214645385742, 0.571061909198761, 0.9993775486946106, 0.5613231658935547, 0.6790478229522705, 0.9668869972229004, 0.8926434516906738, 0.998150110244751, 0.3752707839012146, 0.7241035103797913, 0.9793696999549866, 0.9855697751045227, 0.9929418563842773, 0.38707396388053894, 0.6906514167785645, 0.7194352149963379, 0.9737550020217896, 0.9769790768623352, 0.7632824778556824, 0.9984018206596375, 0.9064459800720215, 0.18029449880123138, 0.9555864334106445, 0.47082361578941345, 0.8445854783058167, 0.9961976408958435, 0.9996258020401001, 0.016285404562950134, 0.9797862768173218, 0.9789343476295471, 0.6965718269348145, 0.929456889629364, 0.07857553660869598, 0.2508743405342102, 0.9878960847854614, 0.4290446937084198, 0.3252272605895996, 0.9829564094543457, 0.24091652035713196, 0.07656016945838928, 0.5977155566215515, 0.9750105738639832, 0.9851598739624023, 0.0841587707400322, 0.9246403574943542, 0.924683153629303, 0.8326748609542847, 0.8962689638137817, 0.8999806642532349, 0.6469327807426453, 0.9893234372138977, 0.6364846229553223, 0.9157769083976746, 0.9134639501571655, 0.9417296051979065, 0.5236753225326538, 0.9883859157562256, 0.994572103023529, 0.9490737915039062, 0.7666839361190796, 0.05586095154285431, 0.8671082258224487, 0.08958669006824493, 0.9662525057792664, 0.863180935382843, 0.07826371490955353, 0.029654473066329956, 0.8202537298202515, 0.8193678855895996, 0.6726822257041931, 0.053837135434150696, 0.5404534935951233, 0.7939488887786865, 0.9560666084289551, 0.19689978659152985, 0.9892736077308655, 0.6561902165412903, 0.8510106205940247, 0.9919231534004211, 0.39516979455947876, 0.6058751344680786, 0.9408396482467651, 0.9979908466339111, 0.5846948027610779, 0.5867642164230347, 0.4021064341068268, 0.985077440738678, 0.9904018044471741, 0.9541239142417908, 0.9093621969223022, 0.39856061339378357, 0.34372425079345703, 0.9893785119056702, 0.9119530320167542, 0.8680511116981506, 0.8937251567840576, 0.9400035738945007, 0.42763081192970276, 0.8077396154403687, 0.9958567023277283, 0.971435546875, 0.9927557110786438, 0.8327069878578186, 0.9251588582992554, 0.9341105818748474, 0.42788881063461304, 0.3989214599132538, 0.9367005825042725, 0.909712553024292, 0.2310834378004074, 0.9438888430595398, 0.9101846814155579, 0.9711501002311707, 0.9735345244407654, 0.9877020716667175, 0.9990891218185425, 0.9342360496520996, 0.9734593629837036, 0.9923996329307556, 0.9601907730102539, 0.9281046390533447, 0.7533091306686401, 0.7259384393692017, 0.9763889908790588, 0.9783994555473328, 0.9370235800743103, 0.8226733803749084, 0.9961638450622559, 0.5054426789283752, 0.45522966980934143, 0.9926992058753967, 0.5690029263496399, 0.9560580253601074, 0.9889578819274902, 0.3061523735523224, 0.7792566418647766, 0.9822801947593689, 0.98919278383255, 0.8303146958351135, 0.8007612228393555, 0.5607864260673523, 0.9961398243904114, 0.9954504370689392, 0.5077736377716064, 0.9986679553985596, 0.9933640956878662, 0.988203763961792, 0.6085231900215149, 0.634841799736023, 0.9917267560958862, 0.7495310306549072, 0.9848021864891052, 0.8878001570701599, 0.9997708201408386, 0.8714559674263, 0.7238084077835083, 0.6227448582649231, 0.9969919919967651, 0.37549078464508057, 0.9228737950325012, 0.6061866879463196, 0.9754403829574585, 0.5099015235900879, 0.6672534346580505, 0.9866340160369873, 0.9868069291114807, 0.973170280456543, 0.0065637147054076195, 0.9835122227668762, 0.9061431288719177, 0.7631167769432068, 0.9974532723426819, 0.9878537654876709, 0.9251089096069336, 0.9986754059791565, 0.9914289116859436, 0.8930298686027527, 0.8475649356842041, 0.8460853695869446, 0.6211795806884766, 0.4515272080898285, 0.8572985529899597, 0.9963578581809998, 0.9992905855178833, 0.6908642053604126, 0.9341023564338684, 0.9744812846183777, 0.9126570820808411, 0.3597397804260254, 0.996735155582428, 0.7556367516517639, 0.9789011478424072, 0.8210905194282532, 0.9890151619911194, 0.9635190367698669, 0.9259965419769287, 0.3007352352142334, 0.6778119206428528, 0.8859574198722839, 0.992181658744812, 0.9556741118431091, 0.734443187713623, 0.9901064038276672, 0.9985382556915283, 0.9916075468063354, 0.8731138706207275, 0.9029278755187988, 0.49384480714797974, 0.8962040543556213, 0.6563790440559387, 0.6388862133026123, 0.770724892616272, 0.9477006196975708, 0.387433797121048, 0.4588368833065033, 0.48914676904678345, 0.40353110432624817, 0.8735103607177734, 0.998050332069397, 0.9391411542892456, 0.9888200163841248, 0.9571083784103394, 0.5565900802612305, 0.9850606322288513, 0.5894267559051514, 0.9892027974128723, 0.4780959188938141, 0.6214516758918762, 0.9949206709861755, 0.902601420879364, 0.9926571249961853, 0.9544288516044617, 0.9832280874252319, 0.9925497770309448, 0.16660954058170319, 0.987622857093811, 0.6452714800834656, 0.9866597652435303, 0.9947892427444458, 0.9498040676116943, 0.6622321605682373, 0.9884218573570251, 0.9903048276901245, 0.6085721850395203, 0.9912579655647278, 0.9987456798553467, 0.3577158749103546, 0.6449611186981201, 0.8839484453201294, 0.0701267197728157, 0.02168971300125122, 0.9701943397521973, 0.1853003352880478, 0.9926935434341431, 0.9655874967575073, 0.12644833326339722, 0.6353821158409119, 0.9829151630401611, 0.9985712766647339, 0.9920903444290161, 0.9940049052238464, 0.37877169251441956, 0.28395840525627136, 0.34128984808921814, 0.646979570388794, 0.38020384311676025, 0.9888713955879211, 0.8186705112457275, 0.9874326586723328, 0.6202074289321899, 0.7629593014717102, 0.9564110040664673, 0.38897910714149475, 0.9991645812988281, 0.990242063999176, 0.9869478940963745, 0.5348106026649475, 0.45004212856292725, 0.3579384386539459, 0.9171419739723206, 0.6252948045730591, 0.9809999465942383, 0.950979471206665, 0.47813668847084045, 0.9623205661773682, 0.4525417983531952, 0.692517876625061, 0.9521982073783875, 0.38859301805496216, 0.20717957615852356, 0.9968785047531128, 0.73753422498703, 0.953485369682312, 0.2722587585449219, 0.9665902853012085, 0.7937547564506531, 0.5261790156364441, 0.9925740957260132, 0.9582844972610474, 0.9581329226493835, 0.15493083000183105, 0.2713158130645752, 0.38436973094940186, 0.9883996248245239, 0.9336928129196167, 0.9745566248893738, 0.8165014982223511, 0.8497852087020874, 0.5337185859680176, 0.9770498275756836, 0.9584037661552429, 0.34828296303749084, 0.7737931609153748, 0.9898911714553833, 0.3764762580394745, 0.8171952962875366, 0.9984408020973206, 0.8759481906890869, 0.28131261467933655, 0.89622563123703, 0.042039308696985245, 0.13348965346813202, 0.05831925570964813, 0.87828528881073, 0.9095441102981567, 0.5125407576560974, 0.6684372425079346, 0.9964631199836731, 0.9052724838256836, 0.5056203603744507, 0.38239017128944397, 0.9878089427947998, 0.9938507080078125, 0.5330935120582581, 0.2195053994655609, 0.241228848695755, 0.37453609704971313, 0.2393054962158203, 0.8678891658782959, 0.9874196648597717, 0.807410717010498, 0.9932730197906494, 0.8852991461753845, 0.9164898991584778, 0.4904252290725708, 0.9210758209228516, 0.5437359809875488, 0.9101729393005371, 0.9170389175415039, 0.9879342317581177, 0.9642086029052734, 0.5247596502304077, 0.9136897921562195, 0.8193400502204895, 0.958114743232727, 0.9967173933982849, 0.9118168354034424, 0.9690924882888794, 0.9938163757324219, 0.9932847023010254, 0.9689028859138489, 0.9909817576408386, 0.08004575967788696, 0.9384862780570984, 0.9523701667785645, 0.30768662691116333, 0.8045921921730042, 0.022876858711242676, 0.6344255805015564, 0.9950337409973145, 0.9581955075263977, 0.19923335313796997, 0.7511065602302551, 0.8819395899772644, 0.9952993392944336, 0.2417975217103958, 0.9960063099861145, 0.9792585968971252, 0.9936415553092957, 0.05750352516770363, 0.4332302510738373, 0.996393620967865, 0.8738720417022705, 0.9872859120368958, 0.9731075167655945, 0.9859549403190613, 0.8990030288696289, 0.33740729093551636, 0.9876390695571899, 0.753365159034729, 0.26337504386901855, 0.8891611099243164, 0.9934635162353516, 0.3217477798461914, 0.8530155420303345, 0.3175033628940582, 0.8380136489868164, 0.984476625919342, 0.47863027453422546, 0.8716307878494263, 0.9206661581993103, 0.08766978979110718, 0.647952675819397, 0.6993924975395203, 0.9906712770462036, 0.8407458066940308, 0.672991931438446, 0.9376529455184937, 0.6018341183662415, 0.7997774481773376, 0.9836037755012512, 0.9055027961730957, 0.9908492565155029, 0.5267338156700134, 0.993553638458252, 0.21057887375354767, 0.9638822078704834, 0.7800063490867615, 0.6889597177505493, 0.9670983552932739, 0.9783535599708557, 0.8690145611763, 0.9115106463432312, 0.9527764916419983, 0.8199130296707153, 0.0850740298628807, 0.7770500183105469, 0.9291905760765076, 0.5247138142585754, 0.9729551076889038, 0.1072062999010086, 0.9455956816673279, 0.6962490081787109, 0.5367363691329956, 0.9509577751159668, 0.41901591420173645, 0.7603703141212463, 0.733748197555542, 0.2944234311580658, 0.9602804780006409, 0.956879198551178, 0.9767192602157593, 0.7045887112617493, 0.893268346786499, 0.8873868584632874, 0.09494648873806, 0.4613102674484253, 0.9119313955307007, 0.9164624214172363, 0.8346415758132935, 0.8397766351699829, 0.6091644167900085, 0.870102047920227, 0.9740361571311951, 0.22453069686889648, 0.8794480562210083, 0.6832219958305359, 0.6551076769828796, 0.5435276031494141, 0.3401133120059967, 0.9573691487312317, 0.9260028600692749, 0.9293773174285889, 0.4591935873031616, 0.35871973633766174, 0.8397849798202515, 0.9693423509597778, 0.38864073157310486, 0.2504444122314453, 0.983314037322998, 0.752615213394165, 0.9547380208969116, 0.9575389623641968, 0.29574984312057495, 0.7588244080543518, 0.9845501184463501, 0.7178035974502563, 0.9857766032218933, 0.9472760558128357, 0.06381268799304962, 0.6468130946159363, 0.04306216165423393, 0.7699649333953857, 0.6106816530227661, 0.5256059765815735, 0.9885155558586121, 0.48494797945022583, 0.8753786087036133, 0.9143475890159607, 0.4896538555622101, 0.971401572227478, 0.05915287137031555, 0.9777711033821106, 0.676344633102417, 0.07911191880702972, 0.9556195139884949, 0.8116024732589722, 0.28384047746658325, 0.35331109166145325, 0.03756556287407875, 0.9642235636711121, 0.5973793864250183, 0.9176079630851746, 0.9914717078208923, 0.13075502216815948, 0.10115353018045425, 0.0085185207426548, 0.9432215690612793, 0.6583431959152222, 0.9667887091636658, 0.863180935382843, 0.03092304617166519, 0.06734776496887207, 0.9732338190078735, 0.8733832836151123, 0.848320484161377, 0.9408310055732727, 0.38539549708366394, 0.9152409434318542, 0.6762906312942505, 0.981844425201416, 0.2166541963815689, 0.5861260890960693, 0.1884002983570099, 0.14367865025997162, 0.09663954377174377, 0.19153878092765808, 0.9106957316398621, 0.956200897693634, 0.6550923585891724, 0.9027183651924133, 0.5410676598548889, 0.8835324645042419, 0.2276567816734314, 0.28835535049438477, 0.9702540636062622, 0.2875281870365143, 0.02769698016345501, 0.8927736282348633, 0.9674390554428101, 0.5535839200019836, 0.9972202777862549, 0.23346607387065887, 0.28024929761886597, 0.9945579767227173, 0.049575675278902054, 0.7380141615867615, 0.844685435295105, 0.012645025737583637, 0.17673109471797943, 0.727238118648529, 0.8896468877792358, 0.2556385099887848, 0.8585350513458252, 0.8017314672470093, 0.9105761647224426, 0.891535758972168, 0.9751244783401489, 0.9147695899009705, 0.9760448932647705, 0.46957674622535706, 0.7460221648216248, 0.9096804261207581, 0.11257337778806686, 0.6818064451217651, 0.5765717625617981, 0.08667446672916412, 0.9200543165206909, 0.9199978113174438, 0.9916223883628845, 0.9517698287963867, 0.9978358149528503, 0.9886130094528198, 0.024776266887784004, 0.24741493165493011, 0.9811671376228333, 0.6003556847572327, 0.9418281316757202, 0.3442560136318207, 0.14912442862987518, 0.815266489982605, 0.6497583985328674, 0.16038140654563904, 0.9264323711395264, 0.9718671441078186, 0.5439797639846802, 0.28394269943237305, 0.8504201173782349, 0.5544599294662476, 0.8922426104545593, 0.677261233329773, 0.9629758596420288, 0.16852399706840515, 0.9960108995437622, 0.6054019331932068, 0.7302828431129456, 0.9427161812782288, 0.998089611530304, 0.6965402364730835, 0.9848185777664185, 0.08620117604732513, 0.704838752746582, 0.7019518613815308, 0.034161221235990524, 0.49450135231018066, 0.057452455163002014, 0.7338621020317078, 0.8563326597213745, 0.8857555985450745, 0.9605709910392761, 0.13684707880020142, 0.9558789134025574, 0.9931938052177429, 0.982982337474823, 0.8860000967979431, 0.8694249391555786, 0.9896034002304077, 0.4472055435180664, 0.6393354535102844, 0.26038798689842224, 0.28537920117378235, 0.7133343815803528, 0.0809500440955162, 0.27539846301078796, 0.34325146675109863, 0.3983426094055176, 0.6208136677742004, 0.7761883735656738, 0.15018363296985626, 0.8383368253707886, 0.27403709292411804, 0.9617533683776855, 0.273214727640152, 0.9192814826965332, 0.2838861346244812, 0.9961451292037964, 0.8631544709205627, 0.5106469392776489, 0.673951268196106, 0.9423558712005615, 0.9933862090110779, 0.8594472408294678, 0.9228663444519043, 0.8791406750679016, 0.4323459565639496, 0.9572737216949463, 0.3531761169433594, 0.9003444314002991, 0.9654176831245422, 0.9639002680778503, 0.9162637591362, 0.5390903353691101, 0.6886522173881531, 0.9484133720397949, 0.9431169033050537, 0.6541135311126709, 0.7807409763336182, 0.876222550868988, 0.11272002756595612, 0.8059059381484985, 0.9365755915641785, 0.5625305771827698, 0.6688840985298157, 0.22594666481018066, 0.5507649183273315, 0.9821059703826904, 0.9908368587493896, 0.039460066705942154, 0.9356555938720703, 0.2830759882926941, 0.03729167580604553, 0.9343898296356201, 0.9941410422325134, 0.8935610055923462, 0.1565486639738083, 0.399790495634079, 0.8443094491958618, 0.1831221729516983, 0.5150840878486633, 0.10012578219175339, 0.3793684244155884, 0.4582386314868927, 0.8852958083152771, 0.9902439713478088, 0.9439780116081238, 0.6710978150367737, 0.9644816517829895, 0.9912880063056946, 0.9843942523002625, 0.3009219467639923, 0.4312208294868469, 0.6641524434089661, 0.5851961970329285, 0.09464678168296814, 0.8011130690574646, 0.9914519786834717, 0.9363517761230469, 0.6207243800163269, 0.9910565614700317, 0.5203431844711304, 0.9453492760658264, 0.3260025084018707, 0.6667425036430359, 0.7937636971473694, 0.9852502942085266, 0.6232665777206421, 0.6545071005821228, 0.013851404190063477, 0.921501636505127, 0.5157472491264343, 0.759430468082428, 0.9865931868553162, 0.48398590087890625, 0.6929869055747986, 0.3894176185131073, 0.32703015208244324, 0.9883352518081665, 0.6522822976112366, 0.5824843645095825, 0.629229724407196, 0.0690336525440216, 0.9334930777549744, 0.9355478882789612, 0.9908018708229065, 0.6976878046989441, 0.9662413597106934, 0.10013902187347412, 0.0360620878636837, 0.9881855249404907, 0.9230179786682129, 0.923433244228363, 0.9989339709281921, 0.9906971454620361, 0.6409769654273987, 0.15909317135810852, 0.6425608396530151, 0.001991123892366886, 0.0009533509728498757, 0.09109917283058167, 3.922398173017427e-05, 0.0010248266626149416, 0.0249225702136755, 0.00012281023373361677, 0.09545997530221939, 0.0030472916550934315, 0.001585370278917253, 0.04447757452726364, 0.002460536314174533, 0.00023823577794246376, 0.0009514245321042836, 0.4408765435218811, 0.00026270427042618394, 0.006374687887728214, 0.0001974297920241952, 0.0007335532573051751, 0.3185182809829712, 0.0017056843498721719, 0.040179286152124405, 0.0009404061129316688, 0.00016056571621447802, 0.008050750009715557, 0.006515298038721085, 0.15073475241661072, 0.007875137962400913, 0.018915651366114616, 0.014619173482060432, 0.003064329968765378, 0.00047388297389261425, 0.6580260396003723, 0.0648377314209938, 0.006960967089980841, 2.460039650031831e-05, 0.011669134721159935, 0.0006019093561917543, 0.007240218110382557, 0.11756662279367447, 0.007757775951176882, 0.00860301312059164, 4.8966121539706364e-06, 4.690476998803206e-05, 0.0006704438128508627, 0.0026796767488121986, 0.18084418773651123, 0.0051604751497507095, 0.0034809489734470844, 0.04412509873509407, 0.006685345433652401, 0.008520909585058689, 0.01915886253118515, 0.011959334835410118, 0.015071644447743893, 0.0001568637089803815, 0.016570309177041054, 0.01010973285883665, 1.3280931852932554e-05, 0.06353465467691422, 1.0990412420142093e-06, 0.18251998722553253, 0.009987290017306805, 0.002772623673081398, 0.00016859422612469643, 0.043724264949560165, 0.0018029081402346492, 0.00018367735901847482, 0.01399635337293148, 0.10577571392059326, 0.035193752497434616, 0.9431498646736145, 0.004868128802627325, 0.0018823847640305758, 2.20973070099717e-05, 5.2914114348823205e-05, 0.00022467349481303245, 2.846653114829678e-05, 0.0017979504773393273, 0.0011228549992665648, 0.00027196138398721814, 0.157637357711792, 0.674692690372467, 0.005455208942294121, 0.01658201590180397, 0.0007762793102301657, 0.011847509071230888, 0.0017629199428483844, 3.8827554817544296e-05, 0.02715744450688362, 0.0002774356980808079, 0.24285759031772614, 0.0010160446399822831, 0.09442419558763504, 0.0011085965670645237, 0.05686735361814499, 0.021450528874993324, 0.00332293170504272, 0.16955018043518066, 0.24619372189044952, 0.00022726775205228478, 0.3129585385322571, 0.29469093680381775, 0.06545806676149368, 0.03477857634425163, 0.032875798642635345, 0.22511635720729828, 0.014017056673765182, 0.0009655167232267559, 0.0003918248985428363, 0.010669701732695103, 0.004127945750951767, 0.00047975798952393234, 0.6267666816711426, 0.0001001919517875649, 0.11181387305259705, 6.822212890256196e-05, 0.00013259904517326504, 0.016787678003311157, 0.2634924650192261, 9.871112706605345e-05, 0.0010265171295031905, 0.0003362359420862049, 0.015506836585700512, 0.0003784403088502586, 1.5123580851650331e-05, 0.00010949771967716515, 0.008927907794713974, 0.0031506752129644156, 0.003251363057643175, 0.0010558944195508957, 0.0014556616079062223, 0.002812332008033991, 0.00013306172331795096, 0.0066369143314659595, 0.0001642603165237233, 0.0002816001360770315, 0.00022650347091257572, 0.00689185643568635, 0.00712012080475688, 0.002093440853059292, 0.016817612573504448, 5.3193190979072824e-05, 0.01399635337293148, 0.0017169308848679066, 0.032352548092603683, 0.0662148967385292, 0.0006690338486805558, 6.904784822836518e-05, 2.941046295745764e-05, 0.023614680394530296, 0.00034975269227288663, 0.00027781844255514443, 0.027222784236073494, 0.0005756030441261828, 0.008231121115386486, 0.10549813508987427, 0.0021794806234538555, 0.0009297450305894017, 8.29754353617318e-05, 0.0028834189288318157, 2.513275649107527e-05, 0.8286420702934265, 1.0085322173836175e-05, 0.5890366435050964, 0.0009401494753547013, 0.0016445176443085074, 0.016311021521687508, 0.0007796650752425194, 0.028110617771744728, 0.0011865139240399003, 0.009194888174533844, 0.0006482150638476014, 0.01589059829711914, 0.0009207715047523379, 0.0005920970579609275, 2.066247907350771e-05, 0.8944664001464844, 7.294995157280937e-06, 0.00041233617230318487, 0.03961773216724396, 1.8558543160906993e-05, 0.0006716931820847094, 0.0016299092676490545, 0.08627194911241531, 0.001949745463207364, 0.0008818283095024526, 0.00010605989518808201, 0.9432215690612793, 0.025234617292881012, 0.00022882106713950634, 0.026391418650746346, 0.012453723698854446, 0.0021985014900565147, 0.0004160438838880509, 0.008520909585058689, 0.007765436079353094, 0.00016704940935596824, 0.004782738164067268, 4.4</t>
+          <t>[0.8115217685699463, 0.37395355105400085, 0.168717160820961, 0.9986792206764221, 0.9915502071380615, 0.43862104415893555, 0.9001944661140442, 0.6022679805755615, 0.6281245946884155, 0.10099578648805618, 0.895571231842041, 0.7244345545768738, 0.7690702676773071, 0.9920682907104492, 0.9997643828392029, 0.5827258825302124, 0.8879521489143372, 0.6976861953735352, 0.09045760333538055, 0.893663763999939, 0.983945906162262, 0.7678812146186829, 0.9210291504859924, 0.11890336871147156, 0.28220850229263306, 0.6312887668609619, 0.9411209225654602, 0.7944315075874329, 0.8027922511100769, 0.2382236123085022, 0.047865647822618484, 0.728169858455658, 0.9790170788764954, 0.9674525856971741, 0.9269551634788513, 0.8818516731262207, 0.9789106249809265, 0.22940312325954437, 0.9696165919303894, 0.8410816192626953, 0.9675644040107727, 0.9712432026863098, 0.9896111488342285, 0.01713825762271881, 0.845513641834259, 0.26641935110092163, 0.9998546838760376, 0.948030948638916, 0.8825000524520874, 0.8477871417999268, 0.9901316165924072, 0.7226178050041199, 0.8251184225082397, 0.8167651891708374, 0.9458205103874207, 0.7180906534194946, 0.9726779460906982, 0.938524067401886, 0.9979214072227478, 0.939812958240509, 0.9540916085243225, 0.9993044137954712, 0.8401150107383728, 0.9928731918334961, 0.9968172311782837, 0.9989544153213501, 0.9028703570365906, 0.33493998646736145, 0.995093584060669, 0.9556233286857605, 0.37684640288352966, 0.8422526121139526, 0.8691566586494446, 0.8600100874900818, 0.9947351217269897, 0.9963864088058472, 0.8642333149909973, 0.9975973963737488, 0.9901037812232971, 0.8603312969207764, 0.5134934186935425, 0.9889304041862488, 0.0470571294426918, 0.9401228427886963, 0.9876419305801392, 0.9293943047523499, 0.805356502532959, 0.13970491290092468, 0.9971554279327393, 0.9980354905128479, 0.8981467485427856, 0.9995494484901428, 0.639968752861023, 0.999656081199646, 0.9417614340782166, 0.7027125358581543, 0.15413972735404968, 0.39529749751091003, 0.807266354560852, 0.9968991279602051, 0.6200008392333984, 0.49505534768104553, 0.9011942148208618, 0.8564265966415405, 0.9893022179603577, 0.8925187587738037, 0.9980146884918213, 0.5061988830566406, 0.29278790950775146, 0.8442283272743225, 0.5655690431594849, 0.9980161190032959, 0.8257195353507996, 0.4401100277900696, 0.9910649657249451, 0.9716492891311646, 0.46978431940078735, 0.7596880793571472, 0.21179844439029694, 0.26442769169807434, 0.9913305044174194, 0.7167582511901855, 0.8698907494544983, 0.9998964071273804, 0.9777269959449768, 0.9968861937522888, 0.2302170842885971, 0.9252005219459534, 0.895564079284668, 0.9850764870643616, 0.1571410894393921, 0.47845548391342163, 0.0059956335462629795, 0.9041122794151306, 0.9115676879882812, 0.9672644734382629, 0.9885730743408203, 0.23869670927524567, 0.6151184439659119, 0.8515372276306152, 0.997136116027832, 0.9319127798080444, 0.9938355088233948, 0.7473540306091309, 0.6537548303604126, 0.9338522553443909, 0.4382953345775604, 0.9462584853172302, 0.9955174326896667, 0.9864975810050964, 0.9485523700714111, 0.21023544669151306, 0.7695316672325134, 0.5060591697692871, 0.9561274647712708, 0.9889792203903198, 0.3594897985458374, 0.9585686922073364, 0.905275821685791, 0.3601885437965393, 0.17011044919490814, 0.7695084810256958, 0.07858432084321976, 0.9400454163551331, 0.6472069025039673, 0.8014397621154785, 0.6133073568344116, 0.2058950513601303, 0.43690648674964905, 0.9675589203834534, 0.0500018484890461, 0.9695245027542114, 0.8997778296470642, 0.48156726360321045, 0.8644524216651917, 0.8856584429740906, 0.7183632254600525, 0.9048774242401123, 0.9815935492515564, 0.7490854263305664, 0.5902761220932007, 0.9324679970741272, 0.04067065194249153, 0.9920795559883118, 0.8499366641044617, 0.578306257724762, 0.9926230907440186, 0.9863061904907227, 0.0519927516579628, 0.9877306818962097, 0.9971709847450256, 0.9780510663986206, 0.3626802861690521, 0.04328054189682007, 0.7831606864929199, 0.9904158115386963, 0.9991255402565002, 0.4114154577255249, 0.8724678158760071, 0.9992542862892151, 0.08480043709278107, 0.8677621483802795, 0.7718481421470642, 0.5060969591140747, 0.6397581696510315, 0.16251060366630554, 0.9749770760536194, 0.08263316005468369, 0.7903035879135132, 0.9958637952804565, 0.01503714732825756, 0.9897317290306091, 0.9964840412139893, 0.179268941283226, 0.9687997102737427, 0.97431480884552, 0.9511722922325134, 0.9045778512954712, 0.05952666327357292, 0.9499034881591797, 0.8807726502418518, 0.40206363797187805, 0.056104131042957306, 0.7829074859619141, 0.0037944125942885876, 0.8739598393440247, 0.8552597165107727, 0.010540110990405083, 0.08526609092950821, 0.021301647648215294, 0.9616134762763977, 0.22963136434555054, 0.9990179538726807, 0.9279997944831848, 0.03846527636051178, 0.4926198124885559, 0.0878492221236229, 0.5073604583740234, 0.03414002060890198, 0.05414087697863579, 0.9547446370124817, 0.003565865568816662, 0.17122475802898407, 0.061560846865177155, 0.8873136043548584, 0.87505042552948, 0.7509778141975403, 0.8662422895431519, 0.8562777638435364, 0.9685824513435364, 0.012211709283292294, 0.9978505373001099, 0.9475907683372498, 0.4218345284461975, 0.8575448989868164, 0.6411551833152771, 0.6366207599639893, 0.9883632063865662, 0.9994969367980957, 0.9978411197662354, 0.059483468532562256, 0.4283405840396881, 0.9731481671333313, 0.12571024894714355, 0.21524183452129364, 0.03259357064962387, 0.4943084418773651, 0.25486254692077637, 0.5723633766174316, 0.07493871450424194, 0.14197728037834167, 0.7528529167175293, 0.9039217233657837, 0.962679386138916, 0.8894106149673462, 0.6709064245223999, 0.018706146627664566, 0.9983416795730591, 0.8761189579963684, 0.9929776787757874, 0.5041075348854065, 0.06811758130788803, 0.9887791872024536, 0.9884737133979797, 0.047629814594984055, 0.7595607042312622, 0.1266992837190628, 0.9989643096923828, 0.006902746390551329, 0.19776059687137604, 0.9944533705711365, 0.707551896572113, 0.24913063645362854, 0.9965967535972595, 0.9782434701919556, 0.92467200756073, 0.6126459836959839, 0.7635974287986755, 0.057046808302402496, 0.10223609954118729, 0.010849476791918278, 0.5044541954994202, 0.995665967464447, 0.5035473108291626, 0.05318398028612137, 0.9206758141517639, 0.21851903200149536, 0.31128358840942383, 0.9860579371452332, 0.9856593608856201, 0.019526546820998192, 0.15310418605804443, 0.40748947858810425, 0.9986181259155273, 0.7148456573486328, 0.943828821182251, 0.638016402721405, 0.8611317276954651, 0.8587309718132019, 0.9938796758651733, 0.07625818997621536, 0.8855258822441101, 0.9955288767814636, 0.9974848031997681, 0.44922441244125366, 0.9918522238731384, 0.045945655554533005, 0.9048632383346558, 0.7607781887054443, 0.789607584476471, 0.9391223192214966, 0.7750083804130554, 0.9912103414535522, 0.9868373870849609, 0.6883354187011719, 0.25537586212158203, 0.3942377269268036, 0.8077623248100281, 0.9314613938331604, 0.09497421234846115, 0.44671252369880676, 0.7101987600326538, 0.9588502645492554, 0.09894698858261108, 0.13732779026031494, 0.7294593453407288, 0.7876484394073486, 0.9980120658874512, 0.7599290013313293, 0.9310458898544312, 0.9759481549263, 0.9946954846382141, 0.16348116099834442, 0.9518391489982605, 0.999275267124176, 0.05641946196556091, 0.9968783855438232, 0.08631648123264313, 0.39760980010032654, 0.9389867186546326, 0.8722013831138611, 0.43388664722442627, 0.05828152969479561, 0.07325588166713715, 0.6208907961845398, 0.9941986799240112, 0.6168347001075745, 0.9569542407989502, 0.3334602117538452, 0.9138697981834412, 0.9006985425949097, 0.47206032276153564, 0.9634162783622742, 0.18340852856636047, 0.9688114523887634, 0.9849008321762085, 0.1313166618347168, 0.9696191549301147, 0.965743362903595, 0.6260483860969543, 0.9308367967605591, 0.9431591033935547, 0.9986351132392883, 0.9335792064666748, 0.9973089694976807, 0.990319013595581, 0.27641117572784424, 0.7925659418106079, 0.9273735880851746, 0.6208198070526123, 0.13972969353199005, 0.9982144832611084, 0.4309338927268982, 0.9993158578872681, 0.8920181393623352, 0.534275233745575, 0.966057538986206, 0.6292253136634827, 0.9992339611053467, 0.839104413986206, 0.008496989496052265, 0.9670974612236023, 0.7407378554344177, 0.7337606549263, 0.7162933349609375, 0.6433799862861633, 0.6689162254333496, 0.1764211803674698, 0.14214929938316345, 0.49504464864730835, 0.9988744854927063, 0.9425013661384583, 0.9774995446205139, 0.9331069588661194, 0.6843019127845764, 0.9720454216003418, 0.12384995073080063, 0.7794131636619568, 0.016083627939224243, 0.9670804738998413, 0.8862833380699158, 0.5883350372314453, 0.8893007636070251, 0.7116320133209229, 0.050412245094776154, 0.04351404681801796, 0.35392439365386963, 0.16116410493850708, 0.0013966131955385208, 0.005547867156565189, 0.6831865906715393, 0.33633941411972046, 0.8813789486885071, 0.14552952349185944, 0.7530829310417175, 0.9131394028663635, 0.005086896009743214, 0.7784944772720337, 0.6036869287490845, 0.8421092629432678, 0.9811644554138184, 0.07492420077323914, 0.9966846108436584, 0.7860280871391296, 0.8531590700149536, 0.9958949089050293, 0.9669786095619202, 0.9964179992675781, 0.9127927422523499, 0.9951015114784241, 0.3402606248855591, 0.24796071648597717, 0.05235183238983154, 0.9954594969749451, 0.19597585499286652, 0.008293245919048786, 0.8987656831741333, 0.1275106519460678, 0.7485796213150024, 0.7866937518119812, 0.9423198103904724, 0.00192705646622926, 0.7442767024040222, 0.7024460434913635, 0.08559288084506989, 0.31484314799308777, 0.522537112236023, 0.6331577301025391, 0.9323642253875732, 0.9910433292388916, 0.987179696559906, 0.9848055243492126, 0.6565545201301575, 0.9801095724105835, 0.6714346408843994, 0.26134300231933594, 0.8217946887016296, 0.6896215677261353, 0.2681545317173004, 0.04042794182896614, 0.2255454659461975, 0.9981641173362732, 0.01816720888018608, 0.23474040627479553, 0.9895159006118774, 0.8875840306282043, 0.9622530937194824, 0.8354842662811279, 0.9468693137168884, 0.004328858107328415, 0.957493245601654, 0.9036787748336792, 0.8227004408836365, 0.9797048568725586, 0.9904680848121643, 0.8610883355140686, 0.29371774196624756, 0.7282561659812927, 0.37099066376686096, 0.930083155632019, 0.04715970158576965, 0.5894634127616882, 0.07336960732936859, 0.9415828585624695, 0.8297345638275146, 0.5874388813972473, 0.10860445350408554, 0.9304443597793579, 0.018951496109366417, 0.8799863457679749, 0.5741539001464844, 0.6630184054374695, 0.9949199557304382, 0.11075637489557266, 0.9855180978775024, 0.35330700874328613, 0.3179847002029419, 0.20894914865493774, 0.9225446581840515, 0.8726209402084351, 0.8592809438705444, 0.9949465394020081, 0.9913083910942078, 0.015735603868961334, 0.9633777737617493, 0.8755700588226318, 0.9311324954032898, 0.9369028210639954, 0.8131267428398132, 0.7105991840362549, 0.15974953770637512, 0.6931902766227722, 0.792633593082428, 0.8022481203079224, 0.3128025531768799, 0.9042098522186279, 0.39620885252952576, 0.7276961207389832, 0.995514452457428, 0.3322756290435791, 0.12946173548698425, 0.20528432726860046, 0.9875696301460266, 0.3379088342189789, 0.005309258121997118, 0.05929940566420555, 0.9934771656990051, 0.7968018054962158, 0.7979546189308167, 0.9114254713058472, 0.9748162627220154, 0.7476983070373535, 0.9717575907707214, 0.023812439292669296, 0.18709123134613037, 0.8311588764190674, 0.480876624584198, 0.7252151966094971, 0.29755085706710815, 0.6140469908714294, 0.8557664752006531, 0.41683658957481384, 0.9862654805183411, 0.9891831874847412, 0.9937783479690552, 0.08827470242977142, 0.9255384206771851, 0.9737354516983032, 0.29170581698417664, 0.5947034955024719, 0.9844558238983154, 0.9369702935218811, 0.40378573536872864, 0.048812706023454666, 0.8872053027153015, 0.9751625657081604, 0.9986801743507385, 0.9648358225822449, 0.9760895371437073, 0.7802860736846924, 0.9554759860038757, 0.024014199152588844, 0.9884703159332275, 0.9603371024131775, 0.8637417554855347, 0.9920796751976013, 0.5816038250923157, 0.9688766002655029, 0.014834694564342499, 0.3492015600204468, 0.5432618856430054, 0.232147678732872, 0.509459912776947, 0.7870631217956543, 0.9871649742126465, 0.9146026968955994, 0.9880003333091736, 0.5633816719055176, 0.6535360813140869, 0.9770463109016418, 0.9444903135299683, 0.13120664656162262, 0.16724000871181488, 0.8500047922134399, 0.4472306966781616, 0.40675005316734314, 0.9644954800605774, 0.9912359714508057, 0.61012202501297, 0.7806327939033508, 0.9920124411582947, 0.9908672571182251, 0.9038223028182983, 0.014535743743181229, 0.004123884253203869, 0.010678942315280437, 0.8727704882621765, 0.925433337688446, 0.5547323822975159, 0.1277007907629013, 0.846216082572937, 0.902630090713501, 0.9769644141197205, 0.6911797523498535, 0.992343008518219, 0.7063048481941223, 0.9102255702018738, 0.5802170634269714, 0.9966285824775696, 0.9671568870544434, 0.7754812836647034, 0.5903339982032776, 0.7733743786811829, 0.00228889100253582, 0.9955496788024902, 0.9988349080085754, 0.9890308976173401, 0.9959450364112854, 0.694015622138977, 0.9896356463432312, 0.015774480998516083, 0.359501451253891, 0.9785165190696716, 0.18587812781333923, 0.8759403824806213, 0.6484653949737549, 0.8359803557395935, 0.8794386982917786, 0.9966436624526978, 0.09464852511882782, 0.43507063388824463, 0.9934491515159607, 0.028065722435712814, 0.30815884470939636, 0.9126667976379395, 0.2199019342660904, 0.0542985200881958, 0.5241231918334961, 0.23773297667503357, 0.832067608833313, 0.1540149599313736, 0.7234841585159302, 0.9370781183242798, 0.3534356951713562, 0.9997462630271912, 0.9453933238983154, 0.9869634509086609, 0.8513391613960266, 0.9942426085472107, 0.013293668627738953, 0.8703872561454773, 0.49034392833709717, 0.9246361255645752, 0.8187591433525085, 0.9781915545463562, 0.9996122717857361, 0.4785022735595703, 0.6675882339477539, 0.9903016686439514, 0.9957043528556824, 0.997328519821167, 0.3690167963504791, 0.7571346759796143, 0.9985660910606384, 0.993606448173523, 0.999231219291687, 0.6898203492164612, 0.8149732947349548, 0.8700802326202393, 0.9754541516304016, 0.998145580291748, 0.22161543369293213, 0.9959903359413147, 0.9917557239532471, 0.5988597273826599, 0.830549418926239, 0.3409477174282074, 0.46434450149536133, 0.9851636290550232, 0.9953483939170837, 0.27150607109069824, 0.6890055537223816, 0.9968642592430115, 0.10170353204011917, 0.9532683491706848, 0.00903753750026226, 0.13071203231811523, 0.9931806325912476, 0.3588595986366272, 0.4960991442203522, 0.9965953230857849, 0.35683509707450867, 0.02593710459768772, 0.2989266514778137, 0.7009572982788086, 0.9858535528182983, 0.31221452355384827, 0.9907117486000061, 0.9862124919891357, 0.8416938781738281, 0.979468584060669, 0.6503746509552002, 0.5282257795333862, 0.9912493228912354, 0.6288058161735535, 0.9815645813941956, 0.5525403618812561, 0.9515116810798645, 0.7456306219100952, 0.9958621263504028, 0.9966326355934143, 0.9682644009590149, 0.9511451125144958, 0.020911548286676407, 0.8899234533309937, 0.37800002098083496, 0.9310591220855713, 0.8073998093605042, 0.6821398138999939, 0.05066927522420883, 0.9973704814910889, 0.9233921766281128, 0.5923807621002197, 0.06120692566037178, 0.5331063270568848, 0.7696627378463745, 0.40045973658561707, 0.033186111599206924, 0.9920116066932678, 0.7837482690811157, 0.7950015068054199, 0.9974186420440674, 0.13995361328125, 0.6540490388870239, 0.9175169467926025, 0.9954990744590759, 0.5711426138877869, 0.9233137965202332, 0.7505393028259277, 0.9976968169212341, 0.8885297179222107, 0.8338698148727417, 0.954841136932373, 0.6992082595825195, 0.33796098828315735, 0.9822281002998352, 0.6546121835708618, 0.9019922018051147, 0.8958942294120789, 0.978263795375824, 0.21745678782463074, 0.855534017086029, 0.9985839128494263, 0.956718921661377, 0.9892334938049316, 0.7476943135261536, 0.9892750382423401, 0.8964704871177673, 0.4555168151855469, 0.44298306107521057, 0.9403058886528015, 0.8534563779830933, 0.3906504809856415, 0.9674169421195984, 0.8358258605003357, 0.8095194697380066, 0.9487684965133667, 0.8762571811676025, 0.9991905093193054, 0.7155581116676331, 0.9755621552467346, 0.9978649020195007, 0.9685395359992981, 0.9654927849769592, 0.539729654788971, 0.6078472137451172, 0.9542381167411804, 0.9427523016929626, 0.9796908497810364, 0.9076147079467773, 0.995758593082428, 0.19734899699687958, 0.30935877561569214, 0.9929096102714539, 0.498096764087677, 0.9375548362731934, 0.9954879879951477, 0.8734259605407715, 0.8328388929367065, 0.8383291363716125, 0.993181049823761, 0.8761317133903503, 0.7799062728881836, 0.6706253290176392, 0.9928954243659973, 0.9840058088302612, 0.7588645219802856, 0.9980942606925964, 0.9958881735801697, 0.9875258207321167, 0.890549898147583, 0.7387189269065857, 0.9970055222511292, 0.8365683555603027, 0.9758656024932861, 0.9135012626647949, 0.9977001547813416, 0.9415814280509949, 0.6518263816833496, 0.6579769253730774, 0.9903256893157959, 0.7535577416419983, 0.9453139305114746, 0.7889525890350342, 0.9823328852653503, 0.6096627116203308, 0.30679354071617126, 0.9699497222900391, 0.9895078539848328, 0.9662497043609619, 0.010317177511751652, 0.9967341423034668, 0.9044155478477478, 0.7700287699699402, 0.9979401230812073, 0.9876573085784912, 0.9209937453269958, 0.9952573180198669, 0.9949429631233215, 0.652210533618927, 0.7270557284355164, 0.9055514931678772, 0.5848612189292908, 0.2124863564968109, 0.8696338534355164, 0.9897650480270386, 0.9976254105567932, 0.780356228351593, 0.9388408660888672, 0.9887229204177856, 0.6034622192382812, 0.16756048798561096, 0.9923726320266724, 0.5739660263061523, 0.9529622197151184, 0.6528414487838745, 0.9193961024284363, 0.8569148778915405, 0.9122883081436157, 0.4523985981941223, 0.8721494078636169, 0.8624363541603088, 0.9984585046768188, 0.9332873821258545, 0.6167470216751099, 0.9885355830192566, 0.9985117316246033, 0.9577023983001709, 0.45105600357055664, 0.7948967814445496, 0.13881169259548187, 0.7970678210258484, 0.8651785850524902, 0.10722491890192032, 0.8208580017089844, 0.9905273914337158, 0.36097002029418945, 0.8098970055580139, 0.5781484842300415, 0.33766838908195496, 0.900128185749054, 0.9950271248817444, 0.9702793955802917, 0.9952428936958313, 0.9838328957557678, 0.12989866733551025, 0.9777829051017761, 0.6812436580657959, 0.9877251982688904, 0.40232619643211365, 0.044659342616796494, 0.9839672446250916, 0.8696565628051758, 0.9383639693260193, 0.9859226942062378, 0.9841237664222717, 0.9931975603103638, 0.17355382442474365, 0.9803815484046936, 0.8497281670570374, 0.9856014847755432, 0.9935954213142395, 0.9716857671737671, 0.6959232091903687, 0.9934477210044861, 0.9841756224632263, 0.4379870295524597, 0.9592292904853821, 0.9992808699607849, 0.5638304948806763, 0.9684600234031677, 0.963844895362854, 0.08130793273448944, 0.026591181755065918, 0.8729803562164307, 0.2619730532169342, 0.9858745336532593, 0.8321119546890259, 0.1363895684480667, 0.6303700804710388, 0.98188316822052, 0.9982643723487854, 0.9915476441383362, 0.9931407570838928, 0.10243453085422516, 0.13272754848003387, 0.41355159878730774, 0.46539896726608276, 0.37312015891075134, 0.9962010979652405, 0.8485661745071411, 0.9933046698570251, 0.7081823348999023, 0.8362635970115662, 0.974017858505249, 0.4875487685203552, 0.9930699467658997, 0.9970833659172058, 0.9693490266799927, 0.314889132976532, 0.22049200534820557, 0.32461902499198914, 0.7362875938415527, 0.8781552910804749, 0.9918398857116699, 0.9301027655601501, 0.695823609828949, 0.9481185674667358, 0.41699936985969543, 0.639252245426178, 0.9585176110267639, 0.1865280419588089, 0.46820321679115295, 0.9908660054206848, 0.8737950325012207, 0.9331162571907043, 0.30673640966415405, 0.9833920001983643, 0.28368934988975525, 0.6370240449905396, 0.988775372505188, 0.8555614352226257, 0.9169320464134216, 0.19057324528694153, 0.2770427465438843, 0.3620733618736267, 0.9906834363937378, 0.9638525247573853, 0.9932075142860413, 0.738523006439209, 0.9217305779457092, 0.640093207359314, 0.9295114278793335, 0.9631354212760925, 0.7135080099105835, 0.8219557404518127, 0.9692613482475281, 0.19685526192188263, 0.8925220966339111, 0.9982205033302307, 0.8920141458511353, 0.42568573355674744, 0.9541783928871155, 0.034919336438179016, 0.2642122507095337, 0.49187976121902466, 0.7793143391609192, 0.6153438687324524, 0.2897048592567444, 0.5204207897186279, 0.9877166152000427, 0.7597677111625671, 0.1094755157828331, 0.3240910768508911, 0.984911322593689, 0.9947951436042786, 0.3328242897987366, 0.16377101838588715, 0.4282802939414978, 0.37770816683769226, 0.36493223905563354, 0.15712349116802216, 0.8906430602073669, 0.5060160756111145, 0.9803026914596558, 0.7063020467758179, 0.9450419545173645, 0.514175534248352, 0.8998345732688904, 0.6741775870323181, 0.8874905109405518, 0.8864296078681946, 0.9834100604057312, 0.9220335483551025, 0.6808854937553406, 0.9557349681854248, 0.7937374711036682, 0.9845779538154602, 0.9984666109085083, 0.8217527866363525, 0.9605043530464172, 0.978058934211731, 0.9933198690414429, 0.9398490786552429, 0.991306722164154, 0.40132763981819153, 0.9787819981575012, 0.9479338526725769, 0.4007817208766937, 0.9404709935188293, 0.10587155073881149, 0.755908191204071, 0.9778755903244019, 0.8343572616577148, 0.5769349932670593, 0.9144764542579651, 0.8651716113090515, 0.9987021684646606, 0.068961501121521, 0.9936307072639465, 0.9133036136627197, 0.9970682263374329, 0.20887358486652374, 0.41558679938316345, 0.9972653388977051, 0.8837334513664246, 0.9450424909591675, 0.8699145913124084, 0.9880678653717041, 0.9130949378013611, 0.3792729079723358, 0.9784911870956421, 0.8917176127433777, 0.3885100483894348, 0.8974951505661011, 0.9648725986480713, 0.3071056306362152, 0.8979209065437317, 0.3783702552318573, 0.8291454315185547, 0.9648664593696594, 0.48071739077568054, 0.8865399956703186, 0.9456040859222412, 0.09221918880939484, 0.8763217329978943, 0.7542263269424438, 0.9851875305175781, 0.9182060360908508, 0.6977581977844238, 0.8387475609779358, 0.933072030544281, 0.7205514907836914, 0.9552148580551147, 0.9213075041770935, 0.9841721653938293, 0.28640344738960266, 0.9969037175178528, 0.3928230106830597, 0.9754374623298645, 0.6345157623291016, 0.6923409700393677, 0.9762724041938782, 0.9642542600631714, 0.8576911687850952, 0.8826443552970886, 0.8781494498252869, 0.9609842300415039, 0.08730897307395935, 0.633709728717804, 0.9377731680870056, 0.5901715755462646, 0.9668496251106262, 0.19812816381454468, 0.8933297991752625, 0.8317432403564453, 0.9072558283805847, 0.6359235048294067, 0.4999547004699707, 0.7735348343849182, 0.7123201489448547, 0.39693859219551086, 0.9583708047866821, 0.936977744102478, 0.982362687587738, 0.561208963394165, 0.8932204842567444, 0.4608529806137085, 0.08429722487926483, 0.5577307939529419, 0.9592882394790649, 0.9521053433418274, 0.6681652069091797, 0.975946307182312, 0.4880610704421997, 0.9217127561569214, 0.9838972687721252, 0.15872548520565033, 0.9336008429527283, 0.8062493205070496, 0.8700688481330872, 0.6064698100090027, 0.08045817166566849, 0.9152687191963196, 0.77083820104599, 0.9792699813842773, 0.366875022649765, 0.8094174265861511, 0.3577766716480255, 0.9227331876754761, 0.6540722250938416, 0.2888181209564209, 0.9496809840202332, 0.5064272880554199, 0.9669077396392822, 0.9890672564506531, 0.7124146223068237, 0.8011036515235901, 0.9864528775215149, 0.815654993057251, 0.9327630996704102, 0.9411120414733887, 0.07352805882692337, 0.5499123334884644, 0.16762198507785797, 0.6153053641319275, 0.33077263832092285, 0.6443902850151062, 0.9796627163887024, 0.8119137287139893, 0.7040886282920837, 0.9145431518554688, 0.09833656996488571, 0.9046937227249146, 0.04124828800559044, 0.9900612831115723, 0.4221780300140381, 0.04588593542575836, 0.9817994236946106, 0.7353065609931946, 0.3016539216041565, 0.4176892936229706, 0.049182258546352386, 0.9606187343597412, 0.7657195925712585, 0.9666778445243835, 0.9965658783912659, 0.1443040370941162, 0.18280251324176788, 0.012311595492064953, 0.9792308211326599, 0.49980583786964417, 0.9642889499664307, 0.8073998093605042, 0.06216786801815033, 0.01891024224460125, 0.9291338920593262, 0.9698328375816345, 0.899836540222168, 0.5020220279693604, 0.27511781454086304, 0.6523024439811707, 0.16644185781478882, 0.9918708801269531, 0.32448694109916687, 0.8148884177207947, 0.10209225118160248, 0.2790483236312866, 0.12863503396511078, 0.3630543649196625, 0.7055181264877319, 0.9088437557220459, 0.6156058311462402, 0.7508867979049683, 0.7929726839065552, 0.4183315336704254, 0.1551750749349594, 0.4700126051902771, 0.9843546152114868, 0.33201393485069275, 0.08722726255655289, 0.9504279494285583, 0.9592559337615967, 0.6916717290878296, 0.9974437952041626, 0.577717661857605, 0.17841729521751404, 0.9949231743812561, 0.00982851441949606, 0.5731220841407776, 0.6765372157096863, 0.03544328734278679, 0.2165682464838028, 0.6109554767608643, 0.7355910539627075, 0.07556050270795822, 0.8050799369812012, 0.5839567184448242, 0.8157675862312317, 0.9348880052566528, 0.9816272854804993, 0.8791979551315308, 0.9744044542312622, 0.25027430057525635, 0.5145974159240723, 0.9046801924705505, 0.6195497512817383, 0.11203393340110779, 0.5442371368408203, 0.3501335084438324, 0.8930145502090454, 0.9356542229652405, 0.9960110187530518, 0.9144120812416077, 0.9962933659553528, 0.9883811473846436, 0.20102936029434204, 0.2683756947517395, 0.9724499583244324, 0.19076724350452423, 0.9373419880867004, 0.04696393385529518, 0.2881465256214142, 0.5886310338973999, 0.7378572821617126, 0.06368496268987656, 0.8209172487258911, 0.9688192009925842, 0.6399618983268738, 0.081980399787426, 0.7729352116584778, 0.4491834044456482, 0.6238610744476318, 0.7513746619224548, 0.9590093493461609, 0.06820275634527206, 0.997869610786438, 0.7840301990509033, 0.7931729555130005, 0.8060623407363892, 0.9979535341262817, 0.43790188431739807, 0.9567577242851257, 0.14402610063552856, 0.5997892618179321, 0.9098194241523743, 0.0034546428360044956, 0.23862098157405853, 0.15135467052459717, 0.9758607149124146, 0.9519423246383667, 0.9160227179527283, 0.8770483732223511, 0.19500887393951416, 0.7719221711158752, 0.9895373582839966, 0.9908130764961243, 0.9385848641395569, 0.45376771688461304, 0.9882239103317261, 0.49918949604034424, 0.3438594341278076, 0.3805243670940399, 0.19241395592689514, 0.902823805809021, 0.056455619633197784, 0.13302955031394958, 0.7645297050476074, 0.38129231333732605, 0.36834293603897095, 0.6741381883621216, 0.091703861951828, 0.5614805221557617, 0.15246230363845825, 0.9464526772499084, 0.2286454439163208, 0.8843569159507751, 0.23940692842006683, 0.9921940565109253, 0.6208751797676086, 0.1455194056034088, 0.7988783121109009, 0.9272121787071228, 0.9451001882553101, 0.76419597864151, 0.8874444961547852, 0.8815828561782837, 0.15277539193630219, 0.9917798638343811, 0.27436909079551697, 0.7267898321151733, 0.9484913945198059, 0.9788557887077332, 0.9047399759292603, 0.2479962408542633, 0.885050892829895, 0.9862031936645508, 0.915188729763031, 0.5963321328163147, 0.31126314401626587, 0.9188847541809082, 0.11994379758834839, 0.5397946238517761, 0.8905521631240845, 0.6345714330673218, 0.7411507368087769, 0.4387447237968445, 0.6284796595573425, 0.9292755126953125, 0.9921079277992249, 0.01045591477304697, 0.9709221124649048, 0.29187148809432983, 0.058028921484947205, 0.9934868812561035, 0.9871296286582947, 0.9245396256446838, 0.19528862833976746, 0.40420037508010864, 0.8617069721221924, 0.7853018045425415, 0.5000655651092529, 0.13934500515460968, 0.5432958602905273, 0.4892207682132721, 0.6922485828399658, 0.96108078956604, 0.9414469003677368, 0.7034049034118652, 0.8319073915481567, 0.9555471539497375, 0.895582914352417, 0.14119262993335724, 0.5688786506652832, 0.5289394855499268, 0.45451003313064575, 0.17956797778606415, 0.5835302472114563, 0.9850180745124817, 0.7166791558265686, 0.5861434936523438, 0.9785594344139099, 0.39257535338401794, 0.9218635559082031, 0.4845031499862671, 0.9141445159912109, 0.7881227135658264, 0.9153504371643066, 0.7137240171432495, 0.707561731338501, 0.04028523340821266, 0.9360426068305969, 0.6695809364318848, 0.9417546391487122, 0.9914470911026001, 0.6666266322135925, 0.4424828290939331, 0.3329398036003113, 0.6401122808456421, 0.9902021288871765, 0.6726135015487671, 0.8344432711601257, 0.5547847151756287, 0.02562529407441616, 0.9597668647766113, 0.915967583656311, 0.9977486729621887, 0.7643001079559326, 0.9559623599052429, 0.16402888298034668, 0.052959512919187546, 0.993198037147522, 0.9576563239097595, 0.7917753458023071, 0.9863085150718689, 0.9654561281204224, 0.302666574716568, 0.4258916974067688, 0.5009640455245972, 7.82755232648924e-05, 0.147171288728714, 0.002244602655991912, 0.08110890537500381, 0.009257515892386436, 1.0942014341708273e-05, 0.02974763698875904, 3.453801036812365e-05, 0.3001297414302826, 0.21495963633060455, 0.724463701248169, 0.00014962253044359386, 0.019965792074799538, 0.004648345522582531, 0.10404252260923386, 0.031017320230603218, 0.0020014026667922735, 0.0011611555237323046, 5.8896173868561164e-05, 0.00845932587981224, 7.342393018916482e-06, 0.00042416242649778724, 5.67134202356101e-06, 0.018694888800382614, 0.010645236819982529, 2.2147434719954617e-05, 0.010462281294167042, 0.058375924825668335, 0.15310418605804443, 7.678807742195204e-05, 0.0001576480717631057, 0.00042949579074047506, 0.10385704040527344, 0.003146251430734992, 0.5164156556129456, 0.021323196589946747, 0.07450550049543381, 0.004002779256552458, 0.061634939163923264, 0.043307509273290634, 0.03827410563826561, 0.0007563733379356563, 0.002024044282734394, 0.0134512297809124, 0.024588875472545624, 6.578391912626103e-05, 0.0002911876072175801, 0.0012843692675232887, 0.0007445023511536419, 0.006934016942977905, 1.4932634258002508e-06, 0.001812694943509996, 0.001061046146787703, 0.9029001593589783, 1.1085806363553274e-05, 0.051517304033041, 0.06656897068023682, 0.0004307228955440223, 0.029466519132256508, 0.017439723014831543, 7.699250272708014e-05, 5.8857658586930484e-05, 0.014828911051154137, 7.364089833572507e-05, 0.00042442636913619936, 0.0036466987803578377, 0.0009676177869550884, 0.0010615445207804441, 0.07734916359186172, 0.012320087291300297, 0.0243810024112463, 0.0005493406788446009, 0.0022297960240393877, 0.039805784821510315, 0.0032185669988393784, 0.004974706098437309, 0.29374292492866516, 4.688898479798809e-05, 0.00026367336977273226, 0.0013633026974275708, 0.026993202045559883, 0.06338980793952942, 0.0009343040292151272, 0.22375747561454773, 0.22183305025100708, 0.0015799776883795857, 0.016399677842855453, 0.001042985008098185, 0.0008884303388185799, 0.00041965729906223714, 0.03754197806119919, 0.04833618924021721, 0.00031753178336657584, 0.0001839420001488179, 0.0525747686624527, 0.05496177822351456, 0.02303837612271309, 0.00045600783778354526, 0.00011162412556586787, 0.0005955032538622618, 0.008039379492402077, 0.06492941826581955, 2.7383624910726212e-05, 0.0003165524685755372, 3.5823119105771184e-05, 0.06062272563576698, 0.0003615504247136414, 0.00131412863265723, 0.0018398110987618566, 0.0007692636572755873, 0.00011449046724010259, 0.0035687400959432125, 5.599472387984861e-06, 8.065284782787785e-05, 0.0016633730847388506, 3.1459076126338914e-06, 0.0238615982234478, 0.020967837423086166, 0.11432461440563202, 1.9674427676363848e-05, 0.004030174575746059, 0.005384077318012714, 0.0003441039298195392, 2.3595152015332133e-05, 0.0033378524240106344, 0.002695768605917692, 7.457628089468926e-05, 0.002101561287418008, 5.58155852559139e-06, 0.00011035422357963398, 7.90622470958624e-06, 0.0013438124442473054, 0.010278153233230114, 0.013708877377212048, 0.40802738070487976, 0.0003794410149566829, 1.998339212150313e-05, 0.0004921647487208247, 0.0331321619451046, 0.00644722580909729, 1.155922745965654e-06, 0.10741497576236725, 0.007162571884691715, 0.00025749477208592, 0.16015124320983887, 0.06298259645700455, 0.03768036141991615, 0.13016235828399658, 0.2571243345737457, 0.2861040234565735, 0.00016575610789004713, 4.342049214756116e-05, 0.006611377000808716, 0.020141489803791046, 0.042037494480609894, 0.0004385135252960026, 0.004205148201435804, 0.00451702531427145, 0.00466981902718544, 0.5571242570877075, 0.3361756205558777, 0.00015194636944215745, 0.0025338504929095507, 0.04325738549232483, 8.764857739151921e-06, 2.3191767468233593e-05, 0.09201253950595856, 0.005122304428368807, 0.015771498903632164, 0.7481220364570618, 0.005359385162591934, 0.00803668424487114, 9.294922347180545e-05, 0.0002269237011205405, 0.0002647697110660374, 1.7041757018887438e-05, 5.000033343094401e-05, 0.00046402725274674594, 0.0007950266008265316, 0.00016336482076440006, 0.001087588956579566, 0.0027400702238082886, 0.0013682584976777434, 0.0004674262891057879, 0.00015377749514300376, 0.000854650919791311, 0.0016507123364135623, 0.0012597625609487295, 0.0003465780755504966, 0.0004041835491079837, 0.00034285287256352603, 0.0002146246115444228, 0.04703374207019806, 0.0005916105001233518, 7.964118412928656e-05, 0.014753732830286026, 0.008</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Outcome_InhospitalMortality</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>neural net</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.7587044534412956</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.7327021121631464</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.8145748987854251</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.702834008097166</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.7714723926380367</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.7587044534412956</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.7117437722419929</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.6941272430668842</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.7571174377224199</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.6663701067615658</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.7242553191489363</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.7117437722419928</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>[1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>[0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>[0.9999745051201411, 0.0012444521603148192, 0.7123082891249414, 0.9993415162915368, 0.8990188277466479, 0.9999999419467771, 0.9945136134531487, 0.6114650533295446, 0.8776905204284069, 0.9999865860142256, 0.9977400681747741, 0.058002452693919335, 0.9998782821368818, 0.9998563961738739, 0.9998355184975107, 0.4552380050735072, 0.9411922282880374, 0.9973804503313334, 0.9906580715176388, 0.015447200463057918, 0.9998947097411485, 0.9015722294890617, 0.9818578374601633, 0.9885503059821599, 0.9698251785095906, 2.2931893945062517e-05, 0.9999998158326961, 0.9998960991463107, 0.9999759079302865, 0.003922235111107994, 0.9849464258924708, 0.11046107570545328, 0.8393575151352399, 0.9988532087575231, 0.10067976519004598, 0.9999923910215223, 0.906536039985589, 0.9804472236048727, 0.9922424286483457, 0.2724194737722774, 0.9666724224499885, 0.9586138502804258, 0.00037624431828133106, 0.9827678959689443, 0.4828092324989348, 2.4205200919171093e-07, 0.999916089856293, 0.9999999916083754, 2.7244235117583187e-05, 0.9999894543682757, 0.939691091338739, 0.9999999938226511, 0.025584598675499406, 0.6108994325559771, 0.9999982145180527, 0.25324688497482983, 0.5840064387917848, 0.04780666252452539, 0.9999991316286336, 0.9995414885335556, 0.9658501390618306, 0.9122546510113693, 0.9992767243612091, 0.9999825586345535, 0.9995066855174879, 0.02725585590829376, 0.7581194592100416, 0.9999735907982175, 0.2891853497209297, 0.00996989288327774, 0.8443339002804556, 0.999070596685878, 0.9482239632773469, 0.9998205703085804, 0.9260417524061312, 0.9999933267260911, 0.999937258576091, 0.8583753429937038, 0.9999998803159128, 3.513516133214475e-07, 0.9998589290920746, 0.9597089696415219, 0.004491293306273457, 0.9889568463793433, 0.7314784923916632, 0.9999889833998562, 0.9995349259437253, 0.9999995301331775, 0.9828456406689074, 0.6798192831452021, 0.9999999612881013, 5.984866578488084e-07, 0.05959115659704971, 0.9729162364039777, 0.1756570337911765, 0.9803294439680759, 0.3323249125179228, 0.9907795414008698, 0.9990456570207481, 0.899759745089562, 0.051333168033064015, 0.9792293857963621, 0.9904943194799014, 0.8750639199484654, 0.9492895118236191, 0.6377635456463012, 0.21158920197883946, 0.6566939370419665, 0.7050063493424443, 0.017223664009110594, 0.4027764001667927, 0.0020593769149200064, 0.041510832441627954, 0.9635146476562654, 0.4363010341006276, 0.9997978728393644, 0.9997989267941867, 0.8984474306313408, 0.3362749209946362, 0.9632354817570479, 0.16872429027637048, 0.7569027430005422, 0.999833445174835, 0.8101178428568526, 0.7476561744941581, 0.24446317977743456, 0.20600376211669352, 0.5171287224483955, 0.28445246053641343, 0.7393603206795358, 0.9618257562259399, 0.9999927754006569, 0.8969707324520735, 0.43745699768460133, 0.9998129216301667, 0.9998794099237708, 0.029133466437732892, 0.9994651671612221, 0.9985922641442174, 0.9453811278935049, 0.9999992481839249, 0.999061141869062, 0.9984601356366006, 0.008034878860138385, 0.7501624902115613, 0.5178135608763337, 0.9999995723997047, 0.4804629842701821, 0.9999974857348694, 0.09963670020335849, 0.0007732869493203121, 0.9999923098691713, 0.5365267834719504, 0.9975849824275022, 0.0010194332771771481, 0.9999750797785679, 0.9987873858941558, 0.01818890570210431, 0.9986969786132512, 0.9276400248361092, 0.9999985635055947, 0.45491660641445736, 0.999987772213573, 0.9999843830417087, 0.2976908743540869, 0.99484521264674, 0.9999993458089002, 0.9231296337597419, 0.9995416559381596, 0.999624649899019, 0.996522179856498, 0.43814200994214253, 0.4461654406196509, 0.9996660971623683, 0.5993795104144516, 0.9561479411309183, 0.9965045116441099, 0.8744344118359091, 0.9725793971792217, 0.9999635972876515, 0.8073744283521587, 0.07967212000548915, 0.8370416602751299, 0.9999522370978166, 0.0008588230816904836, 0.9225795303541071, 0.9022235149920415, 0.9953126883171872, 0.7313354069004253, 0.9959455264941199, 0.9999957147568294, 0.9949439971285984, 0.4744267284005737, 0.527821577827547, 0.08892980483417032, 0.7914433844901941, 0.7427198673660028, 0.9599846365778272, 0.9990024170502361, 1.407560560516876e-06, 0.8286333583654569, 0.9991893542728656, 0.7614628809981769, 0.9997054479088214, 0.27119645607556636, 0.9999935602257884, 0.4581877111349739, 0.9999999865987446, 0.0015964645951988758, 0.9970986947836606, 0.9999764775330181, 0.8613219882582744, 0.9389704006451342, 0.9990054152477362, 0.9699009361970357, 0.9999999934979749, 0.9635936690927135, 0.9864223626419941, 0.998100787518199, 0.0006556357752595272, 0.9992270763418838, 0.2665986098417141, 0.9075198983518006, 0.9849998359193326, 0.9241575904663178, 0.9448331765860689, 0.0018905121615891273, 0.9772908913636422, 0.9883688969378462, 0.9999918953423762, 0.9991704009800113, 0.505767204555049, 0.9874236106143514, 0.999643257954178, 0.08756832855373009, 0.999957031577177, 0.005154221599348094, 0.8008954755357395, 0.9965070375341396, 0.8525100282875554, 0.442225027319502, 0.9971894290396045, 0.6584546889742171, 0.972520842110898, 0.9833813757491215, 0.9999999999999976, 0.99905951496112, 0.8583753429937038, 0.1560245188583055, 8.55343179995917e-05, 0.999998532947711, 0.999996998675959, 0.9999907889207023, 0.8453589559213228, 0.9999745038737887, 0.08580661440272493, 0.989238903225334, 0.9629648274786181, 0.7780548758257638, 0.9988670789972366, 0.981588506511988, 0.8961372035891373, 0.3177854548692819, 0.9998464449838402, 0.9993357310448727, 0.0037949568772685112, 0.9996706283291127, 0.0004556106968638336, 0.9948074879898217, 0.9998513449015378, 0.55921870782028, 0.9425613746092923, 0.4815998519511148, 0.12563763734929032, 0.984751161914519, 0.9167624261771651, 0.5972455633942958, 0.9997691583723407, 0.999945878371958, 0.9413600072120626, 0.009165923273069457, 0.983856118260958, 0.9999996641306566, 0.997403129782329, 0.9946179172627426, 0.0037283389568394665, 0.9999539731383476, 0.9991407961915015, 0.4720649257312036, 0.006716124550145673, 0.9990928376515426, 0.030719317193909194, 0.9999837166696991, 0.836048831112852, 0.9994523517515214, 0.34851746602824013, 0.7310953722570206, 0.9987216123912614, 0.7879394591568428, 0.15893155137110096, 0.00033234645615715655, 0.9989477246327085, 0.027650092259094365, 0.0023581442077440437, 0.9870051734454699, 0.9918474361523731, 0.9999951347514525, 0.9330424267699404, 0.9500371054896395, 0.998615036115764, 0.7875063074667961, 0.561471892838766, 0.9998119982433481, 0.8490722787672665, 0.999999779020412, 0.0017215318740617556, 0.031360439167794615, 0.9431085459333322, 0.6390692640812211, 0.18773619833548655, 0.9993035815848269, 0.8616717727334998, 0.9999991079061459, 0.996992170301263, 0.940127638064442, 0.8046018876984671, 0.998545678850355, 0.05065341311552462, 0.9128385352581383, 0.9999892799322984, 0.7119462510339595, 0.9805118444496302, 0.847822517980638, 0.9679511586262334, 8.695123605936426e-05, 0.21497374474485131, 0.9999985531587962, 0.9999991016219032, 0.9999982615412053, 0.8600628640747839, 0.06102787378957861, 0.8689874846158273, 0.9997477622352803, 0.982592314917472, 0.9943380876686402, 0.5625746469499789, 0.9990920019832435, 0.8858741214582019, 0.9841526564044513, 0.936108785889569, 0.020841669700578477, 0.9999999998964479, 0.8751415605854039, 0.9999925475134761, 0.9546700197765293, 0.9996945939932287, 0.9983800760925032, 0.9231130840572975, 0.9640820883021056, 0.9999517861890156, 0.9114590940864661, 0.0492056404699365, 0.9896510506871429, 0.9987723061928055, 0.9850481153437958, 0.9805555341369478, 0.6411534553901352, 0.67846998163227, 0.8470601435284373, 0.9927985120901405, 0.9979961688545631, 0.9999999783897091, 0.00037701992893456374, 0.9890573692992445, 0.9664421734979199, 0.23962333469348587, 0.988657875852824, 0.9970643765520623, 0.9344241539170598, 0.12150110421571285, 0.4518305200623528, 0.9546532741560153, 0.9729614493408232, 0.9338936600406449, 0.9026256554455638, 0.980814660077348, 0.9904505845316485, 0.4367199748155258, 0.9466696107163641, 0.999995096639439, 0.9949658643367459, 0.001223067012649516, 0.9861375751268422, 0.794392152936807, 0.42444271062347966, 0.953256260194837, 0.9726423567143281, 0.9994197498394322, 3.331876953439021e-06, 0.6314792200975917, 0.9995818726317273, 0.12836368657485242, 0.9511411342550201, 0.9959087764047193, 0.9905258462796899, 0.8645635072388503, 0.9971147751441675, 0.004356442046976137, 0.9998992366312804, 0.9676154789037992, 0.9982020940664104, 0.04551409705124999, 0.43981324652695497, 0.98850094453346, 0.9978924364627538, 0.9986478276240167, 0.5586642842357595, 0.995851654363867, 0.9850267994448442, 0.9654397123464022, 0.018169155416871377, 0.9883291807869253, 0.9494451011763267, 0.9958140151361151, 0.7124256383176452, 0.9977358347159813, 0.7196387675595394, 0.6210724664260123, 0.0012295156873976944, 0.9987427751593879, 0.9915209252716833, 0.9999994039979545, 0.9997379231583382, 0.7930514430436739, 0.9922475319333572, 0.9999974789064726, 0.2946368534017396, 0.9925967320894452, 0.21308004144650128, 0.6774458565488113, 0.9999819534356309, 0.9940385546487033, 0.9905658261745371, 0.016750088970434042, 0.9985819935835271, 0.9908845962999725, 0.9994244003015303, 0.9960736600494206, 0.40979971519105873, 0.9802441291126558, 0.9999985699787518, 0.8768590537250777, 0.8617943722036624, 0.0011652348992319506, 0.9999562199519616, 0.9999997986763, 0.9999979014801412, 0.0028612431489496684, 0.80638678781355, 0.7293982630215511, 0.9982123886606551, 0.9995331979395642, 0.996282226156186, 0.00388078147124203, 0.9994014873064739, 0.9999585023651403, 3.27228789909038e-05, 0.9906828257665495, 0.8159081580165052, 0.9851059050100842, 0.999921870680342, 0.9999999465435776, 0.9999190825599167, 0.00032434370677587876, 0.008395207577319352, 0.003443136794289148, 0.9999813783747374, 0.3081552220860412, 0.9997372040831738, 0.0001190892969590225, 0.9998392989641396, 0.5503198099897784, 0.9994540504898657, 0.5487597594429839, 5.8241433975213736e-05, 0.9999972628015137, 0.9939187965747039, 0.03351619796360384, 0.9999995430799191, 0.00701158095641149, 0.8973514058699661, 0.014477158797762126, 0.711355797078844, 0.4475166775850262, 0.07560813300428541, 0.9971232983756235, 0.9979320051232367, 0.6396333273430648, 0.9997138118067815, 0.999995462288777, 0.052795883293528106, 0.14557347290483097, 0.0008669030481321648, 0.021697154410262067, 0.037672961684784824, 0.13724997296680996, 0.8743094696100465, 0.9794758102156009, 0.9999999480823367, 0.9999990028515833, 0.851603794078216, 0.9999996263699683, 0.012497184746549154, 0.9999841715059905, 0.9695054654033035, 0.8801787599087777, 0.9721321201923788, 0.7891361255367499, 0.9992337582570724, 0.9990015280124135, 0.9703476789503193, 0.9986152362990536, 0.9973274756572635, 0.9640534646907193, 0.8689527472801458, 0.6383661225921389, 0.8506032811354494, 0.8487968496714714, 0.9433949619747966, 0.9992977471038443, 0.9999974387596263, 0.9999880172909802, 0.9999665918387308, 0.012374136319742548, 0.9999941324505027, 0.7614628809981769, 0.922292039173895, 0.9560440158456489, 0.2579543305240549, 0.9969605799317562, 0.0013024183397662892, 0.00840352937638815, 0.8891027177768366, 0.8983384523798228, 0.1037050193409489, 0.9999712013420732, 3.636039888609531e-07, 0.9978290283724893, 0.9995981379808369, 0.014190295162808113, 0.9616408276205818, 0.9999998991370962, 0.9987830547506463, 0.697199102461437, 0.7331076783980982, 0.9568959921698107, 0.011234839134683346, 0.9993564492524334, 0.9999276594298245, 0.9999999127179061, 0.9998891705047495, 0.9999809700444635, 0.9946048926549204, 0.259815536755913, 0.9663564223655058, 0.9999907849980753, 0.999996267217728, 0.7219808225959724, 0.9859911466424864, 0.03357712702071078, 0.19605122725704902, 0.9980989447666481, 0.39452444222383776, 0.005730383682994546, 0.9998291091983321, 0.999343282737175, 0.9999957821843755, 0.9999995169687812, 0.9999999920604278, 0.9992082300155573, 0.9988252019097549, 0.801610789572777, 0.9998177040735615, 0.9945014954644418, 0.8890390225435251, 0.05878011416890338, 0.9770601408943318, 0.9999826683272771, 0.10724742466780544, 0.9999023460643496, 0.9539524707265579, 0.9918803414660582, 0.9924965803537532, 0.9835026051907396, 0.9999961345504614, 0.45726021595982286, 0.999999998672884, 0.9964802679416348, 0.5927184832824058, 0.9876980982529726, 0.8979311892877903, 0.989936523370432, 0.7528663626279295, 0.003157893969434007, 0.00011979561985941839, 0.966760866830555, 0.3215055201813873, 0.13359372831982746, 0.21347957181825064, 7.373409088044205e-06, 0.8447416715524704, 0.9447403905461308, 0.9523349177441887, 0.9999736119474161, 0.21707810456780147, 0.9947788251801033, 0.9999999997015638, 0.9982927944755478, 0.0057417830584373195, 0.9999044444044294, 0.950796002852922, 0.02288424135512441, 0.012636740868074689, 0.9978711158991808, 0.9997938007433758, 0.7062269616617021, 0.12320039506247395, 0.25997125278440564, 0.5685076317418449, 0.9340850601061792, 0.9999966907590937, 0.9896032365769314, 0.9963052650093613, 0.9997945455389962, 0.9999986730814646, 0.9999846205386513, 0.5071622160363088, 0.8196554737743538, 0.9870321617544423, 0.9999959794366359, 0.9919076021259408, 0.999998585080329, 0.9923067509889254, 0.0005060498367225077, 0.9999981965189111, 0.9999127069826189, 0.9999685324707639, 0.002252342689350266, 0.9999969295080745, 0.19238542322097957, 0.9999825797787659, 0.02236712658955567, 0.9999879325040475, 0.9843549045822838, 0.9993680941788831, 0.5997876288444577, 0.9864936683758962, 0.25538445177608704, 0.9999087585528988, 0.2695273575147553, 0.4281855707981516, 0.9477334933359323, 0.11444849990284534, 0.7302042090232405, 0.4871802193694106, 0.48081754864503506, 0.9997750840361791, 0.0001970277305247163, 0.9958348255619903, 0.9953506547613044, 0.9999817089438945, 0.6656866055058269, 0.8319508672285829, 0.26446324262480214, 0.9261163660464922, 0.18530199511840073, 0.7811027002979651, 0.9175989565945809, 0.9972306237453572, 0.002022210126142298, 0.9930201292366426, 0.22083493860701503, 0.0041032389655314035, 0.3741653457835117, 0.6110359303932915, 0.9929515179026446, 0.9988345521802197, 0.0036941056423934427, 0.005316844374519486, 0.05948822512831459, 0.9999864787018942, 0.9999731385138735, 0.9682454464303278, 0.0894388823832195, 0.010809554653581698, 0.8231369281803895, 0.00020300184196040284, 0.9914774945072928, 0.9999913971805271, 0.9975949056991167, 0.999762513732861, 0.9743999460934946, 0.9705335168101678, 0.9167038305398797, 0.8459490836780853, 0.23412448400134836, 0.9999310351197368, 1.3667461305835096e-07, 0.988445162802014, 0.19183820115093483, 0.061202150248705386, 0.9996324594541265, 0.37136759984575496, 0.9998612129391852, 0.9644278435257934, 0.1915546777719795, 0.9754472964935177, 0.9834639168548384, 0.025148665135498627, 0.0007291311261497818, 0.2869939967176249, 0.9795203961530536, 0.9981100693585636, 0.016026942871568046, 0.8356104297189493, 0.9999846918694236, 0.9999999189730321, 0.5646678160241797, 0.992289497785639, 0.9987263122811687, 0.49484293054621675, 0.9849198723891341, 0.9914080900646645, 0.9999841857925077, 0.03637085002384922, 0.9999368998799669, 0.20240987828667056, 0.7245497052591491, 0.9999999997676359, 0.9996437875132493, 0.9974361416724338, 0.5891255185914561, 0.9142955802516757, 0.977950969753212, 0.4237915191087675, 0.9977202169067172, 0.9999999820866193, 0.999640483834536, 0.3472637054282632, 0.9999812176547858, 0.9556713414914356, 0.001905712383979692, 0.8390588937282762, 0.9999909410160615, 0.398466493282288, 0.9999984783425055, 0.9999950716745466, 0.9413843032630049, 0.9999982671058318, 0.9684268853427082, 0.9999999978142682, 0.0009144414412599705, 0.9998246540725586, 0.04798905332172504, 0.8900104789005415, 0.9896554597697917, 0.0004991354359537093, 0.16021131225352325, 0.0018928614228299408, 0.9899559381144536, 0.9975467586364999, 0.05635305547181996, 0.9830868012809807, 0.9967806934014958, 0.9770842662212196, 0.9807041247633511, 0.19183820115093483, 1.7579095082592786e-05, 0.9941627511643967, 0.9993879797131986, 0.9999999869657956, 0.8434721757327647, 0.4070417098993139, 0.705971982485876, 0.9999999999936056, 0.8217777227795677, 0.12402695562647441, 0.7877294628341621, 0.9729392540663773, 0.8619820485020778, 0.999990729971889, 0.000425433432066175, 0.5610454420173124, 0.9626913481560733, 0.7835508411678255, 0.28870629815219073, 0.9999982207152476, 0.12302980121843206, 0.9787652664089003, 0.9970811979354623, 0.7997252871191096, 0.5992591875655693, 0.9999596968332204, 0.9999934798012239, 0.7395654847845089, 0.9999857939031805, 0.9937588800509052, 0.9942076610011311, 5.97810350636501e-06, 0.9944674153456293, 0.18052709732438918, 0.729958245878452, 0.6543896856459971, 0.9999951883478593, 0.9096443268439625, 0.014553094019299278, 0.9998583173182998, 0.8361941005374843, 0.11550160190676928, 0.03229277217145343, 0.27202103327284083, 0.7150661619311021, 0.9830936191118049, 2.3931200929095857e-08, 0.9998590360906112, 0.06373661264738935, 0.9912002339780771, 0.0002819595037107638, 0.9999099207171407, 0.9999994096005016, 0.999941187986733, 0.9999718241617652, 0.7012674802983484, 0.7412373745616, 0.0015887021208245461, 0.9965666382020826, 0.7587218541109765, 0.9999503085098402, 0.013631146357429345, 0.9998658546321455, 0.04797377584426213, 0.006720187445866029, 0.9856791960169934, 0.015579196718316507, 0.05652097188754192, 0.4567065274383248, 0.9996790478559867, 0.9946071525443662, 0.930590281357798, 0.10075423556509248, 0.9999996807205169, 0.0003006028692018635, 3.560093937473539e-05, 0.001017967949133165, 0.9975526509844413, 0.7454566959074191, 0.9769486712881202, 0.0011525159479967113, 0.9441600431578276, 0.9995096798575689, 0.9997006696189675, 0.2004954756286061, 0.48755819936028855, 0.9863699838384736, 0.9812521415244527, 0.9168430981749182, 0.9890558167916125, 0.9935831900448359, 0.9994124114315576, 0.1258156594036633, 0.9997953003843372, 0.9440213802459344, 0.9998058678046906, 0.00024338863699286534, 0.999999934529514, 0.9998947273525075, 0.9970993196334836, 0.9789278017738375, 0.11437178099552776, 0.07949787316843844, 0.9990703513565253, 0.3943909150726805, 0.007347804721108618, 0.61848518848622, 0.6187644243833826, 0.5937148219254657, 0.022909496489515825, 0.9883925382173067, 0.9466267972691557, 0.9988260048963679, 0.9996318146287015, 0.821882052877155, 0.05801392361959379, 0.28562266460124724, 0.5993795104144516, 0.6467414238514617, 0.41295359847156343, 0.9999837526964473, 0.04021409373303775, 0.9987558364580519, 0.9985525233444943, 0.9966285113316288, 0.9340315815291119, 0.26952001852266844, 0.03693311829610827, 0.9999787701779824, 0.12704775145922317, 0.9777445105021586, 0.8246266117993292, 0.9763988081127617, 0.9566438914585685, 0.9702821208663192, 0.9923151202802654, 0.9997649110544503, 0.9999847985112068, 0.4894609642203651, 0.9998631032757751, 0.9901117258315952, 0.04060624802368171, 0.9989386058025511, 0.09593661437188258, 0.003906610788848352, 0.9801835954274143, 0.9999772854447105, 0.9996372969901843, 0.0007266412531385268, 0.020046225420399615, 0.9999978044259494, 0.9999741045012731, 0.46743025898039775, 0.9555786106809192, 0.9999860832601836, 0.9966155993044171, 0.9999564725234513, 0.651912980651072, 0.7055285973091845, 0.9999409728616957, 0.9987064017978049, 0.8464604244291491, 0.9999168534523779, 0.9635936690927135, 0.586181568307964, 0.016281922899206467, 0.2667702395853527, 0.9995722965579246, 0.973423624020668, 2.316586031631397e-07, 0.017136965575014436, 0.8117362260449278, 0.2727924730552914, 0.9999953322082193, 0.0024450141925742887, 0.9546532741560153, 3.3650342528627745e-07, 0.20387618658853893, 0.6471711770887235, 0.9646986616506261, 0.8804589327715433, 0.9853466100130683, 0.9999886219757919, 0.9999983417351361, 0.3225943523521644, 3.360050387533167e-05, 0.9999375497586539, 0.9651032395750044, 0.9998039498316149, 0.8778700088818993, 5.8160678344052566e-05, 0.9999987523665533, 0.7225599349812436, 0.004930525512658345, 0.9999747727438983, 0.20287782258432144, 0.9904791693321183, 0.9921747835765916, 0.9979751515681096, 0.9947046433660289, 0.9999623060534164, 0.9999184588035244, 0.9999915011879037, 0.0724387676421297, 0.010381584144549741, 0.9985856117634712, 0.9136236580162953, 0.8623189782439084, 0.9995106595804829, 0.9999975038427458, 0.9875062862112455, 0.08107300635906634, 0.024702225234915318, 0.9999979255141398, 0.6117605062347393, 0.9953919423050549, 0.9999999966518693, 0.999986369842165, 0.9992422994745462, 0.9994402659656136, 0.46140849013763163, 0.9608073479926262, 0.9961618830158645, 0.9867091858179713, 0.9488325073115975, 0.9990043711869412, 0.00014794461185915726, 3.3184625375038317e-06, 0.9535972844296011, 0.9847341897754309, 0.9999923774124372, 0.9986050432403819, 0.8477409958591909, 0.9998342338191121, 0.6263083469491644, 0.9999351145684506, 0.007647463828895169, 0.9999113389551335, 0.0007810162744436251, 0.40716157724385915, 0.9999944981149413, 0.7038223669662552, 0.9998696518028442, 0.9999999787558367, 0.9958570887854155, 6.356170852198171e-06, 0.9984345059054632, 0.010637393790671551, 0.002235035639309071, 0.1188084844273015, 0.9996235709483868, 0.9996916290852467, 0.17875956463409615, 0.3642489438675861, 0.9965420778946151, 0.9476732942213233, 0.9996926084539458, 0.9997059449976531, 0.0175678076511335, 0.8211721302012653, 0.8484543496520142, 0.983874891306923, 0.9999984907146471, 0.567169110170161, 0.9997298887589706, 0.6613290931822586, 0.8807256124474521, 0.057147891874565857, 0.9566055020815587, 0.023428468696587337, 0.8411526099646602, 0.9919636011576795, 0.18122463412010978, 0.06097528703175468, 6.553638404852768e-05, 0.9005772341864936, 0.9900864938892356, 0.9999988268599096, 0.9999814147072652, 0.9904247928116227, 0.5442633052366977, 0.5638856136668733, 0.01918945770912323, 0.9532667780480292, 0.9703811101367714, 0.9999999975389089, 0.9901064528907445, 0.032154268240239994, 0.9891118786010139, 0.9864838456261763, 0.8147731317134942, 0.014810568146943353, 0.9992799126153106, 0.9999456752349508, 0.9846459767022051, 0.02323475811427922, 0.9999952778465, 0.9955452556969878, 0.9996039540849383, 0.9993722892276324, 0.2990616256591434, 0.9819960156428065, 0.9999818982278579, 0.9994488428711391, 0.9954129457175377, 0.048390090689048294, 0.5578683181613665, 0.874827118585824, 0.9984597275013851, 0.7447609077409881, 0.9999999866987015, 0.00018976057107844086, 0.9894546765700718, 0.9986248499804516, 0.9898656600714584, 0.6224376545418883, 0.9999663816674854, 0.9999892388462949, 0.9999983202986676, 0.9999095977337423, 0.9871851439453871, 0.9997084896905536, 0.6320338384706237, 0.9990961380303849, 0.677221252022324, 0.9999855722127654, 0.9999946429036795, 0.7361066728131862, 0.02091734993849031, 0.08349684823296057, 0.22468463506389608, 0.05057110033032633, 0.972190517885405, 0.9626751262695569, 0.6346998236626966, 0.9995170222188118, 0.928784903608487, 0.983863054369104, 0.9589793651411816, 0.9689562507434163, 0.9811157259930176, 0.04644803006511992, 0.9999976093392026, 0.999699545568214, 0.9624347097545685, 0.9998676276551868, 0.9999561580023106, 0.9922498601566562, 0.9951581164467727, 0.9852564749579192, 0.991818349842428, 0.9995294181901392, 0.5667664349326876, 0.7922158535450475, 0.9999999890700105, 0.9994184642291893, 0.0001697947480620192, 0.7614628809981773, 0.999823347653834, 0.9455615992811578, 0.9999543862270732, 0.9999979759652273, 0.999547220223384, 0.9890125914523843, 0.3932124090247095, 0.9999999176748188, 0.9987811888964583, 0.9999928396700902, 0.9999826490995232, 0.9690131158964421, 0.0013343147970187007, 0.3668369091720202, 0.9767300432521308, 0.9995919007176144, 0.9976917312857118, 0.8690992525450777, 0.05181436345000193, 0.02561002659929903, 0.9883287696019718, 0.03407697674717323, 0.8291467527791525, 0.028227186658135464, 0.998460725216413, 0.7934440701042632, 0.9914873695482526, 0.9664086589029369, 0.9993126196180105, 0.5944145711283267, 0.9999427148476852, 0.9817972242819641, 0.8609022035358154, 0.002203900247567386, 0.9999999866511033, 0.6931950683151705, 0.058409405368050615, 0.8546642183199585, 0.01978034374044559, 0.6733179283155416, 0.9957760504611397, 0.96840151689523, 0.999999794208747, 0.9999836059817647, 0.9880189831759696, 0.002002082341552361, 0.7237035740173066, 0.9994607302012731, 0.8745011415682571, 0.9997524157165419, 0.9964117477446522, 0.9996945302439076, 0.999748004781527, 0.8454197323920859, 0.010563150161082167, 0.9958211185320949, 0.817000399925529, 0.9999967201016048, 0.988161241439121, 0.9947312529423625, 0.9999670881810307, 0.9998940185031137, 0.42611220672633154, 0.9969282297252374, 0.9999602362753639, 0.03265994391493022, 0.1187170270986636, 0.9995482774942805, 0.527821577827547, 0.9655991643047342, 0.9124114849059446, 0.859414838122888, 0.8087983580920335, 0.9718589052042055, 0.9744671021719377, 0.6100575341598825, 1.9849252824055015e-05, 0.26915028794490725, 0.9999999917132972, 0.008509174303929818, 0.949621193053353, 0.0006529639862328755, 0.17629552258074557, 0.9999999999165472, 0.9717858362665086, 1.8098473978772527e-07, 0.9999999135865184, 0.9951927481018141, 0.9993683809213573, 0.902611430221833, 0.9882558680780635, 0.998755508608198, 0.00010548536126220344, 0.055641165417004895, 0.999995547477015, 0.9999999966749762, 0.8750777073586259, 0.9126490702620681, 0.999172712424394, 0.11175534691851671, 0.9838969814859659, 0.99854846305921, 0.9999134235418691, 0.9830670175085977, 0.9995858789417532, 0.008163951045369069, 0.8418912681912419, 0.9999981628920424, 0.9833813757491215, 0.9999999519805386, 0.0006293845866575936, 0.6804071885272585, 0.9999958088609784, 0.9998543445728395, 0.0016640874691775385, 0.9992955047083124, 0.6296747121848805, 0.0006080619457555852, 0.9704597607824356, 0.8982278241888695, 0.9983023153193834, 0.527821577827547, 0.9999999998027178, 0.985189205136708, 0.999296296308414, 0.9999762057409829, 7.039204319496728e-05, 0.9998696928928699, 0.9999793848647219, 0.9979439162674499, 0.5950617390047435, 0.9999995357001501, 0.715231638728593, 0.2751388672767368, 0.6889155158560232, 0.7813297480146014, 0.008606424659404905, 0.9999095022450972, 0.8314779246148748, 0.9341120898742421, 0.9940874157601094, 0.11039665506032172, 0.8667617081007654, 0.18052076555504432, 0.99990587218623, 0.9930637013092944, 0.333521191283744, 2.988756368575367e-07, 0.26119877603064034, 0.9999999994072113, 0.9817520749757639, 0.8016107895727763, 0.9999838480537966, 0.9999999926229111, 0.4379524145547357, 0.9992698419460206, 0.9996017821805161, 0.8684493069103933, 0.8108248966340712, 0.7936628723944184, 0.43081231105444295, 0.7443503886447876, 0.9663680527636875, 0.11178508126875186, 0.9999992491158093, 0.7698333282494968, 0.9999707282296676, 0.00565222313151138, 0.00647876358066238, 0.13217202508446735, 0.0027542742333281998, 0.999616562728686, 0.999998506361964, 0.9427742750276199, 0.7939812308737965, 0.9934821269478217, 0.9833813757491215, 0.9987407590102875, 0.985718883206668, 0.9999386424128762, 0.0165049293745257, 0.3711918522237933, 0.6242358887123962, 0.8785884747918173, 0.5874686571894809, 0.9999999993468784, 0.9999943790041775, 0.42286568668452107, 0.8086377024317062, 0.9999999968318507, 0.9954320828756397, 0.13033792701064517, 0.999978130379791, 0.11259502829763532, 0.9987090367650592, 0.9905786228445078, 0.017265437212408342, 0.9708450559256173, 0.9981437457760369, 0.00043311709906382556, 0.9980950605073081, 0.0030432803344157783, 0.9991012884461108, 0.9826087825962437, 0.9946054508533074, 0.9999481629735517, 0.9996951995916944, 0.058625608627876996, 0.9949435142432845, 0.7783994296839524, 0.9873060894894319, 0.9999999874778825, 0.4196185971783322, 0.9883190480589507, 0.9720292494584244, 0.46516889711927883, 0.999997122073407, 0.9999769358064835, 0.9981420529035875, 0.9732994145571168, 0.9989897281112209, 0.02123673922276711, 0.9999999999934774, 0.9676904295261476, 0.9999697059363901, 0.1164472023457629, 0.9942176265918491, 0.9257931294026815, 0.9247716561457298, 0.9998196511823182, 0.9999138560970416, 0.28332569687567993, 0.07743395944445396, 0.9875189809461156, 0.4962262642101392, 0.8301898228705731, 0.9956114034664352, 0.0888661278501667, 0.7173983684708953, 0.9587482583066685, 0.9999699845773715, 0.991493185353337, 0.9941738711691112, 0.999936325824442, 0.5773342560213072, 0.9087655647266568, 0.9997644503606137, 0.9998742629776834, 0.7614628809981769, 0.5089680760962041, 0.9672409804721984, 0.02339373899441502, 0.9995647581903973, 0.9985106089688363, 0.3458130460037167, 0.9997344279840271, 0.9853947221713562, 0.09126258592275335, 0.9901828962774852, 0.8001219560823707, 0.00236068018951677, 0.9997653586322163, 4.164237384850162e-05, 0.976233892595134, 0.9720410334893166, 0.9925353885855005, 0.9952513490724405, 0.980997685001443, 0.9184344014124416, 0.928412083511397, 0.010275499576351698, 0.9989142107335982, 0.836048831112852, 0.99893636480812, 0.9977813002608653, 0.809540404025659, 0.019643387910876064, 0.9561804564059646, 0.9999990761892302, 0.22929865398644952, 0.229797538913776, 2.429612548275604e-06, 0.06735637272114095, 0.9934870575138148, 0.9557340813474314, 0.008961767719615463, 0.9389200997592405, 0.9999994073629542, 0.9999999989817294, 0.14392189523248367, 0.992925956171917, 0.9999984272707024, 0.9228138374334729, 0.8969171077504269, 0.027384911608250344, 0.992962471135014, 0.5602432788986598, 0.9999999993378199, 0.6379043433958818, 0.0543445200564219, 0.010767184501954193, 0.2616414160661005, 0.7704098597047303, 0.9999674432068922, 0.9931771563942121, 0.09621818171967621, 0.011524549593187867, 0.9953440284892058, 0.9953315123440248, 0.3786148835967879, 0.9905167795474659, 0.6171880060021727, 0.003102904253306349, 0.9523135969653473, 0.9999779164109002, 0.18056959197205213, 0.9669356501056199, 0.29011314475784694, 0.07075109649839442, 0.8459835009891553, 0.8433683860015349, 0.9999999998633802, 0.5673914749173303, 0.005297369560745372, 0.027900212328760197, 0.999963101009425, 0.9999725877212021, 0.9999995073384156, 0.973595001128965, 0.0016255845547434313, 0.8244641288799653, 0.9962933912898808, 0.9675447951953102, 0.8123536788615755, 0.0020850840862573035, 0.9811396198460293, 0.05497068156668428, 0.9999998868477745, 1.681923394505543e-05, 0.0034665842421063636, 0.25662820449566387, 0.9449779929396797, 0.9259290317018812, 0.32819983467087793, 7.764759443078964e-05, 0.9890185435371323, 0.6491646911385889, 0.9793019453158874, 0.9999764854693929, 0.9868367804153804, 0.6615171882069322, 0.9999928216818071, 0.9989588930789738, 0.9289236058834829, 0.023067505370023403, 0.9743459704791468, 0.6975761406996173, 0.37718520517156096, 0.8692426925188476, 0.9999938814321115, 0.9315040088429806, 0.9999483903447391, 0.8982278241888695, 0.01908235011467271, 0.9999992962455612, 0.0009561544645604184, 0.9999991647793963, 0.002813773997357546, 0.9797639717061757, 0.8657964713815491, 0.30845605084640587, 0.9358113647333755, 0.13020820324282806, 0.9999876089168039, 0.5439951179461278, 0.9957219215231472, 0.9993788423144185, 0.9999992653728401, 0.9610031483163168, 0.0016620189250828386, 0.9998492108157698, 0.9903615820885919, 0.9999954490697595, 0.9826713589229796, 0.20083771024200162, 0.07868542024363613, 0.9980474270979257, 0.9999521245754008, 0.023201767383738324, 0.6443860121064156, 0.5077327193169773, 0.010237664741837401, 0.9998691966936145, 0.8925658024645414, 0.9999976695592849, 0.12859418039244172, 0.00015528695778747092, 0.001888414570188429, 2.715478962690477e-05, 0.002261126548681121, 0.5600866631492677, 0.17081831760231728, 0.017372227759196595, 0.005936166994901309, 0.005485143017169118, 0.004426740402317504, 0.028338600135534697, 0.06452937882313581, 0.11937762406041848, 0.998994725973469, 9.409935888545053e-05, 0.9327254347731888, 0.14754551179855324, 0.08472357306704727, 0.9841733069515691, 0.26659177484343327, 0.14599919678867235, 0.014241570784429749, 0.0012593245532394404, 6.07301738483144e-07, 0.011011793640076872, 0.05382768202126011, 0.015576382062676381, 0.9706791893591992, 0.9824425288366775, 0.0003043416967285535, 0.001757460758018687, 0.0022203897111337093, 0.2893433906132164, 0.1710391420931003, 0.05473141459761203, 0.14094798196485647, 0.13804537823030216, 0.9967199781169246, 0.5511071147755918, 0.00063794001480323, 0.03493347080962572, 0.9986965274299899, 0.4905349019605722, 0.16589568679902575, 0.002258020278035517, 0.2687166309826792, 0.006901718368114527, 0.0006501871108268243, 0.0060246743721256695, 0.8252339112224444, 0.031524993478565154, 0.00017829647705457958, 0.00016216293742479101, 0.01756163755807841, 0.09648170893903496, 0.9424615122107377, 0.999949397347797, 0.007152616780023776, 0.4591491579185578, 2.706271482186678e-07, 0.40614587835108007, 0.0014134101662390377, 0.022039703145921487, 0.0030894827010996607, 0.03242446876844455, 0.2735120757034763, 0.9999887900325366, 0.1087621850846408, 0.00013097145622352954, 0.04905115721710959, 3.691188202606546e-05, 0.6418708994203702, 0.003070371198409035, 0.08930777724332363, 0.03331654309872576, 0.7404930056112677, 0.004890131982736358, 0.7982384770950093,</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>[0.1742748857145403, 0.5288757678888288, 0.00035028506458857243, 0.9999999999484785, 0.9998636034801454, 0.9994423730116748, 0.9356179749044296, 0.999929440705031, 0.9999128391947399, 0.2512824948065009, 0.9999979388342843, 0.1764138044939941, 0.8754709848719089, 0.2465859076320179, 0.999999859889468, 0.9957043369103438, 0.9966873104131863, 0.15524973024823635, 0.03993265781726335, 0.9970806918588375, 0.6283863574729506, 0.9999184506379863, 0.998906045518694, 0.006910291863764803, 0.9890272420124306, 0.6266261937976573, 0.9919897565053652, 0.9999042353638639, 0.33242336791915805, 0.3104176338468579, 1.0029069002154752e-05, 0.9999953190836007, 0.9192610547554602, 0.9985051825034669, 0.9999997068969906, 0.9996539928217976, 0.9999268383749725, 0.3001461169135743, 0.9997468646466604, 0.9986439512331776, 0.9997078758919117, 0.9999850037436421, 0.9997360873625084, 0.0005959417426336697, 0.9773172629281093, 0.98395632127123, 0.9999998362621, 0.999641045545498, 0.9999570016247791, 0.9964228252838603, 0.9964122230601197, 0.5034380184945406, 0.9971082763933679, 0.04634372453305334, 0.9999097589256263, 0.999839926236514, 0.9720076803461379, 0.9987992760315292, 0.9999999221659702, 0.9974801104001451, 0.9994706119678352, 0.9999998579756941, 0.9950215138950363, 0.9999963692991324, 0.9999974226746214, 0.9999852729709816, 0.9999885817075248, 0.00025423098843428823, 0.9993686018266915, 0.00873364782601321, 0.3971918811371875, 0.9984506338954219, 0.8825620682919991, 0.9999984593774113, 0.9999998745238263, 0.9985068451959057, 0.9999998967450057, 0.9999985981587064, 0.530153638974396, 0.6814003589859471, 0.008649767376376414, 0.9996287713543359, 0.8385508313623674, 0.9999576762214214, 0.9946588740006798, 0.4579280515768833, 0.873589193074189, 0.24338890797915935, 0.9904429248748438, 0.995738495378918, 0.8949487785175252, 0.9999968340957192, 0.9998217742461265, 0.9999999995823317, 0.9998480904502175, 0.9970238687744765, 0.9776891664431338, 0.9951763893733558, 0.9997598712113366, 0.9997016619195737, 0.7407366973528666, 0.0011478296691703862, 0.999969104482625, 0.9799066902311926, 0.5705954275407996, 0.21065333298618075, 0.9999958783615648, 0.10333501297083726, 1.0238293025393531e-08, 0.9768800380083941, 0.5890836800085495, 0.9999998662144233, 0.4191375562681135, 0.9999347268040378, 0.012612425826148311, 0.9999724438646443, 0.396976321600971, 0.619106597998734, 0.9996255809033353, 0.9912406634287962, 0.9999398446227791, 0.9692610485340337, 0.9907499658287805, 0.9999988858215642, 0.9999999888212946, 0.9321837613070891, 0.2498254158327531, 0.9900374650376198, 0.999979583584476, 0.9999776530255994, 0.015465057592813873, 0.9965063707548328, 0.02269097425619886, 0.9998183086927841, 0.9982531802143428, 0.022855204659507047, 0.9999999379060865, 0.00533709788929464, 0.9931415836378475, 0.4765106238128955, 0.9999998627150823, 0.9999996940122967, 0.9991282917719824, 0.9077844486704595, 0.9996758639095832, 0.9999994256071831, 0.9773034116039891, 0.015764382060134384, 0.9999999830297767, 0.9991653680988024, 0.9987167122866714, 0.9529342806117357, 0.6642926298192832, 0.9988318705657765, 0.6970686282048449, 0.7293613359524833, 0.00033797535437658647, 0.9999944592120487, 0.8054485264726189, 0.9733080726874651, 0.3008337860640559, 0.9968783130707798, 0.9637463276549645, 0.9896019605448851, 0.012908362279303044, 0.9547810789888393, 0.025072277545887197, 0.9834061663701635, 0.11454699774652935, 0.9998645765264645, 0.00016621684981819136, 0.6880761005707866, 0.995887635089177, 0.983962024463721, 0.45058691567126535, 0.6451515478718486, 0.0034292399256618564, 0.9997800906387121, 0.999923079108435, 0.9971557480276796, 0.9999947958443479, 0.9998192512334296, 0.9948605987305196, 0.9999999133485973, 0.060136795156878475, 0.5392427154213043, 0.9832469436191851, 0.9999975441754022, 0.0644440101106195, 0.9909243187213572, 0.9999979153029542, 0.9967844368713641, 0.9995152534525108, 0.4445727931385546, 0.9983399171115249, 0.9956132740339667, 0.9999999442050416, 0.9378281940988429, 0.9740997993907723, 0.9999999532514177, 0.0009952600205916774, 0.9820599848653209, 0.9978403317575071, 0.9939637126725466, 0.04225671913230816, 0.12405422675317086, 0.9999409274584643, 0.5250411383917925, 0.9953065896981679, 0.9999999760126165, 0.03376729370603503, 0.9973625285667075, 0.9999995889631981, 0.017278559306148036, 0.9999994692971085, 0.9988054861699422, 0.9914538205275799, 0.9994437538903699, 0.011548060715806384, 0.9999636732207773, 0.9604739710666734, 0.21822830820279818, 0.906507332109826, 0.9998312058187121, 1.1786300721609781e-07, 0.07225522828078931, 0.9926784079726455, 0.001342327765570495, 0.5484681538377368, 0.00042094266779311556, 0.8281843589682618, 0.14936627155180182, 0.9998947580105334, 0.9991272930269929, 0.8641517259473688, 0.0019041821976492485, 0.0028977750128403924, 0.014234891024642345, 1.7654388386068696e-06, 0.09050382580247375, 0.07699766983436912, 1.790144328799915e-07, 0.0073764828327606245, 1.4149735680271728e-05, 0.3404053803786752, 0.99956435294146, 0.9999939461813909, 0.6729091190151235, 0.9999989140905966, 0.9999533608277494, 0.0018933053675256948, 0.9999888300567225, 0.9893841768333662, 0.2570560914777113, 0.9999997118065791, 0.5043262399055853, 0.4808915300178995, 0.9999954029936909, 0.9999999998923828, 0.9999998304938224, 0.9999884648108873, 2.5618512150385236e-05, 0.9991696988638844, 0.003459087591062925, 0.00828868718848206, 0.002594735368075378, 0.6792713485727273, 0.0017599440502528995, 0.7068271393497331, 0.00034091947213426123, 0.02662732501304652, 0.007020477141521161, 0.9999989400306113, 0.9316876979173798, 0.9999718669380239, 0.3465213411609313, 0.2435157695286903, 0.14338422258306954, 0.8276962481281279, 0.9930402278085578, 0.19043000428994833, 0.06766076176655597, 0.9999168282076346, 0.5354711842098017, 0.4101749334743902, 0.9997433789886905, 0.9999626259455079, 0.9999999920614352, 5.713254008104437e-07, 0.9851129968519268, 0.9999999858448407, 0.09214909060790404, 0.01564405755914074, 0.9971256894980722, 0.9955404409912993, 0.9791684947897817, 0.780491104413716, 0.2925499476398811, 0.0007887214305150108, 0.9388707810946103, 0.00019223567318442662, 0.30941012594166456, 0.999348752047265, 0.44116079486458126, 0.06902565286150134, 0.9982792610332626, 0.9999997687596571, 0.021576554575220938, 0.7881422802386605, 0.9999999998162896, 0.6089269470177598, 0.28617010106499646, 0.9779445513403164, 0.999999338845199, 0.9594640831271372, 0.9999998319768983, 0.8888449817508063, 0.9999985210886881, 0.9992247359243769, 0.9999965302245118, 0.17571182819732847, 0.07333439619067739, 0.9999990462753156, 0.9997815263525642, 0.19553051480689598, 0.9999991680229393, 0.11304387074708393, 0.9714793732936424, 0.8204173130472597, 0.9337804741033223, 0.875848088836454, 0.998823140745359, 0.9999998908603108, 0.9968415696092287, 0.9537456518159834, 0.22367676085041097, 0.5656235264132121, 0.8663977617781422, 0.9931152099221566, 0.03290825191538475, 0.00016753811056179763, 0.9976963147965383, 0.9999884827960387, 0.025329089260286684, 0.24261330604176765, 0.999928904818547, 0.7352727638163229, 0.9999999980573573, 0.9976602418066369, 0.9999999993184157, 0.999999999470979, 0.9999999999113922, 0.8925546065321402, 0.6537113965587077, 0.9342814925135231, 0.9918562537867067, 0.9999942822407066, 0.6405282432750731, 0.9714426833913147, 0.9982869720991553, 0.12758191158174417, 0.20047844361990158, 0.002819697804568432, 0.0031937294980911054, 0.9964198638709594, 0.9969577211731065, 0.031886195153538535, 0.9516700084788737, 0.9998232475338078, 0.131987669828751, 0.996725441543575, 0.05738998433318424, 0.6239935487170964, 0.5262560067516341, 0.7539870237319305, 0.9987660983421331, 0.001351453652465743, 0.9761349125562329, 0.9959353366444574, 0.760883995498122, 0.9891679728668313, 0.9991808241574952, 0.999999769142631, 0.9980247224105488, 0.9989105317250028, 0.9908000251002851, 0.6286270169906921, 0.3108922922307384, 0.9221041851605543, 0.7169717013931597, 0.08961396945222187, 0.9999999237807784, 0.001930872851247956, 0.9999999301622835, 0.999985084287649, 0.5199388366599175, 0.11077987605834742, 0.7031187777100766, 0.9851908846377538, 0.63677579889455, 0.001858188095526266, 0.9996105813736574, 0.4704390667547151, 0.8899823873131162, 0.999236751366985, 0.039644376772478, 0.6649984780561098, 0.7419341393416548, 0.24942351674050237, 1.2334342831542556e-05, 0.999999998927203, 0.9780384882116591, 0.9999342806409621, 0.9999995170751835, 0.9961762578815437, 0.9998564954385992, 0.9641932194398262, 0.99916971639635, 0.00018169585569851243, 0.9966744967385212, 0.9669332407818699, 0.1267108344337286, 0.999357074931145, 0.061499569736520654, 0.004912896725382461, 0.11065259321271281, 0.2552344998875443, 9.84582948631192e-07, 4.254990295045679e-11, 0.0006562729438712077, 0.9999964357333828, 0.00015671500173571645, 0.9999999505933879, 4.273599910483853e-07, 0.9487950216196827, 0.9722428964212505, 2.989541146173211e-06, 0.6581390071341413, 0.525390177597954, 0.34658834456387305, 0.9999994687020085, 7.628718433380495e-07, 0.9999963327891558, 0.9947019872326343, 0.9844468914607307, 0.9997392449305817, 0.9750385089187255, 0.9999906298785222, 0.9886872766583094, 0.9864593159952698, 0.35460298841771754, 0.09689367613359084, 0.09128488659420773, 0.9997049689925354, 0.0575388104686872, 6.293254997410016e-05, 0.5374971583368338, 0.8515722777089942, 0.1082389681135709, 0.986231471142576, 0.999153336269275, 1.2256552630141648e-05, 0.7705822371683296, 0.994855088157589, 0.24249703045746115, 0.6132859370009504, 0.011167611845681253, 0.8786387739795049, 0.9951071532200333, 0.9954473896490855, 0.9984329842935418, 0.9999244160430479, 0.2541142557999492, 0.9999981097994626, 0.9987744055083263, 0.9809196822897869, 0.9602300296053234, 0.01103830384307177, 0.9999999965620716, 0.9994576328902275, 0.8576799943184158, 0.999536906347069, 4.430270842572114e-06, 0.42122948954225675, 0.8577201399372136, 0.9983315011148102, 0.9982372097269953, 0.9992015631362884, 0.9960380371569538, 0.08444655513339692, 0.9999851038313372, 0.06402436166281847, 0.8012012765464002, 0.9948760004111302, 0.9989224302143762, 0.9999736063150331, 0.13584430080714854, 0.9982235975484934, 0.4612796816350781, 0.9980267773058089, 0.5970750574405602, 0.9994258957421392, 0.0020828568064298553, 0.9996407606692673, 0.450843832757395, 0.8539014509081764, 0.0039570065130328505, 0.9998061525421305, 0.0010099081138113342, 0.1896724103798849, 0.9365172335818701, 0.20855877646718504, 0.9999865162935722, 0.8564251698023183, 0.999993878617752, 0.9633277647927889, 0.0001622663981608827, 0.06501216581592589, 0.9883566555550752, 0.12781279850022087, 0.9934765035806475, 0.9999703717701729, 0.9999992477480243, 0.993043970769788, 0.9721588092378818, 0.9984740454607554, 0.8503678039107081, 0.9999562104148801, 0.9976212508719051, 0.9076785617847604, 0.9998664629638465, 0.9933361726718317, 0.9996477648524436, 0.9831896901536233, 0.21017430866823344, 0.9820898507876897, 0.07262384687634141, 0.9891261290313083, 0.9999922507288591, 0.00035036028322789293, 2.0970316930566895e-05, 0.0015991355410829922, 0.2129844354785177, 0.00029277866190834513, 6.657445662268781e-07, 0.005612188187578665, 0.9981462838172903, 0.9715194134416082, 0.46342359575697634, 0.010448334369318956, 0.999998768658321, 0.8173837837591991, 0.9999501674988636, 0.9167543548127375, 0.22870848954693865, 0.999933221740816, 0.9989419423017882, 0.20189201575832774, 0.9900947004248996, 0.23245994824423594, 0.9994644787978381, 0.8888021247365532, 0.9995790129521703, 0.880821254488942, 0.997795700340634, 4.353999985734961e-05, 0.9961623812341762, 0.9760116389632439, 0.8816677297799299, 0.43697024235404386, 0.999995939862895, 0.8985179189414035, 0.9956997726762488, 0.004321092553056329, 0.9747002827499002, 0.9987034869856772, 0.9999944231859065, 0.9999999675911339, 0.9999999979224592, 0.9997841543959323, 0.9999924411790989, 0.016775938591383467, 0.7275041165749724, 0.999787169681863, 0.9999981788568907, 0.997225320325773, 0.9784668417735167, 0.9999835031921651, 4.045497186190069e-05, 0.9999999452845375, 0.06904318230189262, 0.014942035410586637, 0.16068414875239112, 0.998785576870432, 0.9999254805921546, 0.9399769869259014, 0.9695726140119306, 0.005504007950741592, 0.9653034047402911, 0.9930632190882794, 0.9999999999999705, 0.40977769894321747, 0.06551091842571882, 0.9998320872905644, 0.8023245375175535, 0.9997861205036056, 0.9999999915312364, 0.9999857981113901, 0.9858374317649633, 0.16158872731935775, 0.8356315085060156, 0.9942315010107746, 0.9947847961896016, 9.763038538214618e-06, 0.0006933146448927116, 0.38775728014377403, 0.9999604936453232, 0.9919609603870697, 0.9905711981177718, 0.08127679484321901, 0.9941240175021372, 0.9999395573053402, 0.8476349402512954, 0.8828690055101844, 0.994406641512198, 0.9999934252449618, 0.9832084858279138, 0.9997686582525825, 0.978026476758907, 0.9711940530688347, 0.9991812006184584, 0.9999514112486844, 0.9959103753252847, 0.3345732777279822, 0.9993440945117827, 0.9999627618538502, 0.9999982821897343, 0.9999999796266679, 0.9900999857990119, 0.9999048638263266, 0.018824135703769923, 0.40839037718277066, 0.9998682116823078, 0.043007700688385095, 0.9998907971573001, 0.7847990453160936, 0.9999904761796944, 0.9990378313086766, 0.9985055458403652, 0.49426619835486163, 0.151096359469183, 0.9851401064229459, 0.5722217194015395, 0.9945421723327024, 0.9993642138900379, 0.0013068765213725725, 0.886042081088034, 0.9675276679513413, 0.4180210160313504, 0.999907561797725, 0.00039229733433508805, 0.9906684311834776, 0.9997901648939064, 0.511278391236851, 0.9995032302180009, 0.999999982213113, 0.9999865076910324, 0.9999999716323177, 0.9999913270116025, 0.5348902139403504, 0.9997847093642243, 0.9999950507932022, 0.9392368592857608, 0.9999180182862528, 0.9992780555666531, 0.9999983659493408, 0.9999995670801471, 0.6606133510972869, 0.9999971132958276, 0.9999999968389668, 0.2809367010440904, 0.0016764013472284523, 0.9999151611121067, 0.9998951983460346, 0.9999969931040527, 0.999818349495596, 0.9980388526299645, 0.8789913946159099, 0.966251649356728, 0.9941773227300346, 0.9999889919543132, 0.9881212830947986, 0.9999988998188556, 0.9981817196481501, 0.8386102543294525, 0.9999057128414847, 0.996389420438628, 0.939601078783674, 0.999928006124328, 0.9999993069191305, 0.01953015619051514, 0.9949230459246303, 0.7184716549360279, 0.9982463738974879, 0.9993103523939527, 1.0, 0.009761400860940182, 0.9999995965514816, 0.028609141588959736, 0.9911120827720663, 0.9999937637083138, 0.17095725258590252, 0.7957761409516064, 0.18359177678589764, 0.9883988164299108, 0.999999554177968, 0.782696299352562, 0.9999430350975342, 0.9999922381656979, 0.9017103869627043, 0.9988238463435237, 0.9999973830844346, 0.9999995550551878, 0.9999318070082224, 0.9211442200803962, 0.997920522678056, 0.9999993034133815, 0.9999781291932117, 0.04044936737133949, 0.6011953701324873, 0.999987291966165, 0.997097496522469, 0.9637905572496847, 0.07451833390165, 0.7596298236111838, 0.9996428971753527, 0.9999408653646498, 0.03447334001178024, 0.9946566448533201, 0.04043501120583432, 0.987224748819737, 0.9865557551721243, 0.9971852218964948, 0.08284691781934325, 0.9861220059978799, 0.5646200662182236, 0.9955328428227076, 0.06324142554482408, 0.9987138559712446, 0.9993464357488719, 0.9300803140949191, 0.8817755969621047, 0.00421257139845281, 0.964334735373947, 0.9865448958159438, 0.9999905842445636, 0.9946068554405494, 0.9585713104137722, 0.04550526476909988, 0.9645819310986358, 0.9995540577258156, 0.99872600446586, 0.9814544116907896, 0.027497528511286343, 0.7211081739436315, 0.7814500899490049, 0.7889256544202511, 0.6340354308633432, 0.11964235352742424, 0.8008445465734544, 0.25333473436555887, 0.9889957711237611, 0.998045527556485, 0.8216180310428571, 0.9712454936668221, 0.6176927227977739, 0.6938300059653079, 0.9800173546474918, 0.012710358376123363, 0.00629052013460816, 0.989668889272633, 0.9990200899472582, 0.024226194254158912, 0.9975480382362741, 0.8684210888383919, 0.9991181717494408, 0.9231088943572833, 0.9996175225042375, 0.9994980735044449, 0.9188950761752559, 0.20361681861686656, 0.9712196733848625, 0.9381950974059932, 0.2897015425092279, 0.8846801739429161, 0.24271143564999423, 0.3984279785583622, 0.9884459049279073, 0.972528552658502, 0.41749564718915505, 0.9328589812157442, 0.43628962059088144, 0.9645953849123614, 0.9999956749812916, 0.018751533539019847, 0.7305934959334707, 0.9642573015742258, 0.9793204340324252, 0.9228660296305803, 0.9982800607403629, 0.9917127406744122, 0.6184222247695368, 0.951452868876286, 0.45164377721670057, 0.9994603571490326, 0.9999993409856043, 0.0646848653399478, 0.9999999424077943, 0.9977329254227596, 0.9416324151178521, 0.36841584136671257, 0.7537579147375113, 0.9793616339259233, 0.9894161535078916, 0.870761267497177, 0.6553658014053375, 0.9999065960585992, 0.9609611854367182, 0.19815921643299989, 0.1089344184187363, 0.9999991798102271, 0.3206020995444893, 0.9978562095268242, 0.6647882588616373, 0.9990018370250636, 0.9999049737293633, 0.00036523693261623723, 0.8870516209386885, 0.8753664566381434, 0.9999997305034305, 4.841162514223288e-05, 0.9999843447782027, 0.5223360442381471, 0.999176382158852, 0.998265509567491, 0.9976243846088371, 0.5959669620296564, 0.9999873254628353, 0.9999960747049627, 0.8974228232482575, 0.9675779528530711, 0.9807277354402788, 0.16628880762723755, 0.0006812662881129013, 0.9956055544990147, 0.9993531438637412, 0.9998338000829996, 0.9397147263504225, 0.9314472087598508, 0.8281809081483593, 0.7889690897983804, 0.2826969330999087, 0.9378025899270849, 0.6004297056504265, 0.8473817773939777, 0.7603502823476885, 0.9996998151470241, 0.43085101796882624, 0.7662491815159792, 0.7122252190359188, 0.9982597635785878, 0.3307723423786726, 0.9995718797376523, 0.9997602778974167, 0.8566917381552558, 0.9995111479725842, 0.9947523929402536, 0.5203556034467601, 0.016607994781698145, 0.8316756891647192, 0.007754089405212404, 0.9955615822430677, 0.9818151941529563, 0.019534640566294392, 0.7334562378361811, 0.9997270360091288, 0.5829411830320814, 0.0042199950994228136, 0.9905496144634278, 0.8511598837250511, 0.9458155887313457, 0.9998439464480943, 0.9589005738122873, 0.9470472257545862, 0.9994128625228816, 0.5480947074716085, 0.20579296324787968, 0.7711418178252016, 0.5503446918179393, 0.018367502187616767, 0.974712916034712, 0.8222453515493002, 0.9956004650232315, 0.9969168293874326, 0.9999753454701039, 0.9972402645183887, 0.8030963390828809, 0.9971401323026174, 0.999008723860218, 0.3632186392660961, 0.9995861718852533, 0.999957151738017, 0.49590267531932525, 0.987768051859392, 0.8717442164146386, 0.9537153783348733, 0.7393940773566384, 0.2820125135110305, 0.9999594204633235, 0.0029904246972482285, 0.9999814910800535, 0.8415519631050609, 0.1430429163305924, 0.005407547406433387, 0.9957761176954935, 0.00476897554093017, 0.8524177665308876, 0.30341524538214837, 0.015344614079782801, 0.22131642494979137, 0.7607656375882402, 0.9872795796638204, 0.5881461704410064, 0.9837210164708743, 3.7261148729101315e-05, 0.031139489625485378, 0.06694742985045771, 0.9987636210373321, 0.7128776462277844, 0.9999999930207437, 0.9896841712788943, 0.9725132738814077, 0.027136714529401296, 0.07757753886037633, 0.9998071850700303, 0.9432766651029525, 0.9998418818408108, 0.9984507648979088, 0.8774928748256318, 0.051787789815471316, 0.024690271885950823, 0.2988910079163318, 0.9992680856607933, 0.9216924761235349, 0.9481461276212386, 0.7971665845693976, 0.46509984917375474, 0.9594016776690037, 0.006132990286098955, 0.22126968501497107, 0.9965814844195162, 0.761783831918038, 0.9997943934834722, 0.8059791140755044, 0.9992917404657904, 0.9879871118192187, 0.006638716780873334, 0.8805133579157381, 0.11882389515507338, 0.7905369999375154, 0.9955653062480837, 0.9736104394857543, 0.9999693393222735, 0.012972046570485144, 0.10915887080992441, 0.7130764382854207, 0.9988065763257211, 0.9989294713649814, 0.9989970203039549, 0.9999362455055173, 0.9997918845455777, 0.24605734080384137, 0.9621536483546049, 0.9996216641861726, 0.19312627763219728, 0.2218275915455069, 0.9945698563426836, 0.032652933211186154, 0.9586852522658187, 0.9702031940101776, 0.29947295008848457, 0.22793071422521158, 0.9985014045001797, 0.006879609500020477, 0.00017237084688791432, 0.1041524365475114, 0.6942965366462712, 0.07357615098594662, 0.6570878488739534, 0.8492157032051038, 0.9998069977664449, 0.6999114011132768, 0.0016041916550671932, 0.13087711240016825, 0.9992318541097038, 0.9988109723375032, 0.04180196225724767, 0.6529418245671404, 0.16078186418461313, 0.006692936444613116, 0.2606878487847898, 0.6037414656728172, 0.9924381324180569, 0.4452764703347048, 0.9999779191909679, 0.517239342877869, 0.9166540027386584, 0.005536995027635924, 0.7629606822750074, 0.9144886022040508, 0.3648625338365611, 0.7293692400716386, 0.9877714873748717, 0.9248654596480272, 0.8784990464731389, 0.7757652565556198, 0.4554269226441279, 0.3748164552237995, 0.9933795070180429, 0.9559778797335194, 0.9391740842590117, 0.9913088929837504, 0.43668706257697165, 0.9391787545961959, 0.9882798273245652, 0.2818067497004453, 0.9468912232220457, 0.8612962932495655, 0.5316733496893012, 0.95307457095747, 0.08125239118941173, 0.997456114041816, 0.994686108115957, 0.9834509971915155, 0.10721279054078943, 0.9488178526756664, 0.3376337067407238, 0.9499202894684441, 0.9252365665171383, 0.9998068621959061, 0.8355897086339745, 0.9994233265929173, 0.4276773066987554, 0.3082522279997463, 0.12184209403109118, 0.9945103388278206, 0.06393332196782532, 0.9880266962333716, 0.9979870070741316, 0.9953743792791899, 0.01265444534189075, 0.9742629885376936, 0.6205147262803006, 0.03303591384825534, 0.9708199019154112, 0.9288184186530588, 0.17484223101109825, 0.01984324802868392, 0.0013746634626417118, 0.9906349286582706, 0.9757071471714431, 0.9758886857066675, 0.646723007204463, 0.9971340590466481, 0.0056264994511832055, 0.7275080450159769, 0.999917701769364, 0.9999868838276079, 0.9941447971076137, 0.999153962475314, 0.6261633664745371, 0.9994355356598734, 0.9999909636865169, 0.9920172507941176, 0.5255914806670197, 0.7292748905713329, 0.0501417833607814, 0.9994478301819942, 0.9648004439619196, 0.44565521649828627, 0.9999852630881848, 0.9193928405897211, 0.20053343840537577, 0.9990806192946191, 0.9433317547476451, 0.9955031153176009, 0.6084532725208123, 0.8569461790597975, 0.9920663999849548, 0.26153582917397084, 0.9454583942284499, 0.6974719221485762, 0.7815203111340581, 0.00033546834674340944, 0.9972773273747814, 0.4375389748201942, 0.9828149901700953, 0.6618173629517307, 0.9115728072324529, 0.9063436601850062, 0.0038374864294533164, 0.1476626528923209, 0.9893916139296998, 0.9117020542017452, 0.9978584648473078, 0.9473307377732733, 0.9992784063359964, 0.9489495220098751, 0.03577024348767787, 0.8724305218573619, 0.9996094592520289, 0.927080178477067, 0.22928450084802726, 0.9980111615108108, 0.937558806410098, 0.9467814376447156, 0.9947743395607269, 0.010536518027310152, 0.9797617833844041, 0.7006502848601645, 0.5665640397823111, 0.9592365519191753, 0.14890558824644437, 0.7715426524284198, 0.9995042559285964, 0.9345485871357195, 0.5921156101533933, 0.9713838587028597, 0.9979136632867311, 0.9838733128885, 0.6228705128397454, 0.052457616483952994, 0.9915893099659503, 0.9621966701942063, 0.9469362524508351, 0.9289968997967571, 0.0097906192865745, 0.9899497794858161, 0.024740142477302836, 0.6836090966874412, 0.9378923405323268, 0.9294272704845513, 0.00012800984717445412, 0.9955506207518953, 0.31614614141937425, 0.6178930256850207, 0.5048545151329632, 0.833605287583363, 0.4253427904834242, 0.0401790502369923, 0.2494283984293694, 0.9983631513883999, 0.050173732143778786, 0.9997009486416072, 0.0006498169347316894, 0.9969087005155184, 0.09030051040669655, 0.004850481573174394, 0.7219217919475747, 0.9953420897152889, 0.4874799547583198, 0.768774928665923, 0.0005771769553102382, 0.9623882074337273, 0.7977961550089839, 0.9602615900746325, 0.9076644119336786, 0.035231443314700156, 0.7197066638217764, 5.2082215172845294e-05, 0.9561243050091172, 0.02199464755441595, 0.7254340893318489, 0.03447334001178024, 0.12048579302112146, 0.013031078260168643, 0.9928982109969096, 0.9869633747092946, 0.9116330921186913, 0.999892057783118, 0.07599558965648333, 0.9967342749466345, 0.7005109683154367, 0.9830736530921373, 0.08735111241438552, 0.11683052459830362, 0.003383000805108666, 0.7284035296729092, 0.0017547320518206588, 0.03276589416632946, 0.15157886018875308, 0.7770165144514443, 0.08441706510853726, 0.8704261353707292, 0.2053890166742098, 0.0022760263145370006, 0.5481273616145801, 0.026106099384911798, 0.999511465082448, 0.0720328082986933, 0.0006286195508635137, 0.9970565252206627, 0.8066667104209392, 0.9320546595559114, 0.9687070085950864, 0.5994408932849342, 0.8145096241186004, 0.9983677154723452, 0.0001742018110544127, 0.8172218972439912, 0.9977837682535116, 0.0019578825198547783, 0.10272412561083724, 0.9912960446268935, 0.9975826609795189, 0.9684359155434549, 0.9899481918910172, 0.021520846704121358, 0.9804933032305658, 0.9935653142540946, 0.9998896866277038, 0.9988838348167803, 0.9884068726754134, 0.05116173969398701, 0.006351761861556648, 0.034719290727796275, 0.33634938559379335, 0.10114239293444441, 0.6850758009266866, 9.51544714125212e-05, 0.3795012796045776, 0.9980784672297144, 0.9962766345914384, 0.8945836801916053, 0.08442903779978883, 0.743697490817494, 0.7878256421972429, 0.03032063343405114, 0.7617240334073854, 4.2147329569867275e-05, 0.8589707839205617, 0.05189159962640556, 0.8415959720432398, 0.9964795286907259, 0.3644491709176964, 0.035202298698991545, 0.845424765635291, 0.9996041837720798, 0.010889836710266637, 0.05263011866159948, 0.9999275632042007, 0.0029220233909724082, 0.9725572423634726, 0.9959851480181092, 0.9848261312997805, 0.0668300414358067, 0.9898338303766433, 0.4336649050754484, 0.9791643575487741, 0.9985884976840635, 0.17763928055327857, 0.7361935321564181, 0.8376178891762547, 0.09616081461742078, 0.819507833971863, 0.9827853064669775, 0.0025881001295752423, 0.9591703920456461, 4.0932618334486234e-08, 0.9942425207084009, 0.9858110732772413, 0.00851616072805993, 0.9370028115356944, 0.9722092122965343, 0.8315241302589402, 0.977204727026139, 0.8914752747262867, 0.451082395676227, 0.2174133644858964, 0.9999957531259256, 0.30776175945532847, 0.5911845091032504, 0.3919656575194459, 0.13379618101880056, 0.9983431307931472, 0.5620741780041012, 0.11310998183064784, 0.7737259926632705, 0.000588730157143595, 0.0586232256516916, 0.3289507069757731, 0.03721174820583677, 0.0005322934269712574, 0.03984370251205301, 0.9895347712302981, 0.9010572080275633, 0.9998980658801258, 0.8790210938620836, 0.9997071284151792, 0.9696861248653408, 0.9913339357224252, 0.893205030541341, 0.9148864793458843, 0.9963731679826549, 0.014493115836893007, 0.9341990222165156, 0.8351464188099924, 0.23470195049711193, 0.9593752653209243, 0.7660568260450749, 0.9999974810164255, 0.7613213939415805, 0.9965892503124072, 0.918826854061552, 0.6003789916977668, 0.03269943193947217, 0.9999503599261628, 0.9957733346296921, 0.9996107820409219, 0.2370494752293438, 0.9926286673809748, 0.0008506981218303368, 0.509199739185968, 0.13774330555733075, 0.9806665710482191, 0.6817451753179389, 0.17364016225942694, 0.5940705196182049, 0.9246604551503617, 0.9953720469341141, 2.3297199371566213e-05, 0.9999701116826326, 0.9131292598568118, 0.03686593289164335, 0.9588437623800136, 0.15435602316489952, 0.500397510294501, 0.9999999999999607, 0.878208201823617, 0.6293977093049807, 0.9758841337256625, 0.3420302554346952, 0.0008842663126279657, 0.6147986576792736, 0.9468736913942322, 0.2569870212272361, 0.9998666099739747, 0.9935012950816035, 0.9546366837619692, 0.9982737977454279, 0.9995799845982769, 0.9395058152585557, 0.04806558087156772, 0.935017945628509, 0.9589022223165616, 0.006685113708429137, 0.007038518736387066, 0.7154419196032924, 0.9971559117842156, 0.9999565425907412, 0.8616696690672917, 0.9567769350234812, 0.20358140735598101, 0.11620368377865983, 0.0013777129292118166, 0.0386935403330704, 0.9991531667847785, 0.9881398710503404, 0.15506420298009013, 0.38354459453585177, 0.0007811955469021744, 0.882258698106048, 0.010917424681773716, 0.2832726547181889, 0.9716486962564695, 0.5052980815410881, 0.6171949935175303, 0.2854574757098589, 0.07802523080129965, 0.999994201531315, 0.15070466909804514, 1.3973779059502204e-06, 0.9950334066643411, 6.506144264035095e-05, 0.9993138431180822, 0.8287485488846419, 0.9999905632876182, 0.15252852317722757, 0.5290222709960047, 0.31373175706572365, 2.931494489896918e-05, 0.5977036245655891, 0.9837695533021292, 0.933484452841308, 0.9998267096612887, 0.9700618768677242, 0.17063227040154047, 0.42781394567571107, 0.6230027134061008, 3.8851156777385844e-05, 0.9993299069045664, 0.764807097487193, 0.018527907385479367, 0.000789488812952331, 1.4403667714286413e-05, 0.15621073989730694, 0.0037829960167122946, 0.46412607626250096, 0.9717035187268458, 0.999866670791796, 0.9898993362658769, 0.8573107665900636, 0.0003039800399554253, 0.0005279647610377224, 0.05436350083287051, 0.0007621212485432725, 0.4789474350883307, 1.53292253111107e-05, 0.08843390536991845, 0.9968565813649074, 0.2831694413606011, 0.968857301705862, 0.01303913609100301, 0.9870487269431475, 4.433177642620442e-06, 0.2915693760617862, 0.23475321426731507, 0.28621952024545794, 0.029933126696219982, 0.0075825214534508655, 0.003373586834854499, 0.0002729800832742568, 0.12153843167574789, 0.9907098067229861, 0.9928386813308748, 0.9760809032090699, 0.5191367017586473, 1.0290679954629735e-06, 0.15810316485968917, 0.9778548412785238, 0.24140027980006248, 0.4716207902433104, 0.1929925753717392, 0.0032642745087789245, 2.5554457592628625e-06, 0.00664448317482256, 0.006703446108275774, 0.2452017133407146, 0.008711216257395817, 0.0003501867946799679, 0.453000191743024, 0.003944773134538896, 0.8364612607023582, 0.003815779596456078, 0.013138651827870855, 0.6098739092359745, 0.192504949433128, 0.06122226660035848, 0.027804470309433674, 0.0005606981725862155, 2.7279463898850477e-05, 0.48466888804238295, 0.016257360383900667, 2.2532420018589618e-05, 0.7972551003215561, 0.06966112923729151, 1.5057457211091817e-05, 0.5584789847212602, 0.6214922383683241, 0.9980151056315827, 0.30362020144402846, 0.4976047706294101, 0.216735261416347, 0.04207603757723877, 0.009058889070041222, 0.6899476236962722, 0.0001812602013346919, 0.7161083730987792, 0.0008349448308828289, 0.06478800936276902, 0.8295686934171773, 0.39687889806355814, 0.7954128657503898, 0.5878853720426553, 0.02789818988004224, 0.016493917650433156, 0.010733820528487124, 0.8399130977496531, 0.9962400623324433, 0.9723731130561389, 0.008661587146812512, 0.01643007029017922, 0.000861279359036797, 0.5702315665497232, 0.9977682895601238, 0.9975351431958002, 0.2466507207848994, 1.4371675197642357e-08, 0.296658178462667, 0.0004704277976605054, 0.9880826903793509, 0.978243270145898, 0.36997028573523116, 0.9991654534413122, 0.0015132885256645108, 0.013139106079770198, 8.606633524394323e-05, 0.3704369969817706, 0.01626019038133562, 0.001041676968036162, 0.0006045240266896727, 0.8451377585493324, 0.9957235238248591, 0.006621315024794052, 0.9577997221310008, 0.0013307063982898443, 0.9893553379632691, 0.9903725725555274, 4.9712299185075404e-05, 0.057926186246713224, 0.4708626876519683, 0.36405712687229946, 2.0707883035248353e-05, 0.27588846523898775, 0.0016285407846347076, 0.0012166280203183954, 0.0011578846807579848, 2.730565531744606e-07, 4.599189868731026e-11, 0.5812985842258306, 0.035142744435299154, 0.6866898898279536, 0.11074190320868271, 0.9532864609077805, 1.693084929566567e-05, 0.003961266839249718, 3.160793846660828e-05, 0.0174684249518451, 0.0006199444109826377, 1.719649581576276e-05, 0.9017817528570332, 0.0002325237349435088, 0.022377454357082507, 0.20585695042182584, 0.19621043638130625, 0.053555079210322466, 0.6284331049914613, 0.9335792679928971, 0.5474561537356462, 0.6425572095204908, 3.8691382310978925e-07, 0.9956682928222493, 0.9999613044393777, 0.010049885662886546, 0.0006801173403733474, 0.05321736354615086, 0.03400987904213604, 0.043375145870496665, 0.07394078110278068, 0.25296606267745303, 3.2340185290751272e-06, 0.09080848418521291, 1.8576839012004732e-06, 0.36511880559173426, 0.00053784049792857, 0.9999666025070368, 0.00011322814730898454, 0.18195187003058377, 0.999154854972635, 0.9753830257149079, 0.6741800482420005, 0.011177960344768378, 0.47964010349762276, 0.00014080391572969032, 1.3349278264706335e-05, 0.10313517671217051, 0.00215857059233106, 0.9831240622023814, 0.06334852017194174, 0.9990434175180755, 0.1630173176172731, 0.0007168650323008853, 0.9751105935117841, 0.008279319077522208, 0.004284139907384779, 0.6307358116588251, 0.0007808462806137278, 0.006979746842742873, 0.024400897539990713, 0.003542137317273152, 0.00010325641086025054, 0.9973</t>
         </is>
       </c>
     </row>

</xml_diff>